<commit_message>
Latest data: Sat Dec 23 21:10:32 UTC 2023
</commit_message>
<xml_diff>
--- a/docs/particelle_non_trovate.xlsx
+++ b/docs/particelle_non_trovate.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Latest data: Thu Dec 28 20:09:46 UTC 2023
</commit_message>
<xml_diff>
--- a/docs/particelle_non_trovate.xlsx
+++ b/docs/particelle_non_trovate.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C283"/>
+  <dimension ref="A1:C257"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2921,7 +2921,7 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>.507/2</t>
+          <t>5582/2</t>
         </is>
       </c>
       <c r="C192" t="n">
@@ -2934,7 +2934,7 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>.507/3</t>
+          <t>9213/12</t>
         </is>
       </c>
       <c r="C193" t="n">
@@ -2947,11 +2947,11 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>.507/4</t>
+          <t>45</t>
         </is>
       </c>
       <c r="C194" t="n">
-        <v>413</v>
+        <v>283</v>
       </c>
     </row>
     <row r="195">
@@ -2960,11 +2960,11 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>507/5</t>
+          <t>84/1</t>
         </is>
       </c>
       <c r="C195" t="n">
-        <v>413</v>
+        <v>283</v>
       </c>
     </row>
     <row r="196">
@@ -2973,11 +2973,11 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>507/6</t>
+          <t>137</t>
         </is>
       </c>
       <c r="C196" t="n">
-        <v>413</v>
+        <v>41</v>
       </c>
     </row>
     <row r="197">
@@ -2986,11 +2986,11 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>569/8</t>
+          <t>140</t>
         </is>
       </c>
       <c r="C197" t="n">
-        <v>413</v>
+        <v>41</v>
       </c>
     </row>
     <row r="198">
@@ -2999,11 +2999,11 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>.569/5</t>
+          <t>272</t>
         </is>
       </c>
       <c r="C198" t="n">
-        <v>413</v>
+        <v>79</v>
       </c>
     </row>
     <row r="199">
@@ -3012,11 +3012,11 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>7294</t>
+          <t>1845</t>
         </is>
       </c>
       <c r="C199" t="n">
-        <v>413</v>
+        <v>79</v>
       </c>
     </row>
     <row r="200">
@@ -3025,11 +3025,11 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>7293/2</t>
+          <t>100</t>
         </is>
       </c>
       <c r="C200" t="n">
-        <v>413</v>
+        <v>79</v>
       </c>
     </row>
     <row r="201">
@@ -3038,11 +3038,11 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>7293/3</t>
+          <t>1390</t>
         </is>
       </c>
       <c r="C201" t="n">
-        <v>413</v>
+        <v>79</v>
       </c>
     </row>
     <row r="202">
@@ -3051,11 +3051,11 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>7292/1</t>
+          <t>94/6</t>
         </is>
       </c>
       <c r="C202" t="n">
-        <v>413</v>
+        <v>251</v>
       </c>
     </row>
     <row r="203">
@@ -3064,11 +3064,11 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>7191/4</t>
+          <t>243</t>
         </is>
       </c>
       <c r="C203" t="n">
-        <v>413</v>
+        <v>253</v>
       </c>
     </row>
     <row r="204">
@@ -3077,11 +3077,11 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>.1270</t>
+          <t>295</t>
         </is>
       </c>
       <c r="C204" t="n">
-        <v>413</v>
+        <v>253</v>
       </c>
     </row>
     <row r="205">
@@ -3090,11 +3090,11 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>7618/3</t>
+          <t>1403</t>
         </is>
       </c>
       <c r="C205" t="n">
-        <v>413</v>
+        <v>268</v>
       </c>
     </row>
     <row r="206">
@@ -3103,11 +3103,11 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>7618/4</t>
+          <t>1444</t>
         </is>
       </c>
       <c r="C206" t="n">
-        <v>413</v>
+        <v>268</v>
       </c>
     </row>
     <row r="207">
@@ -3116,11 +3116,11 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>361</t>
+          <t>1605</t>
         </is>
       </c>
       <c r="C207" t="n">
-        <v>413</v>
+        <v>268</v>
       </c>
     </row>
     <row r="208">
@@ -3129,11 +3129,11 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>421</t>
+          <t>1823</t>
         </is>
       </c>
       <c r="C208" t="n">
-        <v>413</v>
+        <v>268</v>
       </c>
     </row>
     <row r="209">
@@ -3142,11 +3142,11 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>13094</t>
+          <t>1824</t>
         </is>
       </c>
       <c r="C209" t="n">
-        <v>413</v>
+        <v>268</v>
       </c>
     </row>
     <row r="210">
@@ -3155,11 +3155,11 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>7290/6</t>
+          <t>316</t>
         </is>
       </c>
       <c r="C210" t="n">
-        <v>413</v>
+        <v>442</v>
       </c>
     </row>
     <row r="211">
@@ -3168,11 +3168,11 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>7288</t>
+          <t>53</t>
         </is>
       </c>
       <c r="C211" t="n">
-        <v>413</v>
+        <v>215</v>
       </c>
     </row>
     <row r="212">
@@ -3181,11 +3181,11 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>.343/18</t>
+          <t>454</t>
         </is>
       </c>
       <c r="C212" t="n">
-        <v>404</v>
+        <v>215</v>
       </c>
     </row>
     <row r="213">
@@ -3194,11 +3194,11 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>4523</t>
+          <t>420/80</t>
         </is>
       </c>
       <c r="C213" t="n">
-        <v>404</v>
+        <v>215</v>
       </c>
     </row>
     <row r="214">
@@ -3207,11 +3207,11 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>11766/2</t>
+          <t>420/92</t>
         </is>
       </c>
       <c r="C214" t="n">
-        <v>413</v>
+        <v>215</v>
       </c>
     </row>
     <row r="215">
@@ -3220,11 +3220,11 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>12207</t>
+          <t>420/93</t>
         </is>
       </c>
       <c r="C215" t="n">
-        <v>413</v>
+        <v>215</v>
       </c>
     </row>
     <row r="216">
@@ -3233,11 +3233,11 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>12231</t>
+          <t>420/94</t>
         </is>
       </c>
       <c r="C216" t="n">
-        <v>413</v>
+        <v>215</v>
       </c>
     </row>
     <row r="217">
@@ -3246,11 +3246,11 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>5441</t>
+          <t>420/95</t>
         </is>
       </c>
       <c r="C217" t="n">
-        <v>413</v>
+        <v>215</v>
       </c>
     </row>
     <row r="218">
@@ -3259,11 +3259,11 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>4877</t>
+          <t>420/96</t>
         </is>
       </c>
       <c r="C218" t="n">
-        <v>413</v>
+        <v>215</v>
       </c>
     </row>
     <row r="219">
@@ -3272,11 +3272,11 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>5544</t>
+          <t>420/97</t>
         </is>
       </c>
       <c r="C219" t="n">
-        <v>413</v>
+        <v>215</v>
       </c>
     </row>
     <row r="220">
@@ -3285,11 +3285,11 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>420/101</t>
         </is>
       </c>
       <c r="C220" t="n">
-        <v>283</v>
+        <v>215</v>
       </c>
     </row>
     <row r="221">
@@ -3298,11 +3298,11 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>84/1</t>
+          <t>420/102</t>
         </is>
       </c>
       <c r="C221" t="n">
-        <v>283</v>
+        <v>215</v>
       </c>
     </row>
     <row r="222">
@@ -3311,11 +3311,11 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>137</t>
+          <t>420/106</t>
         </is>
       </c>
       <c r="C222" t="n">
-        <v>41</v>
+        <v>215</v>
       </c>
     </row>
     <row r="223">
@@ -3324,11 +3324,11 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>140</t>
+          <t>420/107</t>
         </is>
       </c>
       <c r="C223" t="n">
-        <v>41</v>
+        <v>215</v>
       </c>
     </row>
     <row r="224">
@@ -3337,11 +3337,11 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>272</t>
+          <t>420/109</t>
         </is>
       </c>
       <c r="C224" t="n">
-        <v>79</v>
+        <v>215</v>
       </c>
     </row>
     <row r="225">
@@ -3350,11 +3350,11 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>1845</t>
+          <t>420/110</t>
         </is>
       </c>
       <c r="C225" t="n">
-        <v>79</v>
+        <v>215</v>
       </c>
     </row>
     <row r="226">
@@ -3363,11 +3363,11 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>705/11</t>
         </is>
       </c>
       <c r="C226" t="n">
-        <v>79</v>
+        <v>215</v>
       </c>
     </row>
     <row r="227">
@@ -3376,11 +3376,11 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>1390</t>
+          <t>756</t>
         </is>
       </c>
       <c r="C227" t="n">
-        <v>79</v>
+        <v>215</v>
       </c>
     </row>
     <row r="228">
@@ -3389,11 +3389,11 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>94/6</t>
+          <t>798/3</t>
         </is>
       </c>
       <c r="C228" t="n">
-        <v>251</v>
+        <v>215</v>
       </c>
     </row>
     <row r="229">
@@ -3402,11 +3402,11 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>243</t>
+          <t>1411/1</t>
         </is>
       </c>
       <c r="C229" t="n">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
     <row r="230">
@@ -3415,11 +3415,11 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>295</t>
+          <t>1411/2</t>
         </is>
       </c>
       <c r="C230" t="n">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
     <row r="231">
@@ -3428,11 +3428,11 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>1403</t>
+          <t>1411/3</t>
         </is>
       </c>
       <c r="C231" t="n">
-        <v>268</v>
+        <v>256</v>
       </c>
     </row>
     <row r="232">
@@ -3441,11 +3441,11 @@
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>1444</t>
+          <t>1411/4</t>
         </is>
       </c>
       <c r="C232" t="n">
-        <v>268</v>
+        <v>256</v>
       </c>
     </row>
     <row r="233">
@@ -3454,11 +3454,11 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>1605</t>
+          <t>1411/5</t>
         </is>
       </c>
       <c r="C233" t="n">
-        <v>268</v>
+        <v>256</v>
       </c>
     </row>
     <row r="234">
@@ -3467,11 +3467,11 @@
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>1823</t>
+          <t>1412</t>
         </is>
       </c>
       <c r="C234" t="n">
-        <v>268</v>
+        <v>256</v>
       </c>
     </row>
     <row r="235">
@@ -3480,11 +3480,11 @@
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>1824</t>
+          <t>1488</t>
         </is>
       </c>
       <c r="C235" t="n">
-        <v>268</v>
+        <v>256</v>
       </c>
     </row>
     <row r="236">
@@ -3493,11 +3493,11 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>316</t>
+          <t>254/2</t>
         </is>
       </c>
       <c r="C236" t="n">
-        <v>442</v>
+        <v>193</v>
       </c>
     </row>
     <row r="237">
@@ -3506,11 +3506,11 @@
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>337/5</t>
         </is>
       </c>
       <c r="C237" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="238">
@@ -3519,11 +3519,11 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>454</t>
+          <t>393/1</t>
         </is>
       </c>
       <c r="C238" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="239">
@@ -3532,11 +3532,11 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>420/80</t>
+          <t>393/2</t>
         </is>
       </c>
       <c r="C239" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="240">
@@ -3545,11 +3545,11 @@
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>420/92</t>
+          <t>393/3</t>
         </is>
       </c>
       <c r="C240" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="241">
@@ -3558,11 +3558,11 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>420/93</t>
+          <t>465</t>
         </is>
       </c>
       <c r="C241" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="242">
@@ -3571,11 +3571,11 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>420/94</t>
+          <t>614</t>
         </is>
       </c>
       <c r="C242" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="243">
@@ -3584,11 +3584,11 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>420/95</t>
+          <t>1303/1</t>
         </is>
       </c>
       <c r="C243" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="244">
@@ -3597,11 +3597,11 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>420/96</t>
+          <t>1303/2</t>
         </is>
       </c>
       <c r="C244" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="245">
@@ -3610,11 +3610,11 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>420/97</t>
+          <t>1309</t>
         </is>
       </c>
       <c r="C245" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="246">
@@ -3623,11 +3623,11 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>420/101</t>
+          <t>1330</t>
         </is>
       </c>
       <c r="C246" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="247">
@@ -3636,11 +3636,11 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>420/102</t>
+          <t>1334</t>
         </is>
       </c>
       <c r="C247" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="248">
@@ -3649,11 +3649,11 @@
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>420/106</t>
+          <t>1346</t>
         </is>
       </c>
       <c r="C248" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="249">
@@ -3662,11 +3662,11 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>420/107</t>
+          <t>1369/1</t>
         </is>
       </c>
       <c r="C249" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="250">
@@ -3675,11 +3675,11 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>420/109</t>
+          <t>1117/2</t>
         </is>
       </c>
       <c r="C250" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="251">
@@ -3688,11 +3688,11 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>420/110</t>
+          <t>1230/85</t>
         </is>
       </c>
       <c r="C251" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="252">
@@ -3701,11 +3701,11 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>705/11</t>
+          <t>1230/86</t>
         </is>
       </c>
       <c r="C252" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="253">
@@ -3714,11 +3714,11 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>756</t>
+          <t>1230/87</t>
         </is>
       </c>
       <c r="C253" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="254">
@@ -3727,11 +3727,11 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>798/3</t>
+          <t>1230/88</t>
         </is>
       </c>
       <c r="C254" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="255">
@@ -3740,11 +3740,11 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>1411/1</t>
+          <t>1230/100</t>
         </is>
       </c>
       <c r="C255" t="n">
-        <v>256</v>
+        <v>193</v>
       </c>
     </row>
     <row r="256">
@@ -3753,11 +3753,11 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>1411/2</t>
+          <t>1230/115</t>
         </is>
       </c>
       <c r="C256" t="n">
-        <v>256</v>
+        <v>193</v>
       </c>
     </row>
     <row r="257">
@@ -3766,348 +3766,10 @@
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>1411/3</t>
+          <t>194/4</t>
         </is>
       </c>
       <c r="C257" t="n">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="258">
-      <c r="A258" s="1" t="n">
-        <v>256</v>
-      </c>
-      <c r="B258" t="inlineStr">
-        <is>
-          <t>1411/4</t>
-        </is>
-      </c>
-      <c r="C258" t="n">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="259">
-      <c r="A259" s="1" t="n">
-        <v>257</v>
-      </c>
-      <c r="B259" t="inlineStr">
-        <is>
-          <t>1411/5</t>
-        </is>
-      </c>
-      <c r="C259" t="n">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="260">
-      <c r="A260" s="1" t="n">
-        <v>258</v>
-      </c>
-      <c r="B260" t="inlineStr">
-        <is>
-          <t>1412</t>
-        </is>
-      </c>
-      <c r="C260" t="n">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="261">
-      <c r="A261" s="1" t="n">
-        <v>259</v>
-      </c>
-      <c r="B261" t="inlineStr">
-        <is>
-          <t>1488</t>
-        </is>
-      </c>
-      <c r="C261" t="n">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="262">
-      <c r="A262" s="1" t="n">
-        <v>260</v>
-      </c>
-      <c r="B262" t="inlineStr">
-        <is>
-          <t>254/2</t>
-        </is>
-      </c>
-      <c r="C262" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="263">
-      <c r="A263" s="1" t="n">
-        <v>261</v>
-      </c>
-      <c r="B263" t="inlineStr">
-        <is>
-          <t>337/5</t>
-        </is>
-      </c>
-      <c r="C263" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="264">
-      <c r="A264" s="1" t="n">
-        <v>262</v>
-      </c>
-      <c r="B264" t="inlineStr">
-        <is>
-          <t>393/1</t>
-        </is>
-      </c>
-      <c r="C264" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="265">
-      <c r="A265" s="1" t="n">
-        <v>263</v>
-      </c>
-      <c r="B265" t="inlineStr">
-        <is>
-          <t>393/2</t>
-        </is>
-      </c>
-      <c r="C265" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="266">
-      <c r="A266" s="1" t="n">
-        <v>264</v>
-      </c>
-      <c r="B266" t="inlineStr">
-        <is>
-          <t>393/3</t>
-        </is>
-      </c>
-      <c r="C266" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="267">
-      <c r="A267" s="1" t="n">
-        <v>265</v>
-      </c>
-      <c r="B267" t="inlineStr">
-        <is>
-          <t>465</t>
-        </is>
-      </c>
-      <c r="C267" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="268">
-      <c r="A268" s="1" t="n">
-        <v>266</v>
-      </c>
-      <c r="B268" t="inlineStr">
-        <is>
-          <t>614</t>
-        </is>
-      </c>
-      <c r="C268" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="269">
-      <c r="A269" s="1" t="n">
-        <v>267</v>
-      </c>
-      <c r="B269" t="inlineStr">
-        <is>
-          <t>1303/1</t>
-        </is>
-      </c>
-      <c r="C269" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="270">
-      <c r="A270" s="1" t="n">
-        <v>268</v>
-      </c>
-      <c r="B270" t="inlineStr">
-        <is>
-          <t>1303/2</t>
-        </is>
-      </c>
-      <c r="C270" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="271">
-      <c r="A271" s="1" t="n">
-        <v>269</v>
-      </c>
-      <c r="B271" t="inlineStr">
-        <is>
-          <t>1309</t>
-        </is>
-      </c>
-      <c r="C271" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="272">
-      <c r="A272" s="1" t="n">
-        <v>270</v>
-      </c>
-      <c r="B272" t="inlineStr">
-        <is>
-          <t>1330</t>
-        </is>
-      </c>
-      <c r="C272" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="273">
-      <c r="A273" s="1" t="n">
-        <v>271</v>
-      </c>
-      <c r="B273" t="inlineStr">
-        <is>
-          <t>1334</t>
-        </is>
-      </c>
-      <c r="C273" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="274">
-      <c r="A274" s="1" t="n">
-        <v>272</v>
-      </c>
-      <c r="B274" t="inlineStr">
-        <is>
-          <t>1346</t>
-        </is>
-      </c>
-      <c r="C274" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="275">
-      <c r="A275" s="1" t="n">
-        <v>273</v>
-      </c>
-      <c r="B275" t="inlineStr">
-        <is>
-          <t>1369/1</t>
-        </is>
-      </c>
-      <c r="C275" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="276">
-      <c r="A276" s="1" t="n">
-        <v>274</v>
-      </c>
-      <c r="B276" t="inlineStr">
-        <is>
-          <t>1117/2</t>
-        </is>
-      </c>
-      <c r="C276" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="277">
-      <c r="A277" s="1" t="n">
-        <v>275</v>
-      </c>
-      <c r="B277" t="inlineStr">
-        <is>
-          <t>1230/85</t>
-        </is>
-      </c>
-      <c r="C277" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="278">
-      <c r="A278" s="1" t="n">
-        <v>276</v>
-      </c>
-      <c r="B278" t="inlineStr">
-        <is>
-          <t>1230/86</t>
-        </is>
-      </c>
-      <c r="C278" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="279">
-      <c r="A279" s="1" t="n">
-        <v>277</v>
-      </c>
-      <c r="B279" t="inlineStr">
-        <is>
-          <t>1230/87</t>
-        </is>
-      </c>
-      <c r="C279" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="280">
-      <c r="A280" s="1" t="n">
-        <v>278</v>
-      </c>
-      <c r="B280" t="inlineStr">
-        <is>
-          <t>1230/88</t>
-        </is>
-      </c>
-      <c r="C280" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="281">
-      <c r="A281" s="1" t="n">
-        <v>279</v>
-      </c>
-      <c r="B281" t="inlineStr">
-        <is>
-          <t>1230/100</t>
-        </is>
-      </c>
-      <c r="C281" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="282">
-      <c r="A282" s="1" t="n">
-        <v>280</v>
-      </c>
-      <c r="B282" t="inlineStr">
-        <is>
-          <t>1230/115</t>
-        </is>
-      </c>
-      <c r="C282" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="283">
-      <c r="A283" s="1" t="n">
-        <v>281</v>
-      </c>
-      <c r="B283" t="inlineStr">
-        <is>
-          <t>194/4</t>
-        </is>
-      </c>
-      <c r="C283" t="n">
         <v>193</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Latest data: Tue Jan  9 16:12:43 UTC 2024
</commit_message>
<xml_diff>
--- a/docs/particelle_non_trovate.xlsx
+++ b/docs/particelle_non_trovate.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C257"/>
+  <dimension ref="A1:C222"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -867,11 +867,11 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>3566/2</t>
+          <t>2189</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35">
@@ -880,11 +880,11 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>3564/2</t>
+          <t>149</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="36">
@@ -893,11 +893,11 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>3564/8</t>
+          <t>1186</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37">
@@ -906,11 +906,11 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>3564/9</t>
+          <t>1220</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38">
@@ -919,11 +919,11 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>3564/10</t>
+          <t>1508</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39">
@@ -932,11 +932,11 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>3564/11</t>
+          <t>1806</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="40">
@@ -945,11 +945,11 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>3564/14</t>
+          <t>1865</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="41">
@@ -958,11 +958,11 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>3564/16</t>
+          <t>1866</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="42">
@@ -971,11 +971,11 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>3564/29</t>
+          <t>3073</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43">
@@ -984,11 +984,11 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>3564/30</t>
+          <t>3074</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="44">
@@ -997,11 +997,11 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>3586</t>
+          <t>3113</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="45">
@@ -1010,11 +1010,11 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>3581</t>
+          <t>141</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>12</v>
+        <v>56</v>
       </c>
     </row>
     <row r="46">
@@ -1023,11 +1023,11 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>3583</t>
+          <t>243</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>12</v>
+        <v>56</v>
       </c>
     </row>
     <row r="47">
@@ -1036,11 +1036,11 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>3591</t>
+          <t>246</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>12</v>
+        <v>56</v>
       </c>
     </row>
     <row r="48">
@@ -1049,11 +1049,11 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>2582</t>
+          <t>536</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>12</v>
+        <v>56</v>
       </c>
     </row>
     <row r="49">
@@ -1062,11 +1062,11 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>2612</t>
+          <t>3181/3</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>12</v>
+        <v>57</v>
       </c>
     </row>
     <row r="50">
@@ -1075,11 +1075,11 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>2528</t>
+          <t>3577</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="51">
@@ -1088,11 +1088,11 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>725/2</t>
+          <t>11008</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="52">
@@ -1101,11 +1101,11 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>1031</t>
+          <t>11029</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="53">
@@ -1114,11 +1114,11 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>1226</t>
+          <t>11846</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="54">
@@ -1127,11 +1127,11 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>3414</t>
+          <t>11861</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="55">
@@ -1140,11 +1140,11 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>3528</t>
+          <t>10564</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="56">
@@ -1153,11 +1153,11 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>3560</t>
+          <t>10563/14</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="57">
@@ -1166,11 +1166,11 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>3599</t>
+          <t>10563/15</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="58">
@@ -1179,11 +1179,11 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>3994</t>
+          <t>3535</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="59">
@@ -1192,11 +1192,11 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>3995</t>
+          <t>3570</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="60">
@@ -1205,11 +1205,11 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>157</t>
+          <t>2168</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="61">
@@ -1218,11 +1218,11 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>3007</t>
+          <t>2762</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="62">
@@ -1231,11 +1231,11 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>.771</t>
+          <t>11867</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="63">
@@ -1244,11 +1244,11 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>.777</t>
+          <t>5009</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>12</v>
+        <v>44</v>
       </c>
     </row>
     <row r="64">
@@ -1257,11 +1257,11 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>613/1</t>
+          <t>5010</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
     <row r="65">
@@ -1270,11 +1270,11 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>663</t>
+          <t>11025/1</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
     <row r="66">
@@ -1283,11 +1283,11 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>589</t>
+          <t>11025/2</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
     <row r="67">
@@ -1296,11 +1296,11 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>.135/2</t>
+          <t>11026/1</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
     <row r="68">
@@ -1309,11 +1309,11 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>.135/5</t>
+          <t>11260</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
     <row r="69">
@@ -1322,11 +1322,11 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>2189</t>
+          <t>13823</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>22</v>
+        <v>154</v>
       </c>
     </row>
     <row r="70">
@@ -1335,11 +1335,11 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>149</t>
+          <t>14724/2</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>22</v>
+        <v>154</v>
       </c>
     </row>
     <row r="71">
@@ -1348,11 +1348,11 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>1186</t>
+          <t>15380</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>22</v>
+        <v>154</v>
       </c>
     </row>
     <row r="72">
@@ -1361,11 +1361,11 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>1220</t>
+          <t>1847/1</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>22</v>
+        <v>154</v>
       </c>
     </row>
     <row r="73">
@@ -1374,11 +1374,11 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>1508</t>
+          <t>220/2</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>22</v>
+        <v>154</v>
       </c>
     </row>
     <row r="74">
@@ -1387,11 +1387,11 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>1806</t>
+          <t>8974/1</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>22</v>
+        <v>154</v>
       </c>
     </row>
     <row r="75">
@@ -1400,11 +1400,11 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>1865</t>
+          <t>8987/1</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>22</v>
+        <v>154</v>
       </c>
     </row>
     <row r="76">
@@ -1413,11 +1413,11 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>1866</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>22</v>
+        <v>174</v>
       </c>
     </row>
     <row r="77">
@@ -1426,11 +1426,11 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>3073</t>
+          <t>469</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>22</v>
+        <v>174</v>
       </c>
     </row>
     <row r="78">
@@ -1439,11 +1439,11 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>3074</t>
+          <t>562</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>22</v>
+        <v>174</v>
       </c>
     </row>
     <row r="79">
@@ -1452,11 +1452,11 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>3113</t>
+          <t>173</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>22</v>
+        <v>174</v>
       </c>
     </row>
     <row r="80">
@@ -1465,11 +1465,11 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>141</t>
+          <t>697</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>56</v>
+        <v>188</v>
       </c>
     </row>
     <row r="81">
@@ -1478,11 +1478,11 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>243</t>
+          <t>777</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>56</v>
+        <v>188</v>
       </c>
     </row>
     <row r="82">
@@ -1491,11 +1491,11 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>246</t>
+          <t>948</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>56</v>
+        <v>188</v>
       </c>
     </row>
     <row r="83">
@@ -1504,11 +1504,11 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>536</t>
+          <t>205</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>56</v>
+        <v>214</v>
       </c>
     </row>
     <row r="84">
@@ -1517,11 +1517,11 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>3181/3</t>
+          <t>206</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>57</v>
+        <v>214</v>
       </c>
     </row>
     <row r="85">
@@ -1530,11 +1530,11 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>3577</t>
+          <t>198</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>44</v>
+        <v>214</v>
       </c>
     </row>
     <row r="86">
@@ -1543,11 +1543,11 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>11008</t>
+          <t>253/3</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>44</v>
+        <v>153</v>
       </c>
     </row>
     <row r="87">
@@ -1556,11 +1556,11 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>11029</t>
+          <t>1094</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>44</v>
+        <v>266</v>
       </c>
     </row>
     <row r="88">
@@ -1569,11 +1569,11 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>11846</t>
+          <t>1096</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>44</v>
+        <v>266</v>
       </c>
     </row>
     <row r="89">
@@ -1582,11 +1582,11 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>11861</t>
+          <t>1097</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>44</v>
+        <v>266</v>
       </c>
     </row>
     <row r="90">
@@ -1595,11 +1595,11 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>10564</t>
+          <t>1150</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>44</v>
+        <v>266</v>
       </c>
     </row>
     <row r="91">
@@ -1608,11 +1608,11 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>10563/14</t>
+          <t>1183</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>44</v>
+        <v>266</v>
       </c>
     </row>
     <row r="92">
@@ -1621,11 +1621,11 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>10563/15</t>
+          <t>842</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>44</v>
+        <v>266</v>
       </c>
     </row>
     <row r="93">
@@ -1634,11 +1634,11 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>3535</t>
+          <t>587</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>44</v>
+        <v>213</v>
       </c>
     </row>
     <row r="94">
@@ -1647,11 +1647,11 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>3570</t>
+          <t>588</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>44</v>
+        <v>213</v>
       </c>
     </row>
     <row r="95">
@@ -1660,11 +1660,11 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>2168</t>
+          <t>51</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>44</v>
+        <v>213</v>
       </c>
     </row>
     <row r="96">
@@ -1673,11 +1673,11 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>2762</t>
+          <t>642/2</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>44</v>
+        <v>213</v>
       </c>
     </row>
     <row r="97">
@@ -1686,11 +1686,11 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>11867</t>
+          <t>116</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>44</v>
+        <v>213</v>
       </c>
     </row>
     <row r="98">
@@ -1699,11 +1699,11 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>5009</t>
+          <t>151</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>44</v>
+        <v>213</v>
       </c>
     </row>
     <row r="99">
@@ -1712,11 +1712,11 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>5010</t>
+          <t>466</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>44</v>
+        <v>213</v>
       </c>
     </row>
     <row r="100">
@@ -1725,11 +1725,11 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>11025/1</t>
+          <t>1479</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>44</v>
+        <v>265</v>
       </c>
     </row>
     <row r="101">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>11025/2</t>
+          <t>2243</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>44</v>
+        <v>265</v>
       </c>
     </row>
     <row r="102">
@@ -1751,11 +1751,11 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>11026/1</t>
+          <t>901</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>44</v>
+        <v>265</v>
       </c>
     </row>
     <row r="103">
@@ -1764,11 +1764,11 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>11260</t>
+          <t>842</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>44</v>
+        <v>265</v>
       </c>
     </row>
     <row r="104">
@@ -1777,11 +1777,11 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>13823</t>
+          <t>656</t>
         </is>
       </c>
       <c r="C104" t="n">
-        <v>154</v>
+        <v>245</v>
       </c>
     </row>
     <row r="105">
@@ -1790,11 +1790,11 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>14724/2</t>
+          <t>811</t>
         </is>
       </c>
       <c r="C105" t="n">
-        <v>154</v>
+        <v>245</v>
       </c>
     </row>
     <row r="106">
@@ -1803,11 +1803,11 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>15380</t>
+          <t>370</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>154</v>
+        <v>245</v>
       </c>
     </row>
     <row r="107">
@@ -1816,11 +1816,11 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>1847/1</t>
+          <t>537</t>
         </is>
       </c>
       <c r="C107" t="n">
-        <v>154</v>
+        <v>245</v>
       </c>
     </row>
     <row r="108">
@@ -1829,11 +1829,11 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>220/2</t>
+          <t>4812</t>
         </is>
       </c>
       <c r="C108" t="n">
-        <v>154</v>
+        <v>245</v>
       </c>
     </row>
     <row r="109">
@@ -1842,11 +1842,11 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>8974/1</t>
+          <t>5016</t>
         </is>
       </c>
       <c r="C109" t="n">
-        <v>154</v>
+        <v>245</v>
       </c>
     </row>
     <row r="110">
@@ -1855,11 +1855,11 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>8987/1</t>
+          <t>51</t>
         </is>
       </c>
       <c r="C110" t="n">
-        <v>154</v>
+        <v>245</v>
       </c>
     </row>
     <row r="111">
@@ -1868,11 +1868,11 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1858</t>
         </is>
       </c>
       <c r="C111" t="n">
-        <v>174</v>
+        <v>245</v>
       </c>
     </row>
     <row r="112">
@@ -1881,11 +1881,11 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>469</t>
+          <t>2421</t>
         </is>
       </c>
       <c r="C112" t="n">
-        <v>174</v>
+        <v>245</v>
       </c>
     </row>
     <row r="113">
@@ -1894,11 +1894,11 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>562</t>
+          <t>2436</t>
         </is>
       </c>
       <c r="C113" t="n">
-        <v>174</v>
+        <v>245</v>
       </c>
     </row>
     <row r="114">
@@ -1907,11 +1907,11 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>173</t>
+          <t>609</t>
         </is>
       </c>
       <c r="C114" t="n">
-        <v>174</v>
+        <v>414</v>
       </c>
     </row>
     <row r="115">
@@ -1920,11 +1920,11 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>697</t>
+          <t>912</t>
         </is>
       </c>
       <c r="C115" t="n">
-        <v>188</v>
+        <v>414</v>
       </c>
     </row>
     <row r="116">
@@ -1933,11 +1933,11 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>777</t>
+          <t>1419</t>
         </is>
       </c>
       <c r="C116" t="n">
-        <v>188</v>
+        <v>414</v>
       </c>
     </row>
     <row r="117">
@@ -1946,11 +1946,11 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>948</t>
+          <t>31</t>
         </is>
       </c>
       <c r="C117" t="n">
-        <v>188</v>
+        <v>282</v>
       </c>
     </row>
     <row r="118">
@@ -1959,11 +1959,11 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>205</t>
+          <t>722</t>
         </is>
       </c>
       <c r="C118" t="n">
-        <v>214</v>
+        <v>282</v>
       </c>
     </row>
     <row r="119">
@@ -1972,11 +1972,11 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>206</t>
+          <t>410</t>
         </is>
       </c>
       <c r="C119" t="n">
-        <v>214</v>
+        <v>282</v>
       </c>
     </row>
     <row r="120">
@@ -1985,11 +1985,11 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>198</t>
+          <t>412</t>
         </is>
       </c>
       <c r="C120" t="n">
-        <v>214</v>
+        <v>282</v>
       </c>
     </row>
     <row r="121">
@@ -1998,11 +1998,11 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>253/3</t>
+          <t>461</t>
         </is>
       </c>
       <c r="C121" t="n">
-        <v>153</v>
+        <v>282</v>
       </c>
     </row>
     <row r="122">
@@ -2011,11 +2011,11 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>1094</t>
+          <t>467</t>
         </is>
       </c>
       <c r="C122" t="n">
-        <v>266</v>
+        <v>282</v>
       </c>
     </row>
     <row r="123">
@@ -2024,11 +2024,11 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>1096</t>
+          <t>468</t>
         </is>
       </c>
       <c r="C123" t="n">
-        <v>266</v>
+        <v>282</v>
       </c>
     </row>
     <row r="124">
@@ -2037,11 +2037,11 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>1097</t>
+          <t>.315</t>
         </is>
       </c>
       <c r="C124" t="n">
-        <v>266</v>
+        <v>282</v>
       </c>
     </row>
     <row r="125">
@@ -2050,11 +2050,11 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>1150</t>
+          <t>1826</t>
         </is>
       </c>
       <c r="C125" t="n">
-        <v>266</v>
+        <v>282</v>
       </c>
     </row>
     <row r="126">
@@ -2063,11 +2063,11 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>1183</t>
+          <t>86</t>
         </is>
       </c>
       <c r="C126" t="n">
-        <v>266</v>
+        <v>340</v>
       </c>
     </row>
     <row r="127">
@@ -2076,11 +2076,11 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>842</t>
+          <t>397</t>
         </is>
       </c>
       <c r="C127" t="n">
-        <v>266</v>
+        <v>340</v>
       </c>
     </row>
     <row r="128">
@@ -2089,11 +2089,11 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>587</t>
+          <t>488</t>
         </is>
       </c>
       <c r="C128" t="n">
-        <v>213</v>
+        <v>340</v>
       </c>
     </row>
     <row r="129">
@@ -2102,11 +2102,11 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>588</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C129" t="n">
-        <v>213</v>
+        <v>255</v>
       </c>
     </row>
     <row r="130">
@@ -2115,11 +2115,11 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>1082</t>
         </is>
       </c>
       <c r="C130" t="n">
-        <v>213</v>
+        <v>255</v>
       </c>
     </row>
     <row r="131">
@@ -2128,11 +2128,11 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>642/2</t>
+          <t>403</t>
         </is>
       </c>
       <c r="C131" t="n">
-        <v>213</v>
+        <v>97</v>
       </c>
     </row>
     <row r="132">
@@ -2141,11 +2141,11 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>116</t>
+          <t>746</t>
         </is>
       </c>
       <c r="C132" t="n">
-        <v>213</v>
+        <v>97</v>
       </c>
     </row>
     <row r="133">
@@ -2154,11 +2154,11 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>151</t>
+          <t>749</t>
         </is>
       </c>
       <c r="C133" t="n">
-        <v>213</v>
+        <v>97</v>
       </c>
     </row>
     <row r="134">
@@ -2167,11 +2167,11 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>466</t>
+          <t>754</t>
         </is>
       </c>
       <c r="C134" t="n">
-        <v>213</v>
+        <v>97</v>
       </c>
     </row>
     <row r="135">
@@ -2180,11 +2180,11 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>1479</t>
+          <t>755</t>
         </is>
       </c>
       <c r="C135" t="n">
-        <v>265</v>
+        <v>97</v>
       </c>
     </row>
     <row r="136">
@@ -2193,11 +2193,11 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>2243</t>
+          <t>757</t>
         </is>
       </c>
       <c r="C136" t="n">
-        <v>265</v>
+        <v>97</v>
       </c>
     </row>
     <row r="137">
@@ -2206,11 +2206,11 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>901</t>
+          <t>758</t>
         </is>
       </c>
       <c r="C137" t="n">
-        <v>265</v>
+        <v>97</v>
       </c>
     </row>
     <row r="138">
@@ -2219,11 +2219,11 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>842</t>
+          <t>825/63</t>
         </is>
       </c>
       <c r="C138" t="n">
-        <v>265</v>
+        <v>97</v>
       </c>
     </row>
     <row r="139">
@@ -2232,11 +2232,11 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>656</t>
+          <t>1900/4</t>
         </is>
       </c>
       <c r="C139" t="n">
-        <v>245</v>
+        <v>317</v>
       </c>
     </row>
     <row r="140">
@@ -2245,11 +2245,11 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>811</t>
+          <t>9609</t>
         </is>
       </c>
       <c r="C140" t="n">
-        <v>245</v>
+        <v>390</v>
       </c>
     </row>
     <row r="141">
@@ -2258,11 +2258,11 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>370</t>
+          <t>9608/2</t>
         </is>
       </c>
       <c r="C141" t="n">
-        <v>245</v>
+        <v>390</v>
       </c>
     </row>
     <row r="142">
@@ -2271,11 +2271,11 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>537</t>
+          <t>371</t>
         </is>
       </c>
       <c r="C142" t="n">
-        <v>245</v>
+        <v>404</v>
       </c>
     </row>
     <row r="143">
@@ -2284,11 +2284,11 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>4812</t>
+          <t>373</t>
         </is>
       </c>
       <c r="C143" t="n">
-        <v>245</v>
+        <v>404</v>
       </c>
     </row>
     <row r="144">
@@ -2297,11 +2297,11 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>5016</t>
+          <t>1741</t>
         </is>
       </c>
       <c r="C144" t="n">
-        <v>245</v>
+        <v>404</v>
       </c>
     </row>
     <row r="145">
@@ -2310,11 +2310,11 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>1820</t>
         </is>
       </c>
       <c r="C145" t="n">
-        <v>245</v>
+        <v>404</v>
       </c>
     </row>
     <row r="146">
@@ -2323,11 +2323,11 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>1858</t>
+          <t>156</t>
         </is>
       </c>
       <c r="C146" t="n">
-        <v>245</v>
+        <v>404</v>
       </c>
     </row>
     <row r="147">
@@ -2336,11 +2336,11 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>2421</t>
+          <t>4708</t>
         </is>
       </c>
       <c r="C147" t="n">
-        <v>245</v>
+        <v>404</v>
       </c>
     </row>
     <row r="148">
@@ -2349,11 +2349,11 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>2436</t>
+          <t>162/3</t>
         </is>
       </c>
       <c r="C148" t="n">
-        <v>245</v>
+        <v>404</v>
       </c>
     </row>
     <row r="149">
@@ -2362,11 +2362,11 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>609</t>
+          <t>1193</t>
         </is>
       </c>
       <c r="C149" t="n">
-        <v>414</v>
+        <v>404</v>
       </c>
     </row>
     <row r="150">
@@ -2375,11 +2375,11 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>912</t>
+          <t>2762</t>
         </is>
       </c>
       <c r="C150" t="n">
-        <v>414</v>
+        <v>404</v>
       </c>
     </row>
     <row r="151">
@@ -2388,11 +2388,11 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>1419</t>
+          <t>2766/3</t>
         </is>
       </c>
       <c r="C151" t="n">
-        <v>414</v>
+        <v>404</v>
       </c>
     </row>
     <row r="152">
@@ -2401,11 +2401,11 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>2736/8</t>
         </is>
       </c>
       <c r="C152" t="n">
-        <v>282</v>
+        <v>404</v>
       </c>
     </row>
     <row r="153">
@@ -2414,11 +2414,11 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>722</t>
+          <t>2769/1</t>
         </is>
       </c>
       <c r="C153" t="n">
-        <v>282</v>
+        <v>404</v>
       </c>
     </row>
     <row r="154">
@@ -2427,11 +2427,11 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>410</t>
+          <t>2768</t>
         </is>
       </c>
       <c r="C154" t="n">
-        <v>282</v>
+        <v>404</v>
       </c>
     </row>
     <row r="155">
@@ -2440,11 +2440,11 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>412</t>
+          <t>2767</t>
         </is>
       </c>
       <c r="C155" t="n">
-        <v>282</v>
+        <v>404</v>
       </c>
     </row>
     <row r="156">
@@ -2453,11 +2453,11 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>461</t>
+          <t>679/2</t>
         </is>
       </c>
       <c r="C156" t="n">
-        <v>282</v>
+        <v>404</v>
       </c>
     </row>
     <row r="157">
@@ -2466,11 +2466,11 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>467</t>
+          <t>5582/2</t>
         </is>
       </c>
       <c r="C157" t="n">
-        <v>282</v>
+        <v>413</v>
       </c>
     </row>
     <row r="158">
@@ -2479,11 +2479,11 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>468</t>
+          <t>9213/12</t>
         </is>
       </c>
       <c r="C158" t="n">
-        <v>282</v>
+        <v>413</v>
       </c>
     </row>
     <row r="159">
@@ -2492,11 +2492,11 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>.315</t>
+          <t>45</t>
         </is>
       </c>
       <c r="C159" t="n">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="160">
@@ -2505,11 +2505,11 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>1826</t>
+          <t>84/1</t>
         </is>
       </c>
       <c r="C160" t="n">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="161">
@@ -2518,11 +2518,11 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>86</t>
+          <t>137</t>
         </is>
       </c>
       <c r="C161" t="n">
-        <v>340</v>
+        <v>41</v>
       </c>
     </row>
     <row r="162">
@@ -2531,11 +2531,11 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>397</t>
+          <t>140</t>
         </is>
       </c>
       <c r="C162" t="n">
-        <v>340</v>
+        <v>41</v>
       </c>
     </row>
     <row r="163">
@@ -2544,11 +2544,11 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>488</t>
+          <t>272</t>
         </is>
       </c>
       <c r="C163" t="n">
-        <v>340</v>
+        <v>79</v>
       </c>
     </row>
     <row r="164">
@@ -2557,11 +2557,11 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1845</t>
         </is>
       </c>
       <c r="C164" t="n">
-        <v>255</v>
+        <v>79</v>
       </c>
     </row>
     <row r="165">
@@ -2570,11 +2570,11 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>1082</t>
+          <t>100</t>
         </is>
       </c>
       <c r="C165" t="n">
-        <v>255</v>
+        <v>79</v>
       </c>
     </row>
     <row r="166">
@@ -2583,11 +2583,11 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>403</t>
+          <t>1390</t>
         </is>
       </c>
       <c r="C166" t="n">
-        <v>97</v>
+        <v>79</v>
       </c>
     </row>
     <row r="167">
@@ -2596,11 +2596,11 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>746</t>
+          <t>94/6</t>
         </is>
       </c>
       <c r="C167" t="n">
-        <v>97</v>
+        <v>251</v>
       </c>
     </row>
     <row r="168">
@@ -2609,11 +2609,11 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>749</t>
+          <t>243</t>
         </is>
       </c>
       <c r="C168" t="n">
-        <v>97</v>
+        <v>253</v>
       </c>
     </row>
     <row r="169">
@@ -2622,11 +2622,11 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>754</t>
+          <t>295</t>
         </is>
       </c>
       <c r="C169" t="n">
-        <v>97</v>
+        <v>253</v>
       </c>
     </row>
     <row r="170">
@@ -2635,11 +2635,11 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>755</t>
+          <t>1403</t>
         </is>
       </c>
       <c r="C170" t="n">
-        <v>97</v>
+        <v>268</v>
       </c>
     </row>
     <row r="171">
@@ -2648,11 +2648,11 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>757</t>
+          <t>1444</t>
         </is>
       </c>
       <c r="C171" t="n">
-        <v>97</v>
+        <v>268</v>
       </c>
     </row>
     <row r="172">
@@ -2661,11 +2661,11 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>758</t>
+          <t>1605</t>
         </is>
       </c>
       <c r="C172" t="n">
-        <v>97</v>
+        <v>268</v>
       </c>
     </row>
     <row r="173">
@@ -2674,11 +2674,11 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>825/63</t>
+          <t>1823</t>
         </is>
       </c>
       <c r="C173" t="n">
-        <v>97</v>
+        <v>268</v>
       </c>
     </row>
     <row r="174">
@@ -2687,11 +2687,11 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>1900/4</t>
+          <t>1824</t>
         </is>
       </c>
       <c r="C174" t="n">
-        <v>317</v>
+        <v>268</v>
       </c>
     </row>
     <row r="175">
@@ -2700,11 +2700,11 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>9609</t>
+          <t>316</t>
         </is>
       </c>
       <c r="C175" t="n">
-        <v>390</v>
+        <v>442</v>
       </c>
     </row>
     <row r="176">
@@ -2713,11 +2713,11 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>9608/2</t>
+          <t>53</t>
         </is>
       </c>
       <c r="C176" t="n">
-        <v>390</v>
+        <v>215</v>
       </c>
     </row>
     <row r="177">
@@ -2726,11 +2726,11 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>371</t>
+          <t>454</t>
         </is>
       </c>
       <c r="C177" t="n">
-        <v>404</v>
+        <v>215</v>
       </c>
     </row>
     <row r="178">
@@ -2739,11 +2739,11 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>373</t>
+          <t>420/80</t>
         </is>
       </c>
       <c r="C178" t="n">
-        <v>404</v>
+        <v>215</v>
       </c>
     </row>
     <row r="179">
@@ -2752,11 +2752,11 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>1741</t>
+          <t>420/92</t>
         </is>
       </c>
       <c r="C179" t="n">
-        <v>404</v>
+        <v>215</v>
       </c>
     </row>
     <row r="180">
@@ -2765,11 +2765,11 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>1820</t>
+          <t>420/93</t>
         </is>
       </c>
       <c r="C180" t="n">
-        <v>404</v>
+        <v>215</v>
       </c>
     </row>
     <row r="181">
@@ -2778,11 +2778,11 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>156</t>
+          <t>420/94</t>
         </is>
       </c>
       <c r="C181" t="n">
-        <v>404</v>
+        <v>215</v>
       </c>
     </row>
     <row r="182">
@@ -2791,11 +2791,11 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>4708</t>
+          <t>420/95</t>
         </is>
       </c>
       <c r="C182" t="n">
-        <v>404</v>
+        <v>215</v>
       </c>
     </row>
     <row r="183">
@@ -2804,11 +2804,11 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>162/3</t>
+          <t>420/96</t>
         </is>
       </c>
       <c r="C183" t="n">
-        <v>404</v>
+        <v>215</v>
       </c>
     </row>
     <row r="184">
@@ -2817,11 +2817,11 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>1193</t>
+          <t>420/97</t>
         </is>
       </c>
       <c r="C184" t="n">
-        <v>404</v>
+        <v>215</v>
       </c>
     </row>
     <row r="185">
@@ -2830,11 +2830,11 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>2762</t>
+          <t>420/101</t>
         </is>
       </c>
       <c r="C185" t="n">
-        <v>404</v>
+        <v>215</v>
       </c>
     </row>
     <row r="186">
@@ -2843,11 +2843,11 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>2766/3</t>
+          <t>420/102</t>
         </is>
       </c>
       <c r="C186" t="n">
-        <v>404</v>
+        <v>215</v>
       </c>
     </row>
     <row r="187">
@@ -2856,11 +2856,11 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>2736/8</t>
+          <t>420/106</t>
         </is>
       </c>
       <c r="C187" t="n">
-        <v>404</v>
+        <v>215</v>
       </c>
     </row>
     <row r="188">
@@ -2869,11 +2869,11 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>2769/1</t>
+          <t>420/107</t>
         </is>
       </c>
       <c r="C188" t="n">
-        <v>404</v>
+        <v>215</v>
       </c>
     </row>
     <row r="189">
@@ -2882,11 +2882,11 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>2768</t>
+          <t>420/109</t>
         </is>
       </c>
       <c r="C189" t="n">
-        <v>404</v>
+        <v>215</v>
       </c>
     </row>
     <row r="190">
@@ -2895,11 +2895,11 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>2767</t>
+          <t>420/110</t>
         </is>
       </c>
       <c r="C190" t="n">
-        <v>404</v>
+        <v>215</v>
       </c>
     </row>
     <row r="191">
@@ -2908,11 +2908,11 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>679/2</t>
+          <t>705/11</t>
         </is>
       </c>
       <c r="C191" t="n">
-        <v>404</v>
+        <v>215</v>
       </c>
     </row>
     <row r="192">
@@ -2921,11 +2921,11 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>5582/2</t>
+          <t>756</t>
         </is>
       </c>
       <c r="C192" t="n">
-        <v>413</v>
+        <v>215</v>
       </c>
     </row>
     <row r="193">
@@ -2934,11 +2934,11 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>9213/12</t>
+          <t>798/3</t>
         </is>
       </c>
       <c r="C193" t="n">
-        <v>413</v>
+        <v>215</v>
       </c>
     </row>
     <row r="194">
@@ -2947,11 +2947,11 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>1411/1</t>
         </is>
       </c>
       <c r="C194" t="n">
-        <v>283</v>
+        <v>256</v>
       </c>
     </row>
     <row r="195">
@@ -2960,11 +2960,11 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>84/1</t>
+          <t>1411/2</t>
         </is>
       </c>
       <c r="C195" t="n">
-        <v>283</v>
+        <v>256</v>
       </c>
     </row>
     <row r="196">
@@ -2973,11 +2973,11 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>137</t>
+          <t>1411/3</t>
         </is>
       </c>
       <c r="C196" t="n">
-        <v>41</v>
+        <v>256</v>
       </c>
     </row>
     <row r="197">
@@ -2986,11 +2986,11 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>140</t>
+          <t>1411/4</t>
         </is>
       </c>
       <c r="C197" t="n">
-        <v>41</v>
+        <v>256</v>
       </c>
     </row>
     <row r="198">
@@ -2999,11 +2999,11 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>272</t>
+          <t>1411/5</t>
         </is>
       </c>
       <c r="C198" t="n">
-        <v>79</v>
+        <v>256</v>
       </c>
     </row>
     <row r="199">
@@ -3012,11 +3012,11 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>1845</t>
+          <t>1412</t>
         </is>
       </c>
       <c r="C199" t="n">
-        <v>79</v>
+        <v>256</v>
       </c>
     </row>
     <row r="200">
@@ -3025,11 +3025,11 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>1488</t>
         </is>
       </c>
       <c r="C200" t="n">
-        <v>79</v>
+        <v>256</v>
       </c>
     </row>
     <row r="201">
@@ -3038,11 +3038,11 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>1390</t>
+          <t>254/2</t>
         </is>
       </c>
       <c r="C201" t="n">
-        <v>79</v>
+        <v>193</v>
       </c>
     </row>
     <row r="202">
@@ -3051,11 +3051,11 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>94/6</t>
+          <t>337/5</t>
         </is>
       </c>
       <c r="C202" t="n">
-        <v>251</v>
+        <v>193</v>
       </c>
     </row>
     <row r="203">
@@ -3064,11 +3064,11 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>243</t>
+          <t>393/1</t>
         </is>
       </c>
       <c r="C203" t="n">
-        <v>253</v>
+        <v>193</v>
       </c>
     </row>
     <row r="204">
@@ -3077,11 +3077,11 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>295</t>
+          <t>393/2</t>
         </is>
       </c>
       <c r="C204" t="n">
-        <v>253</v>
+        <v>193</v>
       </c>
     </row>
     <row r="205">
@@ -3090,11 +3090,11 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>1403</t>
+          <t>393/3</t>
         </is>
       </c>
       <c r="C205" t="n">
-        <v>268</v>
+        <v>193</v>
       </c>
     </row>
     <row r="206">
@@ -3103,11 +3103,11 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>1444</t>
+          <t>465</t>
         </is>
       </c>
       <c r="C206" t="n">
-        <v>268</v>
+        <v>193</v>
       </c>
     </row>
     <row r="207">
@@ -3116,11 +3116,11 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>1605</t>
+          <t>614</t>
         </is>
       </c>
       <c r="C207" t="n">
-        <v>268</v>
+        <v>193</v>
       </c>
     </row>
     <row r="208">
@@ -3129,11 +3129,11 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>1823</t>
+          <t>1303/1</t>
         </is>
       </c>
       <c r="C208" t="n">
-        <v>268</v>
+        <v>193</v>
       </c>
     </row>
     <row r="209">
@@ -3142,11 +3142,11 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>1824</t>
+          <t>1303/2</t>
         </is>
       </c>
       <c r="C209" t="n">
-        <v>268</v>
+        <v>193</v>
       </c>
     </row>
     <row r="210">
@@ -3155,11 +3155,11 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>316</t>
+          <t>1309</t>
         </is>
       </c>
       <c r="C210" t="n">
-        <v>442</v>
+        <v>193</v>
       </c>
     </row>
     <row r="211">
@@ -3168,11 +3168,11 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>1330</t>
         </is>
       </c>
       <c r="C211" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="212">
@@ -3181,11 +3181,11 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>454</t>
+          <t>1334</t>
         </is>
       </c>
       <c r="C212" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="213">
@@ -3194,11 +3194,11 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>420/80</t>
+          <t>1346</t>
         </is>
       </c>
       <c r="C213" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="214">
@@ -3207,11 +3207,11 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>420/92</t>
+          <t>1369/1</t>
         </is>
       </c>
       <c r="C214" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="215">
@@ -3220,11 +3220,11 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>420/93</t>
+          <t>1117/2</t>
         </is>
       </c>
       <c r="C215" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="216">
@@ -3233,11 +3233,11 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>420/94</t>
+          <t>1230/85</t>
         </is>
       </c>
       <c r="C216" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="217">
@@ -3246,11 +3246,11 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>420/95</t>
+          <t>1230/86</t>
         </is>
       </c>
       <c r="C217" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="218">
@@ -3259,11 +3259,11 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>420/96</t>
+          <t>1230/87</t>
         </is>
       </c>
       <c r="C218" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="219">
@@ -3272,11 +3272,11 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>420/97</t>
+          <t>1230/88</t>
         </is>
       </c>
       <c r="C219" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="220">
@@ -3285,11 +3285,11 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>420/101</t>
+          <t>1230/100</t>
         </is>
       </c>
       <c r="C220" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="221">
@@ -3298,11 +3298,11 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>420/102</t>
+          <t>1230/115</t>
         </is>
       </c>
       <c r="C221" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="222">
@@ -3311,465 +3311,10 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>420/106</t>
+          <t>194/4</t>
         </is>
       </c>
       <c r="C222" t="n">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="223">
-      <c r="A223" s="1" t="n">
-        <v>221</v>
-      </c>
-      <c r="B223" t="inlineStr">
-        <is>
-          <t>420/107</t>
-        </is>
-      </c>
-      <c r="C223" t="n">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="224">
-      <c r="A224" s="1" t="n">
-        <v>222</v>
-      </c>
-      <c r="B224" t="inlineStr">
-        <is>
-          <t>420/109</t>
-        </is>
-      </c>
-      <c r="C224" t="n">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="225">
-      <c r="A225" s="1" t="n">
-        <v>223</v>
-      </c>
-      <c r="B225" t="inlineStr">
-        <is>
-          <t>420/110</t>
-        </is>
-      </c>
-      <c r="C225" t="n">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="226">
-      <c r="A226" s="1" t="n">
-        <v>224</v>
-      </c>
-      <c r="B226" t="inlineStr">
-        <is>
-          <t>705/11</t>
-        </is>
-      </c>
-      <c r="C226" t="n">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="227">
-      <c r="A227" s="1" t="n">
-        <v>225</v>
-      </c>
-      <c r="B227" t="inlineStr">
-        <is>
-          <t>756</t>
-        </is>
-      </c>
-      <c r="C227" t="n">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="228">
-      <c r="A228" s="1" t="n">
-        <v>226</v>
-      </c>
-      <c r="B228" t="inlineStr">
-        <is>
-          <t>798/3</t>
-        </is>
-      </c>
-      <c r="C228" t="n">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="229">
-      <c r="A229" s="1" t="n">
-        <v>227</v>
-      </c>
-      <c r="B229" t="inlineStr">
-        <is>
-          <t>1411/1</t>
-        </is>
-      </c>
-      <c r="C229" t="n">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="230">
-      <c r="A230" s="1" t="n">
-        <v>228</v>
-      </c>
-      <c r="B230" t="inlineStr">
-        <is>
-          <t>1411/2</t>
-        </is>
-      </c>
-      <c r="C230" t="n">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="231">
-      <c r="A231" s="1" t="n">
-        <v>229</v>
-      </c>
-      <c r="B231" t="inlineStr">
-        <is>
-          <t>1411/3</t>
-        </is>
-      </c>
-      <c r="C231" t="n">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="232">
-      <c r="A232" s="1" t="n">
-        <v>230</v>
-      </c>
-      <c r="B232" t="inlineStr">
-        <is>
-          <t>1411/4</t>
-        </is>
-      </c>
-      <c r="C232" t="n">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="233">
-      <c r="A233" s="1" t="n">
-        <v>231</v>
-      </c>
-      <c r="B233" t="inlineStr">
-        <is>
-          <t>1411/5</t>
-        </is>
-      </c>
-      <c r="C233" t="n">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="234">
-      <c r="A234" s="1" t="n">
-        <v>232</v>
-      </c>
-      <c r="B234" t="inlineStr">
-        <is>
-          <t>1412</t>
-        </is>
-      </c>
-      <c r="C234" t="n">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="235">
-      <c r="A235" s="1" t="n">
-        <v>233</v>
-      </c>
-      <c r="B235" t="inlineStr">
-        <is>
-          <t>1488</t>
-        </is>
-      </c>
-      <c r="C235" t="n">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="236">
-      <c r="A236" s="1" t="n">
-        <v>234</v>
-      </c>
-      <c r="B236" t="inlineStr">
-        <is>
-          <t>254/2</t>
-        </is>
-      </c>
-      <c r="C236" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="237">
-      <c r="A237" s="1" t="n">
-        <v>235</v>
-      </c>
-      <c r="B237" t="inlineStr">
-        <is>
-          <t>337/5</t>
-        </is>
-      </c>
-      <c r="C237" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="238">
-      <c r="A238" s="1" t="n">
-        <v>236</v>
-      </c>
-      <c r="B238" t="inlineStr">
-        <is>
-          <t>393/1</t>
-        </is>
-      </c>
-      <c r="C238" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="239">
-      <c r="A239" s="1" t="n">
-        <v>237</v>
-      </c>
-      <c r="B239" t="inlineStr">
-        <is>
-          <t>393/2</t>
-        </is>
-      </c>
-      <c r="C239" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="240">
-      <c r="A240" s="1" t="n">
-        <v>238</v>
-      </c>
-      <c r="B240" t="inlineStr">
-        <is>
-          <t>393/3</t>
-        </is>
-      </c>
-      <c r="C240" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="241">
-      <c r="A241" s="1" t="n">
-        <v>239</v>
-      </c>
-      <c r="B241" t="inlineStr">
-        <is>
-          <t>465</t>
-        </is>
-      </c>
-      <c r="C241" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="242">
-      <c r="A242" s="1" t="n">
-        <v>240</v>
-      </c>
-      <c r="B242" t="inlineStr">
-        <is>
-          <t>614</t>
-        </is>
-      </c>
-      <c r="C242" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="243">
-      <c r="A243" s="1" t="n">
-        <v>241</v>
-      </c>
-      <c r="B243" t="inlineStr">
-        <is>
-          <t>1303/1</t>
-        </is>
-      </c>
-      <c r="C243" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="244">
-      <c r="A244" s="1" t="n">
-        <v>242</v>
-      </c>
-      <c r="B244" t="inlineStr">
-        <is>
-          <t>1303/2</t>
-        </is>
-      </c>
-      <c r="C244" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="245">
-      <c r="A245" s="1" t="n">
-        <v>243</v>
-      </c>
-      <c r="B245" t="inlineStr">
-        <is>
-          <t>1309</t>
-        </is>
-      </c>
-      <c r="C245" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="246">
-      <c r="A246" s="1" t="n">
-        <v>244</v>
-      </c>
-      <c r="B246" t="inlineStr">
-        <is>
-          <t>1330</t>
-        </is>
-      </c>
-      <c r="C246" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="247">
-      <c r="A247" s="1" t="n">
-        <v>245</v>
-      </c>
-      <c r="B247" t="inlineStr">
-        <is>
-          <t>1334</t>
-        </is>
-      </c>
-      <c r="C247" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="248">
-      <c r="A248" s="1" t="n">
-        <v>246</v>
-      </c>
-      <c r="B248" t="inlineStr">
-        <is>
-          <t>1346</t>
-        </is>
-      </c>
-      <c r="C248" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="249">
-      <c r="A249" s="1" t="n">
-        <v>247</v>
-      </c>
-      <c r="B249" t="inlineStr">
-        <is>
-          <t>1369/1</t>
-        </is>
-      </c>
-      <c r="C249" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="250">
-      <c r="A250" s="1" t="n">
-        <v>248</v>
-      </c>
-      <c r="B250" t="inlineStr">
-        <is>
-          <t>1117/2</t>
-        </is>
-      </c>
-      <c r="C250" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="251">
-      <c r="A251" s="1" t="n">
-        <v>249</v>
-      </c>
-      <c r="B251" t="inlineStr">
-        <is>
-          <t>1230/85</t>
-        </is>
-      </c>
-      <c r="C251" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="252">
-      <c r="A252" s="1" t="n">
-        <v>250</v>
-      </c>
-      <c r="B252" t="inlineStr">
-        <is>
-          <t>1230/86</t>
-        </is>
-      </c>
-      <c r="C252" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="253">
-      <c r="A253" s="1" t="n">
-        <v>251</v>
-      </c>
-      <c r="B253" t="inlineStr">
-        <is>
-          <t>1230/87</t>
-        </is>
-      </c>
-      <c r="C253" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="254">
-      <c r="A254" s="1" t="n">
-        <v>252</v>
-      </c>
-      <c r="B254" t="inlineStr">
-        <is>
-          <t>1230/88</t>
-        </is>
-      </c>
-      <c r="C254" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="255">
-      <c r="A255" s="1" t="n">
-        <v>253</v>
-      </c>
-      <c r="B255" t="inlineStr">
-        <is>
-          <t>1230/100</t>
-        </is>
-      </c>
-      <c r="C255" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="256">
-      <c r="A256" s="1" t="n">
-        <v>254</v>
-      </c>
-      <c r="B256" t="inlineStr">
-        <is>
-          <t>1230/115</t>
-        </is>
-      </c>
-      <c r="C256" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="257">
-      <c r="A257" s="1" t="n">
-        <v>255</v>
-      </c>
-      <c r="B257" t="inlineStr">
-        <is>
-          <t>194/4</t>
-        </is>
-      </c>
-      <c r="C257" t="n">
         <v>193</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Latest data: Thu Jan 11 12:15:15 UTC 2024
</commit_message>
<xml_diff>
--- a/docs/particelle_non_trovate.xlsx
+++ b/docs/particelle_non_trovate.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Latest data: Thu Jan 11 14:48:42 UTC 2024
</commit_message>
<xml_diff>
--- a/docs/particelle_non_trovate.xlsx
+++ b/docs/particelle_non_trovate.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Latest data: Mon Jan 15 12:15:44 UTC 2024
</commit_message>
<xml_diff>
--- a/docs/particelle_non_trovate.xlsx
+++ b/docs/particelle_non_trovate.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C223"/>
+  <dimension ref="A1:C239"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2479,7 +2479,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>5582/2</t>
+          <t>.507/2</t>
         </is>
       </c>
       <c r="C158" t="n">
@@ -2492,7 +2492,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>9213/12</t>
+          <t>.507/3</t>
         </is>
       </c>
       <c r="C159" t="n">
@@ -2505,11 +2505,11 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>.507/4</t>
         </is>
       </c>
       <c r="C160" t="n">
-        <v>283</v>
+        <v>413</v>
       </c>
     </row>
     <row r="161">
@@ -2518,11 +2518,11 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>84/1</t>
+          <t>507/5</t>
         </is>
       </c>
       <c r="C161" t="n">
-        <v>283</v>
+        <v>413</v>
       </c>
     </row>
     <row r="162">
@@ -2531,11 +2531,11 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>137</t>
+          <t>507/6</t>
         </is>
       </c>
       <c r="C162" t="n">
-        <v>41</v>
+        <v>413</v>
       </c>
     </row>
     <row r="163">
@@ -2544,11 +2544,11 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>140</t>
+          <t>569/8</t>
         </is>
       </c>
       <c r="C163" t="n">
-        <v>41</v>
+        <v>413</v>
       </c>
     </row>
     <row r="164">
@@ -2557,11 +2557,11 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>272</t>
+          <t>.569/5</t>
         </is>
       </c>
       <c r="C164" t="n">
-        <v>79</v>
+        <v>413</v>
       </c>
     </row>
     <row r="165">
@@ -2570,11 +2570,11 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>1845</t>
+          <t>7294</t>
         </is>
       </c>
       <c r="C165" t="n">
-        <v>79</v>
+        <v>413</v>
       </c>
     </row>
     <row r="166">
@@ -2583,11 +2583,11 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>7293/2</t>
         </is>
       </c>
       <c r="C166" t="n">
-        <v>79</v>
+        <v>413</v>
       </c>
     </row>
     <row r="167">
@@ -2596,11 +2596,11 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>1390</t>
+          <t>7293/3</t>
         </is>
       </c>
       <c r="C167" t="n">
-        <v>79</v>
+        <v>413</v>
       </c>
     </row>
     <row r="168">
@@ -2609,11 +2609,11 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>94/6</t>
+          <t>1.391</t>
         </is>
       </c>
       <c r="C168" t="n">
-        <v>251</v>
+        <v>413</v>
       </c>
     </row>
     <row r="169">
@@ -2622,11 +2622,11 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>243</t>
+          <t>7292/1</t>
         </is>
       </c>
       <c r="C169" t="n">
-        <v>253</v>
+        <v>413</v>
       </c>
     </row>
     <row r="170">
@@ -2635,11 +2635,11 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>295</t>
+          <t>1.358</t>
         </is>
       </c>
       <c r="C170" t="n">
-        <v>253</v>
+        <v>413</v>
       </c>
     </row>
     <row r="171">
@@ -2648,11 +2648,11 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>1403</t>
+          <t>1.359</t>
         </is>
       </c>
       <c r="C171" t="n">
-        <v>268</v>
+        <v>413</v>
       </c>
     </row>
     <row r="172">
@@ -2661,11 +2661,11 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>1444</t>
+          <t>7191/4</t>
         </is>
       </c>
       <c r="C172" t="n">
-        <v>268</v>
+        <v>413</v>
       </c>
     </row>
     <row r="173">
@@ -2674,11 +2674,11 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>1605</t>
+          <t>1.270</t>
         </is>
       </c>
       <c r="C173" t="n">
-        <v>268</v>
+        <v>413</v>
       </c>
     </row>
     <row r="174">
@@ -2687,11 +2687,11 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>1823</t>
+          <t>7618/3</t>
         </is>
       </c>
       <c r="C174" t="n">
-        <v>268</v>
+        <v>413</v>
       </c>
     </row>
     <row r="175">
@@ -2700,11 +2700,11 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>1824</t>
+          <t>7618/4</t>
         </is>
       </c>
       <c r="C175" t="n">
-        <v>268</v>
+        <v>413</v>
       </c>
     </row>
     <row r="176">
@@ -2713,11 +2713,11 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>316</t>
+          <t>114</t>
         </is>
       </c>
       <c r="C176" t="n">
-        <v>442</v>
+        <v>413</v>
       </c>
     </row>
     <row r="177">
@@ -2726,11 +2726,11 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>361</t>
         </is>
       </c>
       <c r="C177" t="n">
-        <v>215</v>
+        <v>413</v>
       </c>
     </row>
     <row r="178">
@@ -2739,11 +2739,11 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>454</t>
+          <t>421</t>
         </is>
       </c>
       <c r="C178" t="n">
-        <v>215</v>
+        <v>413</v>
       </c>
     </row>
     <row r="179">
@@ -2752,11 +2752,11 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>420/80</t>
+          <t>13094</t>
         </is>
       </c>
       <c r="C179" t="n">
-        <v>215</v>
+        <v>413</v>
       </c>
     </row>
     <row r="180">
@@ -2765,11 +2765,11 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>420/92</t>
+          <t>7290/6</t>
         </is>
       </c>
       <c r="C180" t="n">
-        <v>215</v>
+        <v>413</v>
       </c>
     </row>
     <row r="181">
@@ -2778,11 +2778,11 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>420/93</t>
+          <t>7288</t>
         </is>
       </c>
       <c r="C181" t="n">
-        <v>215</v>
+        <v>413</v>
       </c>
     </row>
     <row r="182">
@@ -2791,11 +2791,11 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>420/94</t>
+          <t>45</t>
         </is>
       </c>
       <c r="C182" t="n">
-        <v>215</v>
+        <v>283</v>
       </c>
     </row>
     <row r="183">
@@ -2804,11 +2804,11 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>420/95</t>
+          <t>84/1</t>
         </is>
       </c>
       <c r="C183" t="n">
-        <v>215</v>
+        <v>283</v>
       </c>
     </row>
     <row r="184">
@@ -2817,11 +2817,11 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>420/96</t>
+          <t>137</t>
         </is>
       </c>
       <c r="C184" t="n">
-        <v>215</v>
+        <v>41</v>
       </c>
     </row>
     <row r="185">
@@ -2830,11 +2830,11 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>420/97</t>
+          <t>140</t>
         </is>
       </c>
       <c r="C185" t="n">
-        <v>215</v>
+        <v>41</v>
       </c>
     </row>
     <row r="186">
@@ -2843,11 +2843,11 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>420/101</t>
+          <t>272</t>
         </is>
       </c>
       <c r="C186" t="n">
-        <v>215</v>
+        <v>79</v>
       </c>
     </row>
     <row r="187">
@@ -2856,11 +2856,11 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>420/102</t>
+          <t>1881/8</t>
         </is>
       </c>
       <c r="C187" t="n">
-        <v>215</v>
+        <v>79</v>
       </c>
     </row>
     <row r="188">
@@ -2869,11 +2869,11 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>420/106</t>
+          <t>94/6</t>
         </is>
       </c>
       <c r="C188" t="n">
-        <v>215</v>
+        <v>251</v>
       </c>
     </row>
     <row r="189">
@@ -2882,11 +2882,11 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>420/107</t>
+          <t>243</t>
         </is>
       </c>
       <c r="C189" t="n">
-        <v>215</v>
+        <v>253</v>
       </c>
     </row>
     <row r="190">
@@ -2895,11 +2895,11 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>420/109</t>
+          <t>295</t>
         </is>
       </c>
       <c r="C190" t="n">
-        <v>215</v>
+        <v>253</v>
       </c>
     </row>
     <row r="191">
@@ -2908,11 +2908,11 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>420/110</t>
+          <t>1403</t>
         </is>
       </c>
       <c r="C191" t="n">
-        <v>215</v>
+        <v>268</v>
       </c>
     </row>
     <row r="192">
@@ -2921,11 +2921,11 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>705/11</t>
+          <t>316</t>
         </is>
       </c>
       <c r="C192" t="n">
-        <v>215</v>
+        <v>442</v>
       </c>
     </row>
     <row r="193">
@@ -2934,7 +2934,7 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>756</t>
+          <t>53</t>
         </is>
       </c>
       <c r="C193" t="n">
@@ -2947,7 +2947,7 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>798/3</t>
+          <t>454</t>
         </is>
       </c>
       <c r="C194" t="n">
@@ -2960,11 +2960,11 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>1411/1</t>
+          <t>420/80</t>
         </is>
       </c>
       <c r="C195" t="n">
-        <v>256</v>
+        <v>215</v>
       </c>
     </row>
     <row r="196">
@@ -2973,11 +2973,11 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>1411/2</t>
+          <t>420/92</t>
         </is>
       </c>
       <c r="C196" t="n">
-        <v>256</v>
+        <v>215</v>
       </c>
     </row>
     <row r="197">
@@ -2986,11 +2986,11 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>1411/3</t>
+          <t>420/93</t>
         </is>
       </c>
       <c r="C197" t="n">
-        <v>256</v>
+        <v>215</v>
       </c>
     </row>
     <row r="198">
@@ -2999,11 +2999,11 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>1411/4</t>
+          <t>420/94</t>
         </is>
       </c>
       <c r="C198" t="n">
-        <v>256</v>
+        <v>215</v>
       </c>
     </row>
     <row r="199">
@@ -3012,11 +3012,11 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>1411/5</t>
+          <t>420/95</t>
         </is>
       </c>
       <c r="C199" t="n">
-        <v>256</v>
+        <v>215</v>
       </c>
     </row>
     <row r="200">
@@ -3025,11 +3025,11 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>1412</t>
+          <t>420/96</t>
         </is>
       </c>
       <c r="C200" t="n">
-        <v>256</v>
+        <v>215</v>
       </c>
     </row>
     <row r="201">
@@ -3038,11 +3038,11 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>1488</t>
+          <t>420/97</t>
         </is>
       </c>
       <c r="C201" t="n">
-        <v>256</v>
+        <v>215</v>
       </c>
     </row>
     <row r="202">
@@ -3051,11 +3051,11 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>254/2</t>
+          <t>420/101</t>
         </is>
       </c>
       <c r="C202" t="n">
-        <v>193</v>
+        <v>215</v>
       </c>
     </row>
     <row r="203">
@@ -3064,11 +3064,11 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>337/5</t>
+          <t>420/102</t>
         </is>
       </c>
       <c r="C203" t="n">
-        <v>193</v>
+        <v>215</v>
       </c>
     </row>
     <row r="204">
@@ -3077,11 +3077,11 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>393/1</t>
+          <t>420/106</t>
         </is>
       </c>
       <c r="C204" t="n">
-        <v>193</v>
+        <v>215</v>
       </c>
     </row>
     <row r="205">
@@ -3090,11 +3090,11 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>393/2</t>
+          <t>420/107</t>
         </is>
       </c>
       <c r="C205" t="n">
-        <v>193</v>
+        <v>215</v>
       </c>
     </row>
     <row r="206">
@@ -3103,11 +3103,11 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>393/3</t>
+          <t>420/109</t>
         </is>
       </c>
       <c r="C206" t="n">
-        <v>193</v>
+        <v>215</v>
       </c>
     </row>
     <row r="207">
@@ -3116,11 +3116,11 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>465</t>
+          <t>420/110</t>
         </is>
       </c>
       <c r="C207" t="n">
-        <v>193</v>
+        <v>215</v>
       </c>
     </row>
     <row r="208">
@@ -3129,11 +3129,11 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>614</t>
+          <t>705/11</t>
         </is>
       </c>
       <c r="C208" t="n">
-        <v>193</v>
+        <v>215</v>
       </c>
     </row>
     <row r="209">
@@ -3142,11 +3142,11 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>1303/1</t>
+          <t>756</t>
         </is>
       </c>
       <c r="C209" t="n">
-        <v>193</v>
+        <v>215</v>
       </c>
     </row>
     <row r="210">
@@ -3155,11 +3155,11 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>1303/2</t>
+          <t>798/3</t>
         </is>
       </c>
       <c r="C210" t="n">
-        <v>193</v>
+        <v>215</v>
       </c>
     </row>
     <row r="211">
@@ -3168,11 +3168,11 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>1309</t>
+          <t>1411/1</t>
         </is>
       </c>
       <c r="C211" t="n">
-        <v>193</v>
+        <v>256</v>
       </c>
     </row>
     <row r="212">
@@ -3181,11 +3181,11 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>1330</t>
+          <t>1411/2</t>
         </is>
       </c>
       <c r="C212" t="n">
-        <v>193</v>
+        <v>256</v>
       </c>
     </row>
     <row r="213">
@@ -3194,11 +3194,11 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>1334</t>
+          <t>1411/3</t>
         </is>
       </c>
       <c r="C213" t="n">
-        <v>193</v>
+        <v>256</v>
       </c>
     </row>
     <row r="214">
@@ -3207,11 +3207,11 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>1346</t>
+          <t>1411/4</t>
         </is>
       </c>
       <c r="C214" t="n">
-        <v>193</v>
+        <v>256</v>
       </c>
     </row>
     <row r="215">
@@ -3220,11 +3220,11 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>1369/1</t>
+          <t>1411/5</t>
         </is>
       </c>
       <c r="C215" t="n">
-        <v>193</v>
+        <v>256</v>
       </c>
     </row>
     <row r="216">
@@ -3233,11 +3233,11 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>1117/2</t>
+          <t>1412</t>
         </is>
       </c>
       <c r="C216" t="n">
-        <v>193</v>
+        <v>256</v>
       </c>
     </row>
     <row r="217">
@@ -3246,11 +3246,11 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>1230/85</t>
+          <t>1488</t>
         </is>
       </c>
       <c r="C217" t="n">
-        <v>193</v>
+        <v>256</v>
       </c>
     </row>
     <row r="218">
@@ -3259,7 +3259,7 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>1230/86</t>
+          <t>254/2</t>
         </is>
       </c>
       <c r="C218" t="n">
@@ -3272,7 +3272,7 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>1230/87</t>
+          <t>337/5</t>
         </is>
       </c>
       <c r="C219" t="n">
@@ -3285,7 +3285,7 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>1230/88</t>
+          <t>393/1</t>
         </is>
       </c>
       <c r="C220" t="n">
@@ -3298,7 +3298,7 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>1230/100</t>
+          <t>393/2</t>
         </is>
       </c>
       <c r="C221" t="n">
@@ -3311,7 +3311,7 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>1230/115</t>
+          <t>393/3</t>
         </is>
       </c>
       <c r="C222" t="n">
@@ -3324,10 +3324,218 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
+          <t>465</t>
+        </is>
+      </c>
+      <c r="C223" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" s="1" t="n">
+        <v>222</v>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>614</t>
+        </is>
+      </c>
+      <c r="C224" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" s="1" t="n">
+        <v>223</v>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>1303/1</t>
+        </is>
+      </c>
+      <c r="C225" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" s="1" t="n">
+        <v>224</v>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>1303/2</t>
+        </is>
+      </c>
+      <c r="C226" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" s="1" t="n">
+        <v>225</v>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>1309</t>
+        </is>
+      </c>
+      <c r="C227" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" s="1" t="n">
+        <v>226</v>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>1330</t>
+        </is>
+      </c>
+      <c r="C228" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" s="1" t="n">
+        <v>227</v>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>1334</t>
+        </is>
+      </c>
+      <c r="C229" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" s="1" t="n">
+        <v>228</v>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>1346</t>
+        </is>
+      </c>
+      <c r="C230" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" s="1" t="n">
+        <v>229</v>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>1369/1</t>
+        </is>
+      </c>
+      <c r="C231" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" s="1" t="n">
+        <v>230</v>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>1117/2</t>
+        </is>
+      </c>
+      <c r="C232" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" s="1" t="n">
+        <v>231</v>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>1230/85</t>
+        </is>
+      </c>
+      <c r="C233" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" s="1" t="n">
+        <v>232</v>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>1230/86</t>
+        </is>
+      </c>
+      <c r="C234" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" s="1" t="n">
+        <v>233</v>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>1230/87</t>
+        </is>
+      </c>
+      <c r="C235" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" s="1" t="n">
+        <v>234</v>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>1230/88</t>
+        </is>
+      </c>
+      <c r="C236" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" s="1" t="n">
+        <v>235</v>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>1230/100</t>
+        </is>
+      </c>
+      <c r="C237" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" s="1" t="n">
+        <v>236</v>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>1230/115</t>
+        </is>
+      </c>
+      <c r="C238" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" s="1" t="n">
+        <v>237</v>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
           <t>194/4</t>
         </is>
       </c>
-      <c r="C223" t="n">
+      <c r="C239" t="n">
         <v>193</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Latest data: Thu Feb  1 20:10:27 UTC 2024
</commit_message>
<xml_diff>
--- a/docs/particelle_non_trovate.xlsx
+++ b/docs/particelle_non_trovate.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C239"/>
+  <dimension ref="A1:C220"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>391</t>
         </is>
       </c>
       <c r="C77" t="n">
@@ -1439,11 +1439,11 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>469</t>
+          <t>587</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>174</v>
+        <v>213</v>
       </c>
     </row>
     <row r="79">
@@ -1452,11 +1452,11 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>562</t>
+          <t>588</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>174</v>
+        <v>213</v>
       </c>
     </row>
     <row r="80">
@@ -1465,11 +1465,11 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>173</t>
+          <t>51</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>174</v>
+        <v>213</v>
       </c>
     </row>
     <row r="81">
@@ -1478,11 +1478,11 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>697</t>
+          <t>642/2</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>188</v>
+        <v>213</v>
       </c>
     </row>
     <row r="82">
@@ -1491,11 +1491,11 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>777</t>
+          <t>116</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>188</v>
+        <v>213</v>
       </c>
     </row>
     <row r="83">
@@ -1504,11 +1504,11 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>948</t>
+          <t>151</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>188</v>
+        <v>213</v>
       </c>
     </row>
     <row r="84">
@@ -1517,11 +1517,11 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>205</t>
+          <t>466</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="85">
@@ -1530,11 +1530,11 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>206</t>
+          <t>1479</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>214</v>
+        <v>265</v>
       </c>
     </row>
     <row r="86">
@@ -1543,11 +1543,11 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>198</t>
+          <t>2243</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>214</v>
+        <v>265</v>
       </c>
     </row>
     <row r="87">
@@ -1556,11 +1556,11 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>253/3</t>
+          <t>901</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>153</v>
+        <v>265</v>
       </c>
     </row>
     <row r="88">
@@ -1569,11 +1569,11 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>1094</t>
+          <t>842</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="89">
@@ -1582,11 +1582,11 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>1096</t>
+          <t>656</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>266</v>
+        <v>245</v>
       </c>
     </row>
     <row r="90">
@@ -1595,11 +1595,11 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>1097</t>
+          <t>811</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>266</v>
+        <v>245</v>
       </c>
     </row>
     <row r="91">
@@ -1608,11 +1608,11 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>1150</t>
+          <t>370</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>266</v>
+        <v>245</v>
       </c>
     </row>
     <row r="92">
@@ -1621,11 +1621,11 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>1183</t>
+          <t>537</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>266</v>
+        <v>245</v>
       </c>
     </row>
     <row r="93">
@@ -1634,11 +1634,11 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>842</t>
+          <t>4812</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>266</v>
+        <v>245</v>
       </c>
     </row>
     <row r="94">
@@ -1647,11 +1647,11 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>587</t>
+          <t>5016</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>213</v>
+        <v>245</v>
       </c>
     </row>
     <row r="95">
@@ -1660,11 +1660,11 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>588</t>
+          <t>51</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>213</v>
+        <v>245</v>
       </c>
     </row>
     <row r="96">
@@ -1673,11 +1673,11 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>1858</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>213</v>
+        <v>245</v>
       </c>
     </row>
     <row r="97">
@@ -1686,11 +1686,11 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>642/2</t>
+          <t>2421</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>213</v>
+        <v>245</v>
       </c>
     </row>
     <row r="98">
@@ -1699,11 +1699,11 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>116</t>
+          <t>2436</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>213</v>
+        <v>245</v>
       </c>
     </row>
     <row r="99">
@@ -1712,11 +1712,11 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>151</t>
+          <t>609</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>213</v>
+        <v>414</v>
       </c>
     </row>
     <row r="100">
@@ -1725,11 +1725,11 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>466</t>
+          <t>912</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>213</v>
+        <v>414</v>
       </c>
     </row>
     <row r="101">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>1479</t>
+          <t>1419</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>265</v>
+        <v>414</v>
       </c>
     </row>
     <row r="102">
@@ -1751,11 +1751,11 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>2243</t>
+          <t>31</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>265</v>
+        <v>282</v>
       </c>
     </row>
     <row r="103">
@@ -1764,11 +1764,11 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>901</t>
+          <t>722</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>265</v>
+        <v>282</v>
       </c>
     </row>
     <row r="104">
@@ -1777,11 +1777,11 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>842</t>
+          <t>410</t>
         </is>
       </c>
       <c r="C104" t="n">
-        <v>265</v>
+        <v>282</v>
       </c>
     </row>
     <row r="105">
@@ -1790,11 +1790,11 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>656</t>
+          <t>412</t>
         </is>
       </c>
       <c r="C105" t="n">
-        <v>245</v>
+        <v>282</v>
       </c>
     </row>
     <row r="106">
@@ -1803,11 +1803,11 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>811</t>
+          <t>461</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>245</v>
+        <v>282</v>
       </c>
     </row>
     <row r="107">
@@ -1816,11 +1816,11 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>370</t>
+          <t>467</t>
         </is>
       </c>
       <c r="C107" t="n">
-        <v>245</v>
+        <v>282</v>
       </c>
     </row>
     <row r="108">
@@ -1829,11 +1829,11 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>537</t>
+          <t>468</t>
         </is>
       </c>
       <c r="C108" t="n">
-        <v>245</v>
+        <v>282</v>
       </c>
     </row>
     <row r="109">
@@ -1842,11 +1842,11 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>4812</t>
+          <t>.315</t>
         </is>
       </c>
       <c r="C109" t="n">
-        <v>245</v>
+        <v>282</v>
       </c>
     </row>
     <row r="110">
@@ -1855,11 +1855,11 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>5016</t>
+          <t>1826</t>
         </is>
       </c>
       <c r="C110" t="n">
-        <v>245</v>
+        <v>282</v>
       </c>
     </row>
     <row r="111">
@@ -1868,11 +1868,11 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>86</t>
         </is>
       </c>
       <c r="C111" t="n">
-        <v>245</v>
+        <v>340</v>
       </c>
     </row>
     <row r="112">
@@ -1881,11 +1881,11 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>1858</t>
+          <t>397</t>
         </is>
       </c>
       <c r="C112" t="n">
-        <v>245</v>
+        <v>340</v>
       </c>
     </row>
     <row r="113">
@@ -1894,11 +1894,11 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>2421</t>
+          <t>488</t>
         </is>
       </c>
       <c r="C113" t="n">
-        <v>245</v>
+        <v>340</v>
       </c>
     </row>
     <row r="114">
@@ -1907,11 +1907,11 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>2436</t>
+          <t>403</t>
         </is>
       </c>
       <c r="C114" t="n">
-        <v>245</v>
+        <v>97</v>
       </c>
     </row>
     <row r="115">
@@ -1920,11 +1920,11 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>609</t>
+          <t>746</t>
         </is>
       </c>
       <c r="C115" t="n">
-        <v>414</v>
+        <v>97</v>
       </c>
     </row>
     <row r="116">
@@ -1933,11 +1933,11 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>912</t>
+          <t>749</t>
         </is>
       </c>
       <c r="C116" t="n">
-        <v>414</v>
+        <v>97</v>
       </c>
     </row>
     <row r="117">
@@ -1946,11 +1946,11 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>1419</t>
+          <t>754</t>
         </is>
       </c>
       <c r="C117" t="n">
-        <v>414</v>
+        <v>97</v>
       </c>
     </row>
     <row r="118">
@@ -1959,11 +1959,11 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>755</t>
         </is>
       </c>
       <c r="C118" t="n">
-        <v>282</v>
+        <v>97</v>
       </c>
     </row>
     <row r="119">
@@ -1972,11 +1972,11 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>722</t>
+          <t>757</t>
         </is>
       </c>
       <c r="C119" t="n">
-        <v>282</v>
+        <v>97</v>
       </c>
     </row>
     <row r="120">
@@ -1985,11 +1985,11 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>410</t>
+          <t>758</t>
         </is>
       </c>
       <c r="C120" t="n">
-        <v>282</v>
+        <v>97</v>
       </c>
     </row>
     <row r="121">
@@ -1998,11 +1998,11 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>412</t>
+          <t>825/63</t>
         </is>
       </c>
       <c r="C121" t="n">
-        <v>282</v>
+        <v>97</v>
       </c>
     </row>
     <row r="122">
@@ -2011,11 +2011,11 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>461</t>
+          <t>1900/4</t>
         </is>
       </c>
       <c r="C122" t="n">
-        <v>282</v>
+        <v>317</v>
       </c>
     </row>
     <row r="123">
@@ -2024,11 +2024,11 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>467</t>
+          <t>9609</t>
         </is>
       </c>
       <c r="C123" t="n">
-        <v>282</v>
+        <v>390</v>
       </c>
     </row>
     <row r="124">
@@ -2037,11 +2037,11 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>468</t>
+          <t>9608/2</t>
         </is>
       </c>
       <c r="C124" t="n">
-        <v>282</v>
+        <v>390</v>
       </c>
     </row>
     <row r="125">
@@ -2050,11 +2050,11 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>.315</t>
+          <t>371</t>
         </is>
       </c>
       <c r="C125" t="n">
-        <v>282</v>
+        <v>404</v>
       </c>
     </row>
     <row r="126">
@@ -2063,11 +2063,11 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>1826</t>
+          <t>373</t>
         </is>
       </c>
       <c r="C126" t="n">
-        <v>282</v>
+        <v>404</v>
       </c>
     </row>
     <row r="127">
@@ -2076,11 +2076,11 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>86</t>
+          <t>1741</t>
         </is>
       </c>
       <c r="C127" t="n">
-        <v>340</v>
+        <v>404</v>
       </c>
     </row>
     <row r="128">
@@ -2089,11 +2089,11 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>397</t>
+          <t>1820</t>
         </is>
       </c>
       <c r="C128" t="n">
-        <v>340</v>
+        <v>404</v>
       </c>
     </row>
     <row r="129">
@@ -2102,11 +2102,11 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>488</t>
+          <t>156</t>
         </is>
       </c>
       <c r="C129" t="n">
-        <v>340</v>
+        <v>404</v>
       </c>
     </row>
     <row r="130">
@@ -2115,11 +2115,11 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4708</t>
         </is>
       </c>
       <c r="C130" t="n">
-        <v>255</v>
+        <v>404</v>
       </c>
     </row>
     <row r="131">
@@ -2128,11 +2128,11 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>1082</t>
+          <t>162/3</t>
         </is>
       </c>
       <c r="C131" t="n">
-        <v>255</v>
+        <v>404</v>
       </c>
     </row>
     <row r="132">
@@ -2141,11 +2141,11 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>403</t>
+          <t>1193</t>
         </is>
       </c>
       <c r="C132" t="n">
-        <v>97</v>
+        <v>404</v>
       </c>
     </row>
     <row r="133">
@@ -2154,11 +2154,11 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>746</t>
+          <t>2762</t>
         </is>
       </c>
       <c r="C133" t="n">
-        <v>97</v>
+        <v>404</v>
       </c>
     </row>
     <row r="134">
@@ -2167,11 +2167,11 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>749</t>
+          <t>2766/3</t>
         </is>
       </c>
       <c r="C134" t="n">
-        <v>97</v>
+        <v>404</v>
       </c>
     </row>
     <row r="135">
@@ -2180,11 +2180,11 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>754</t>
+          <t>2736/8</t>
         </is>
       </c>
       <c r="C135" t="n">
-        <v>97</v>
+        <v>404</v>
       </c>
     </row>
     <row r="136">
@@ -2193,11 +2193,11 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>755</t>
+          <t>2769/1</t>
         </is>
       </c>
       <c r="C136" t="n">
-        <v>97</v>
+        <v>404</v>
       </c>
     </row>
     <row r="137">
@@ -2206,11 +2206,11 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>757</t>
+          <t>2768</t>
         </is>
       </c>
       <c r="C137" t="n">
-        <v>97</v>
+        <v>404</v>
       </c>
     </row>
     <row r="138">
@@ -2219,11 +2219,11 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>758</t>
+          <t>2767</t>
         </is>
       </c>
       <c r="C138" t="n">
-        <v>97</v>
+        <v>404</v>
       </c>
     </row>
     <row r="139">
@@ -2232,11 +2232,11 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>825/63</t>
+          <t>679/2</t>
         </is>
       </c>
       <c r="C139" t="n">
-        <v>97</v>
+        <v>404</v>
       </c>
     </row>
     <row r="140">
@@ -2245,11 +2245,11 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>1900/4</t>
+          <t>.507/2</t>
         </is>
       </c>
       <c r="C140" t="n">
-        <v>317</v>
+        <v>413</v>
       </c>
     </row>
     <row r="141">
@@ -2258,11 +2258,11 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>9609</t>
+          <t>.507/3</t>
         </is>
       </c>
       <c r="C141" t="n">
-        <v>390</v>
+        <v>413</v>
       </c>
     </row>
     <row r="142">
@@ -2271,11 +2271,11 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>9608/2</t>
+          <t>.507/4</t>
         </is>
       </c>
       <c r="C142" t="n">
-        <v>390</v>
+        <v>413</v>
       </c>
     </row>
     <row r="143">
@@ -2284,11 +2284,11 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>371</t>
+          <t>507/5</t>
         </is>
       </c>
       <c r="C143" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="144">
@@ -2297,11 +2297,11 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>373</t>
+          <t>507/6</t>
         </is>
       </c>
       <c r="C144" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="145">
@@ -2310,11 +2310,11 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>1741</t>
+          <t>569/8</t>
         </is>
       </c>
       <c r="C145" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="146">
@@ -2323,11 +2323,11 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>1820</t>
+          <t>.569/5</t>
         </is>
       </c>
       <c r="C146" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="147">
@@ -2336,11 +2336,11 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>156</t>
+          <t>7294</t>
         </is>
       </c>
       <c r="C147" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="148">
@@ -2349,11 +2349,11 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>4708</t>
+          <t>7293/2</t>
         </is>
       </c>
       <c r="C148" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="149">
@@ -2362,11 +2362,11 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>162/3</t>
+          <t>7293/3</t>
         </is>
       </c>
       <c r="C149" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="150">
@@ -2375,11 +2375,11 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>1193</t>
+          <t>1391</t>
         </is>
       </c>
       <c r="C150" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="151">
@@ -2388,11 +2388,11 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>2762</t>
+          <t>7292/1</t>
         </is>
       </c>
       <c r="C151" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="152">
@@ -2401,11 +2401,11 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>2766/3</t>
+          <t>1358</t>
         </is>
       </c>
       <c r="C152" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="153">
@@ -2414,11 +2414,11 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>2736/8</t>
+          <t>7191/4</t>
         </is>
       </c>
       <c r="C153" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="154">
@@ -2427,11 +2427,11 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>2769/1</t>
+          <t>7618/3</t>
         </is>
       </c>
       <c r="C154" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="155">
@@ -2440,11 +2440,11 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>2768</t>
+          <t>7618/4</t>
         </is>
       </c>
       <c r="C155" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="156">
@@ -2453,11 +2453,11 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>2767</t>
+          <t>114</t>
         </is>
       </c>
       <c r="C156" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="157">
@@ -2466,11 +2466,11 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>679/2</t>
+          <t>361</t>
         </is>
       </c>
       <c r="C157" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="158">
@@ -2479,7 +2479,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>.507/2</t>
+          <t>421</t>
         </is>
       </c>
       <c r="C158" t="n">
@@ -2492,7 +2492,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>.507/3</t>
+          <t>13094</t>
         </is>
       </c>
       <c r="C159" t="n">
@@ -2505,7 +2505,7 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>.507/4</t>
+          <t>7290/6</t>
         </is>
       </c>
       <c r="C160" t="n">
@@ -2518,7 +2518,7 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>507/5</t>
+          <t>7288</t>
         </is>
       </c>
       <c r="C161" t="n">
@@ -2531,11 +2531,11 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>507/6</t>
+          <t>45</t>
         </is>
       </c>
       <c r="C162" t="n">
-        <v>413</v>
+        <v>283</v>
       </c>
     </row>
     <row r="163">
@@ -2544,11 +2544,11 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>569/8</t>
+          <t>84/1</t>
         </is>
       </c>
       <c r="C163" t="n">
-        <v>413</v>
+        <v>283</v>
       </c>
     </row>
     <row r="164">
@@ -2557,11 +2557,11 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>.569/5</t>
+          <t>137</t>
         </is>
       </c>
       <c r="C164" t="n">
-        <v>413</v>
+        <v>41</v>
       </c>
     </row>
     <row r="165">
@@ -2570,11 +2570,11 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>7294</t>
+          <t>140</t>
         </is>
       </c>
       <c r="C165" t="n">
-        <v>413</v>
+        <v>41</v>
       </c>
     </row>
     <row r="166">
@@ -2583,11 +2583,11 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>7293/2</t>
+          <t>272</t>
         </is>
       </c>
       <c r="C166" t="n">
-        <v>413</v>
+        <v>79</v>
       </c>
     </row>
     <row r="167">
@@ -2596,11 +2596,11 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>7293/3</t>
+          <t>1881/8</t>
         </is>
       </c>
       <c r="C167" t="n">
-        <v>413</v>
+        <v>79</v>
       </c>
     </row>
     <row r="168">
@@ -2609,11 +2609,11 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>1.391</t>
+          <t>94/6</t>
         </is>
       </c>
       <c r="C168" t="n">
-        <v>413</v>
+        <v>251</v>
       </c>
     </row>
     <row r="169">
@@ -2622,11 +2622,11 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>7292/1</t>
+          <t>243</t>
         </is>
       </c>
       <c r="C169" t="n">
-        <v>413</v>
+        <v>253</v>
       </c>
     </row>
     <row r="170">
@@ -2635,11 +2635,11 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>1.358</t>
+          <t>295</t>
         </is>
       </c>
       <c r="C170" t="n">
-        <v>413</v>
+        <v>253</v>
       </c>
     </row>
     <row r="171">
@@ -2648,11 +2648,11 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>1.359</t>
+          <t>1403</t>
         </is>
       </c>
       <c r="C171" t="n">
-        <v>413</v>
+        <v>268</v>
       </c>
     </row>
     <row r="172">
@@ -2661,11 +2661,11 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>7191/4</t>
+          <t>316</t>
         </is>
       </c>
       <c r="C172" t="n">
-        <v>413</v>
+        <v>442</v>
       </c>
     </row>
     <row r="173">
@@ -2674,11 +2674,11 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>1.270</t>
+          <t>53</t>
         </is>
       </c>
       <c r="C173" t="n">
-        <v>413</v>
+        <v>215</v>
       </c>
     </row>
     <row r="174">
@@ -2687,11 +2687,11 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>7618/3</t>
+          <t>454</t>
         </is>
       </c>
       <c r="C174" t="n">
-        <v>413</v>
+        <v>215</v>
       </c>
     </row>
     <row r="175">
@@ -2700,11 +2700,11 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>7618/4</t>
+          <t>420/80</t>
         </is>
       </c>
       <c r="C175" t="n">
-        <v>413</v>
+        <v>215</v>
       </c>
     </row>
     <row r="176">
@@ -2713,11 +2713,11 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>114</t>
+          <t>420/92</t>
         </is>
       </c>
       <c r="C176" t="n">
-        <v>413</v>
+        <v>215</v>
       </c>
     </row>
     <row r="177">
@@ -2726,11 +2726,11 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>361</t>
+          <t>420/93</t>
         </is>
       </c>
       <c r="C177" t="n">
-        <v>413</v>
+        <v>215</v>
       </c>
     </row>
     <row r="178">
@@ -2739,11 +2739,11 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>421</t>
+          <t>420/94</t>
         </is>
       </c>
       <c r="C178" t="n">
-        <v>413</v>
+        <v>215</v>
       </c>
     </row>
     <row r="179">
@@ -2752,11 +2752,11 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>13094</t>
+          <t>420/95</t>
         </is>
       </c>
       <c r="C179" t="n">
-        <v>413</v>
+        <v>215</v>
       </c>
     </row>
     <row r="180">
@@ -2765,11 +2765,11 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>7290/6</t>
+          <t>420/96</t>
         </is>
       </c>
       <c r="C180" t="n">
-        <v>413</v>
+        <v>215</v>
       </c>
     </row>
     <row r="181">
@@ -2778,11 +2778,11 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>7288</t>
+          <t>420/97</t>
         </is>
       </c>
       <c r="C181" t="n">
-        <v>413</v>
+        <v>215</v>
       </c>
     </row>
     <row r="182">
@@ -2791,11 +2791,11 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>420/101</t>
         </is>
       </c>
       <c r="C182" t="n">
-        <v>283</v>
+        <v>215</v>
       </c>
     </row>
     <row r="183">
@@ -2804,11 +2804,11 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>84/1</t>
+          <t>420/102</t>
         </is>
       </c>
       <c r="C183" t="n">
-        <v>283</v>
+        <v>215</v>
       </c>
     </row>
     <row r="184">
@@ -2817,11 +2817,11 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>137</t>
+          <t>420/106</t>
         </is>
       </c>
       <c r="C184" t="n">
-        <v>41</v>
+        <v>215</v>
       </c>
     </row>
     <row r="185">
@@ -2830,11 +2830,11 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>140</t>
+          <t>420/107</t>
         </is>
       </c>
       <c r="C185" t="n">
-        <v>41</v>
+        <v>215</v>
       </c>
     </row>
     <row r="186">
@@ -2843,11 +2843,11 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>272</t>
+          <t>420/109</t>
         </is>
       </c>
       <c r="C186" t="n">
-        <v>79</v>
+        <v>215</v>
       </c>
     </row>
     <row r="187">
@@ -2856,11 +2856,11 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>1881/8</t>
+          <t>420/110</t>
         </is>
       </c>
       <c r="C187" t="n">
-        <v>79</v>
+        <v>215</v>
       </c>
     </row>
     <row r="188">
@@ -2869,11 +2869,11 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>94/6</t>
+          <t>705/11</t>
         </is>
       </c>
       <c r="C188" t="n">
-        <v>251</v>
+        <v>215</v>
       </c>
     </row>
     <row r="189">
@@ -2882,11 +2882,11 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>243</t>
+          <t>756</t>
         </is>
       </c>
       <c r="C189" t="n">
-        <v>253</v>
+        <v>215</v>
       </c>
     </row>
     <row r="190">
@@ -2895,11 +2895,11 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>295</t>
+          <t>798/3</t>
         </is>
       </c>
       <c r="C190" t="n">
-        <v>253</v>
+        <v>215</v>
       </c>
     </row>
     <row r="191">
@@ -2908,11 +2908,11 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>1403</t>
+          <t>1411/1</t>
         </is>
       </c>
       <c r="C191" t="n">
-        <v>268</v>
+        <v>256</v>
       </c>
     </row>
     <row r="192">
@@ -2921,11 +2921,11 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>316</t>
+          <t>1411/2</t>
         </is>
       </c>
       <c r="C192" t="n">
-        <v>442</v>
+        <v>256</v>
       </c>
     </row>
     <row r="193">
@@ -2934,11 +2934,11 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>1411/3</t>
         </is>
       </c>
       <c r="C193" t="n">
-        <v>215</v>
+        <v>256</v>
       </c>
     </row>
     <row r="194">
@@ -2947,11 +2947,11 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>454</t>
+          <t>1411/4</t>
         </is>
       </c>
       <c r="C194" t="n">
-        <v>215</v>
+        <v>256</v>
       </c>
     </row>
     <row r="195">
@@ -2960,11 +2960,11 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>420/80</t>
+          <t>1411/5</t>
         </is>
       </c>
       <c r="C195" t="n">
-        <v>215</v>
+        <v>256</v>
       </c>
     </row>
     <row r="196">
@@ -2973,11 +2973,11 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>420/92</t>
+          <t>1412</t>
         </is>
       </c>
       <c r="C196" t="n">
-        <v>215</v>
+        <v>256</v>
       </c>
     </row>
     <row r="197">
@@ -2986,11 +2986,11 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>420/93</t>
+          <t>1488</t>
         </is>
       </c>
       <c r="C197" t="n">
-        <v>215</v>
+        <v>256</v>
       </c>
     </row>
     <row r="198">
@@ -2999,11 +2999,11 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>420/94</t>
+          <t>1117/2</t>
         </is>
       </c>
       <c r="C198" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="199">
@@ -3012,11 +3012,11 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>420/95</t>
+          <t>1230/100</t>
         </is>
       </c>
       <c r="C199" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="200">
@@ -3025,11 +3025,11 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>420/96</t>
+          <t>1230/115</t>
         </is>
       </c>
       <c r="C200" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="201">
@@ -3038,11 +3038,11 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>420/97</t>
+          <t>1230/85</t>
         </is>
       </c>
       <c r="C201" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="202">
@@ -3051,11 +3051,11 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>420/101</t>
+          <t>1230/86</t>
         </is>
       </c>
       <c r="C202" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="203">
@@ -3064,11 +3064,11 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>420/102</t>
+          <t>1230/87</t>
         </is>
       </c>
       <c r="C203" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="204">
@@ -3077,11 +3077,11 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>420/106</t>
+          <t>1230/88</t>
         </is>
       </c>
       <c r="C204" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="205">
@@ -3090,11 +3090,11 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>420/107</t>
+          <t>1303/1</t>
         </is>
       </c>
       <c r="C205" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="206">
@@ -3103,11 +3103,11 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>420/109</t>
+          <t>1303/2</t>
         </is>
       </c>
       <c r="C206" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="207">
@@ -3116,11 +3116,11 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>420/110</t>
+          <t>1309</t>
         </is>
       </c>
       <c r="C207" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="208">
@@ -3129,11 +3129,11 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>705/11</t>
+          <t>1330</t>
         </is>
       </c>
       <c r="C208" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="209">
@@ -3142,11 +3142,11 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>756</t>
+          <t>1334</t>
         </is>
       </c>
       <c r="C209" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="210">
@@ -3155,11 +3155,11 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>798/3</t>
+          <t>1346</t>
         </is>
       </c>
       <c r="C210" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="211">
@@ -3168,11 +3168,11 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>1411/1</t>
+          <t>1369/1</t>
         </is>
       </c>
       <c r="C211" t="n">
-        <v>256</v>
+        <v>193</v>
       </c>
     </row>
     <row r="212">
@@ -3181,11 +3181,11 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>1411/2</t>
+          <t>194/4</t>
         </is>
       </c>
       <c r="C212" t="n">
-        <v>256</v>
+        <v>193</v>
       </c>
     </row>
     <row r="213">
@@ -3194,11 +3194,11 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>1411/3</t>
+          <t>254/2</t>
         </is>
       </c>
       <c r="C213" t="n">
-        <v>256</v>
+        <v>193</v>
       </c>
     </row>
     <row r="214">
@@ -3207,11 +3207,11 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>1411/4</t>
+          <t>337/5</t>
         </is>
       </c>
       <c r="C214" t="n">
-        <v>256</v>
+        <v>193</v>
       </c>
     </row>
     <row r="215">
@@ -3220,11 +3220,11 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>1411/5</t>
+          <t>393/1</t>
         </is>
       </c>
       <c r="C215" t="n">
-        <v>256</v>
+        <v>193</v>
       </c>
     </row>
     <row r="216">
@@ -3233,11 +3233,11 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>1412</t>
+          <t>393/2</t>
         </is>
       </c>
       <c r="C216" t="n">
-        <v>256</v>
+        <v>193</v>
       </c>
     </row>
     <row r="217">
@@ -3246,11 +3246,11 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>1488</t>
+          <t>393/3</t>
         </is>
       </c>
       <c r="C217" t="n">
-        <v>256</v>
+        <v>193</v>
       </c>
     </row>
     <row r="218">
@@ -3259,7 +3259,7 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>254/2</t>
+          <t>465</t>
         </is>
       </c>
       <c r="C218" t="n">
@@ -3272,7 +3272,7 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>337/5</t>
+          <t>614</t>
         </is>
       </c>
       <c r="C219" t="n">
@@ -3285,257 +3285,10 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>393/1</t>
+          <t>384/1</t>
         </is>
       </c>
       <c r="C220" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="221">
-      <c r="A221" s="1" t="n">
-        <v>219</v>
-      </c>
-      <c r="B221" t="inlineStr">
-        <is>
-          <t>393/2</t>
-        </is>
-      </c>
-      <c r="C221" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="222">
-      <c r="A222" s="1" t="n">
-        <v>220</v>
-      </c>
-      <c r="B222" t="inlineStr">
-        <is>
-          <t>393/3</t>
-        </is>
-      </c>
-      <c r="C222" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="223">
-      <c r="A223" s="1" t="n">
-        <v>221</v>
-      </c>
-      <c r="B223" t="inlineStr">
-        <is>
-          <t>465</t>
-        </is>
-      </c>
-      <c r="C223" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="224">
-      <c r="A224" s="1" t="n">
-        <v>222</v>
-      </c>
-      <c r="B224" t="inlineStr">
-        <is>
-          <t>614</t>
-        </is>
-      </c>
-      <c r="C224" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="225">
-      <c r="A225" s="1" t="n">
-        <v>223</v>
-      </c>
-      <c r="B225" t="inlineStr">
-        <is>
-          <t>1303/1</t>
-        </is>
-      </c>
-      <c r="C225" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="226">
-      <c r="A226" s="1" t="n">
-        <v>224</v>
-      </c>
-      <c r="B226" t="inlineStr">
-        <is>
-          <t>1303/2</t>
-        </is>
-      </c>
-      <c r="C226" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="227">
-      <c r="A227" s="1" t="n">
-        <v>225</v>
-      </c>
-      <c r="B227" t="inlineStr">
-        <is>
-          <t>1309</t>
-        </is>
-      </c>
-      <c r="C227" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="228">
-      <c r="A228" s="1" t="n">
-        <v>226</v>
-      </c>
-      <c r="B228" t="inlineStr">
-        <is>
-          <t>1330</t>
-        </is>
-      </c>
-      <c r="C228" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="229">
-      <c r="A229" s="1" t="n">
-        <v>227</v>
-      </c>
-      <c r="B229" t="inlineStr">
-        <is>
-          <t>1334</t>
-        </is>
-      </c>
-      <c r="C229" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="230">
-      <c r="A230" s="1" t="n">
-        <v>228</v>
-      </c>
-      <c r="B230" t="inlineStr">
-        <is>
-          <t>1346</t>
-        </is>
-      </c>
-      <c r="C230" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="231">
-      <c r="A231" s="1" t="n">
-        <v>229</v>
-      </c>
-      <c r="B231" t="inlineStr">
-        <is>
-          <t>1369/1</t>
-        </is>
-      </c>
-      <c r="C231" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="232">
-      <c r="A232" s="1" t="n">
-        <v>230</v>
-      </c>
-      <c r="B232" t="inlineStr">
-        <is>
-          <t>1117/2</t>
-        </is>
-      </c>
-      <c r="C232" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="233">
-      <c r="A233" s="1" t="n">
-        <v>231</v>
-      </c>
-      <c r="B233" t="inlineStr">
-        <is>
-          <t>1230/85</t>
-        </is>
-      </c>
-      <c r="C233" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="234">
-      <c r="A234" s="1" t="n">
-        <v>232</v>
-      </c>
-      <c r="B234" t="inlineStr">
-        <is>
-          <t>1230/86</t>
-        </is>
-      </c>
-      <c r="C234" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="235">
-      <c r="A235" s="1" t="n">
-        <v>233</v>
-      </c>
-      <c r="B235" t="inlineStr">
-        <is>
-          <t>1230/87</t>
-        </is>
-      </c>
-      <c r="C235" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="236">
-      <c r="A236" s="1" t="n">
-        <v>234</v>
-      </c>
-      <c r="B236" t="inlineStr">
-        <is>
-          <t>1230/88</t>
-        </is>
-      </c>
-      <c r="C236" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="237">
-      <c r="A237" s="1" t="n">
-        <v>235</v>
-      </c>
-      <c r="B237" t="inlineStr">
-        <is>
-          <t>1230/100</t>
-        </is>
-      </c>
-      <c r="C237" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="238">
-      <c r="A238" s="1" t="n">
-        <v>236</v>
-      </c>
-      <c r="B238" t="inlineStr">
-        <is>
-          <t>1230/115</t>
-        </is>
-      </c>
-      <c r="C238" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="239">
-      <c r="A239" s="1" t="n">
-        <v>237</v>
-      </c>
-      <c r="B239" t="inlineStr">
-        <is>
-          <t>194/4</t>
-        </is>
-      </c>
-      <c r="C239" t="n">
         <v>193</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Latest data: Wed Feb 14 12:15:36 UTC 2024
</commit_message>
<xml_diff>
--- a/docs/particelle_non_trovate.xlsx
+++ b/docs/particelle_non_trovate.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C220"/>
+  <dimension ref="A1:C197"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1439,7 +1439,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>587</t>
+          <t>466</t>
         </is>
       </c>
       <c r="C78" t="n">
@@ -1452,11 +1452,11 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>588</t>
+          <t>31</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>213</v>
+        <v>282</v>
       </c>
     </row>
     <row r="80">
@@ -1465,11 +1465,11 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>722</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>213</v>
+        <v>282</v>
       </c>
     </row>
     <row r="81">
@@ -1478,11 +1478,11 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>642/2</t>
+          <t>410</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>213</v>
+        <v>282</v>
       </c>
     </row>
     <row r="82">
@@ -1491,11 +1491,11 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>116</t>
+          <t>412</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>213</v>
+        <v>282</v>
       </c>
     </row>
     <row r="83">
@@ -1504,11 +1504,11 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>151</t>
+          <t>461</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>213</v>
+        <v>282</v>
       </c>
     </row>
     <row r="84">
@@ -1517,11 +1517,11 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>466</t>
+          <t>467</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>213</v>
+        <v>282</v>
       </c>
     </row>
     <row r="85">
@@ -1530,11 +1530,11 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>1479</t>
+          <t>468</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>265</v>
+        <v>282</v>
       </c>
     </row>
     <row r="86">
@@ -1543,11 +1543,11 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>2243</t>
+          <t>.315</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>265</v>
+        <v>282</v>
       </c>
     </row>
     <row r="87">
@@ -1556,11 +1556,11 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>901</t>
+          <t>1826</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>265</v>
+        <v>282</v>
       </c>
     </row>
     <row r="88">
@@ -1569,11 +1569,11 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>842</t>
+          <t>86</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>265</v>
+        <v>340</v>
       </c>
     </row>
     <row r="89">
@@ -1582,11 +1582,11 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>656</t>
+          <t>397</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>245</v>
+        <v>340</v>
       </c>
     </row>
     <row r="90">
@@ -1595,11 +1595,11 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>811</t>
+          <t>488</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>245</v>
+        <v>340</v>
       </c>
     </row>
     <row r="91">
@@ -1608,11 +1608,11 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>370</t>
+          <t>403</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>245</v>
+        <v>97</v>
       </c>
     </row>
     <row r="92">
@@ -1621,11 +1621,11 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>537</t>
+          <t>746</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>245</v>
+        <v>97</v>
       </c>
     </row>
     <row r="93">
@@ -1634,11 +1634,11 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>4812</t>
+          <t>749</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>245</v>
+        <v>97</v>
       </c>
     </row>
     <row r="94">
@@ -1647,11 +1647,11 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>5016</t>
+          <t>754</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>245</v>
+        <v>97</v>
       </c>
     </row>
     <row r="95">
@@ -1660,11 +1660,11 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>755</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>245</v>
+        <v>97</v>
       </c>
     </row>
     <row r="96">
@@ -1673,11 +1673,11 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>1858</t>
+          <t>757</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>245</v>
+        <v>97</v>
       </c>
     </row>
     <row r="97">
@@ -1686,11 +1686,11 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>2421</t>
+          <t>758</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>245</v>
+        <v>97</v>
       </c>
     </row>
     <row r="98">
@@ -1699,11 +1699,11 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>2436</t>
+          <t>825/63</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>245</v>
+        <v>97</v>
       </c>
     </row>
     <row r="99">
@@ -1712,11 +1712,11 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>609</t>
+          <t>1900/4</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>414</v>
+        <v>317</v>
       </c>
     </row>
     <row r="100">
@@ -1725,11 +1725,11 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>912</t>
+          <t>9609</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>414</v>
+        <v>390</v>
       </c>
     </row>
     <row r="101">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>1419</t>
+          <t>9608/2</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>414</v>
+        <v>390</v>
       </c>
     </row>
     <row r="102">
@@ -1751,11 +1751,11 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>371</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>282</v>
+        <v>404</v>
       </c>
     </row>
     <row r="103">
@@ -1764,11 +1764,11 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>722</t>
+          <t>373</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>282</v>
+        <v>404</v>
       </c>
     </row>
     <row r="104">
@@ -1777,11 +1777,11 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>410</t>
+          <t>1741</t>
         </is>
       </c>
       <c r="C104" t="n">
-        <v>282</v>
+        <v>404</v>
       </c>
     </row>
     <row r="105">
@@ -1790,11 +1790,11 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>412</t>
+          <t>1820</t>
         </is>
       </c>
       <c r="C105" t="n">
-        <v>282</v>
+        <v>404</v>
       </c>
     </row>
     <row r="106">
@@ -1803,11 +1803,11 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>461</t>
+          <t>156</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>282</v>
+        <v>404</v>
       </c>
     </row>
     <row r="107">
@@ -1816,11 +1816,11 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>467</t>
+          <t>4708</t>
         </is>
       </c>
       <c r="C107" t="n">
-        <v>282</v>
+        <v>404</v>
       </c>
     </row>
     <row r="108">
@@ -1829,11 +1829,11 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>468</t>
+          <t>162/3</t>
         </is>
       </c>
       <c r="C108" t="n">
-        <v>282</v>
+        <v>404</v>
       </c>
     </row>
     <row r="109">
@@ -1842,11 +1842,11 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>.315</t>
+          <t>1193</t>
         </is>
       </c>
       <c r="C109" t="n">
-        <v>282</v>
+        <v>404</v>
       </c>
     </row>
     <row r="110">
@@ -1855,11 +1855,11 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>1826</t>
+          <t>2762</t>
         </is>
       </c>
       <c r="C110" t="n">
-        <v>282</v>
+        <v>404</v>
       </c>
     </row>
     <row r="111">
@@ -1868,11 +1868,11 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>86</t>
+          <t>2766/3</t>
         </is>
       </c>
       <c r="C111" t="n">
-        <v>340</v>
+        <v>404</v>
       </c>
     </row>
     <row r="112">
@@ -1881,11 +1881,11 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>397</t>
+          <t>2736/8</t>
         </is>
       </c>
       <c r="C112" t="n">
-        <v>340</v>
+        <v>404</v>
       </c>
     </row>
     <row r="113">
@@ -1894,11 +1894,11 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>488</t>
+          <t>2769/1</t>
         </is>
       </c>
       <c r="C113" t="n">
-        <v>340</v>
+        <v>404</v>
       </c>
     </row>
     <row r="114">
@@ -1907,11 +1907,11 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>403</t>
+          <t>2768</t>
         </is>
       </c>
       <c r="C114" t="n">
-        <v>97</v>
+        <v>404</v>
       </c>
     </row>
     <row r="115">
@@ -1920,11 +1920,11 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>746</t>
+          <t>2767</t>
         </is>
       </c>
       <c r="C115" t="n">
-        <v>97</v>
+        <v>404</v>
       </c>
     </row>
     <row r="116">
@@ -1933,11 +1933,11 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>749</t>
+          <t>679/2</t>
         </is>
       </c>
       <c r="C116" t="n">
-        <v>97</v>
+        <v>404</v>
       </c>
     </row>
     <row r="117">
@@ -1946,11 +1946,11 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>754</t>
+          <t>.507/2</t>
         </is>
       </c>
       <c r="C117" t="n">
-        <v>97</v>
+        <v>413</v>
       </c>
     </row>
     <row r="118">
@@ -1959,11 +1959,11 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>755</t>
+          <t>.507/3</t>
         </is>
       </c>
       <c r="C118" t="n">
-        <v>97</v>
+        <v>413</v>
       </c>
     </row>
     <row r="119">
@@ -1972,11 +1972,11 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>757</t>
+          <t>.507/4</t>
         </is>
       </c>
       <c r="C119" t="n">
-        <v>97</v>
+        <v>413</v>
       </c>
     </row>
     <row r="120">
@@ -1985,11 +1985,11 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>758</t>
+          <t>507/5</t>
         </is>
       </c>
       <c r="C120" t="n">
-        <v>97</v>
+        <v>413</v>
       </c>
     </row>
     <row r="121">
@@ -1998,11 +1998,11 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>825/63</t>
+          <t>507/6</t>
         </is>
       </c>
       <c r="C121" t="n">
-        <v>97</v>
+        <v>413</v>
       </c>
     </row>
     <row r="122">
@@ -2011,11 +2011,11 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>1900/4</t>
+          <t>569/8</t>
         </is>
       </c>
       <c r="C122" t="n">
-        <v>317</v>
+        <v>413</v>
       </c>
     </row>
     <row r="123">
@@ -2024,11 +2024,11 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>9609</t>
+          <t>.569/5</t>
         </is>
       </c>
       <c r="C123" t="n">
-        <v>390</v>
+        <v>413</v>
       </c>
     </row>
     <row r="124">
@@ -2037,11 +2037,11 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>9608/2</t>
+          <t>7294</t>
         </is>
       </c>
       <c r="C124" t="n">
-        <v>390</v>
+        <v>413</v>
       </c>
     </row>
     <row r="125">
@@ -2050,11 +2050,11 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>371</t>
+          <t>7293/2</t>
         </is>
       </c>
       <c r="C125" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="126">
@@ -2063,11 +2063,11 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>373</t>
+          <t>7293/3</t>
         </is>
       </c>
       <c r="C126" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="127">
@@ -2076,11 +2076,11 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>1741</t>
+          <t>1391</t>
         </is>
       </c>
       <c r="C127" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="128">
@@ -2089,11 +2089,11 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>1820</t>
+          <t>7292/1</t>
         </is>
       </c>
       <c r="C128" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="129">
@@ -2102,11 +2102,11 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>156</t>
+          <t>1358</t>
         </is>
       </c>
       <c r="C129" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="130">
@@ -2115,11 +2115,11 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>4708</t>
+          <t>7191/4</t>
         </is>
       </c>
       <c r="C130" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="131">
@@ -2128,11 +2128,11 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>162/3</t>
+          <t>7618/3</t>
         </is>
       </c>
       <c r="C131" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="132">
@@ -2141,11 +2141,11 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>1193</t>
+          <t>7618/4</t>
         </is>
       </c>
       <c r="C132" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="133">
@@ -2154,11 +2154,11 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>2762</t>
+          <t>114</t>
         </is>
       </c>
       <c r="C133" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="134">
@@ -2167,11 +2167,11 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>2766/3</t>
+          <t>361</t>
         </is>
       </c>
       <c r="C134" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="135">
@@ -2180,11 +2180,11 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>2736/8</t>
+          <t>421</t>
         </is>
       </c>
       <c r="C135" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="136">
@@ -2193,11 +2193,11 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>2769/1</t>
+          <t>13094</t>
         </is>
       </c>
       <c r="C136" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="137">
@@ -2206,11 +2206,11 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>2768</t>
+          <t>7290/6</t>
         </is>
       </c>
       <c r="C137" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="138">
@@ -2219,11 +2219,11 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>2767</t>
+          <t>7288</t>
         </is>
       </c>
       <c r="C138" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="139">
@@ -2232,11 +2232,11 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>679/2</t>
+          <t>45</t>
         </is>
       </c>
       <c r="C139" t="n">
-        <v>404</v>
+        <v>283</v>
       </c>
     </row>
     <row r="140">
@@ -2245,11 +2245,11 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>.507/2</t>
+          <t>84/1</t>
         </is>
       </c>
       <c r="C140" t="n">
-        <v>413</v>
+        <v>283</v>
       </c>
     </row>
     <row r="141">
@@ -2258,11 +2258,11 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>.507/3</t>
+          <t>137</t>
         </is>
       </c>
       <c r="C141" t="n">
-        <v>413</v>
+        <v>41</v>
       </c>
     </row>
     <row r="142">
@@ -2271,11 +2271,11 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>.507/4</t>
+          <t>140</t>
         </is>
       </c>
       <c r="C142" t="n">
-        <v>413</v>
+        <v>41</v>
       </c>
     </row>
     <row r="143">
@@ -2284,11 +2284,11 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>507/5</t>
+          <t>272</t>
         </is>
       </c>
       <c r="C143" t="n">
-        <v>413</v>
+        <v>79</v>
       </c>
     </row>
     <row r="144">
@@ -2297,11 +2297,11 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>507/6</t>
+          <t>1881/8</t>
         </is>
       </c>
       <c r="C144" t="n">
-        <v>413</v>
+        <v>79</v>
       </c>
     </row>
     <row r="145">
@@ -2310,11 +2310,11 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>569/8</t>
+          <t>94/6</t>
         </is>
       </c>
       <c r="C145" t="n">
-        <v>413</v>
+        <v>251</v>
       </c>
     </row>
     <row r="146">
@@ -2323,11 +2323,11 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>.569/5</t>
+          <t>243</t>
         </is>
       </c>
       <c r="C146" t="n">
-        <v>413</v>
+        <v>253</v>
       </c>
     </row>
     <row r="147">
@@ -2336,11 +2336,11 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>7294</t>
+          <t>295</t>
         </is>
       </c>
       <c r="C147" t="n">
-        <v>413</v>
+        <v>253</v>
       </c>
     </row>
     <row r="148">
@@ -2349,11 +2349,11 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>7293/2</t>
+          <t>1403</t>
         </is>
       </c>
       <c r="C148" t="n">
-        <v>413</v>
+        <v>268</v>
       </c>
     </row>
     <row r="149">
@@ -2362,11 +2362,11 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>7293/3</t>
+          <t>316</t>
         </is>
       </c>
       <c r="C149" t="n">
-        <v>413</v>
+        <v>442</v>
       </c>
     </row>
     <row r="150">
@@ -2375,11 +2375,11 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>1391</t>
+          <t>53</t>
         </is>
       </c>
       <c r="C150" t="n">
-        <v>413</v>
+        <v>215</v>
       </c>
     </row>
     <row r="151">
@@ -2388,11 +2388,11 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>7292/1</t>
+          <t>454</t>
         </is>
       </c>
       <c r="C151" t="n">
-        <v>413</v>
+        <v>215</v>
       </c>
     </row>
     <row r="152">
@@ -2401,11 +2401,11 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>1358</t>
+          <t>420/80</t>
         </is>
       </c>
       <c r="C152" t="n">
-        <v>413</v>
+        <v>215</v>
       </c>
     </row>
     <row r="153">
@@ -2414,11 +2414,11 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>7191/4</t>
+          <t>420/92</t>
         </is>
       </c>
       <c r="C153" t="n">
-        <v>413</v>
+        <v>215</v>
       </c>
     </row>
     <row r="154">
@@ -2427,11 +2427,11 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>7618/3</t>
+          <t>420/93</t>
         </is>
       </c>
       <c r="C154" t="n">
-        <v>413</v>
+        <v>215</v>
       </c>
     </row>
     <row r="155">
@@ -2440,11 +2440,11 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>7618/4</t>
+          <t>420/94</t>
         </is>
       </c>
       <c r="C155" t="n">
-        <v>413</v>
+        <v>215</v>
       </c>
     </row>
     <row r="156">
@@ -2453,11 +2453,11 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>114</t>
+          <t>420/95</t>
         </is>
       </c>
       <c r="C156" t="n">
-        <v>413</v>
+        <v>215</v>
       </c>
     </row>
     <row r="157">
@@ -2466,11 +2466,11 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>361</t>
+          <t>420/96</t>
         </is>
       </c>
       <c r="C157" t="n">
-        <v>413</v>
+        <v>215</v>
       </c>
     </row>
     <row r="158">
@@ -2479,11 +2479,11 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>421</t>
+          <t>420/97</t>
         </is>
       </c>
       <c r="C158" t="n">
-        <v>413</v>
+        <v>215</v>
       </c>
     </row>
     <row r="159">
@@ -2492,11 +2492,11 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>13094</t>
+          <t>420/101</t>
         </is>
       </c>
       <c r="C159" t="n">
-        <v>413</v>
+        <v>215</v>
       </c>
     </row>
     <row r="160">
@@ -2505,11 +2505,11 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>7290/6</t>
+          <t>420/102</t>
         </is>
       </c>
       <c r="C160" t="n">
-        <v>413</v>
+        <v>215</v>
       </c>
     </row>
     <row r="161">
@@ -2518,11 +2518,11 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>7288</t>
+          <t>420/106</t>
         </is>
       </c>
       <c r="C161" t="n">
-        <v>413</v>
+        <v>215</v>
       </c>
     </row>
     <row r="162">
@@ -2531,11 +2531,11 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>420/107</t>
         </is>
       </c>
       <c r="C162" t="n">
-        <v>283</v>
+        <v>215</v>
       </c>
     </row>
     <row r="163">
@@ -2544,11 +2544,11 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>84/1</t>
+          <t>420/109</t>
         </is>
       </c>
       <c r="C163" t="n">
-        <v>283</v>
+        <v>215</v>
       </c>
     </row>
     <row r="164">
@@ -2557,11 +2557,11 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>137</t>
+          <t>420/110</t>
         </is>
       </c>
       <c r="C164" t="n">
-        <v>41</v>
+        <v>215</v>
       </c>
     </row>
     <row r="165">
@@ -2570,11 +2570,11 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>140</t>
+          <t>705/11</t>
         </is>
       </c>
       <c r="C165" t="n">
-        <v>41</v>
+        <v>215</v>
       </c>
     </row>
     <row r="166">
@@ -2583,11 +2583,11 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>272</t>
+          <t>756</t>
         </is>
       </c>
       <c r="C166" t="n">
-        <v>79</v>
+        <v>215</v>
       </c>
     </row>
     <row r="167">
@@ -2596,11 +2596,11 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>1881/8</t>
+          <t>798/3</t>
         </is>
       </c>
       <c r="C167" t="n">
-        <v>79</v>
+        <v>215</v>
       </c>
     </row>
     <row r="168">
@@ -2609,11 +2609,11 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>94/6</t>
+          <t>1411/1</t>
         </is>
       </c>
       <c r="C168" t="n">
-        <v>251</v>
+        <v>256</v>
       </c>
     </row>
     <row r="169">
@@ -2622,11 +2622,11 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>243</t>
+          <t>1411/2</t>
         </is>
       </c>
       <c r="C169" t="n">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
     <row r="170">
@@ -2635,11 +2635,11 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>295</t>
+          <t>1411/3</t>
         </is>
       </c>
       <c r="C170" t="n">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
     <row r="171">
@@ -2648,11 +2648,11 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>1403</t>
+          <t>1411/4</t>
         </is>
       </c>
       <c r="C171" t="n">
-        <v>268</v>
+        <v>256</v>
       </c>
     </row>
     <row r="172">
@@ -2661,11 +2661,11 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>316</t>
+          <t>1411/5</t>
         </is>
       </c>
       <c r="C172" t="n">
-        <v>442</v>
+        <v>256</v>
       </c>
     </row>
     <row r="173">
@@ -2674,11 +2674,11 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>1412</t>
         </is>
       </c>
       <c r="C173" t="n">
-        <v>215</v>
+        <v>256</v>
       </c>
     </row>
     <row r="174">
@@ -2687,11 +2687,11 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>454</t>
+          <t>1488</t>
         </is>
       </c>
       <c r="C174" t="n">
-        <v>215</v>
+        <v>256</v>
       </c>
     </row>
     <row r="175">
@@ -2700,11 +2700,11 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>420/80</t>
+          <t>1117/2</t>
         </is>
       </c>
       <c r="C175" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="176">
@@ -2713,11 +2713,11 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>420/92</t>
+          <t>1230/100</t>
         </is>
       </c>
       <c r="C176" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="177">
@@ -2726,11 +2726,11 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>420/93</t>
+          <t>1230/115</t>
         </is>
       </c>
       <c r="C177" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="178">
@@ -2739,11 +2739,11 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>420/94</t>
+          <t>1230/85</t>
         </is>
       </c>
       <c r="C178" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="179">
@@ -2752,11 +2752,11 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>420/95</t>
+          <t>1230/86</t>
         </is>
       </c>
       <c r="C179" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="180">
@@ -2765,11 +2765,11 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>420/96</t>
+          <t>1230/87</t>
         </is>
       </c>
       <c r="C180" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="181">
@@ -2778,11 +2778,11 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>420/97</t>
+          <t>1230/88</t>
         </is>
       </c>
       <c r="C181" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="182">
@@ -2791,11 +2791,11 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>420/101</t>
+          <t>1303/1</t>
         </is>
       </c>
       <c r="C182" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="183">
@@ -2804,11 +2804,11 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>420/102</t>
+          <t>1303/2</t>
         </is>
       </c>
       <c r="C183" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="184">
@@ -2817,11 +2817,11 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>420/106</t>
+          <t>1309</t>
         </is>
       </c>
       <c r="C184" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="185">
@@ -2830,11 +2830,11 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>420/107</t>
+          <t>1330</t>
         </is>
       </c>
       <c r="C185" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="186">
@@ -2843,11 +2843,11 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>420/109</t>
+          <t>1334</t>
         </is>
       </c>
       <c r="C186" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="187">
@@ -2856,11 +2856,11 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>420/110</t>
+          <t>1346</t>
         </is>
       </c>
       <c r="C187" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="188">
@@ -2869,11 +2869,11 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>705/11</t>
+          <t>1369/1</t>
         </is>
       </c>
       <c r="C188" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="189">
@@ -2882,11 +2882,11 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>756</t>
+          <t>194/4</t>
         </is>
       </c>
       <c r="C189" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="190">
@@ -2895,11 +2895,11 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>798/3</t>
+          <t>254/2</t>
         </is>
       </c>
       <c r="C190" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="191">
@@ -2908,11 +2908,11 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>1411/1</t>
+          <t>337/5</t>
         </is>
       </c>
       <c r="C191" t="n">
-        <v>256</v>
+        <v>193</v>
       </c>
     </row>
     <row r="192">
@@ -2921,11 +2921,11 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>1411/2</t>
+          <t>393/1</t>
         </is>
       </c>
       <c r="C192" t="n">
-        <v>256</v>
+        <v>193</v>
       </c>
     </row>
     <row r="193">
@@ -2934,11 +2934,11 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>1411/3</t>
+          <t>393/2</t>
         </is>
       </c>
       <c r="C193" t="n">
-        <v>256</v>
+        <v>193</v>
       </c>
     </row>
     <row r="194">
@@ -2947,11 +2947,11 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>1411/4</t>
+          <t>393/3</t>
         </is>
       </c>
       <c r="C194" t="n">
-        <v>256</v>
+        <v>193</v>
       </c>
     </row>
     <row r="195">
@@ -2960,11 +2960,11 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>1411/5</t>
+          <t>465</t>
         </is>
       </c>
       <c r="C195" t="n">
-        <v>256</v>
+        <v>193</v>
       </c>
     </row>
     <row r="196">
@@ -2973,11 +2973,11 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>1412</t>
+          <t>614</t>
         </is>
       </c>
       <c r="C196" t="n">
-        <v>256</v>
+        <v>193</v>
       </c>
     </row>
     <row r="197">
@@ -2986,309 +2986,10 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>1488</t>
+          <t>384/1</t>
         </is>
       </c>
       <c r="C197" t="n">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="198">
-      <c r="A198" s="1" t="n">
-        <v>196</v>
-      </c>
-      <c r="B198" t="inlineStr">
-        <is>
-          <t>1117/2</t>
-        </is>
-      </c>
-      <c r="C198" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="199">
-      <c r="A199" s="1" t="n">
-        <v>197</v>
-      </c>
-      <c r="B199" t="inlineStr">
-        <is>
-          <t>1230/100</t>
-        </is>
-      </c>
-      <c r="C199" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="200">
-      <c r="A200" s="1" t="n">
-        <v>198</v>
-      </c>
-      <c r="B200" t="inlineStr">
-        <is>
-          <t>1230/115</t>
-        </is>
-      </c>
-      <c r="C200" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="201">
-      <c r="A201" s="1" t="n">
-        <v>199</v>
-      </c>
-      <c r="B201" t="inlineStr">
-        <is>
-          <t>1230/85</t>
-        </is>
-      </c>
-      <c r="C201" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="202">
-      <c r="A202" s="1" t="n">
-        <v>200</v>
-      </c>
-      <c r="B202" t="inlineStr">
-        <is>
-          <t>1230/86</t>
-        </is>
-      </c>
-      <c r="C202" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="203">
-      <c r="A203" s="1" t="n">
-        <v>201</v>
-      </c>
-      <c r="B203" t="inlineStr">
-        <is>
-          <t>1230/87</t>
-        </is>
-      </c>
-      <c r="C203" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="204">
-      <c r="A204" s="1" t="n">
-        <v>202</v>
-      </c>
-      <c r="B204" t="inlineStr">
-        <is>
-          <t>1230/88</t>
-        </is>
-      </c>
-      <c r="C204" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="205">
-      <c r="A205" s="1" t="n">
-        <v>203</v>
-      </c>
-      <c r="B205" t="inlineStr">
-        <is>
-          <t>1303/1</t>
-        </is>
-      </c>
-      <c r="C205" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="206">
-      <c r="A206" s="1" t="n">
-        <v>204</v>
-      </c>
-      <c r="B206" t="inlineStr">
-        <is>
-          <t>1303/2</t>
-        </is>
-      </c>
-      <c r="C206" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="207">
-      <c r="A207" s="1" t="n">
-        <v>205</v>
-      </c>
-      <c r="B207" t="inlineStr">
-        <is>
-          <t>1309</t>
-        </is>
-      </c>
-      <c r="C207" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="208">
-      <c r="A208" s="1" t="n">
-        <v>206</v>
-      </c>
-      <c r="B208" t="inlineStr">
-        <is>
-          <t>1330</t>
-        </is>
-      </c>
-      <c r="C208" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="209">
-      <c r="A209" s="1" t="n">
-        <v>207</v>
-      </c>
-      <c r="B209" t="inlineStr">
-        <is>
-          <t>1334</t>
-        </is>
-      </c>
-      <c r="C209" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="210">
-      <c r="A210" s="1" t="n">
-        <v>208</v>
-      </c>
-      <c r="B210" t="inlineStr">
-        <is>
-          <t>1346</t>
-        </is>
-      </c>
-      <c r="C210" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="211">
-      <c r="A211" s="1" t="n">
-        <v>209</v>
-      </c>
-      <c r="B211" t="inlineStr">
-        <is>
-          <t>1369/1</t>
-        </is>
-      </c>
-      <c r="C211" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="212">
-      <c r="A212" s="1" t="n">
-        <v>210</v>
-      </c>
-      <c r="B212" t="inlineStr">
-        <is>
-          <t>194/4</t>
-        </is>
-      </c>
-      <c r="C212" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="213">
-      <c r="A213" s="1" t="n">
-        <v>211</v>
-      </c>
-      <c r="B213" t="inlineStr">
-        <is>
-          <t>254/2</t>
-        </is>
-      </c>
-      <c r="C213" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="214">
-      <c r="A214" s="1" t="n">
-        <v>212</v>
-      </c>
-      <c r="B214" t="inlineStr">
-        <is>
-          <t>337/5</t>
-        </is>
-      </c>
-      <c r="C214" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="215">
-      <c r="A215" s="1" t="n">
-        <v>213</v>
-      </c>
-      <c r="B215" t="inlineStr">
-        <is>
-          <t>393/1</t>
-        </is>
-      </c>
-      <c r="C215" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="216">
-      <c r="A216" s="1" t="n">
-        <v>214</v>
-      </c>
-      <c r="B216" t="inlineStr">
-        <is>
-          <t>393/2</t>
-        </is>
-      </c>
-      <c r="C216" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="217">
-      <c r="A217" s="1" t="n">
-        <v>215</v>
-      </c>
-      <c r="B217" t="inlineStr">
-        <is>
-          <t>393/3</t>
-        </is>
-      </c>
-      <c r="C217" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="218">
-      <c r="A218" s="1" t="n">
-        <v>216</v>
-      </c>
-      <c r="B218" t="inlineStr">
-        <is>
-          <t>465</t>
-        </is>
-      </c>
-      <c r="C218" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="219">
-      <c r="A219" s="1" t="n">
-        <v>217</v>
-      </c>
-      <c r="B219" t="inlineStr">
-        <is>
-          <t>614</t>
-        </is>
-      </c>
-      <c r="C219" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="220">
-      <c r="A220" s="1" t="n">
-        <v>218</v>
-      </c>
-      <c r="B220" t="inlineStr">
-        <is>
-          <t>384/1</t>
-        </is>
-      </c>
-      <c r="C220" t="n">
         <v>193</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Latest data: Sun Mar  3 16:08:27 UTC 2024
</commit_message>
<xml_diff>
--- a/docs/particelle_non_trovate.xlsx
+++ b/docs/particelle_non_trovate.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C197"/>
+  <dimension ref="A1:C186"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -880,11 +880,11 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>2189</t>
+          <t>141</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>22</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36">
@@ -893,11 +893,11 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>149</t>
+          <t>243</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>22</v>
+        <v>56</v>
       </c>
     </row>
     <row r="37">
@@ -906,11 +906,11 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>1186</t>
+          <t>246</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>22</v>
+        <v>56</v>
       </c>
     </row>
     <row r="38">
@@ -919,11 +919,11 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>1220</t>
+          <t>536</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>22</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39">
@@ -932,11 +932,11 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>1508</t>
+          <t>3181/3</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>22</v>
+        <v>57</v>
       </c>
     </row>
     <row r="40">
@@ -945,11 +945,11 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>1806</t>
+          <t>3577</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>22</v>
+        <v>44</v>
       </c>
     </row>
     <row r="41">
@@ -958,11 +958,11 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>1865</t>
+          <t>11008</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>22</v>
+        <v>44</v>
       </c>
     </row>
     <row r="42">
@@ -971,11 +971,11 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>1866</t>
+          <t>11029</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>22</v>
+        <v>44</v>
       </c>
     </row>
     <row r="43">
@@ -984,11 +984,11 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>3073</t>
+          <t>11846</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>22</v>
+        <v>44</v>
       </c>
     </row>
     <row r="44">
@@ -997,11 +997,11 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>3074</t>
+          <t>11861</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>22</v>
+        <v>44</v>
       </c>
     </row>
     <row r="45">
@@ -1010,11 +1010,11 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>3113</t>
+          <t>10564</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>22</v>
+        <v>44</v>
       </c>
     </row>
     <row r="46">
@@ -1023,11 +1023,11 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>141</t>
+          <t>10563/14</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>56</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47">
@@ -1036,11 +1036,11 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>243</t>
+          <t>10563/15</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>56</v>
+        <v>44</v>
       </c>
     </row>
     <row r="48">
@@ -1049,11 +1049,11 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>246</t>
+          <t>3535</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>56</v>
+        <v>44</v>
       </c>
     </row>
     <row r="49">
@@ -1062,11 +1062,11 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>536</t>
+          <t>3570</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>56</v>
+        <v>44</v>
       </c>
     </row>
     <row r="50">
@@ -1075,11 +1075,11 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>3181/3</t>
+          <t>2168</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>57</v>
+        <v>44</v>
       </c>
     </row>
     <row r="51">
@@ -1088,7 +1088,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>3577</t>
+          <t>2762</t>
         </is>
       </c>
       <c r="C51" t="n">
@@ -1101,7 +1101,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>11008</t>
+          <t>11867</t>
         </is>
       </c>
       <c r="C52" t="n">
@@ -1114,7 +1114,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>11029</t>
+          <t>5009</t>
         </is>
       </c>
       <c r="C53" t="n">
@@ -1127,7 +1127,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>11846</t>
+          <t>5010</t>
         </is>
       </c>
       <c r="C54" t="n">
@@ -1140,7 +1140,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>11861</t>
+          <t>11025/1</t>
         </is>
       </c>
       <c r="C55" t="n">
@@ -1153,7 +1153,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>10564</t>
+          <t>11025/2</t>
         </is>
       </c>
       <c r="C56" t="n">
@@ -1166,7 +1166,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>10563/14</t>
+          <t>11026/1</t>
         </is>
       </c>
       <c r="C57" t="n">
@@ -1179,7 +1179,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>10563/15</t>
+          <t>11260</t>
         </is>
       </c>
       <c r="C58" t="n">
@@ -1192,11 +1192,11 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>3535</t>
+          <t>13823</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>44</v>
+        <v>154</v>
       </c>
     </row>
     <row r="60">
@@ -1205,11 +1205,11 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>3570</t>
+          <t>14724/2</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>44</v>
+        <v>154</v>
       </c>
     </row>
     <row r="61">
@@ -1218,11 +1218,11 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>2168</t>
+          <t>15380</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>44</v>
+        <v>154</v>
       </c>
     </row>
     <row r="62">
@@ -1231,11 +1231,11 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>2762</t>
+          <t>1847/1</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>44</v>
+        <v>154</v>
       </c>
     </row>
     <row r="63">
@@ -1244,11 +1244,11 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>11867</t>
+          <t>220/2</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>44</v>
+        <v>154</v>
       </c>
     </row>
     <row r="64">
@@ -1257,11 +1257,11 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>5009</t>
+          <t>8974/1</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>44</v>
+        <v>154</v>
       </c>
     </row>
     <row r="65">
@@ -1270,11 +1270,11 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>5010</t>
+          <t>8987/1</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>44</v>
+        <v>154</v>
       </c>
     </row>
     <row r="66">
@@ -1283,11 +1283,11 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>11025/1</t>
+          <t>391</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>44</v>
+        <v>174</v>
       </c>
     </row>
     <row r="67">
@@ -1296,11 +1296,11 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>11025/2</t>
+          <t>466</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>44</v>
+        <v>213</v>
       </c>
     </row>
     <row r="68">
@@ -1309,11 +1309,11 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>11026/1</t>
+          <t>31</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>44</v>
+        <v>282</v>
       </c>
     </row>
     <row r="69">
@@ -1322,11 +1322,11 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>11260</t>
+          <t>722</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>44</v>
+        <v>282</v>
       </c>
     </row>
     <row r="70">
@@ -1335,11 +1335,11 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>13823</t>
+          <t>410</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>154</v>
+        <v>282</v>
       </c>
     </row>
     <row r="71">
@@ -1348,11 +1348,11 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>14724/2</t>
+          <t>412</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>154</v>
+        <v>282</v>
       </c>
     </row>
     <row r="72">
@@ -1361,11 +1361,11 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>15380</t>
+          <t>461</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>154</v>
+        <v>282</v>
       </c>
     </row>
     <row r="73">
@@ -1374,11 +1374,11 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>1847/1</t>
+          <t>467</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>154</v>
+        <v>282</v>
       </c>
     </row>
     <row r="74">
@@ -1387,11 +1387,11 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>220/2</t>
+          <t>468</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>154</v>
+        <v>282</v>
       </c>
     </row>
     <row r="75">
@@ -1400,11 +1400,11 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>8974/1</t>
+          <t>.315</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>154</v>
+        <v>282</v>
       </c>
     </row>
     <row r="76">
@@ -1413,11 +1413,11 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>8987/1</t>
+          <t>1826</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>154</v>
+        <v>282</v>
       </c>
     </row>
     <row r="77">
@@ -1426,11 +1426,11 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>391</t>
+          <t>86</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>174</v>
+        <v>340</v>
       </c>
     </row>
     <row r="78">
@@ -1439,11 +1439,11 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>466</t>
+          <t>397</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>213</v>
+        <v>340</v>
       </c>
     </row>
     <row r="79">
@@ -1452,11 +1452,11 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>488</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>282</v>
+        <v>340</v>
       </c>
     </row>
     <row r="80">
@@ -1465,11 +1465,11 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>722</t>
+          <t>403</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>282</v>
+        <v>97</v>
       </c>
     </row>
     <row r="81">
@@ -1478,11 +1478,11 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>410</t>
+          <t>746</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>282</v>
+        <v>97</v>
       </c>
     </row>
     <row r="82">
@@ -1491,11 +1491,11 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>412</t>
+          <t>749</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>282</v>
+        <v>97</v>
       </c>
     </row>
     <row r="83">
@@ -1504,11 +1504,11 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>461</t>
+          <t>754</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>282</v>
+        <v>97</v>
       </c>
     </row>
     <row r="84">
@@ -1517,11 +1517,11 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>467</t>
+          <t>755</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>282</v>
+        <v>97</v>
       </c>
     </row>
     <row r="85">
@@ -1530,11 +1530,11 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>468</t>
+          <t>757</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>282</v>
+        <v>97</v>
       </c>
     </row>
     <row r="86">
@@ -1543,11 +1543,11 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>.315</t>
+          <t>758</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>282</v>
+        <v>97</v>
       </c>
     </row>
     <row r="87">
@@ -1556,11 +1556,11 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>1826</t>
+          <t>825/63</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>282</v>
+        <v>97</v>
       </c>
     </row>
     <row r="88">
@@ -1569,11 +1569,11 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>86</t>
+          <t>1900/4</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>340</v>
+        <v>317</v>
       </c>
     </row>
     <row r="89">
@@ -1582,11 +1582,11 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>397</t>
+          <t>9609</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>340</v>
+        <v>390</v>
       </c>
     </row>
     <row r="90">
@@ -1595,11 +1595,11 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>488</t>
+          <t>9608/2</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>340</v>
+        <v>390</v>
       </c>
     </row>
     <row r="91">
@@ -1608,11 +1608,11 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>403</t>
+          <t>371</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>97</v>
+        <v>404</v>
       </c>
     </row>
     <row r="92">
@@ -1621,11 +1621,11 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>746</t>
+          <t>373</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>97</v>
+        <v>404</v>
       </c>
     </row>
     <row r="93">
@@ -1634,11 +1634,11 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>749</t>
+          <t>1741</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>97</v>
+        <v>404</v>
       </c>
     </row>
     <row r="94">
@@ -1647,11 +1647,11 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>754</t>
+          <t>1820</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>97</v>
+        <v>404</v>
       </c>
     </row>
     <row r="95">
@@ -1660,11 +1660,11 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>755</t>
+          <t>156</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>97</v>
+        <v>404</v>
       </c>
     </row>
     <row r="96">
@@ -1673,11 +1673,11 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>757</t>
+          <t>4708</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>97</v>
+        <v>404</v>
       </c>
     </row>
     <row r="97">
@@ -1686,11 +1686,11 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>758</t>
+          <t>162/3</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>97</v>
+        <v>404</v>
       </c>
     </row>
     <row r="98">
@@ -1699,11 +1699,11 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>825/63</t>
+          <t>1193</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>97</v>
+        <v>404</v>
       </c>
     </row>
     <row r="99">
@@ -1712,11 +1712,11 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>1900/4</t>
+          <t>2762</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>317</v>
+        <v>404</v>
       </c>
     </row>
     <row r="100">
@@ -1725,11 +1725,11 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>9609</t>
+          <t>2766/3</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>390</v>
+        <v>404</v>
       </c>
     </row>
     <row r="101">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>9608/2</t>
+          <t>2736/8</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>390</v>
+        <v>404</v>
       </c>
     </row>
     <row r="102">
@@ -1751,7 +1751,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>371</t>
+          <t>2769/1</t>
         </is>
       </c>
       <c r="C102" t="n">
@@ -1764,7 +1764,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>373</t>
+          <t>2768</t>
         </is>
       </c>
       <c r="C103" t="n">
@@ -1777,7 +1777,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>1741</t>
+          <t>2767</t>
         </is>
       </c>
       <c r="C104" t="n">
@@ -1790,7 +1790,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>1820</t>
+          <t>679/2</t>
         </is>
       </c>
       <c r="C105" t="n">
@@ -1803,11 +1803,11 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>156</t>
+          <t>.507/2</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="107">
@@ -1816,11 +1816,11 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>4708</t>
+          <t>.507/3</t>
         </is>
       </c>
       <c r="C107" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="108">
@@ -1829,11 +1829,11 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>162/3</t>
+          <t>.507/4</t>
         </is>
       </c>
       <c r="C108" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="109">
@@ -1842,11 +1842,11 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>1193</t>
+          <t>507/5</t>
         </is>
       </c>
       <c r="C109" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="110">
@@ -1855,11 +1855,11 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>2762</t>
+          <t>507/6</t>
         </is>
       </c>
       <c r="C110" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="111">
@@ -1868,11 +1868,11 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>2766/3</t>
+          <t>569/8</t>
         </is>
       </c>
       <c r="C111" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="112">
@@ -1881,11 +1881,11 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>2736/8</t>
+          <t>.569/5</t>
         </is>
       </c>
       <c r="C112" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="113">
@@ -1894,11 +1894,11 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>2769/1</t>
+          <t>7294</t>
         </is>
       </c>
       <c r="C113" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="114">
@@ -1907,11 +1907,11 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>2768</t>
+          <t>7293/2</t>
         </is>
       </c>
       <c r="C114" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="115">
@@ -1920,11 +1920,11 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>2767</t>
+          <t>7293/3</t>
         </is>
       </c>
       <c r="C115" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="116">
@@ -1933,11 +1933,11 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>679/2</t>
+          <t>1391</t>
         </is>
       </c>
       <c r="C116" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="117">
@@ -1946,7 +1946,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>.507/2</t>
+          <t>7292/1</t>
         </is>
       </c>
       <c r="C117" t="n">
@@ -1959,7 +1959,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>.507/3</t>
+          <t>1358</t>
         </is>
       </c>
       <c r="C118" t="n">
@@ -1972,7 +1972,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>.507/4</t>
+          <t>7191/4</t>
         </is>
       </c>
       <c r="C119" t="n">
@@ -1985,7 +1985,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>507/5</t>
+          <t>7618/3</t>
         </is>
       </c>
       <c r="C120" t="n">
@@ -1998,7 +1998,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>507/6</t>
+          <t>7618/4</t>
         </is>
       </c>
       <c r="C121" t="n">
@@ -2011,7 +2011,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>569/8</t>
+          <t>114</t>
         </is>
       </c>
       <c r="C122" t="n">
@@ -2024,7 +2024,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>.569/5</t>
+          <t>361</t>
         </is>
       </c>
       <c r="C123" t="n">
@@ -2037,7 +2037,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>7294</t>
+          <t>421</t>
         </is>
       </c>
       <c r="C124" t="n">
@@ -2050,7 +2050,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>7293/2</t>
+          <t>13094</t>
         </is>
       </c>
       <c r="C125" t="n">
@@ -2063,7 +2063,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>7293/3</t>
+          <t>7290/6</t>
         </is>
       </c>
       <c r="C126" t="n">
@@ -2076,7 +2076,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>1391</t>
+          <t>7288</t>
         </is>
       </c>
       <c r="C127" t="n">
@@ -2089,11 +2089,11 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>7292/1</t>
+          <t>45</t>
         </is>
       </c>
       <c r="C128" t="n">
-        <v>413</v>
+        <v>283</v>
       </c>
     </row>
     <row r="129">
@@ -2102,11 +2102,11 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>1358</t>
+          <t>84/1</t>
         </is>
       </c>
       <c r="C129" t="n">
-        <v>413</v>
+        <v>283</v>
       </c>
     </row>
     <row r="130">
@@ -2115,11 +2115,11 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>7191/4</t>
+          <t>137</t>
         </is>
       </c>
       <c r="C130" t="n">
-        <v>413</v>
+        <v>41</v>
       </c>
     </row>
     <row r="131">
@@ -2128,11 +2128,11 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>7618/3</t>
+          <t>140</t>
         </is>
       </c>
       <c r="C131" t="n">
-        <v>413</v>
+        <v>41</v>
       </c>
     </row>
     <row r="132">
@@ -2141,11 +2141,11 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>7618/4</t>
+          <t>272</t>
         </is>
       </c>
       <c r="C132" t="n">
-        <v>413</v>
+        <v>79</v>
       </c>
     </row>
     <row r="133">
@@ -2154,11 +2154,11 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>114</t>
+          <t>1881/8</t>
         </is>
       </c>
       <c r="C133" t="n">
-        <v>413</v>
+        <v>79</v>
       </c>
     </row>
     <row r="134">
@@ -2167,11 +2167,11 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>361</t>
+          <t>94/6</t>
         </is>
       </c>
       <c r="C134" t="n">
-        <v>413</v>
+        <v>251</v>
       </c>
     </row>
     <row r="135">
@@ -2180,11 +2180,11 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>421</t>
+          <t>243</t>
         </is>
       </c>
       <c r="C135" t="n">
-        <v>413</v>
+        <v>253</v>
       </c>
     </row>
     <row r="136">
@@ -2193,11 +2193,11 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>13094</t>
+          <t>295</t>
         </is>
       </c>
       <c r="C136" t="n">
-        <v>413</v>
+        <v>253</v>
       </c>
     </row>
     <row r="137">
@@ -2206,11 +2206,11 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>7290/6</t>
+          <t>1403</t>
         </is>
       </c>
       <c r="C137" t="n">
-        <v>413</v>
+        <v>268</v>
       </c>
     </row>
     <row r="138">
@@ -2219,11 +2219,11 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>7288</t>
+          <t>316</t>
         </is>
       </c>
       <c r="C138" t="n">
-        <v>413</v>
+        <v>442</v>
       </c>
     </row>
     <row r="139">
@@ -2232,11 +2232,11 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>53</t>
         </is>
       </c>
       <c r="C139" t="n">
-        <v>283</v>
+        <v>215</v>
       </c>
     </row>
     <row r="140">
@@ -2245,11 +2245,11 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>84/1</t>
+          <t>454</t>
         </is>
       </c>
       <c r="C140" t="n">
-        <v>283</v>
+        <v>215</v>
       </c>
     </row>
     <row r="141">
@@ -2258,11 +2258,11 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>137</t>
+          <t>420/80</t>
         </is>
       </c>
       <c r="C141" t="n">
-        <v>41</v>
+        <v>215</v>
       </c>
     </row>
     <row r="142">
@@ -2271,11 +2271,11 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>140</t>
+          <t>420/92</t>
         </is>
       </c>
       <c r="C142" t="n">
-        <v>41</v>
+        <v>215</v>
       </c>
     </row>
     <row r="143">
@@ -2284,11 +2284,11 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>272</t>
+          <t>420/93</t>
         </is>
       </c>
       <c r="C143" t="n">
-        <v>79</v>
+        <v>215</v>
       </c>
     </row>
     <row r="144">
@@ -2297,11 +2297,11 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>1881/8</t>
+          <t>420/94</t>
         </is>
       </c>
       <c r="C144" t="n">
-        <v>79</v>
+        <v>215</v>
       </c>
     </row>
     <row r="145">
@@ -2310,11 +2310,11 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>94/6</t>
+          <t>420/95</t>
         </is>
       </c>
       <c r="C145" t="n">
-        <v>251</v>
+        <v>215</v>
       </c>
     </row>
     <row r="146">
@@ -2323,11 +2323,11 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>243</t>
+          <t>420/96</t>
         </is>
       </c>
       <c r="C146" t="n">
-        <v>253</v>
+        <v>215</v>
       </c>
     </row>
     <row r="147">
@@ -2336,11 +2336,11 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>295</t>
+          <t>420/97</t>
         </is>
       </c>
       <c r="C147" t="n">
-        <v>253</v>
+        <v>215</v>
       </c>
     </row>
     <row r="148">
@@ -2349,11 +2349,11 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>1403</t>
+          <t>420/101</t>
         </is>
       </c>
       <c r="C148" t="n">
-        <v>268</v>
+        <v>215</v>
       </c>
     </row>
     <row r="149">
@@ -2362,11 +2362,11 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>316</t>
+          <t>420/102</t>
         </is>
       </c>
       <c r="C149" t="n">
-        <v>442</v>
+        <v>215</v>
       </c>
     </row>
     <row r="150">
@@ -2375,7 +2375,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>420/106</t>
         </is>
       </c>
       <c r="C150" t="n">
@@ -2388,7 +2388,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>454</t>
+          <t>420/107</t>
         </is>
       </c>
       <c r="C151" t="n">
@@ -2401,7 +2401,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>420/80</t>
+          <t>420/109</t>
         </is>
       </c>
       <c r="C152" t="n">
@@ -2414,7 +2414,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>420/92</t>
+          <t>420/110</t>
         </is>
       </c>
       <c r="C153" t="n">
@@ -2427,7 +2427,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>420/93</t>
+          <t>705/11</t>
         </is>
       </c>
       <c r="C154" t="n">
@@ -2440,7 +2440,7 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>420/94</t>
+          <t>756</t>
         </is>
       </c>
       <c r="C155" t="n">
@@ -2453,7 +2453,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>420/95</t>
+          <t>798/3</t>
         </is>
       </c>
       <c r="C156" t="n">
@@ -2466,11 +2466,11 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>420/96</t>
+          <t>1411/1</t>
         </is>
       </c>
       <c r="C157" t="n">
-        <v>215</v>
+        <v>256</v>
       </c>
     </row>
     <row r="158">
@@ -2479,11 +2479,11 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>420/97</t>
+          <t>1411/2</t>
         </is>
       </c>
       <c r="C158" t="n">
-        <v>215</v>
+        <v>256</v>
       </c>
     </row>
     <row r="159">
@@ -2492,11 +2492,11 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>420/101</t>
+          <t>1411/3</t>
         </is>
       </c>
       <c r="C159" t="n">
-        <v>215</v>
+        <v>256</v>
       </c>
     </row>
     <row r="160">
@@ -2505,11 +2505,11 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>420/102</t>
+          <t>1411/4</t>
         </is>
       </c>
       <c r="C160" t="n">
-        <v>215</v>
+        <v>256</v>
       </c>
     </row>
     <row r="161">
@@ -2518,11 +2518,11 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>420/106</t>
+          <t>1411/5</t>
         </is>
       </c>
       <c r="C161" t="n">
-        <v>215</v>
+        <v>256</v>
       </c>
     </row>
     <row r="162">
@@ -2531,11 +2531,11 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>420/107</t>
+          <t>1412</t>
         </is>
       </c>
       <c r="C162" t="n">
-        <v>215</v>
+        <v>256</v>
       </c>
     </row>
     <row r="163">
@@ -2544,11 +2544,11 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>420/109</t>
+          <t>1488</t>
         </is>
       </c>
       <c r="C163" t="n">
-        <v>215</v>
+        <v>256</v>
       </c>
     </row>
     <row r="164">
@@ -2557,11 +2557,11 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>420/110</t>
+          <t>1117/2</t>
         </is>
       </c>
       <c r="C164" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="165">
@@ -2570,11 +2570,11 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>705/11</t>
+          <t>1230/100</t>
         </is>
       </c>
       <c r="C165" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="166">
@@ -2583,11 +2583,11 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>756</t>
+          <t>1230/115</t>
         </is>
       </c>
       <c r="C166" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="167">
@@ -2596,11 +2596,11 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>798/3</t>
+          <t>1230/85</t>
         </is>
       </c>
       <c r="C167" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="168">
@@ -2609,11 +2609,11 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>1411/1</t>
+          <t>1230/86</t>
         </is>
       </c>
       <c r="C168" t="n">
-        <v>256</v>
+        <v>193</v>
       </c>
     </row>
     <row r="169">
@@ -2622,11 +2622,11 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>1411/2</t>
+          <t>1230/87</t>
         </is>
       </c>
       <c r="C169" t="n">
-        <v>256</v>
+        <v>193</v>
       </c>
     </row>
     <row r="170">
@@ -2635,11 +2635,11 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>1411/3</t>
+          <t>1230/88</t>
         </is>
       </c>
       <c r="C170" t="n">
-        <v>256</v>
+        <v>193</v>
       </c>
     </row>
     <row r="171">
@@ -2648,11 +2648,11 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>1411/4</t>
+          <t>1303/1</t>
         </is>
       </c>
       <c r="C171" t="n">
-        <v>256</v>
+        <v>193</v>
       </c>
     </row>
     <row r="172">
@@ -2661,11 +2661,11 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>1411/5</t>
+          <t>1303/2</t>
         </is>
       </c>
       <c r="C172" t="n">
-        <v>256</v>
+        <v>193</v>
       </c>
     </row>
     <row r="173">
@@ -2674,11 +2674,11 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>1412</t>
+          <t>1309</t>
         </is>
       </c>
       <c r="C173" t="n">
-        <v>256</v>
+        <v>193</v>
       </c>
     </row>
     <row r="174">
@@ -2687,11 +2687,11 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>1488</t>
+          <t>1330</t>
         </is>
       </c>
       <c r="C174" t="n">
-        <v>256</v>
+        <v>193</v>
       </c>
     </row>
     <row r="175">
@@ -2700,7 +2700,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>1117/2</t>
+          <t>1334</t>
         </is>
       </c>
       <c r="C175" t="n">
@@ -2713,7 +2713,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>1230/100</t>
+          <t>1346</t>
         </is>
       </c>
       <c r="C176" t="n">
@@ -2726,7 +2726,7 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>1230/115</t>
+          <t>1369/1</t>
         </is>
       </c>
       <c r="C177" t="n">
@@ -2739,7 +2739,7 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>1230/85</t>
+          <t>194/4</t>
         </is>
       </c>
       <c r="C178" t="n">
@@ -2752,7 +2752,7 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>1230/86</t>
+          <t>254/2</t>
         </is>
       </c>
       <c r="C179" t="n">
@@ -2765,7 +2765,7 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>1230/87</t>
+          <t>337/5</t>
         </is>
       </c>
       <c r="C180" t="n">
@@ -2778,7 +2778,7 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>1230/88</t>
+          <t>393/1</t>
         </is>
       </c>
       <c r="C181" t="n">
@@ -2791,7 +2791,7 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>1303/1</t>
+          <t>393/2</t>
         </is>
       </c>
       <c r="C182" t="n">
@@ -2804,7 +2804,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>1303/2</t>
+          <t>393/3</t>
         </is>
       </c>
       <c r="C183" t="n">
@@ -2817,7 +2817,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>1309</t>
+          <t>465</t>
         </is>
       </c>
       <c r="C184" t="n">
@@ -2830,7 +2830,7 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>1330</t>
+          <t>614</t>
         </is>
       </c>
       <c r="C185" t="n">
@@ -2843,153 +2843,10 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>1334</t>
+          <t>384/1</t>
         </is>
       </c>
       <c r="C186" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="187">
-      <c r="A187" s="1" t="n">
-        <v>185</v>
-      </c>
-      <c r="B187" t="inlineStr">
-        <is>
-          <t>1346</t>
-        </is>
-      </c>
-      <c r="C187" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="188">
-      <c r="A188" s="1" t="n">
-        <v>186</v>
-      </c>
-      <c r="B188" t="inlineStr">
-        <is>
-          <t>1369/1</t>
-        </is>
-      </c>
-      <c r="C188" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="189">
-      <c r="A189" s="1" t="n">
-        <v>187</v>
-      </c>
-      <c r="B189" t="inlineStr">
-        <is>
-          <t>194/4</t>
-        </is>
-      </c>
-      <c r="C189" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="190">
-      <c r="A190" s="1" t="n">
-        <v>188</v>
-      </c>
-      <c r="B190" t="inlineStr">
-        <is>
-          <t>254/2</t>
-        </is>
-      </c>
-      <c r="C190" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="191">
-      <c r="A191" s="1" t="n">
-        <v>189</v>
-      </c>
-      <c r="B191" t="inlineStr">
-        <is>
-          <t>337/5</t>
-        </is>
-      </c>
-      <c r="C191" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="192">
-      <c r="A192" s="1" t="n">
-        <v>190</v>
-      </c>
-      <c r="B192" t="inlineStr">
-        <is>
-          <t>393/1</t>
-        </is>
-      </c>
-      <c r="C192" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="193">
-      <c r="A193" s="1" t="n">
-        <v>191</v>
-      </c>
-      <c r="B193" t="inlineStr">
-        <is>
-          <t>393/2</t>
-        </is>
-      </c>
-      <c r="C193" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="194">
-      <c r="A194" s="1" t="n">
-        <v>192</v>
-      </c>
-      <c r="B194" t="inlineStr">
-        <is>
-          <t>393/3</t>
-        </is>
-      </c>
-      <c r="C194" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="195">
-      <c r="A195" s="1" t="n">
-        <v>193</v>
-      </c>
-      <c r="B195" t="inlineStr">
-        <is>
-          <t>465</t>
-        </is>
-      </c>
-      <c r="C195" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="196">
-      <c r="A196" s="1" t="n">
-        <v>194</v>
-      </c>
-      <c r="B196" t="inlineStr">
-        <is>
-          <t>614</t>
-        </is>
-      </c>
-      <c r="C196" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="197">
-      <c r="A197" s="1" t="n">
-        <v>195</v>
-      </c>
-      <c r="B197" t="inlineStr">
-        <is>
-          <t>384/1</t>
-        </is>
-      </c>
-      <c r="C197" t="n">
         <v>193</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Latest data: Sun Mar  3 20:07:27 UTC 2024
</commit_message>
<xml_diff>
--- a/docs/particelle_non_trovate.xlsx
+++ b/docs/particelle_non_trovate.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C186"/>
+  <dimension ref="A1:C171"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -880,11 +880,11 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>141</t>
+          <t>2181/2</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="36">
@@ -893,11 +893,11 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>243</t>
+          <t>3577</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>56</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37">
@@ -906,11 +906,11 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>246</t>
+          <t>11008</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>56</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38">
@@ -919,11 +919,11 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>536</t>
+          <t>11029</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>56</v>
+        <v>44</v>
       </c>
     </row>
     <row r="39">
@@ -932,11 +932,11 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>3181/3</t>
+          <t>11846</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>57</v>
+        <v>44</v>
       </c>
     </row>
     <row r="40">
@@ -945,7 +945,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>3577</t>
+          <t>11861</t>
         </is>
       </c>
       <c r="C40" t="n">
@@ -958,7 +958,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>11008</t>
+          <t>10564</t>
         </is>
       </c>
       <c r="C41" t="n">
@@ -971,7 +971,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>11029</t>
+          <t>10563/14</t>
         </is>
       </c>
       <c r="C42" t="n">
@@ -984,7 +984,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>11846</t>
+          <t>10563/15</t>
         </is>
       </c>
       <c r="C43" t="n">
@@ -997,7 +997,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>11861</t>
+          <t>3535</t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -1010,7 +1010,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>10564</t>
+          <t>3570</t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -1023,7 +1023,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>10563/14</t>
+          <t>2168</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -1036,7 +1036,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>10563/15</t>
+          <t>2762</t>
         </is>
       </c>
       <c r="C47" t="n">
@@ -1049,7 +1049,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>3535</t>
+          <t>11867</t>
         </is>
       </c>
       <c r="C48" t="n">
@@ -1062,7 +1062,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>3570</t>
+          <t>5009</t>
         </is>
       </c>
       <c r="C49" t="n">
@@ -1075,7 +1075,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>2168</t>
+          <t>5010</t>
         </is>
       </c>
       <c r="C50" t="n">
@@ -1088,7 +1088,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>2762</t>
+          <t>11025/1</t>
         </is>
       </c>
       <c r="C51" t="n">
@@ -1101,7 +1101,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>11867</t>
+          <t>11025/2</t>
         </is>
       </c>
       <c r="C52" t="n">
@@ -1114,7 +1114,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>5009</t>
+          <t>11026/1</t>
         </is>
       </c>
       <c r="C53" t="n">
@@ -1127,7 +1127,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>5010</t>
+          <t>11260</t>
         </is>
       </c>
       <c r="C54" t="n">
@@ -1140,11 +1140,11 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>11025/1</t>
+          <t>13823</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>44</v>
+        <v>154</v>
       </c>
     </row>
     <row r="56">
@@ -1153,11 +1153,11 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>11025/2</t>
+          <t>14724/2</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>44</v>
+        <v>154</v>
       </c>
     </row>
     <row r="57">
@@ -1166,11 +1166,11 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>11026/1</t>
+          <t>15380</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>44</v>
+        <v>154</v>
       </c>
     </row>
     <row r="58">
@@ -1179,11 +1179,11 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>11260</t>
+          <t>1847/1</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>44</v>
+        <v>154</v>
       </c>
     </row>
     <row r="59">
@@ -1192,7 +1192,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>13823</t>
+          <t>220/2</t>
         </is>
       </c>
       <c r="C59" t="n">
@@ -1205,7 +1205,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>14724/2</t>
+          <t>8974/1</t>
         </is>
       </c>
       <c r="C60" t="n">
@@ -1218,7 +1218,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>15380</t>
+          <t>8987/1</t>
         </is>
       </c>
       <c r="C61" t="n">
@@ -1231,11 +1231,11 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>1847/1</t>
+          <t>391</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>154</v>
+        <v>174</v>
       </c>
     </row>
     <row r="63">
@@ -1244,11 +1244,11 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>220/2</t>
+          <t>466</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>154</v>
+        <v>213</v>
       </c>
     </row>
     <row r="64">
@@ -1257,11 +1257,11 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>8974/1</t>
+          <t>.315</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>154</v>
+        <v>282</v>
       </c>
     </row>
     <row r="65">
@@ -1270,11 +1270,11 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>8987/1</t>
+          <t>403</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>154</v>
+        <v>97</v>
       </c>
     </row>
     <row r="66">
@@ -1283,11 +1283,11 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>391</t>
+          <t>746</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>174</v>
+        <v>97</v>
       </c>
     </row>
     <row r="67">
@@ -1296,11 +1296,11 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>466</t>
+          <t>749</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>213</v>
+        <v>97</v>
       </c>
     </row>
     <row r="68">
@@ -1309,11 +1309,11 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>754</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>282</v>
+        <v>97</v>
       </c>
     </row>
     <row r="69">
@@ -1322,11 +1322,11 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>722</t>
+          <t>755</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>282</v>
+        <v>97</v>
       </c>
     </row>
     <row r="70">
@@ -1335,11 +1335,11 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>410</t>
+          <t>757</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>282</v>
+        <v>97</v>
       </c>
     </row>
     <row r="71">
@@ -1348,11 +1348,11 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>412</t>
+          <t>758</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>282</v>
+        <v>97</v>
       </c>
     </row>
     <row r="72">
@@ -1361,11 +1361,11 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>461</t>
+          <t>825/63</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>282</v>
+        <v>97</v>
       </c>
     </row>
     <row r="73">
@@ -1374,11 +1374,11 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>467</t>
+          <t>1900/4</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>282</v>
+        <v>317</v>
       </c>
     </row>
     <row r="74">
@@ -1387,11 +1387,11 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>468</t>
+          <t>9609</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>282</v>
+        <v>390</v>
       </c>
     </row>
     <row r="75">
@@ -1400,11 +1400,11 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>.315</t>
+          <t>9608/2</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>282</v>
+        <v>390</v>
       </c>
     </row>
     <row r="76">
@@ -1413,11 +1413,11 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>1826</t>
+          <t>371</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>282</v>
+        <v>404</v>
       </c>
     </row>
     <row r="77">
@@ -1426,11 +1426,11 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>86</t>
+          <t>373</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>340</v>
+        <v>404</v>
       </c>
     </row>
     <row r="78">
@@ -1439,11 +1439,11 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>397</t>
+          <t>1741</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>340</v>
+        <v>404</v>
       </c>
     </row>
     <row r="79">
@@ -1452,11 +1452,11 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>488</t>
+          <t>1820</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>340</v>
+        <v>404</v>
       </c>
     </row>
     <row r="80">
@@ -1465,11 +1465,11 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>403</t>
+          <t>156</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>97</v>
+        <v>404</v>
       </c>
     </row>
     <row r="81">
@@ -1478,11 +1478,11 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>746</t>
+          <t>4708</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>97</v>
+        <v>404</v>
       </c>
     </row>
     <row r="82">
@@ -1491,11 +1491,11 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>749</t>
+          <t>162/3</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>97</v>
+        <v>404</v>
       </c>
     </row>
     <row r="83">
@@ -1504,11 +1504,11 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>754</t>
+          <t>1193</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>97</v>
+        <v>404</v>
       </c>
     </row>
     <row r="84">
@@ -1517,11 +1517,11 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>755</t>
+          <t>2762</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>97</v>
+        <v>404</v>
       </c>
     </row>
     <row r="85">
@@ -1530,11 +1530,11 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>757</t>
+          <t>2766/3</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>97</v>
+        <v>404</v>
       </c>
     </row>
     <row r="86">
@@ -1543,11 +1543,11 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>758</t>
+          <t>2736/8</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>97</v>
+        <v>404</v>
       </c>
     </row>
     <row r="87">
@@ -1556,11 +1556,11 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>825/63</t>
+          <t>2769/1</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>97</v>
+        <v>404</v>
       </c>
     </row>
     <row r="88">
@@ -1569,11 +1569,11 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>1900/4</t>
+          <t>2768</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>317</v>
+        <v>404</v>
       </c>
     </row>
     <row r="89">
@@ -1582,11 +1582,11 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>9609</t>
+          <t>2767</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>390</v>
+        <v>404</v>
       </c>
     </row>
     <row r="90">
@@ -1595,11 +1595,11 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>9608/2</t>
+          <t>679/2</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>390</v>
+        <v>404</v>
       </c>
     </row>
     <row r="91">
@@ -1608,11 +1608,11 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>371</t>
+          <t>.507/2</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="92">
@@ -1621,11 +1621,11 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>373</t>
+          <t>.507/3</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="93">
@@ -1634,11 +1634,11 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>1741</t>
+          <t>.507/4</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="94">
@@ -1647,11 +1647,11 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>1820</t>
+          <t>507/5</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="95">
@@ -1660,11 +1660,11 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>156</t>
+          <t>507/6</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="96">
@@ -1673,11 +1673,11 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>4708</t>
+          <t>569/8</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="97">
@@ -1686,11 +1686,11 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>162/3</t>
+          <t>.569/5</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="98">
@@ -1699,11 +1699,11 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>1193</t>
+          <t>7294</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="99">
@@ -1712,11 +1712,11 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>2762</t>
+          <t>7293/2</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="100">
@@ -1725,11 +1725,11 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>2766/3</t>
+          <t>7293/3</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="101">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>2736/8</t>
+          <t>1391</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="102">
@@ -1751,11 +1751,11 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>2769/1</t>
+          <t>7292/1</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="103">
@@ -1764,11 +1764,11 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>2768</t>
+          <t>1358</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="104">
@@ -1777,11 +1777,11 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>2767</t>
+          <t>7191/4</t>
         </is>
       </c>
       <c r="C104" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="105">
@@ -1790,11 +1790,11 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>679/2</t>
+          <t>7618/3</t>
         </is>
       </c>
       <c r="C105" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="106">
@@ -1803,7 +1803,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>.507/2</t>
+          <t>7618/4</t>
         </is>
       </c>
       <c r="C106" t="n">
@@ -1816,7 +1816,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>.507/3</t>
+          <t>114</t>
         </is>
       </c>
       <c r="C107" t="n">
@@ -1829,7 +1829,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>.507/4</t>
+          <t>361</t>
         </is>
       </c>
       <c r="C108" t="n">
@@ -1842,7 +1842,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>507/5</t>
+          <t>421</t>
         </is>
       </c>
       <c r="C109" t="n">
@@ -1855,7 +1855,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>507/6</t>
+          <t>13094</t>
         </is>
       </c>
       <c r="C110" t="n">
@@ -1868,7 +1868,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>569/8</t>
+          <t>7290/6</t>
         </is>
       </c>
       <c r="C111" t="n">
@@ -1881,7 +1881,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>.569/5</t>
+          <t>7288</t>
         </is>
       </c>
       <c r="C112" t="n">
@@ -1894,11 +1894,11 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>7294</t>
+          <t>45</t>
         </is>
       </c>
       <c r="C113" t="n">
-        <v>413</v>
+        <v>283</v>
       </c>
     </row>
     <row r="114">
@@ -1907,11 +1907,11 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>7293/2</t>
+          <t>84/1</t>
         </is>
       </c>
       <c r="C114" t="n">
-        <v>413</v>
+        <v>283</v>
       </c>
     </row>
     <row r="115">
@@ -1920,11 +1920,11 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>7293/3</t>
+          <t>137</t>
         </is>
       </c>
       <c r="C115" t="n">
-        <v>413</v>
+        <v>41</v>
       </c>
     </row>
     <row r="116">
@@ -1933,11 +1933,11 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>1391</t>
+          <t>140</t>
         </is>
       </c>
       <c r="C116" t="n">
-        <v>413</v>
+        <v>41</v>
       </c>
     </row>
     <row r="117">
@@ -1946,11 +1946,11 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>7292/1</t>
+          <t>272</t>
         </is>
       </c>
       <c r="C117" t="n">
-        <v>413</v>
+        <v>79</v>
       </c>
     </row>
     <row r="118">
@@ -1959,11 +1959,11 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>1358</t>
+          <t>1881/8</t>
         </is>
       </c>
       <c r="C118" t="n">
-        <v>413</v>
+        <v>79</v>
       </c>
     </row>
     <row r="119">
@@ -1972,11 +1972,11 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>7191/4</t>
+          <t>94/6</t>
         </is>
       </c>
       <c r="C119" t="n">
-        <v>413</v>
+        <v>251</v>
       </c>
     </row>
     <row r="120">
@@ -1985,11 +1985,11 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>7618/3</t>
+          <t>243</t>
         </is>
       </c>
       <c r="C120" t="n">
-        <v>413</v>
+        <v>253</v>
       </c>
     </row>
     <row r="121">
@@ -1998,11 +1998,11 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>7618/4</t>
+          <t>295</t>
         </is>
       </c>
       <c r="C121" t="n">
-        <v>413</v>
+        <v>253</v>
       </c>
     </row>
     <row r="122">
@@ -2011,11 +2011,11 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>114</t>
+          <t>1403</t>
         </is>
       </c>
       <c r="C122" t="n">
-        <v>413</v>
+        <v>268</v>
       </c>
     </row>
     <row r="123">
@@ -2024,11 +2024,11 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>361</t>
+          <t>316</t>
         </is>
       </c>
       <c r="C123" t="n">
-        <v>413</v>
+        <v>442</v>
       </c>
     </row>
     <row r="124">
@@ -2037,11 +2037,11 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>421</t>
+          <t>53</t>
         </is>
       </c>
       <c r="C124" t="n">
-        <v>413</v>
+        <v>215</v>
       </c>
     </row>
     <row r="125">
@@ -2050,11 +2050,11 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>13094</t>
+          <t>454</t>
         </is>
       </c>
       <c r="C125" t="n">
-        <v>413</v>
+        <v>215</v>
       </c>
     </row>
     <row r="126">
@@ -2063,11 +2063,11 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>7290/6</t>
+          <t>420/80</t>
         </is>
       </c>
       <c r="C126" t="n">
-        <v>413</v>
+        <v>215</v>
       </c>
     </row>
     <row r="127">
@@ -2076,11 +2076,11 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>7288</t>
+          <t>420/92</t>
         </is>
       </c>
       <c r="C127" t="n">
-        <v>413</v>
+        <v>215</v>
       </c>
     </row>
     <row r="128">
@@ -2089,11 +2089,11 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>420/93</t>
         </is>
       </c>
       <c r="C128" t="n">
-        <v>283</v>
+        <v>215</v>
       </c>
     </row>
     <row r="129">
@@ -2102,11 +2102,11 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>84/1</t>
+          <t>420/94</t>
         </is>
       </c>
       <c r="C129" t="n">
-        <v>283</v>
+        <v>215</v>
       </c>
     </row>
     <row r="130">
@@ -2115,11 +2115,11 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>137</t>
+          <t>420/95</t>
         </is>
       </c>
       <c r="C130" t="n">
-        <v>41</v>
+        <v>215</v>
       </c>
     </row>
     <row r="131">
@@ -2128,11 +2128,11 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>140</t>
+          <t>420/96</t>
         </is>
       </c>
       <c r="C131" t="n">
-        <v>41</v>
+        <v>215</v>
       </c>
     </row>
     <row r="132">
@@ -2141,11 +2141,11 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>272</t>
+          <t>420/97</t>
         </is>
       </c>
       <c r="C132" t="n">
-        <v>79</v>
+        <v>215</v>
       </c>
     </row>
     <row r="133">
@@ -2154,11 +2154,11 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>1881/8</t>
+          <t>420/101</t>
         </is>
       </c>
       <c r="C133" t="n">
-        <v>79</v>
+        <v>215</v>
       </c>
     </row>
     <row r="134">
@@ -2167,11 +2167,11 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>94/6</t>
+          <t>420/102</t>
         </is>
       </c>
       <c r="C134" t="n">
-        <v>251</v>
+        <v>215</v>
       </c>
     </row>
     <row r="135">
@@ -2180,11 +2180,11 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>243</t>
+          <t>420/106</t>
         </is>
       </c>
       <c r="C135" t="n">
-        <v>253</v>
+        <v>215</v>
       </c>
     </row>
     <row r="136">
@@ -2193,11 +2193,11 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>295</t>
+          <t>420/107</t>
         </is>
       </c>
       <c r="C136" t="n">
-        <v>253</v>
+        <v>215</v>
       </c>
     </row>
     <row r="137">
@@ -2206,11 +2206,11 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>1403</t>
+          <t>420/109</t>
         </is>
       </c>
       <c r="C137" t="n">
-        <v>268</v>
+        <v>215</v>
       </c>
     </row>
     <row r="138">
@@ -2219,11 +2219,11 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>316</t>
+          <t>420/110</t>
         </is>
       </c>
       <c r="C138" t="n">
-        <v>442</v>
+        <v>215</v>
       </c>
     </row>
     <row r="139">
@@ -2232,7 +2232,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>705/11</t>
         </is>
       </c>
       <c r="C139" t="n">
@@ -2245,7 +2245,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>454</t>
+          <t>756</t>
         </is>
       </c>
       <c r="C140" t="n">
@@ -2258,7 +2258,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>420/80</t>
+          <t>798/3</t>
         </is>
       </c>
       <c r="C141" t="n">
@@ -2271,11 +2271,11 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>420/92</t>
+          <t>1411/1</t>
         </is>
       </c>
       <c r="C142" t="n">
-        <v>215</v>
+        <v>256</v>
       </c>
     </row>
     <row r="143">
@@ -2284,11 +2284,11 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>420/93</t>
+          <t>1411/2</t>
         </is>
       </c>
       <c r="C143" t="n">
-        <v>215</v>
+        <v>256</v>
       </c>
     </row>
     <row r="144">
@@ -2297,11 +2297,11 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>420/94</t>
+          <t>1411/3</t>
         </is>
       </c>
       <c r="C144" t="n">
-        <v>215</v>
+        <v>256</v>
       </c>
     </row>
     <row r="145">
@@ -2310,11 +2310,11 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>420/95</t>
+          <t>1411/4</t>
         </is>
       </c>
       <c r="C145" t="n">
-        <v>215</v>
+        <v>256</v>
       </c>
     </row>
     <row r="146">
@@ -2323,11 +2323,11 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>420/96</t>
+          <t>1411/5</t>
         </is>
       </c>
       <c r="C146" t="n">
-        <v>215</v>
+        <v>256</v>
       </c>
     </row>
     <row r="147">
@@ -2336,11 +2336,11 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>420/97</t>
+          <t>1412</t>
         </is>
       </c>
       <c r="C147" t="n">
-        <v>215</v>
+        <v>256</v>
       </c>
     </row>
     <row r="148">
@@ -2349,11 +2349,11 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>420/101</t>
+          <t>1488</t>
         </is>
       </c>
       <c r="C148" t="n">
-        <v>215</v>
+        <v>256</v>
       </c>
     </row>
     <row r="149">
@@ -2362,11 +2362,11 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>420/102</t>
+          <t>1117/2</t>
         </is>
       </c>
       <c r="C149" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="150">
@@ -2375,11 +2375,11 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>420/106</t>
+          <t>1230/100</t>
         </is>
       </c>
       <c r="C150" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="151">
@@ -2388,11 +2388,11 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>420/107</t>
+          <t>1230/115</t>
         </is>
       </c>
       <c r="C151" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="152">
@@ -2401,11 +2401,11 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>420/109</t>
+          <t>1230/85</t>
         </is>
       </c>
       <c r="C152" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="153">
@@ -2414,11 +2414,11 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>420/110</t>
+          <t>1230/86</t>
         </is>
       </c>
       <c r="C153" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="154">
@@ -2427,11 +2427,11 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>705/11</t>
+          <t>1230/87</t>
         </is>
       </c>
       <c r="C154" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="155">
@@ -2440,11 +2440,11 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>756</t>
+          <t>1230/88</t>
         </is>
       </c>
       <c r="C155" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="156">
@@ -2453,11 +2453,11 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>798/3</t>
+          <t>1303/1</t>
         </is>
       </c>
       <c r="C156" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="157">
@@ -2466,11 +2466,11 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>1411/1</t>
+          <t>1303/2</t>
         </is>
       </c>
       <c r="C157" t="n">
-        <v>256</v>
+        <v>193</v>
       </c>
     </row>
     <row r="158">
@@ -2479,11 +2479,11 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>1411/2</t>
+          <t>1309</t>
         </is>
       </c>
       <c r="C158" t="n">
-        <v>256</v>
+        <v>193</v>
       </c>
     </row>
     <row r="159">
@@ -2492,11 +2492,11 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>1411/3</t>
+          <t>1330</t>
         </is>
       </c>
       <c r="C159" t="n">
-        <v>256</v>
+        <v>193</v>
       </c>
     </row>
     <row r="160">
@@ -2505,11 +2505,11 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>1411/4</t>
+          <t>1334</t>
         </is>
       </c>
       <c r="C160" t="n">
-        <v>256</v>
+        <v>193</v>
       </c>
     </row>
     <row r="161">
@@ -2518,11 +2518,11 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>1411/5</t>
+          <t>1346</t>
         </is>
       </c>
       <c r="C161" t="n">
-        <v>256</v>
+        <v>193</v>
       </c>
     </row>
     <row r="162">
@@ -2531,11 +2531,11 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>1412</t>
+          <t>1369/1</t>
         </is>
       </c>
       <c r="C162" t="n">
-        <v>256</v>
+        <v>193</v>
       </c>
     </row>
     <row r="163">
@@ -2544,11 +2544,11 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>1488</t>
+          <t>194/4</t>
         </is>
       </c>
       <c r="C163" t="n">
-        <v>256</v>
+        <v>193</v>
       </c>
     </row>
     <row r="164">
@@ -2557,7 +2557,7 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>1117/2</t>
+          <t>254/2</t>
         </is>
       </c>
       <c r="C164" t="n">
@@ -2570,7 +2570,7 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>1230/100</t>
+          <t>337/5</t>
         </is>
       </c>
       <c r="C165" t="n">
@@ -2583,7 +2583,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>1230/115</t>
+          <t>393/1</t>
         </is>
       </c>
       <c r="C166" t="n">
@@ -2596,7 +2596,7 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>1230/85</t>
+          <t>393/2</t>
         </is>
       </c>
       <c r="C167" t="n">
@@ -2609,7 +2609,7 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>1230/86</t>
+          <t>393/3</t>
         </is>
       </c>
       <c r="C168" t="n">
@@ -2622,7 +2622,7 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>1230/87</t>
+          <t>465</t>
         </is>
       </c>
       <c r="C169" t="n">
@@ -2635,7 +2635,7 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>1230/88</t>
+          <t>614</t>
         </is>
       </c>
       <c r="C170" t="n">
@@ -2648,205 +2648,10 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>1303/1</t>
+          <t>384/1</t>
         </is>
       </c>
       <c r="C171" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="172">
-      <c r="A172" s="1" t="n">
-        <v>170</v>
-      </c>
-      <c r="B172" t="inlineStr">
-        <is>
-          <t>1303/2</t>
-        </is>
-      </c>
-      <c r="C172" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="173">
-      <c r="A173" s="1" t="n">
-        <v>171</v>
-      </c>
-      <c r="B173" t="inlineStr">
-        <is>
-          <t>1309</t>
-        </is>
-      </c>
-      <c r="C173" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="174">
-      <c r="A174" s="1" t="n">
-        <v>172</v>
-      </c>
-      <c r="B174" t="inlineStr">
-        <is>
-          <t>1330</t>
-        </is>
-      </c>
-      <c r="C174" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="175">
-      <c r="A175" s="1" t="n">
-        <v>173</v>
-      </c>
-      <c r="B175" t="inlineStr">
-        <is>
-          <t>1334</t>
-        </is>
-      </c>
-      <c r="C175" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="176">
-      <c r="A176" s="1" t="n">
-        <v>174</v>
-      </c>
-      <c r="B176" t="inlineStr">
-        <is>
-          <t>1346</t>
-        </is>
-      </c>
-      <c r="C176" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="177">
-      <c r="A177" s="1" t="n">
-        <v>175</v>
-      </c>
-      <c r="B177" t="inlineStr">
-        <is>
-          <t>1369/1</t>
-        </is>
-      </c>
-      <c r="C177" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="178">
-      <c r="A178" s="1" t="n">
-        <v>176</v>
-      </c>
-      <c r="B178" t="inlineStr">
-        <is>
-          <t>194/4</t>
-        </is>
-      </c>
-      <c r="C178" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="179">
-      <c r="A179" s="1" t="n">
-        <v>177</v>
-      </c>
-      <c r="B179" t="inlineStr">
-        <is>
-          <t>254/2</t>
-        </is>
-      </c>
-      <c r="C179" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="180">
-      <c r="A180" s="1" t="n">
-        <v>178</v>
-      </c>
-      <c r="B180" t="inlineStr">
-        <is>
-          <t>337/5</t>
-        </is>
-      </c>
-      <c r="C180" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="181">
-      <c r="A181" s="1" t="n">
-        <v>179</v>
-      </c>
-      <c r="B181" t="inlineStr">
-        <is>
-          <t>393/1</t>
-        </is>
-      </c>
-      <c r="C181" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="182">
-      <c r="A182" s="1" t="n">
-        <v>180</v>
-      </c>
-      <c r="B182" t="inlineStr">
-        <is>
-          <t>393/2</t>
-        </is>
-      </c>
-      <c r="C182" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" s="1" t="n">
-        <v>181</v>
-      </c>
-      <c r="B183" t="inlineStr">
-        <is>
-          <t>393/3</t>
-        </is>
-      </c>
-      <c r="C183" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="184">
-      <c r="A184" s="1" t="n">
-        <v>182</v>
-      </c>
-      <c r="B184" t="inlineStr">
-        <is>
-          <t>465</t>
-        </is>
-      </c>
-      <c r="C184" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="185">
-      <c r="A185" s="1" t="n">
-        <v>183</v>
-      </c>
-      <c r="B185" t="inlineStr">
-        <is>
-          <t>614</t>
-        </is>
-      </c>
-      <c r="C185" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="186">
-      <c r="A186" s="1" t="n">
-        <v>184</v>
-      </c>
-      <c r="B186" t="inlineStr">
-        <is>
-          <t>384/1</t>
-        </is>
-      </c>
-      <c r="C186" t="n">
         <v>193</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Latest data: Mon Mar  4 16:14:26 UTC 2024
</commit_message>
<xml_diff>
--- a/docs/particelle_non_trovate.xlsx
+++ b/docs/particelle_non_trovate.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C171"/>
+  <dimension ref="A1:C154"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -893,7 +893,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>3577</t>
+          <t>9769/2</t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -906,7 +906,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>11008</t>
+          <t>9783/231</t>
         </is>
       </c>
       <c r="C37" t="n">
@@ -919,11 +919,11 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>11029</t>
+          <t>13823</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>44</v>
+        <v>154</v>
       </c>
     </row>
     <row r="39">
@@ -932,11 +932,11 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>11846</t>
+          <t>14724/2</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>44</v>
+        <v>154</v>
       </c>
     </row>
     <row r="40">
@@ -945,11 +945,11 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>11861</t>
+          <t>15380</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>44</v>
+        <v>154</v>
       </c>
     </row>
     <row r="41">
@@ -958,11 +958,11 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>10564</t>
+          <t>1847/1</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>44</v>
+        <v>154</v>
       </c>
     </row>
     <row r="42">
@@ -971,11 +971,11 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>10563/14</t>
+          <t>220/2</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>44</v>
+        <v>154</v>
       </c>
     </row>
     <row r="43">
@@ -984,11 +984,11 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>10563/15</t>
+          <t>8974/1</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>44</v>
+        <v>154</v>
       </c>
     </row>
     <row r="44">
@@ -997,11 +997,11 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>3535</t>
+          <t>8987/1</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>44</v>
+        <v>154</v>
       </c>
     </row>
     <row r="45">
@@ -1010,11 +1010,11 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>3570</t>
+          <t>391</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>44</v>
+        <v>174</v>
       </c>
     </row>
     <row r="46">
@@ -1023,11 +1023,11 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>2168</t>
+          <t>466</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>44</v>
+        <v>213</v>
       </c>
     </row>
     <row r="47">
@@ -1036,11 +1036,11 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>2762</t>
+          <t>.315</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>44</v>
+        <v>282</v>
       </c>
     </row>
     <row r="48">
@@ -1049,11 +1049,11 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>11867</t>
+          <t>403</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>44</v>
+        <v>97</v>
       </c>
     </row>
     <row r="49">
@@ -1062,11 +1062,11 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>5009</t>
+          <t>746</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>44</v>
+        <v>97</v>
       </c>
     </row>
     <row r="50">
@@ -1075,11 +1075,11 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>5010</t>
+          <t>749</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>44</v>
+        <v>97</v>
       </c>
     </row>
     <row r="51">
@@ -1088,11 +1088,11 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>11025/1</t>
+          <t>754</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>44</v>
+        <v>97</v>
       </c>
     </row>
     <row r="52">
@@ -1101,11 +1101,11 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>11025/2</t>
+          <t>755</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>44</v>
+        <v>97</v>
       </c>
     </row>
     <row r="53">
@@ -1114,11 +1114,11 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>11026/1</t>
+          <t>757</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>44</v>
+        <v>97</v>
       </c>
     </row>
     <row r="54">
@@ -1127,11 +1127,11 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>11260</t>
+          <t>758</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>44</v>
+        <v>97</v>
       </c>
     </row>
     <row r="55">
@@ -1140,11 +1140,11 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>13823</t>
+          <t>825/63</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>154</v>
+        <v>97</v>
       </c>
     </row>
     <row r="56">
@@ -1153,11 +1153,11 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>14724/2</t>
+          <t>1900/4</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>154</v>
+        <v>317</v>
       </c>
     </row>
     <row r="57">
@@ -1166,11 +1166,11 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>15380</t>
+          <t>9609</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>154</v>
+        <v>390</v>
       </c>
     </row>
     <row r="58">
@@ -1179,11 +1179,11 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>1847/1</t>
+          <t>9608/2</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>154</v>
+        <v>390</v>
       </c>
     </row>
     <row r="59">
@@ -1192,11 +1192,11 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>220/2</t>
+          <t>371</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>154</v>
+        <v>404</v>
       </c>
     </row>
     <row r="60">
@@ -1205,11 +1205,11 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>8974/1</t>
+          <t>373</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>154</v>
+        <v>404</v>
       </c>
     </row>
     <row r="61">
@@ -1218,11 +1218,11 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>8987/1</t>
+          <t>1741</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>154</v>
+        <v>404</v>
       </c>
     </row>
     <row r="62">
@@ -1231,11 +1231,11 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>391</t>
+          <t>1820</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>174</v>
+        <v>404</v>
       </c>
     </row>
     <row r="63">
@@ -1244,11 +1244,11 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>466</t>
+          <t>156</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>213</v>
+        <v>404</v>
       </c>
     </row>
     <row r="64">
@@ -1257,11 +1257,11 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>.315</t>
+          <t>4708</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>282</v>
+        <v>404</v>
       </c>
     </row>
     <row r="65">
@@ -1270,11 +1270,11 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>403</t>
+          <t>162/3</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>97</v>
+        <v>404</v>
       </c>
     </row>
     <row r="66">
@@ -1283,11 +1283,11 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>746</t>
+          <t>1193</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>97</v>
+        <v>404</v>
       </c>
     </row>
     <row r="67">
@@ -1296,11 +1296,11 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>749</t>
+          <t>2762</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>97</v>
+        <v>404</v>
       </c>
     </row>
     <row r="68">
@@ -1309,11 +1309,11 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>754</t>
+          <t>2766/3</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>97</v>
+        <v>404</v>
       </c>
     </row>
     <row r="69">
@@ -1322,11 +1322,11 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>755</t>
+          <t>2736/8</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>97</v>
+        <v>404</v>
       </c>
     </row>
     <row r="70">
@@ -1335,11 +1335,11 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>757</t>
+          <t>2769/1</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>97</v>
+        <v>404</v>
       </c>
     </row>
     <row r="71">
@@ -1348,11 +1348,11 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>758</t>
+          <t>2768</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>97</v>
+        <v>404</v>
       </c>
     </row>
     <row r="72">
@@ -1361,11 +1361,11 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>825/63</t>
+          <t>2767</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>97</v>
+        <v>404</v>
       </c>
     </row>
     <row r="73">
@@ -1374,11 +1374,11 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>1900/4</t>
+          <t>679/2</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>317</v>
+        <v>404</v>
       </c>
     </row>
     <row r="74">
@@ -1387,11 +1387,11 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>9609</t>
+          <t>.507/2</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>390</v>
+        <v>413</v>
       </c>
     </row>
     <row r="75">
@@ -1400,11 +1400,11 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>9608/2</t>
+          <t>.507/3</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>390</v>
+        <v>413</v>
       </c>
     </row>
     <row r="76">
@@ -1413,11 +1413,11 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>371</t>
+          <t>.507/4</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="77">
@@ -1426,11 +1426,11 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>373</t>
+          <t>507/5</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="78">
@@ -1439,11 +1439,11 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>1741</t>
+          <t>507/6</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="79">
@@ -1452,11 +1452,11 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>1820</t>
+          <t>569/8</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="80">
@@ -1465,11 +1465,11 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>156</t>
+          <t>.569/5</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="81">
@@ -1478,11 +1478,11 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>4708</t>
+          <t>7294</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="82">
@@ -1491,11 +1491,11 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>162/3</t>
+          <t>7293/2</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="83">
@@ -1504,11 +1504,11 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>1193</t>
+          <t>7293/3</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="84">
@@ -1517,11 +1517,11 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>2762</t>
+          <t>1391</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="85">
@@ -1530,11 +1530,11 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>2766/3</t>
+          <t>7292/1</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="86">
@@ -1543,11 +1543,11 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>2736/8</t>
+          <t>1358</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="87">
@@ -1556,11 +1556,11 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>2769/1</t>
+          <t>7191/4</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="88">
@@ -1569,11 +1569,11 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>2768</t>
+          <t>7618/3</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="89">
@@ -1582,11 +1582,11 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>2767</t>
+          <t>7618/4</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="90">
@@ -1595,11 +1595,11 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>679/2</t>
+          <t>114</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="91">
@@ -1608,7 +1608,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>.507/2</t>
+          <t>361</t>
         </is>
       </c>
       <c r="C91" t="n">
@@ -1621,7 +1621,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>.507/3</t>
+          <t>421</t>
         </is>
       </c>
       <c r="C92" t="n">
@@ -1634,7 +1634,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>.507/4</t>
+          <t>13094</t>
         </is>
       </c>
       <c r="C93" t="n">
@@ -1647,7 +1647,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>507/5</t>
+          <t>7290/6</t>
         </is>
       </c>
       <c r="C94" t="n">
@@ -1660,7 +1660,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>507/6</t>
+          <t>7288</t>
         </is>
       </c>
       <c r="C95" t="n">
@@ -1673,11 +1673,11 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>569/8</t>
+          <t>45</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>413</v>
+        <v>283</v>
       </c>
     </row>
     <row r="97">
@@ -1686,11 +1686,11 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>.569/5</t>
+          <t>84/1</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>413</v>
+        <v>283</v>
       </c>
     </row>
     <row r="98">
@@ -1699,11 +1699,11 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>7294</t>
+          <t>137</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>413</v>
+        <v>41</v>
       </c>
     </row>
     <row r="99">
@@ -1712,11 +1712,11 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>7293/2</t>
+          <t>140</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>413</v>
+        <v>41</v>
       </c>
     </row>
     <row r="100">
@@ -1725,11 +1725,11 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>7293/3</t>
+          <t>272</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>413</v>
+        <v>79</v>
       </c>
     </row>
     <row r="101">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>1391</t>
+          <t>1881/8</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>413</v>
+        <v>79</v>
       </c>
     </row>
     <row r="102">
@@ -1751,11 +1751,11 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>7292/1</t>
+          <t>94/6</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>413</v>
+        <v>251</v>
       </c>
     </row>
     <row r="103">
@@ -1764,11 +1764,11 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>1358</t>
+          <t>243</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>413</v>
+        <v>253</v>
       </c>
     </row>
     <row r="104">
@@ -1777,11 +1777,11 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>7191/4</t>
+          <t>295</t>
         </is>
       </c>
       <c r="C104" t="n">
-        <v>413</v>
+        <v>253</v>
       </c>
     </row>
     <row r="105">
@@ -1790,11 +1790,11 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>7618/3</t>
+          <t>1403</t>
         </is>
       </c>
       <c r="C105" t="n">
-        <v>413</v>
+        <v>268</v>
       </c>
     </row>
     <row r="106">
@@ -1803,11 +1803,11 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>7618/4</t>
+          <t>316</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>413</v>
+        <v>442</v>
       </c>
     </row>
     <row r="107">
@@ -1816,11 +1816,11 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>114</t>
+          <t>53</t>
         </is>
       </c>
       <c r="C107" t="n">
-        <v>413</v>
+        <v>215</v>
       </c>
     </row>
     <row r="108">
@@ -1829,11 +1829,11 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>361</t>
+          <t>454</t>
         </is>
       </c>
       <c r="C108" t="n">
-        <v>413</v>
+        <v>215</v>
       </c>
     </row>
     <row r="109">
@@ -1842,11 +1842,11 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>421</t>
+          <t>420/80</t>
         </is>
       </c>
       <c r="C109" t="n">
-        <v>413</v>
+        <v>215</v>
       </c>
     </row>
     <row r="110">
@@ -1855,11 +1855,11 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>13094</t>
+          <t>420/92</t>
         </is>
       </c>
       <c r="C110" t="n">
-        <v>413</v>
+        <v>215</v>
       </c>
     </row>
     <row r="111">
@@ -1868,11 +1868,11 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>7290/6</t>
+          <t>420/93</t>
         </is>
       </c>
       <c r="C111" t="n">
-        <v>413</v>
+        <v>215</v>
       </c>
     </row>
     <row r="112">
@@ -1881,11 +1881,11 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>7288</t>
+          <t>420/94</t>
         </is>
       </c>
       <c r="C112" t="n">
-        <v>413</v>
+        <v>215</v>
       </c>
     </row>
     <row r="113">
@@ -1894,11 +1894,11 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>420/95</t>
         </is>
       </c>
       <c r="C113" t="n">
-        <v>283</v>
+        <v>215</v>
       </c>
     </row>
     <row r="114">
@@ -1907,11 +1907,11 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>84/1</t>
+          <t>420/96</t>
         </is>
       </c>
       <c r="C114" t="n">
-        <v>283</v>
+        <v>215</v>
       </c>
     </row>
     <row r="115">
@@ -1920,11 +1920,11 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>137</t>
+          <t>420/97</t>
         </is>
       </c>
       <c r="C115" t="n">
-        <v>41</v>
+        <v>215</v>
       </c>
     </row>
     <row r="116">
@@ -1933,11 +1933,11 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>140</t>
+          <t>420/101</t>
         </is>
       </c>
       <c r="C116" t="n">
-        <v>41</v>
+        <v>215</v>
       </c>
     </row>
     <row r="117">
@@ -1946,11 +1946,11 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>272</t>
+          <t>420/102</t>
         </is>
       </c>
       <c r="C117" t="n">
-        <v>79</v>
+        <v>215</v>
       </c>
     </row>
     <row r="118">
@@ -1959,11 +1959,11 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>1881/8</t>
+          <t>420/106</t>
         </is>
       </c>
       <c r="C118" t="n">
-        <v>79</v>
+        <v>215</v>
       </c>
     </row>
     <row r="119">
@@ -1972,11 +1972,11 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>94/6</t>
+          <t>420/107</t>
         </is>
       </c>
       <c r="C119" t="n">
-        <v>251</v>
+        <v>215</v>
       </c>
     </row>
     <row r="120">
@@ -1985,11 +1985,11 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>243</t>
+          <t>420/109</t>
         </is>
       </c>
       <c r="C120" t="n">
-        <v>253</v>
+        <v>215</v>
       </c>
     </row>
     <row r="121">
@@ -1998,11 +1998,11 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>295</t>
+          <t>420/110</t>
         </is>
       </c>
       <c r="C121" t="n">
-        <v>253</v>
+        <v>215</v>
       </c>
     </row>
     <row r="122">
@@ -2011,11 +2011,11 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>1403</t>
+          <t>705/11</t>
         </is>
       </c>
       <c r="C122" t="n">
-        <v>268</v>
+        <v>215</v>
       </c>
     </row>
     <row r="123">
@@ -2024,11 +2024,11 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>316</t>
+          <t>756</t>
         </is>
       </c>
       <c r="C123" t="n">
-        <v>442</v>
+        <v>215</v>
       </c>
     </row>
     <row r="124">
@@ -2037,7 +2037,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>798/3</t>
         </is>
       </c>
       <c r="C124" t="n">
@@ -2050,11 +2050,11 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>454</t>
+          <t>1411/1</t>
         </is>
       </c>
       <c r="C125" t="n">
-        <v>215</v>
+        <v>256</v>
       </c>
     </row>
     <row r="126">
@@ -2063,11 +2063,11 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>420/80</t>
+          <t>1411/2</t>
         </is>
       </c>
       <c r="C126" t="n">
-        <v>215</v>
+        <v>256</v>
       </c>
     </row>
     <row r="127">
@@ -2076,11 +2076,11 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>420/92</t>
+          <t>1411/3</t>
         </is>
       </c>
       <c r="C127" t="n">
-        <v>215</v>
+        <v>256</v>
       </c>
     </row>
     <row r="128">
@@ -2089,11 +2089,11 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>420/93</t>
+          <t>1411/4</t>
         </is>
       </c>
       <c r="C128" t="n">
-        <v>215</v>
+        <v>256</v>
       </c>
     </row>
     <row r="129">
@@ -2102,11 +2102,11 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>420/94</t>
+          <t>1411/5</t>
         </is>
       </c>
       <c r="C129" t="n">
-        <v>215</v>
+        <v>256</v>
       </c>
     </row>
     <row r="130">
@@ -2115,11 +2115,11 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>420/95</t>
+          <t>1412</t>
         </is>
       </c>
       <c r="C130" t="n">
-        <v>215</v>
+        <v>256</v>
       </c>
     </row>
     <row r="131">
@@ -2128,11 +2128,11 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>420/96</t>
+          <t>1488</t>
         </is>
       </c>
       <c r="C131" t="n">
-        <v>215</v>
+        <v>256</v>
       </c>
     </row>
     <row r="132">
@@ -2141,11 +2141,11 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>420/97</t>
+          <t>1117/2</t>
         </is>
       </c>
       <c r="C132" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="133">
@@ -2154,11 +2154,11 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>420/101</t>
+          <t>1230/100</t>
         </is>
       </c>
       <c r="C133" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="134">
@@ -2167,11 +2167,11 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>420/102</t>
+          <t>1230/115</t>
         </is>
       </c>
       <c r="C134" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="135">
@@ -2180,11 +2180,11 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>420/106</t>
+          <t>1230/85</t>
         </is>
       </c>
       <c r="C135" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="136">
@@ -2193,11 +2193,11 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>420/107</t>
+          <t>1230/86</t>
         </is>
       </c>
       <c r="C136" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="137">
@@ -2206,11 +2206,11 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>420/109</t>
+          <t>1230/87</t>
         </is>
       </c>
       <c r="C137" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="138">
@@ -2219,11 +2219,11 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>420/110</t>
+          <t>1230/88</t>
         </is>
       </c>
       <c r="C138" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="139">
@@ -2232,11 +2232,11 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>705/11</t>
+          <t>1303/1</t>
         </is>
       </c>
       <c r="C139" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="140">
@@ -2245,11 +2245,11 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>756</t>
+          <t>1303/2</t>
         </is>
       </c>
       <c r="C140" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="141">
@@ -2258,11 +2258,11 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>798/3</t>
+          <t>1309</t>
         </is>
       </c>
       <c r="C141" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="142">
@@ -2271,11 +2271,11 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>1411/1</t>
+          <t>1330</t>
         </is>
       </c>
       <c r="C142" t="n">
-        <v>256</v>
+        <v>193</v>
       </c>
     </row>
     <row r="143">
@@ -2284,11 +2284,11 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>1411/2</t>
+          <t>1334</t>
         </is>
       </c>
       <c r="C143" t="n">
-        <v>256</v>
+        <v>193</v>
       </c>
     </row>
     <row r="144">
@@ -2297,11 +2297,11 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>1411/3</t>
+          <t>1346</t>
         </is>
       </c>
       <c r="C144" t="n">
-        <v>256</v>
+        <v>193</v>
       </c>
     </row>
     <row r="145">
@@ -2310,11 +2310,11 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>1411/4</t>
+          <t>1369/1</t>
         </is>
       </c>
       <c r="C145" t="n">
-        <v>256</v>
+        <v>193</v>
       </c>
     </row>
     <row r="146">
@@ -2323,11 +2323,11 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>1411/5</t>
+          <t>194/4</t>
         </is>
       </c>
       <c r="C146" t="n">
-        <v>256</v>
+        <v>193</v>
       </c>
     </row>
     <row r="147">
@@ -2336,11 +2336,11 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>1412</t>
+          <t>254/2</t>
         </is>
       </c>
       <c r="C147" t="n">
-        <v>256</v>
+        <v>193</v>
       </c>
     </row>
     <row r="148">
@@ -2349,11 +2349,11 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>1488</t>
+          <t>337/5</t>
         </is>
       </c>
       <c r="C148" t="n">
-        <v>256</v>
+        <v>193</v>
       </c>
     </row>
     <row r="149">
@@ -2362,7 +2362,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>1117/2</t>
+          <t>393/1</t>
         </is>
       </c>
       <c r="C149" t="n">
@@ -2375,7 +2375,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>1230/100</t>
+          <t>393/2</t>
         </is>
       </c>
       <c r="C150" t="n">
@@ -2388,7 +2388,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>1230/115</t>
+          <t>393/3</t>
         </is>
       </c>
       <c r="C151" t="n">
@@ -2401,7 +2401,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>1230/85</t>
+          <t>465</t>
         </is>
       </c>
       <c r="C152" t="n">
@@ -2414,7 +2414,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>1230/86</t>
+          <t>614</t>
         </is>
       </c>
       <c r="C153" t="n">
@@ -2427,231 +2427,10 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>1230/87</t>
+          <t>384/1</t>
         </is>
       </c>
       <c r="C154" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="155">
-      <c r="A155" s="1" t="n">
-        <v>153</v>
-      </c>
-      <c r="B155" t="inlineStr">
-        <is>
-          <t>1230/88</t>
-        </is>
-      </c>
-      <c r="C155" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="156">
-      <c r="A156" s="1" t="n">
-        <v>154</v>
-      </c>
-      <c r="B156" t="inlineStr">
-        <is>
-          <t>1303/1</t>
-        </is>
-      </c>
-      <c r="C156" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="157">
-      <c r="A157" s="1" t="n">
-        <v>155</v>
-      </c>
-      <c r="B157" t="inlineStr">
-        <is>
-          <t>1303/2</t>
-        </is>
-      </c>
-      <c r="C157" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="158">
-      <c r="A158" s="1" t="n">
-        <v>156</v>
-      </c>
-      <c r="B158" t="inlineStr">
-        <is>
-          <t>1309</t>
-        </is>
-      </c>
-      <c r="C158" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="159">
-      <c r="A159" s="1" t="n">
-        <v>157</v>
-      </c>
-      <c r="B159" t="inlineStr">
-        <is>
-          <t>1330</t>
-        </is>
-      </c>
-      <c r="C159" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="160">
-      <c r="A160" s="1" t="n">
-        <v>158</v>
-      </c>
-      <c r="B160" t="inlineStr">
-        <is>
-          <t>1334</t>
-        </is>
-      </c>
-      <c r="C160" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="161">
-      <c r="A161" s="1" t="n">
-        <v>159</v>
-      </c>
-      <c r="B161" t="inlineStr">
-        <is>
-          <t>1346</t>
-        </is>
-      </c>
-      <c r="C161" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="162">
-      <c r="A162" s="1" t="n">
-        <v>160</v>
-      </c>
-      <c r="B162" t="inlineStr">
-        <is>
-          <t>1369/1</t>
-        </is>
-      </c>
-      <c r="C162" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="163">
-      <c r="A163" s="1" t="n">
-        <v>161</v>
-      </c>
-      <c r="B163" t="inlineStr">
-        <is>
-          <t>194/4</t>
-        </is>
-      </c>
-      <c r="C163" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="164">
-      <c r="A164" s="1" t="n">
-        <v>162</v>
-      </c>
-      <c r="B164" t="inlineStr">
-        <is>
-          <t>254/2</t>
-        </is>
-      </c>
-      <c r="C164" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="165">
-      <c r="A165" s="1" t="n">
-        <v>163</v>
-      </c>
-      <c r="B165" t="inlineStr">
-        <is>
-          <t>337/5</t>
-        </is>
-      </c>
-      <c r="C165" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="166">
-      <c r="A166" s="1" t="n">
-        <v>164</v>
-      </c>
-      <c r="B166" t="inlineStr">
-        <is>
-          <t>393/1</t>
-        </is>
-      </c>
-      <c r="C166" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="167">
-      <c r="A167" s="1" t="n">
-        <v>165</v>
-      </c>
-      <c r="B167" t="inlineStr">
-        <is>
-          <t>393/2</t>
-        </is>
-      </c>
-      <c r="C167" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="168">
-      <c r="A168" s="1" t="n">
-        <v>166</v>
-      </c>
-      <c r="B168" t="inlineStr">
-        <is>
-          <t>393/3</t>
-        </is>
-      </c>
-      <c r="C168" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="169">
-      <c r="A169" s="1" t="n">
-        <v>167</v>
-      </c>
-      <c r="B169" t="inlineStr">
-        <is>
-          <t>465</t>
-        </is>
-      </c>
-      <c r="C169" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="170">
-      <c r="A170" s="1" t="n">
-        <v>168</v>
-      </c>
-      <c r="B170" t="inlineStr">
-        <is>
-          <t>614</t>
-        </is>
-      </c>
-      <c r="C170" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="171">
-      <c r="A171" s="1" t="n">
-        <v>169</v>
-      </c>
-      <c r="B171" t="inlineStr">
-        <is>
-          <t>384/1</t>
-        </is>
-      </c>
-      <c r="C171" t="n">
         <v>193</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Latest data: Wed Mar  6 16:11:12 UTC 2024
</commit_message>
<xml_diff>
--- a/docs/particelle_non_trovate.xlsx
+++ b/docs/particelle_non_trovate.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Latest data: Thu Mar  7 20:07:52 UTC 2024
</commit_message>
<xml_diff>
--- a/docs/particelle_non_trovate.xlsx
+++ b/docs/particelle_non_trovate.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1215"/>
+  <dimension ref="A1:C1178"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13360,7 +13360,7 @@
       </c>
       <c r="B995" t="inlineStr">
         <is>
-          <t>9609</t>
+          <t>1272/3</t>
         </is>
       </c>
       <c r="C995" t="n">
@@ -13373,11 +13373,11 @@
       </c>
       <c r="B996" t="inlineStr">
         <is>
-          <t>9608/2</t>
+          <t>765</t>
         </is>
       </c>
       <c r="C996" t="n">
-        <v>390</v>
+        <v>404</v>
       </c>
     </row>
     <row r="997">
@@ -13386,11 +13386,11 @@
       </c>
       <c r="B997" t="inlineStr">
         <is>
-          <t>371</t>
+          <t>134</t>
         </is>
       </c>
       <c r="C997" t="n">
-        <v>404</v>
+        <v>41</v>
       </c>
     </row>
     <row r="998">
@@ -13399,11 +13399,11 @@
       </c>
       <c r="B998" t="inlineStr">
         <is>
-          <t>373</t>
+          <t>135</t>
         </is>
       </c>
       <c r="C998" t="n">
-        <v>404</v>
+        <v>41</v>
       </c>
     </row>
     <row r="999">
@@ -13412,11 +13412,11 @@
       </c>
       <c r="B999" t="inlineStr">
         <is>
-          <t>1741</t>
+          <t>136</t>
         </is>
       </c>
       <c r="C999" t="n">
-        <v>404</v>
+        <v>41</v>
       </c>
     </row>
     <row r="1000">
@@ -13425,11 +13425,11 @@
       </c>
       <c r="B1000" t="inlineStr">
         <is>
-          <t>1820</t>
+          <t>137/1</t>
         </is>
       </c>
       <c r="C1000" t="n">
-        <v>404</v>
+        <v>41</v>
       </c>
     </row>
     <row r="1001">
@@ -13438,11 +13438,11 @@
       </c>
       <c r="B1001" t="inlineStr">
         <is>
-          <t>156</t>
+          <t>137/8</t>
         </is>
       </c>
       <c r="C1001" t="n">
-        <v>404</v>
+        <v>41</v>
       </c>
     </row>
     <row r="1002">
@@ -13451,11 +13451,11 @@
       </c>
       <c r="B1002" t="inlineStr">
         <is>
-          <t>4708</t>
+          <t>138/1</t>
         </is>
       </c>
       <c r="C1002" t="n">
-        <v>404</v>
+        <v>41</v>
       </c>
     </row>
     <row r="1003">
@@ -13464,11 +13464,11 @@
       </c>
       <c r="B1003" t="inlineStr">
         <is>
-          <t>162/3</t>
+          <t>138/3</t>
         </is>
       </c>
       <c r="C1003" t="n">
-        <v>404</v>
+        <v>41</v>
       </c>
     </row>
     <row r="1004">
@@ -13477,11 +13477,11 @@
       </c>
       <c r="B1004" t="inlineStr">
         <is>
-          <t>1193</t>
+          <t>138/4</t>
         </is>
       </c>
       <c r="C1004" t="n">
-        <v>404</v>
+        <v>41</v>
       </c>
     </row>
     <row r="1005">
@@ -13490,11 +13490,11 @@
       </c>
       <c r="B1005" t="inlineStr">
         <is>
-          <t>2762</t>
+          <t>138/5</t>
         </is>
       </c>
       <c r="C1005" t="n">
-        <v>404</v>
+        <v>41</v>
       </c>
     </row>
     <row r="1006">
@@ -13503,11 +13503,11 @@
       </c>
       <c r="B1006" t="inlineStr">
         <is>
-          <t>2766/3</t>
+          <t>138/19</t>
         </is>
       </c>
       <c r="C1006" t="n">
-        <v>404</v>
+        <v>41</v>
       </c>
     </row>
     <row r="1007">
@@ -13516,11 +13516,11 @@
       </c>
       <c r="B1007" t="inlineStr">
         <is>
-          <t>2736/8</t>
+          <t>138/20</t>
         </is>
       </c>
       <c r="C1007" t="n">
-        <v>404</v>
+        <v>41</v>
       </c>
     </row>
     <row r="1008">
@@ -13529,11 +13529,11 @@
       </c>
       <c r="B1008" t="inlineStr">
         <is>
-          <t>2769/1</t>
+          <t>280</t>
         </is>
       </c>
       <c r="C1008" t="n">
-        <v>404</v>
+        <v>41</v>
       </c>
     </row>
     <row r="1009">
@@ -13542,11 +13542,11 @@
       </c>
       <c r="B1009" t="inlineStr">
         <is>
-          <t>2768</t>
+          <t>3057</t>
         </is>
       </c>
       <c r="C1009" t="n">
-        <v>404</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1010">
@@ -13555,11 +13555,11 @@
       </c>
       <c r="B1010" t="inlineStr">
         <is>
-          <t>2767</t>
+          <t>3071</t>
         </is>
       </c>
       <c r="C1010" t="n">
-        <v>404</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1011">
@@ -13568,11 +13568,11 @@
       </c>
       <c r="B1011" t="inlineStr">
         <is>
-          <t>679/2</t>
+          <t>.547</t>
         </is>
       </c>
       <c r="C1011" t="n">
-        <v>404</v>
+        <v>79</v>
       </c>
     </row>
     <row r="1012">
@@ -13581,11 +13581,11 @@
       </c>
       <c r="B1012" t="inlineStr">
         <is>
-          <t>.507/2</t>
+          <t>.548</t>
         </is>
       </c>
       <c r="C1012" t="n">
-        <v>413</v>
+        <v>79</v>
       </c>
     </row>
     <row r="1013">
@@ -13594,11 +13594,11 @@
       </c>
       <c r="B1013" t="inlineStr">
         <is>
-          <t>.507/3</t>
+          <t>2160</t>
         </is>
       </c>
       <c r="C1013" t="n">
-        <v>413</v>
+        <v>79</v>
       </c>
     </row>
     <row r="1014">
@@ -13607,11 +13607,11 @@
       </c>
       <c r="B1014" t="inlineStr">
         <is>
-          <t>.507/4</t>
+          <t>2185</t>
         </is>
       </c>
       <c r="C1014" t="n">
-        <v>413</v>
+        <v>79</v>
       </c>
     </row>
     <row r="1015">
@@ -13620,11 +13620,11 @@
       </c>
       <c r="B1015" t="inlineStr">
         <is>
-          <t>507/5</t>
+          <t>3070</t>
         </is>
       </c>
       <c r="C1015" t="n">
-        <v>413</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1016">
@@ -13633,11 +13633,11 @@
       </c>
       <c r="B1016" t="inlineStr">
         <is>
-          <t>507/6</t>
+          <t>94/6</t>
         </is>
       </c>
       <c r="C1016" t="n">
-        <v>413</v>
+        <v>251</v>
       </c>
     </row>
     <row r="1017">
@@ -13646,11 +13646,11 @@
       </c>
       <c r="B1017" t="inlineStr">
         <is>
-          <t>569/8</t>
+          <t>1389/1</t>
         </is>
       </c>
       <c r="C1017" t="n">
-        <v>413</v>
+        <v>79</v>
       </c>
     </row>
     <row r="1018">
@@ -13659,11 +13659,11 @@
       </c>
       <c r="B1018" t="inlineStr">
         <is>
-          <t>.569/5</t>
+          <t>1389/2</t>
         </is>
       </c>
       <c r="C1018" t="n">
-        <v>413</v>
+        <v>79</v>
       </c>
     </row>
     <row r="1019">
@@ -13672,11 +13672,11 @@
       </c>
       <c r="B1019" t="inlineStr">
         <is>
-          <t>7294</t>
+          <t>1389/3</t>
         </is>
       </c>
       <c r="C1019" t="n">
-        <v>413</v>
+        <v>79</v>
       </c>
     </row>
     <row r="1020">
@@ -13685,11 +13685,11 @@
       </c>
       <c r="B1020" t="inlineStr">
         <is>
-          <t>7293/2</t>
+          <t>1389/4</t>
         </is>
       </c>
       <c r="C1020" t="n">
-        <v>413</v>
+        <v>79</v>
       </c>
     </row>
     <row r="1021">
@@ -13698,11 +13698,11 @@
       </c>
       <c r="B1021" t="inlineStr">
         <is>
-          <t>7293/3</t>
+          <t>1389/5</t>
         </is>
       </c>
       <c r="C1021" t="n">
-        <v>413</v>
+        <v>79</v>
       </c>
     </row>
     <row r="1022">
@@ -13711,11 +13711,11 @@
       </c>
       <c r="B1022" t="inlineStr">
         <is>
-          <t>1391</t>
+          <t>1389/6</t>
         </is>
       </c>
       <c r="C1022" t="n">
-        <v>413</v>
+        <v>79</v>
       </c>
     </row>
     <row r="1023">
@@ -13724,11 +13724,11 @@
       </c>
       <c r="B1023" t="inlineStr">
         <is>
-          <t>7292/1</t>
+          <t>2023/2</t>
         </is>
       </c>
       <c r="C1023" t="n">
-        <v>413</v>
+        <v>79</v>
       </c>
     </row>
     <row r="1024">
@@ -13737,11 +13737,11 @@
       </c>
       <c r="B1024" t="inlineStr">
         <is>
-          <t>1358</t>
+          <t>2028/1</t>
         </is>
       </c>
       <c r="C1024" t="n">
-        <v>413</v>
+        <v>79</v>
       </c>
     </row>
     <row r="1025">
@@ -13750,11 +13750,11 @@
       </c>
       <c r="B1025" t="inlineStr">
         <is>
-          <t>7191/4</t>
+          <t>2027/1</t>
         </is>
       </c>
       <c r="C1025" t="n">
-        <v>413</v>
+        <v>79</v>
       </c>
     </row>
     <row r="1026">
@@ -13763,11 +13763,11 @@
       </c>
       <c r="B1026" t="inlineStr">
         <is>
-          <t>7618/3</t>
+          <t>100/3</t>
         </is>
       </c>
       <c r="C1026" t="n">
-        <v>413</v>
+        <v>79</v>
       </c>
     </row>
     <row r="1027">
@@ -13776,11 +13776,11 @@
       </c>
       <c r="B1027" t="inlineStr">
         <is>
-          <t>7618/4</t>
+          <t>100/4</t>
         </is>
       </c>
       <c r="C1027" t="n">
-        <v>413</v>
+        <v>79</v>
       </c>
     </row>
     <row r="1028">
@@ -13789,11 +13789,11 @@
       </c>
       <c r="B1028" t="inlineStr">
         <is>
-          <t>114</t>
+          <t>100/5</t>
         </is>
       </c>
       <c r="C1028" t="n">
-        <v>413</v>
+        <v>79</v>
       </c>
     </row>
     <row r="1029">
@@ -13802,11 +13802,11 @@
       </c>
       <c r="B1029" t="inlineStr">
         <is>
-          <t>361</t>
+          <t>100/6</t>
         </is>
       </c>
       <c r="C1029" t="n">
-        <v>413</v>
+        <v>79</v>
       </c>
     </row>
     <row r="1030">
@@ -13815,11 +13815,11 @@
       </c>
       <c r="B1030" t="inlineStr">
         <is>
-          <t>421</t>
+          <t>275</t>
         </is>
       </c>
       <c r="C1030" t="n">
-        <v>413</v>
+        <v>79</v>
       </c>
     </row>
     <row r="1031">
@@ -13828,11 +13828,11 @@
       </c>
       <c r="B1031" t="inlineStr">
         <is>
-          <t>13094</t>
+          <t>327</t>
         </is>
       </c>
       <c r="C1031" t="n">
-        <v>413</v>
+        <v>79</v>
       </c>
     </row>
     <row r="1032">
@@ -13841,11 +13841,11 @@
       </c>
       <c r="B1032" t="inlineStr">
         <is>
-          <t>7290/6</t>
+          <t>410/2</t>
         </is>
       </c>
       <c r="C1032" t="n">
-        <v>413</v>
+        <v>79</v>
       </c>
     </row>
     <row r="1033">
@@ -13854,11 +13854,11 @@
       </c>
       <c r="B1033" t="inlineStr">
         <is>
-          <t>7288</t>
+          <t>.615</t>
         </is>
       </c>
       <c r="C1033" t="n">
-        <v>413</v>
+        <v>79</v>
       </c>
     </row>
     <row r="1034">
@@ -13867,11 +13867,11 @@
       </c>
       <c r="B1034" t="inlineStr">
         <is>
-          <t>134</t>
+          <t>.616</t>
         </is>
       </c>
       <c r="C1034" t="n">
-        <v>41</v>
+        <v>79</v>
       </c>
     </row>
     <row r="1035">
@@ -13880,11 +13880,11 @@
       </c>
       <c r="B1035" t="inlineStr">
         <is>
-          <t>135</t>
+          <t>.617</t>
         </is>
       </c>
       <c r="C1035" t="n">
-        <v>41</v>
+        <v>79</v>
       </c>
     </row>
     <row r="1036">
@@ -13893,11 +13893,11 @@
       </c>
       <c r="B1036" t="inlineStr">
         <is>
-          <t>136</t>
+          <t>.618</t>
         </is>
       </c>
       <c r="C1036" t="n">
-        <v>41</v>
+        <v>79</v>
       </c>
     </row>
     <row r="1037">
@@ -13906,11 +13906,11 @@
       </c>
       <c r="B1037" t="inlineStr">
         <is>
-          <t>137/1</t>
+          <t>.619</t>
         </is>
       </c>
       <c r="C1037" t="n">
-        <v>41</v>
+        <v>79</v>
       </c>
     </row>
     <row r="1038">
@@ -13919,11 +13919,11 @@
       </c>
       <c r="B1038" t="inlineStr">
         <is>
-          <t>137/8</t>
+          <t>874</t>
         </is>
       </c>
       <c r="C1038" t="n">
-        <v>41</v>
+        <v>79</v>
       </c>
     </row>
     <row r="1039">
@@ -13932,11 +13932,11 @@
       </c>
       <c r="B1039" t="inlineStr">
         <is>
-          <t>138/1</t>
+          <t>912</t>
         </is>
       </c>
       <c r="C1039" t="n">
-        <v>41</v>
+        <v>79</v>
       </c>
     </row>
     <row r="1040">
@@ -13945,11 +13945,11 @@
       </c>
       <c r="B1040" t="inlineStr">
         <is>
-          <t>138/3</t>
+          <t>1390/1</t>
         </is>
       </c>
       <c r="C1040" t="n">
-        <v>41</v>
+        <v>79</v>
       </c>
     </row>
     <row r="1041">
@@ -13958,11 +13958,11 @@
       </c>
       <c r="B1041" t="inlineStr">
         <is>
-          <t>138/4</t>
+          <t>1390/2</t>
         </is>
       </c>
       <c r="C1041" t="n">
-        <v>41</v>
+        <v>79</v>
       </c>
     </row>
     <row r="1042">
@@ -13971,11 +13971,11 @@
       </c>
       <c r="B1042" t="inlineStr">
         <is>
-          <t>138/5</t>
+          <t>1489</t>
         </is>
       </c>
       <c r="C1042" t="n">
-        <v>41</v>
+        <v>79</v>
       </c>
     </row>
     <row r="1043">
@@ -13984,11 +13984,11 @@
       </c>
       <c r="B1043" t="inlineStr">
         <is>
-          <t>138/19</t>
+          <t>1545</t>
         </is>
       </c>
       <c r="C1043" t="n">
-        <v>41</v>
+        <v>79</v>
       </c>
     </row>
     <row r="1044">
@@ -13997,11 +13997,11 @@
       </c>
       <c r="B1044" t="inlineStr">
         <is>
-          <t>138/20</t>
+          <t>1786</t>
         </is>
       </c>
       <c r="C1044" t="n">
-        <v>41</v>
+        <v>79</v>
       </c>
     </row>
     <row r="1045">
@@ -14010,11 +14010,11 @@
       </c>
       <c r="B1045" t="inlineStr">
         <is>
-          <t>280</t>
+          <t>1845/1</t>
         </is>
       </c>
       <c r="C1045" t="n">
-        <v>41</v>
+        <v>79</v>
       </c>
     </row>
     <row r="1046">
@@ -14023,11 +14023,11 @@
       </c>
       <c r="B1046" t="inlineStr">
         <is>
-          <t>3057</t>
+          <t>1845/2</t>
         </is>
       </c>
       <c r="C1046" t="n">
-        <v>4</v>
+        <v>79</v>
       </c>
     </row>
     <row r="1047">
@@ -14036,11 +14036,11 @@
       </c>
       <c r="B1047" t="inlineStr">
         <is>
-          <t>3071</t>
+          <t>1880</t>
         </is>
       </c>
       <c r="C1047" t="n">
-        <v>4</v>
+        <v>79</v>
       </c>
     </row>
     <row r="1048">
@@ -14049,7 +14049,7 @@
       </c>
       <c r="B1048" t="inlineStr">
         <is>
-          <t>.547</t>
+          <t>1881/1</t>
         </is>
       </c>
       <c r="C1048" t="n">
@@ -14062,7 +14062,7 @@
       </c>
       <c r="B1049" t="inlineStr">
         <is>
-          <t>.548</t>
+          <t>1883</t>
         </is>
       </c>
       <c r="C1049" t="n">
@@ -14075,7 +14075,7 @@
       </c>
       <c r="B1050" t="inlineStr">
         <is>
-          <t>2160</t>
+          <t>1884</t>
         </is>
       </c>
       <c r="C1050" t="n">
@@ -14088,7 +14088,7 @@
       </c>
       <c r="B1051" t="inlineStr">
         <is>
-          <t>2185</t>
+          <t>1948</t>
         </is>
       </c>
       <c r="C1051" t="n">
@@ -14101,11 +14101,11 @@
       </c>
       <c r="B1052" t="inlineStr">
         <is>
-          <t>3070</t>
+          <t>1989</t>
         </is>
       </c>
       <c r="C1052" t="n">
-        <v>4</v>
+        <v>79</v>
       </c>
     </row>
     <row r="1053">
@@ -14114,11 +14114,11 @@
       </c>
       <c r="B1053" t="inlineStr">
         <is>
-          <t>94/6</t>
+          <t>2125</t>
         </is>
       </c>
       <c r="C1053" t="n">
-        <v>251</v>
+        <v>79</v>
       </c>
     </row>
     <row r="1054">
@@ -14127,7 +14127,7 @@
       </c>
       <c r="B1054" t="inlineStr">
         <is>
-          <t>1389/1</t>
+          <t>2151</t>
         </is>
       </c>
       <c r="C1054" t="n">
@@ -14140,7 +14140,7 @@
       </c>
       <c r="B1055" t="inlineStr">
         <is>
-          <t>1389/2</t>
+          <t>2343</t>
         </is>
       </c>
       <c r="C1055" t="n">
@@ -14151,482 +14151,260 @@
       <c r="A1056" s="1" t="n">
         <v>1054</v>
       </c>
-      <c r="B1056" t="inlineStr">
-        <is>
-          <t>1389/3</t>
-        </is>
-      </c>
-      <c r="C1056" t="n">
-        <v>79</v>
-      </c>
+      <c r="B1056" t="inlineStr"/>
+      <c r="C1056" t="inlineStr"/>
     </row>
     <row r="1057">
       <c r="A1057" s="1" t="n">
         <v>1055</v>
       </c>
-      <c r="B1057" t="inlineStr">
-        <is>
-          <t>1389/4</t>
-        </is>
-      </c>
-      <c r="C1057" t="n">
-        <v>79</v>
-      </c>
+      <c r="B1057" t="inlineStr"/>
+      <c r="C1057" t="inlineStr"/>
     </row>
     <row r="1058">
       <c r="A1058" s="1" t="n">
         <v>1056</v>
       </c>
-      <c r="B1058" t="inlineStr">
-        <is>
-          <t>1389/5</t>
-        </is>
-      </c>
-      <c r="C1058" t="n">
-        <v>79</v>
-      </c>
+      <c r="B1058" t="inlineStr"/>
+      <c r="C1058" t="inlineStr"/>
     </row>
     <row r="1059">
       <c r="A1059" s="1" t="n">
         <v>1057</v>
       </c>
-      <c r="B1059" t="inlineStr">
-        <is>
-          <t>1389/6</t>
-        </is>
-      </c>
-      <c r="C1059" t="n">
-        <v>79</v>
-      </c>
+      <c r="B1059" t="inlineStr"/>
+      <c r="C1059" t="inlineStr"/>
     </row>
     <row r="1060">
       <c r="A1060" s="1" t="n">
         <v>1058</v>
       </c>
-      <c r="B1060" t="inlineStr">
-        <is>
-          <t>2023/2</t>
-        </is>
-      </c>
-      <c r="C1060" t="n">
-        <v>79</v>
-      </c>
+      <c r="B1060" t="inlineStr"/>
+      <c r="C1060" t="inlineStr"/>
     </row>
     <row r="1061">
       <c r="A1061" s="1" t="n">
         <v>1059</v>
       </c>
-      <c r="B1061" t="inlineStr">
-        <is>
-          <t>2028/1</t>
-        </is>
-      </c>
-      <c r="C1061" t="n">
-        <v>79</v>
-      </c>
+      <c r="B1061" t="inlineStr"/>
+      <c r="C1061" t="inlineStr"/>
     </row>
     <row r="1062">
       <c r="A1062" s="1" t="n">
         <v>1060</v>
       </c>
-      <c r="B1062" t="inlineStr">
-        <is>
-          <t>2027/1</t>
-        </is>
-      </c>
-      <c r="C1062" t="n">
-        <v>79</v>
-      </c>
+      <c r="B1062" t="inlineStr"/>
+      <c r="C1062" t="inlineStr"/>
     </row>
     <row r="1063">
       <c r="A1063" s="1" t="n">
         <v>1061</v>
       </c>
-      <c r="B1063" t="inlineStr">
-        <is>
-          <t>100/3</t>
-        </is>
-      </c>
-      <c r="C1063" t="n">
-        <v>79</v>
-      </c>
+      <c r="B1063" t="inlineStr"/>
+      <c r="C1063" t="inlineStr"/>
     </row>
     <row r="1064">
       <c r="A1064" s="1" t="n">
         <v>1062</v>
       </c>
-      <c r="B1064" t="inlineStr">
-        <is>
-          <t>100/4</t>
-        </is>
-      </c>
-      <c r="C1064" t="n">
-        <v>79</v>
-      </c>
+      <c r="B1064" t="inlineStr"/>
+      <c r="C1064" t="inlineStr"/>
     </row>
     <row r="1065">
       <c r="A1065" s="1" t="n">
         <v>1063</v>
       </c>
-      <c r="B1065" t="inlineStr">
-        <is>
-          <t>100/5</t>
-        </is>
-      </c>
-      <c r="C1065" t="n">
-        <v>79</v>
-      </c>
+      <c r="B1065" t="inlineStr"/>
+      <c r="C1065" t="inlineStr"/>
     </row>
     <row r="1066">
       <c r="A1066" s="1" t="n">
         <v>1064</v>
       </c>
-      <c r="B1066" t="inlineStr">
-        <is>
-          <t>100/6</t>
-        </is>
-      </c>
-      <c r="C1066" t="n">
-        <v>79</v>
-      </c>
+      <c r="B1066" t="inlineStr"/>
+      <c r="C1066" t="inlineStr"/>
     </row>
     <row r="1067">
       <c r="A1067" s="1" t="n">
         <v>1065</v>
       </c>
-      <c r="B1067" t="inlineStr">
-        <is>
-          <t>275</t>
-        </is>
-      </c>
-      <c r="C1067" t="n">
-        <v>79</v>
-      </c>
+      <c r="B1067" t="inlineStr"/>
+      <c r="C1067" t="inlineStr"/>
     </row>
     <row r="1068">
       <c r="A1068" s="1" t="n">
         <v>1066</v>
       </c>
-      <c r="B1068" t="inlineStr">
-        <is>
-          <t>327</t>
-        </is>
-      </c>
-      <c r="C1068" t="n">
-        <v>79</v>
-      </c>
+      <c r="B1068" t="inlineStr"/>
+      <c r="C1068" t="inlineStr"/>
     </row>
     <row r="1069">
       <c r="A1069" s="1" t="n">
         <v>1067</v>
       </c>
-      <c r="B1069" t="inlineStr">
-        <is>
-          <t>410/2</t>
-        </is>
-      </c>
-      <c r="C1069" t="n">
-        <v>79</v>
-      </c>
+      <c r="B1069" t="inlineStr"/>
+      <c r="C1069" t="inlineStr"/>
     </row>
     <row r="1070">
       <c r="A1070" s="1" t="n">
         <v>1068</v>
       </c>
-      <c r="B1070" t="inlineStr">
-        <is>
-          <t>.615</t>
-        </is>
-      </c>
-      <c r="C1070" t="n">
-        <v>79</v>
-      </c>
+      <c r="B1070" t="inlineStr"/>
+      <c r="C1070" t="inlineStr"/>
     </row>
     <row r="1071">
       <c r="A1071" s="1" t="n">
         <v>1069</v>
       </c>
-      <c r="B1071" t="inlineStr">
-        <is>
-          <t>.616</t>
-        </is>
-      </c>
-      <c r="C1071" t="n">
-        <v>79</v>
-      </c>
+      <c r="B1071" t="inlineStr"/>
+      <c r="C1071" t="inlineStr"/>
     </row>
     <row r="1072">
       <c r="A1072" s="1" t="n">
         <v>1070</v>
       </c>
-      <c r="B1072" t="inlineStr">
-        <is>
-          <t>.617</t>
-        </is>
-      </c>
-      <c r="C1072" t="n">
-        <v>79</v>
-      </c>
+      <c r="B1072" t="inlineStr"/>
+      <c r="C1072" t="inlineStr"/>
     </row>
     <row r="1073">
       <c r="A1073" s="1" t="n">
         <v>1071</v>
       </c>
-      <c r="B1073" t="inlineStr">
-        <is>
-          <t>.618</t>
-        </is>
-      </c>
-      <c r="C1073" t="n">
-        <v>79</v>
-      </c>
+      <c r="B1073" t="inlineStr"/>
+      <c r="C1073" t="inlineStr"/>
     </row>
     <row r="1074">
       <c r="A1074" s="1" t="n">
         <v>1072</v>
       </c>
-      <c r="B1074" t="inlineStr">
-        <is>
-          <t>.619</t>
-        </is>
-      </c>
-      <c r="C1074" t="n">
-        <v>79</v>
-      </c>
+      <c r="B1074" t="inlineStr"/>
+      <c r="C1074" t="inlineStr"/>
     </row>
     <row r="1075">
       <c r="A1075" s="1" t="n">
         <v>1073</v>
       </c>
-      <c r="B1075" t="inlineStr">
-        <is>
-          <t>874</t>
-        </is>
-      </c>
-      <c r="C1075" t="n">
-        <v>79</v>
-      </c>
+      <c r="B1075" t="inlineStr"/>
+      <c r="C1075" t="inlineStr"/>
     </row>
     <row r="1076">
       <c r="A1076" s="1" t="n">
         <v>1074</v>
       </c>
-      <c r="B1076" t="inlineStr">
-        <is>
-          <t>912</t>
-        </is>
-      </c>
-      <c r="C1076" t="n">
-        <v>79</v>
-      </c>
+      <c r="B1076" t="inlineStr"/>
+      <c r="C1076" t="inlineStr"/>
     </row>
     <row r="1077">
       <c r="A1077" s="1" t="n">
         <v>1075</v>
       </c>
-      <c r="B1077" t="inlineStr">
-        <is>
-          <t>1390/1</t>
-        </is>
-      </c>
-      <c r="C1077" t="n">
-        <v>79</v>
-      </c>
+      <c r="B1077" t="inlineStr"/>
+      <c r="C1077" t="inlineStr"/>
     </row>
     <row r="1078">
       <c r="A1078" s="1" t="n">
         <v>1076</v>
       </c>
-      <c r="B1078" t="inlineStr">
-        <is>
-          <t>1390/2</t>
-        </is>
-      </c>
-      <c r="C1078" t="n">
-        <v>79</v>
-      </c>
+      <c r="B1078" t="inlineStr"/>
+      <c r="C1078" t="inlineStr"/>
     </row>
     <row r="1079">
       <c r="A1079" s="1" t="n">
         <v>1077</v>
       </c>
-      <c r="B1079" t="inlineStr">
-        <is>
-          <t>1489</t>
-        </is>
-      </c>
-      <c r="C1079" t="n">
-        <v>79</v>
-      </c>
+      <c r="B1079" t="inlineStr"/>
+      <c r="C1079" t="inlineStr"/>
     </row>
     <row r="1080">
       <c r="A1080" s="1" t="n">
         <v>1078</v>
       </c>
-      <c r="B1080" t="inlineStr">
-        <is>
-          <t>1545</t>
-        </is>
-      </c>
-      <c r="C1080" t="n">
-        <v>79</v>
-      </c>
+      <c r="B1080" t="inlineStr"/>
+      <c r="C1080" t="inlineStr"/>
     </row>
     <row r="1081">
       <c r="A1081" s="1" t="n">
         <v>1079</v>
       </c>
-      <c r="B1081" t="inlineStr">
-        <is>
-          <t>1786</t>
-        </is>
-      </c>
-      <c r="C1081" t="n">
-        <v>79</v>
-      </c>
+      <c r="B1081" t="inlineStr"/>
+      <c r="C1081" t="inlineStr"/>
     </row>
     <row r="1082">
       <c r="A1082" s="1" t="n">
         <v>1080</v>
       </c>
-      <c r="B1082" t="inlineStr">
-        <is>
-          <t>1845/1</t>
-        </is>
-      </c>
-      <c r="C1082" t="n">
-        <v>79</v>
-      </c>
+      <c r="B1082" t="inlineStr"/>
+      <c r="C1082" t="inlineStr"/>
     </row>
     <row r="1083">
       <c r="A1083" s="1" t="n">
         <v>1081</v>
       </c>
-      <c r="B1083" t="inlineStr">
-        <is>
-          <t>1845/2</t>
-        </is>
-      </c>
-      <c r="C1083" t="n">
-        <v>79</v>
-      </c>
+      <c r="B1083" t="inlineStr"/>
+      <c r="C1083" t="inlineStr"/>
     </row>
     <row r="1084">
       <c r="A1084" s="1" t="n">
         <v>1082</v>
       </c>
-      <c r="B1084" t="inlineStr">
-        <is>
-          <t>1880</t>
-        </is>
-      </c>
-      <c r="C1084" t="n">
-        <v>79</v>
-      </c>
+      <c r="B1084" t="inlineStr"/>
+      <c r="C1084" t="inlineStr"/>
     </row>
     <row r="1085">
       <c r="A1085" s="1" t="n">
         <v>1083</v>
       </c>
-      <c r="B1085" t="inlineStr">
-        <is>
-          <t>1881/1</t>
-        </is>
-      </c>
-      <c r="C1085" t="n">
-        <v>79</v>
-      </c>
+      <c r="B1085" t="inlineStr"/>
+      <c r="C1085" t="inlineStr"/>
     </row>
     <row r="1086">
       <c r="A1086" s="1" t="n">
         <v>1084</v>
       </c>
-      <c r="B1086" t="inlineStr">
-        <is>
-          <t>1883</t>
-        </is>
-      </c>
-      <c r="C1086" t="n">
-        <v>79</v>
-      </c>
+      <c r="B1086" t="inlineStr"/>
+      <c r="C1086" t="inlineStr"/>
     </row>
     <row r="1087">
       <c r="A1087" s="1" t="n">
         <v>1085</v>
       </c>
-      <c r="B1087" t="inlineStr">
-        <is>
-          <t>1884</t>
-        </is>
-      </c>
-      <c r="C1087" t="n">
-        <v>79</v>
-      </c>
+      <c r="B1087" t="inlineStr"/>
+      <c r="C1087" t="inlineStr"/>
     </row>
     <row r="1088">
       <c r="A1088" s="1" t="n">
         <v>1086</v>
       </c>
-      <c r="B1088" t="inlineStr">
-        <is>
-          <t>1948</t>
-        </is>
-      </c>
-      <c r="C1088" t="n">
-        <v>79</v>
-      </c>
+      <c r="B1088" t="inlineStr"/>
+      <c r="C1088" t="inlineStr"/>
     </row>
     <row r="1089">
       <c r="A1089" s="1" t="n">
         <v>1087</v>
       </c>
-      <c r="B1089" t="inlineStr">
-        <is>
-          <t>1989</t>
-        </is>
-      </c>
-      <c r="C1089" t="n">
-        <v>79</v>
-      </c>
+      <c r="B1089" t="inlineStr"/>
+      <c r="C1089" t="inlineStr"/>
     </row>
     <row r="1090">
       <c r="A1090" s="1" t="n">
         <v>1088</v>
       </c>
-      <c r="B1090" t="inlineStr">
-        <is>
-          <t>2125</t>
-        </is>
-      </c>
-      <c r="C1090" t="n">
-        <v>79</v>
-      </c>
+      <c r="B1090" t="inlineStr"/>
+      <c r="C1090" t="inlineStr"/>
     </row>
     <row r="1091">
       <c r="A1091" s="1" t="n">
         <v>1089</v>
       </c>
-      <c r="B1091" t="inlineStr">
-        <is>
-          <t>2151</t>
-        </is>
-      </c>
-      <c r="C1091" t="n">
-        <v>79</v>
-      </c>
+      <c r="B1091" t="inlineStr"/>
+      <c r="C1091" t="inlineStr"/>
     </row>
     <row r="1092">
       <c r="A1092" s="1" t="n">
         <v>1090</v>
       </c>
-      <c r="B1092" t="inlineStr">
-        <is>
-          <t>2343</t>
-        </is>
-      </c>
-      <c r="C1092" t="n">
-        <v>79</v>
-      </c>
+      <c r="B1092" t="inlineStr"/>
+      <c r="C1092" t="inlineStr"/>
     </row>
     <row r="1093">
       <c r="A1093" s="1" t="n">
@@ -14877,260 +14655,482 @@
       <c r="A1128" s="1" t="n">
         <v>1126</v>
       </c>
-      <c r="B1128" t="inlineStr"/>
-      <c r="C1128" t="inlineStr"/>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>316</t>
+        </is>
+      </c>
+      <c r="C1128" t="n">
+        <v>442</v>
+      </c>
     </row>
     <row r="1129">
       <c r="A1129" s="1" t="n">
         <v>1127</v>
       </c>
-      <c r="B1129" t="inlineStr"/>
-      <c r="C1129" t="inlineStr"/>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>390</t>
+        </is>
+      </c>
+      <c r="C1129" t="n">
+        <v>85</v>
+      </c>
     </row>
     <row r="1130">
       <c r="A1130" s="1" t="n">
         <v>1128</v>
       </c>
-      <c r="B1130" t="inlineStr"/>
-      <c r="C1130" t="inlineStr"/>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>391/1</t>
+        </is>
+      </c>
+      <c r="C1130" t="n">
+        <v>85</v>
+      </c>
     </row>
     <row r="1131">
       <c r="A1131" s="1" t="n">
         <v>1129</v>
       </c>
-      <c r="B1131" t="inlineStr"/>
-      <c r="C1131" t="inlineStr"/>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="C1131" t="n">
+        <v>215</v>
+      </c>
     </row>
     <row r="1132">
       <c r="A1132" s="1" t="n">
         <v>1130</v>
       </c>
-      <c r="B1132" t="inlineStr"/>
-      <c r="C1132" t="inlineStr"/>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>454</t>
+        </is>
+      </c>
+      <c r="C1132" t="n">
+        <v>215</v>
+      </c>
     </row>
     <row r="1133">
       <c r="A1133" s="1" t="n">
         <v>1131</v>
       </c>
-      <c r="B1133" t="inlineStr"/>
-      <c r="C1133" t="inlineStr"/>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>420/80</t>
+        </is>
+      </c>
+      <c r="C1133" t="n">
+        <v>215</v>
+      </c>
     </row>
     <row r="1134">
       <c r="A1134" s="1" t="n">
         <v>1132</v>
       </c>
-      <c r="B1134" t="inlineStr"/>
-      <c r="C1134" t="inlineStr"/>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>420/92</t>
+        </is>
+      </c>
+      <c r="C1134" t="n">
+        <v>215</v>
+      </c>
     </row>
     <row r="1135">
       <c r="A1135" s="1" t="n">
         <v>1133</v>
       </c>
-      <c r="B1135" t="inlineStr"/>
-      <c r="C1135" t="inlineStr"/>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>420/93</t>
+        </is>
+      </c>
+      <c r="C1135" t="n">
+        <v>215</v>
+      </c>
     </row>
     <row r="1136">
       <c r="A1136" s="1" t="n">
         <v>1134</v>
       </c>
-      <c r="B1136" t="inlineStr"/>
-      <c r="C1136" t="inlineStr"/>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>420/94</t>
+        </is>
+      </c>
+      <c r="C1136" t="n">
+        <v>215</v>
+      </c>
     </row>
     <row r="1137">
       <c r="A1137" s="1" t="n">
         <v>1135</v>
       </c>
-      <c r="B1137" t="inlineStr"/>
-      <c r="C1137" t="inlineStr"/>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>420/95</t>
+        </is>
+      </c>
+      <c r="C1137" t="n">
+        <v>215</v>
+      </c>
     </row>
     <row r="1138">
       <c r="A1138" s="1" t="n">
         <v>1136</v>
       </c>
-      <c r="B1138" t="inlineStr"/>
-      <c r="C1138" t="inlineStr"/>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>420/96</t>
+        </is>
+      </c>
+      <c r="C1138" t="n">
+        <v>215</v>
+      </c>
     </row>
     <row r="1139">
       <c r="A1139" s="1" t="n">
         <v>1137</v>
       </c>
-      <c r="B1139" t="inlineStr"/>
-      <c r="C1139" t="inlineStr"/>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>420/97</t>
+        </is>
+      </c>
+      <c r="C1139" t="n">
+        <v>215</v>
+      </c>
     </row>
     <row r="1140">
       <c r="A1140" s="1" t="n">
         <v>1138</v>
       </c>
-      <c r="B1140" t="inlineStr"/>
-      <c r="C1140" t="inlineStr"/>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>420/101</t>
+        </is>
+      </c>
+      <c r="C1140" t="n">
+        <v>215</v>
+      </c>
     </row>
     <row r="1141">
       <c r="A1141" s="1" t="n">
         <v>1139</v>
       </c>
-      <c r="B1141" t="inlineStr"/>
-      <c r="C1141" t="inlineStr"/>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>420/102</t>
+        </is>
+      </c>
+      <c r="C1141" t="n">
+        <v>215</v>
+      </c>
     </row>
     <row r="1142">
       <c r="A1142" s="1" t="n">
         <v>1140</v>
       </c>
-      <c r="B1142" t="inlineStr"/>
-      <c r="C1142" t="inlineStr"/>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>420/106</t>
+        </is>
+      </c>
+      <c r="C1142" t="n">
+        <v>215</v>
+      </c>
     </row>
     <row r="1143">
       <c r="A1143" s="1" t="n">
         <v>1141</v>
       </c>
-      <c r="B1143" t="inlineStr"/>
-      <c r="C1143" t="inlineStr"/>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>420/107</t>
+        </is>
+      </c>
+      <c r="C1143" t="n">
+        <v>215</v>
+      </c>
     </row>
     <row r="1144">
       <c r="A1144" s="1" t="n">
         <v>1142</v>
       </c>
-      <c r="B1144" t="inlineStr"/>
-      <c r="C1144" t="inlineStr"/>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>420/109</t>
+        </is>
+      </c>
+      <c r="C1144" t="n">
+        <v>215</v>
+      </c>
     </row>
     <row r="1145">
       <c r="A1145" s="1" t="n">
         <v>1143</v>
       </c>
-      <c r="B1145" t="inlineStr"/>
-      <c r="C1145" t="inlineStr"/>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>420/110</t>
+        </is>
+      </c>
+      <c r="C1145" t="n">
+        <v>215</v>
+      </c>
     </row>
     <row r="1146">
       <c r="A1146" s="1" t="n">
         <v>1144</v>
       </c>
-      <c r="B1146" t="inlineStr"/>
-      <c r="C1146" t="inlineStr"/>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>705/11</t>
+        </is>
+      </c>
+      <c r="C1146" t="n">
+        <v>215</v>
+      </c>
     </row>
     <row r="1147">
       <c r="A1147" s="1" t="n">
         <v>1145</v>
       </c>
-      <c r="B1147" t="inlineStr"/>
-      <c r="C1147" t="inlineStr"/>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>756</t>
+        </is>
+      </c>
+      <c r="C1147" t="n">
+        <v>215</v>
+      </c>
     </row>
     <row r="1148">
       <c r="A1148" s="1" t="n">
         <v>1146</v>
       </c>
-      <c r="B1148" t="inlineStr"/>
-      <c r="C1148" t="inlineStr"/>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>798/3</t>
+        </is>
+      </c>
+      <c r="C1148" t="n">
+        <v>215</v>
+      </c>
     </row>
     <row r="1149">
       <c r="A1149" s="1" t="n">
         <v>1147</v>
       </c>
-      <c r="B1149" t="inlineStr"/>
-      <c r="C1149" t="inlineStr"/>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>1411/1</t>
+        </is>
+      </c>
+      <c r="C1149" t="n">
+        <v>256</v>
+      </c>
     </row>
     <row r="1150">
       <c r="A1150" s="1" t="n">
         <v>1148</v>
       </c>
-      <c r="B1150" t="inlineStr"/>
-      <c r="C1150" t="inlineStr"/>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>1411/2</t>
+        </is>
+      </c>
+      <c r="C1150" t="n">
+        <v>256</v>
+      </c>
     </row>
     <row r="1151">
       <c r="A1151" s="1" t="n">
         <v>1149</v>
       </c>
-      <c r="B1151" t="inlineStr"/>
-      <c r="C1151" t="inlineStr"/>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>1411/3</t>
+        </is>
+      </c>
+      <c r="C1151" t="n">
+        <v>256</v>
+      </c>
     </row>
     <row r="1152">
       <c r="A1152" s="1" t="n">
         <v>1150</v>
       </c>
-      <c r="B1152" t="inlineStr"/>
-      <c r="C1152" t="inlineStr"/>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>1411/4</t>
+        </is>
+      </c>
+      <c r="C1152" t="n">
+        <v>256</v>
+      </c>
     </row>
     <row r="1153">
       <c r="A1153" s="1" t="n">
         <v>1151</v>
       </c>
-      <c r="B1153" t="inlineStr"/>
-      <c r="C1153" t="inlineStr"/>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>1411/5</t>
+        </is>
+      </c>
+      <c r="C1153" t="n">
+        <v>256</v>
+      </c>
     </row>
     <row r="1154">
       <c r="A1154" s="1" t="n">
         <v>1152</v>
       </c>
-      <c r="B1154" t="inlineStr"/>
-      <c r="C1154" t="inlineStr"/>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>1412</t>
+        </is>
+      </c>
+      <c r="C1154" t="n">
+        <v>256</v>
+      </c>
     </row>
     <row r="1155">
       <c r="A1155" s="1" t="n">
         <v>1153</v>
       </c>
-      <c r="B1155" t="inlineStr"/>
-      <c r="C1155" t="inlineStr"/>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>1488</t>
+        </is>
+      </c>
+      <c r="C1155" t="n">
+        <v>256</v>
+      </c>
     </row>
     <row r="1156">
       <c r="A1156" s="1" t="n">
         <v>1154</v>
       </c>
-      <c r="B1156" t="inlineStr"/>
-      <c r="C1156" t="inlineStr"/>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>1117/2</t>
+        </is>
+      </c>
+      <c r="C1156" t="n">
+        <v>193</v>
+      </c>
     </row>
     <row r="1157">
       <c r="A1157" s="1" t="n">
         <v>1155</v>
       </c>
-      <c r="B1157" t="inlineStr"/>
-      <c r="C1157" t="inlineStr"/>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>1230/100</t>
+        </is>
+      </c>
+      <c r="C1157" t="n">
+        <v>193</v>
+      </c>
     </row>
     <row r="1158">
       <c r="A1158" s="1" t="n">
         <v>1156</v>
       </c>
-      <c r="B1158" t="inlineStr"/>
-      <c r="C1158" t="inlineStr"/>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>1230/115</t>
+        </is>
+      </c>
+      <c r="C1158" t="n">
+        <v>193</v>
+      </c>
     </row>
     <row r="1159">
       <c r="A1159" s="1" t="n">
         <v>1157</v>
       </c>
-      <c r="B1159" t="inlineStr"/>
-      <c r="C1159" t="inlineStr"/>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>1230/85</t>
+        </is>
+      </c>
+      <c r="C1159" t="n">
+        <v>193</v>
+      </c>
     </row>
     <row r="1160">
       <c r="A1160" s="1" t="n">
         <v>1158</v>
       </c>
-      <c r="B1160" t="inlineStr"/>
-      <c r="C1160" t="inlineStr"/>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>1230/86</t>
+        </is>
+      </c>
+      <c r="C1160" t="n">
+        <v>193</v>
+      </c>
     </row>
     <row r="1161">
       <c r="A1161" s="1" t="n">
         <v>1159</v>
       </c>
-      <c r="B1161" t="inlineStr"/>
-      <c r="C1161" t="inlineStr"/>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>1230/87</t>
+        </is>
+      </c>
+      <c r="C1161" t="n">
+        <v>193</v>
+      </c>
     </row>
     <row r="1162">
       <c r="A1162" s="1" t="n">
         <v>1160</v>
       </c>
-      <c r="B1162" t="inlineStr"/>
-      <c r="C1162" t="inlineStr"/>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>1230/88</t>
+        </is>
+      </c>
+      <c r="C1162" t="n">
+        <v>193</v>
+      </c>
     </row>
     <row r="1163">
       <c r="A1163" s="1" t="n">
         <v>1161</v>
       </c>
-      <c r="B1163" t="inlineStr"/>
-      <c r="C1163" t="inlineStr"/>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>1303/1</t>
+        </is>
+      </c>
+      <c r="C1163" t="n">
+        <v>193</v>
+      </c>
     </row>
     <row r="1164">
       <c r="A1164" s="1" t="n">
         <v>1162</v>
       </c>
-      <c r="B1164" t="inlineStr"/>
-      <c r="C1164" t="inlineStr"/>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>1303/2</t>
+        </is>
+      </c>
+      <c r="C1164" t="n">
+        <v>193</v>
+      </c>
     </row>
     <row r="1165">
       <c r="A1165" s="1" t="n">
@@ -15138,11 +15138,11 @@
       </c>
       <c r="B1165" t="inlineStr">
         <is>
-          <t>316</t>
+          <t>1309</t>
         </is>
       </c>
       <c r="C1165" t="n">
-        <v>442</v>
+        <v>193</v>
       </c>
     </row>
     <row r="1166">
@@ -15151,11 +15151,11 @@
       </c>
       <c r="B1166" t="inlineStr">
         <is>
-          <t>390</t>
+          <t>1330</t>
         </is>
       </c>
       <c r="C1166" t="n">
-        <v>85</v>
+        <v>193</v>
       </c>
     </row>
     <row r="1167">
@@ -15164,11 +15164,11 @@
       </c>
       <c r="B1167" t="inlineStr">
         <is>
-          <t>391/1</t>
+          <t>1334</t>
         </is>
       </c>
       <c r="C1167" t="n">
-        <v>85</v>
+        <v>193</v>
       </c>
     </row>
     <row r="1168">
@@ -15177,11 +15177,11 @@
       </c>
       <c r="B1168" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>1346</t>
         </is>
       </c>
       <c r="C1168" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="1169">
@@ -15190,11 +15190,11 @@
       </c>
       <c r="B1169" t="inlineStr">
         <is>
-          <t>454</t>
+          <t>1369/1</t>
         </is>
       </c>
       <c r="C1169" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="1170">
@@ -15203,11 +15203,11 @@
       </c>
       <c r="B1170" t="inlineStr">
         <is>
-          <t>420/80</t>
+          <t>194/4</t>
         </is>
       </c>
       <c r="C1170" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="1171">
@@ -15216,11 +15216,11 @@
       </c>
       <c r="B1171" t="inlineStr">
         <is>
-          <t>420/92</t>
+          <t>254/2</t>
         </is>
       </c>
       <c r="C1171" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="1172">
@@ -15229,11 +15229,11 @@
       </c>
       <c r="B1172" t="inlineStr">
         <is>
-          <t>420/93</t>
+          <t>337/5</t>
         </is>
       </c>
       <c r="C1172" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="1173">
@@ -15242,11 +15242,11 @@
       </c>
       <c r="B1173" t="inlineStr">
         <is>
-          <t>420/94</t>
+          <t>393/1</t>
         </is>
       </c>
       <c r="C1173" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="1174">
@@ -15255,11 +15255,11 @@
       </c>
       <c r="B1174" t="inlineStr">
         <is>
-          <t>420/95</t>
+          <t>393/2</t>
         </is>
       </c>
       <c r="C1174" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="1175">
@@ -15268,11 +15268,11 @@
       </c>
       <c r="B1175" t="inlineStr">
         <is>
-          <t>420/96</t>
+          <t>393/3</t>
         </is>
       </c>
       <c r="C1175" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="1176">
@@ -15281,11 +15281,11 @@
       </c>
       <c r="B1176" t="inlineStr">
         <is>
-          <t>420/97</t>
+          <t>465</t>
         </is>
       </c>
       <c r="C1176" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="1177">
@@ -15294,11 +15294,11 @@
       </c>
       <c r="B1177" t="inlineStr">
         <is>
-          <t>420/101</t>
+          <t>614</t>
         </is>
       </c>
       <c r="C1177" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="1178">
@@ -15307,491 +15307,10 @@
       </c>
       <c r="B1178" t="inlineStr">
         <is>
-          <t>420/102</t>
+          <t>384/1</t>
         </is>
       </c>
       <c r="C1178" t="n">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="1179">
-      <c r="A1179" s="1" t="n">
-        <v>1177</v>
-      </c>
-      <c r="B1179" t="inlineStr">
-        <is>
-          <t>420/106</t>
-        </is>
-      </c>
-      <c r="C1179" t="n">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="1180">
-      <c r="A1180" s="1" t="n">
-        <v>1178</v>
-      </c>
-      <c r="B1180" t="inlineStr">
-        <is>
-          <t>420/107</t>
-        </is>
-      </c>
-      <c r="C1180" t="n">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="1181">
-      <c r="A1181" s="1" t="n">
-        <v>1179</v>
-      </c>
-      <c r="B1181" t="inlineStr">
-        <is>
-          <t>420/109</t>
-        </is>
-      </c>
-      <c r="C1181" t="n">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="1182">
-      <c r="A1182" s="1" t="n">
-        <v>1180</v>
-      </c>
-      <c r="B1182" t="inlineStr">
-        <is>
-          <t>420/110</t>
-        </is>
-      </c>
-      <c r="C1182" t="n">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="1183">
-      <c r="A1183" s="1" t="n">
-        <v>1181</v>
-      </c>
-      <c r="B1183" t="inlineStr">
-        <is>
-          <t>705/11</t>
-        </is>
-      </c>
-      <c r="C1183" t="n">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="1184">
-      <c r="A1184" s="1" t="n">
-        <v>1182</v>
-      </c>
-      <c r="B1184" t="inlineStr">
-        <is>
-          <t>756</t>
-        </is>
-      </c>
-      <c r="C1184" t="n">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="1185">
-      <c r="A1185" s="1" t="n">
-        <v>1183</v>
-      </c>
-      <c r="B1185" t="inlineStr">
-        <is>
-          <t>798/3</t>
-        </is>
-      </c>
-      <c r="C1185" t="n">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="1186">
-      <c r="A1186" s="1" t="n">
-        <v>1184</v>
-      </c>
-      <c r="B1186" t="inlineStr">
-        <is>
-          <t>1411/1</t>
-        </is>
-      </c>
-      <c r="C1186" t="n">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="1187">
-      <c r="A1187" s="1" t="n">
-        <v>1185</v>
-      </c>
-      <c r="B1187" t="inlineStr">
-        <is>
-          <t>1411/2</t>
-        </is>
-      </c>
-      <c r="C1187" t="n">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="1188">
-      <c r="A1188" s="1" t="n">
-        <v>1186</v>
-      </c>
-      <c r="B1188" t="inlineStr">
-        <is>
-          <t>1411/3</t>
-        </is>
-      </c>
-      <c r="C1188" t="n">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="1189">
-      <c r="A1189" s="1" t="n">
-        <v>1187</v>
-      </c>
-      <c r="B1189" t="inlineStr">
-        <is>
-          <t>1411/4</t>
-        </is>
-      </c>
-      <c r="C1189" t="n">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="1190">
-      <c r="A1190" s="1" t="n">
-        <v>1188</v>
-      </c>
-      <c r="B1190" t="inlineStr">
-        <is>
-          <t>1411/5</t>
-        </is>
-      </c>
-      <c r="C1190" t="n">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="1191">
-      <c r="A1191" s="1" t="n">
-        <v>1189</v>
-      </c>
-      <c r="B1191" t="inlineStr">
-        <is>
-          <t>1412</t>
-        </is>
-      </c>
-      <c r="C1191" t="n">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="1192">
-      <c r="A1192" s="1" t="n">
-        <v>1190</v>
-      </c>
-      <c r="B1192" t="inlineStr">
-        <is>
-          <t>1488</t>
-        </is>
-      </c>
-      <c r="C1192" t="n">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="1193">
-      <c r="A1193" s="1" t="n">
-        <v>1191</v>
-      </c>
-      <c r="B1193" t="inlineStr">
-        <is>
-          <t>1117/2</t>
-        </is>
-      </c>
-      <c r="C1193" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="1194">
-      <c r="A1194" s="1" t="n">
-        <v>1192</v>
-      </c>
-      <c r="B1194" t="inlineStr">
-        <is>
-          <t>1230/100</t>
-        </is>
-      </c>
-      <c r="C1194" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="1195">
-      <c r="A1195" s="1" t="n">
-        <v>1193</v>
-      </c>
-      <c r="B1195" t="inlineStr">
-        <is>
-          <t>1230/115</t>
-        </is>
-      </c>
-      <c r="C1195" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="1196">
-      <c r="A1196" s="1" t="n">
-        <v>1194</v>
-      </c>
-      <c r="B1196" t="inlineStr">
-        <is>
-          <t>1230/85</t>
-        </is>
-      </c>
-      <c r="C1196" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="1197">
-      <c r="A1197" s="1" t="n">
-        <v>1195</v>
-      </c>
-      <c r="B1197" t="inlineStr">
-        <is>
-          <t>1230/86</t>
-        </is>
-      </c>
-      <c r="C1197" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="1198">
-      <c r="A1198" s="1" t="n">
-        <v>1196</v>
-      </c>
-      <c r="B1198" t="inlineStr">
-        <is>
-          <t>1230/87</t>
-        </is>
-      </c>
-      <c r="C1198" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="1199">
-      <c r="A1199" s="1" t="n">
-        <v>1197</v>
-      </c>
-      <c r="B1199" t="inlineStr">
-        <is>
-          <t>1230/88</t>
-        </is>
-      </c>
-      <c r="C1199" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="1200">
-      <c r="A1200" s="1" t="n">
-        <v>1198</v>
-      </c>
-      <c r="B1200" t="inlineStr">
-        <is>
-          <t>1303/1</t>
-        </is>
-      </c>
-      <c r="C1200" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="1201">
-      <c r="A1201" s="1" t="n">
-        <v>1199</v>
-      </c>
-      <c r="B1201" t="inlineStr">
-        <is>
-          <t>1303/2</t>
-        </is>
-      </c>
-      <c r="C1201" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="1202">
-      <c r="A1202" s="1" t="n">
-        <v>1200</v>
-      </c>
-      <c r="B1202" t="inlineStr">
-        <is>
-          <t>1309</t>
-        </is>
-      </c>
-      <c r="C1202" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="1203">
-      <c r="A1203" s="1" t="n">
-        <v>1201</v>
-      </c>
-      <c r="B1203" t="inlineStr">
-        <is>
-          <t>1330</t>
-        </is>
-      </c>
-      <c r="C1203" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="1204">
-      <c r="A1204" s="1" t="n">
-        <v>1202</v>
-      </c>
-      <c r="B1204" t="inlineStr">
-        <is>
-          <t>1334</t>
-        </is>
-      </c>
-      <c r="C1204" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="1205">
-      <c r="A1205" s="1" t="n">
-        <v>1203</v>
-      </c>
-      <c r="B1205" t="inlineStr">
-        <is>
-          <t>1346</t>
-        </is>
-      </c>
-      <c r="C1205" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="1206">
-      <c r="A1206" s="1" t="n">
-        <v>1204</v>
-      </c>
-      <c r="B1206" t="inlineStr">
-        <is>
-          <t>1369/1</t>
-        </is>
-      </c>
-      <c r="C1206" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="1207">
-      <c r="A1207" s="1" t="n">
-        <v>1205</v>
-      </c>
-      <c r="B1207" t="inlineStr">
-        <is>
-          <t>194/4</t>
-        </is>
-      </c>
-      <c r="C1207" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="1208">
-      <c r="A1208" s="1" t="n">
-        <v>1206</v>
-      </c>
-      <c r="B1208" t="inlineStr">
-        <is>
-          <t>254/2</t>
-        </is>
-      </c>
-      <c r="C1208" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="1209">
-      <c r="A1209" s="1" t="n">
-        <v>1207</v>
-      </c>
-      <c r="B1209" t="inlineStr">
-        <is>
-          <t>337/5</t>
-        </is>
-      </c>
-      <c r="C1209" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="1210">
-      <c r="A1210" s="1" t="n">
-        <v>1208</v>
-      </c>
-      <c r="B1210" t="inlineStr">
-        <is>
-          <t>393/1</t>
-        </is>
-      </c>
-      <c r="C1210" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="1211">
-      <c r="A1211" s="1" t="n">
-        <v>1209</v>
-      </c>
-      <c r="B1211" t="inlineStr">
-        <is>
-          <t>393/2</t>
-        </is>
-      </c>
-      <c r="C1211" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="1212">
-      <c r="A1212" s="1" t="n">
-        <v>1210</v>
-      </c>
-      <c r="B1212" t="inlineStr">
-        <is>
-          <t>393/3</t>
-        </is>
-      </c>
-      <c r="C1212" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="1213">
-      <c r="A1213" s="1" t="n">
-        <v>1211</v>
-      </c>
-      <c r="B1213" t="inlineStr">
-        <is>
-          <t>465</t>
-        </is>
-      </c>
-      <c r="C1213" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="1214">
-      <c r="A1214" s="1" t="n">
-        <v>1212</v>
-      </c>
-      <c r="B1214" t="inlineStr">
-        <is>
-          <t>614</t>
-        </is>
-      </c>
-      <c r="C1214" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="1215">
-      <c r="A1215" s="1" t="n">
-        <v>1213</v>
-      </c>
-      <c r="B1215" t="inlineStr">
-        <is>
-          <t>384/1</t>
-        </is>
-      </c>
-      <c r="C1215" t="n">
         <v>193</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Latest data: Fri Mar  8 00:31:39 UTC 2024
</commit_message>
<xml_diff>
--- a/docs/particelle_non_trovate.xlsx
+++ b/docs/particelle_non_trovate.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1178"/>
+  <dimension ref="A1:C1182"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15314,6 +15314,58 @@
         <v>193</v>
       </c>
     </row>
+    <row r="1179">
+      <c r="A1179" s="1" t="n">
+        <v>1177</v>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>4523</t>
+        </is>
+      </c>
+      <c r="C1179" t="n">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" s="1" t="n">
+        <v>1178</v>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>1911/5</t>
+        </is>
+      </c>
+      <c r="C1180" t="n">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" s="1" t="n">
+        <v>1179</v>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>1912/5</t>
+        </is>
+      </c>
+      <c r="C1181" t="n">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" s="1" t="n">
+        <v>1180</v>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>1912/5</t>
+        </is>
+      </c>
+      <c r="C1182" t="n">
+        <v>404</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Latest data: Sat Mar  9 20:10:04 UTC 2024
</commit_message>
<xml_diff>
--- a/docs/particelle_non_trovate.xlsx
+++ b/docs/particelle_non_trovate.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Latest data: Sun Mar 10 12:13:53 UTC 2024
</commit_message>
<xml_diff>
--- a/docs/particelle_non_trovate.xlsx
+++ b/docs/particelle_non_trovate.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C91"/>
+  <dimension ref="A1:C88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -659,7 +659,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>15380</t>
+          <t>8974/1</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -672,7 +672,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>1847/1</t>
+          <t>15380</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -685,11 +685,11 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>220/2</t>
+          <t>391</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>154</v>
+        <v>174</v>
       </c>
     </row>
     <row r="21">
@@ -698,11 +698,11 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>8974/1</t>
+          <t>466</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>154</v>
+        <v>213</v>
       </c>
     </row>
     <row r="22">
@@ -711,11 +711,11 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>8987/1</t>
+          <t>.315</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>154</v>
+        <v>282</v>
       </c>
     </row>
     <row r="23">
@@ -724,11 +724,11 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>391</t>
+          <t>403</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>174</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24">
@@ -737,11 +737,11 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>466</t>
+          <t>746</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>213</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25">
@@ -750,11 +750,11 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>.315</t>
+          <t>749</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>282</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26">
@@ -763,7 +763,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>403</t>
+          <t>754</t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -776,7 +776,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>746</t>
+          <t>755</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -789,7 +789,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>749</t>
+          <t>757</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -802,7 +802,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>754</t>
+          <t>758</t>
         </is>
       </c>
       <c r="C29" t="n">
@@ -815,7 +815,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>755</t>
+          <t>825/63</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -828,11 +828,11 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>757</t>
+          <t>1900/4</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>97</v>
+        <v>317</v>
       </c>
     </row>
     <row r="32">
@@ -841,11 +841,11 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>758</t>
+          <t>1272/3</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>97</v>
+        <v>390</v>
       </c>
     </row>
     <row r="33">
@@ -854,11 +854,11 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>825/63</t>
+          <t>765</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>97</v>
+        <v>404</v>
       </c>
     </row>
     <row r="34">
@@ -867,11 +867,11 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>1900/4</t>
+          <t>94/6</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>317</v>
+        <v>251</v>
       </c>
     </row>
     <row r="35">
@@ -880,11 +880,11 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>1272/3</t>
+          <t>2681/1</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>390</v>
+        <v>442</v>
       </c>
     </row>
     <row r="36">
@@ -893,11 +893,11 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>765</t>
+          <t>789</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>404</v>
+        <v>443</v>
       </c>
     </row>
     <row r="37">
@@ -906,11 +906,11 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>94/6</t>
+          <t>53</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>251</v>
+        <v>215</v>
       </c>
     </row>
     <row r="38">
@@ -919,11 +919,11 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>2681/1</t>
+          <t>454</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>442</v>
+        <v>215</v>
       </c>
     </row>
     <row r="39">
@@ -932,11 +932,11 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>789</t>
+          <t>420/80</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>443</v>
+        <v>215</v>
       </c>
     </row>
     <row r="40">
@@ -945,7 +945,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>420/92</t>
         </is>
       </c>
       <c r="C40" t="n">
@@ -958,7 +958,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>454</t>
+          <t>420/93</t>
         </is>
       </c>
       <c r="C41" t="n">
@@ -971,7 +971,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>420/80</t>
+          <t>420/94</t>
         </is>
       </c>
       <c r="C42" t="n">
@@ -984,7 +984,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>420/92</t>
+          <t>420/95</t>
         </is>
       </c>
       <c r="C43" t="n">
@@ -997,7 +997,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>420/93</t>
+          <t>420/96</t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -1010,7 +1010,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>420/94</t>
+          <t>420/97</t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -1023,7 +1023,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>420/95</t>
+          <t>420/101</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -1036,7 +1036,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>420/96</t>
+          <t>420/102</t>
         </is>
       </c>
       <c r="C47" t="n">
@@ -1049,7 +1049,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>420/97</t>
+          <t>420/106</t>
         </is>
       </c>
       <c r="C48" t="n">
@@ -1062,7 +1062,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>420/101</t>
+          <t>420/107</t>
         </is>
       </c>
       <c r="C49" t="n">
@@ -1075,7 +1075,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>420/102</t>
+          <t>420/109</t>
         </is>
       </c>
       <c r="C50" t="n">
@@ -1088,7 +1088,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>420/106</t>
+          <t>420/110</t>
         </is>
       </c>
       <c r="C51" t="n">
@@ -1101,7 +1101,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>420/107</t>
+          <t>705/11</t>
         </is>
       </c>
       <c r="C52" t="n">
@@ -1114,7 +1114,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>420/109</t>
+          <t>756</t>
         </is>
       </c>
       <c r="C53" t="n">
@@ -1127,7 +1127,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>420/110</t>
+          <t>798/3</t>
         </is>
       </c>
       <c r="C54" t="n">
@@ -1140,11 +1140,11 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>705/11</t>
+          <t>1411/1</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>215</v>
+        <v>256</v>
       </c>
     </row>
     <row r="56">
@@ -1153,11 +1153,11 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>756</t>
+          <t>1411/2</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>215</v>
+        <v>256</v>
       </c>
     </row>
     <row r="57">
@@ -1166,11 +1166,11 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>798/3</t>
+          <t>1411/3</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>215</v>
+        <v>256</v>
       </c>
     </row>
     <row r="58">
@@ -1179,7 +1179,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>1411/1</t>
+          <t>1411/4</t>
         </is>
       </c>
       <c r="C58" t="n">
@@ -1192,7 +1192,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>1411/2</t>
+          <t>1411/5</t>
         </is>
       </c>
       <c r="C59" t="n">
@@ -1205,7 +1205,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>1411/3</t>
+          <t>1412</t>
         </is>
       </c>
       <c r="C60" t="n">
@@ -1218,7 +1218,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>1411/4</t>
+          <t>1488</t>
         </is>
       </c>
       <c r="C61" t="n">
@@ -1231,11 +1231,11 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>1411/5</t>
+          <t>1117/2</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>256</v>
+        <v>193</v>
       </c>
     </row>
     <row r="63">
@@ -1244,11 +1244,11 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>1412</t>
+          <t>1230/100</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>256</v>
+        <v>193</v>
       </c>
     </row>
     <row r="64">
@@ -1257,11 +1257,11 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>1488</t>
+          <t>1230/115</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>256</v>
+        <v>193</v>
       </c>
     </row>
     <row r="65">
@@ -1270,7 +1270,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>1117/2</t>
+          <t>1230/85</t>
         </is>
       </c>
       <c r="C65" t="n">
@@ -1283,7 +1283,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>1230/100</t>
+          <t>1230/86</t>
         </is>
       </c>
       <c r="C66" t="n">
@@ -1296,7 +1296,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>1230/115</t>
+          <t>1230/87</t>
         </is>
       </c>
       <c r="C67" t="n">
@@ -1309,7 +1309,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>1230/85</t>
+          <t>1230/88</t>
         </is>
       </c>
       <c r="C68" t="n">
@@ -1322,7 +1322,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>1230/86</t>
+          <t>1303/1</t>
         </is>
       </c>
       <c r="C69" t="n">
@@ -1335,7 +1335,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>1230/87</t>
+          <t>1303/2</t>
         </is>
       </c>
       <c r="C70" t="n">
@@ -1348,7 +1348,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>1230/88</t>
+          <t>1309</t>
         </is>
       </c>
       <c r="C71" t="n">
@@ -1361,7 +1361,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>1303/1</t>
+          <t>1330</t>
         </is>
       </c>
       <c r="C72" t="n">
@@ -1374,7 +1374,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>1303/2</t>
+          <t>1334</t>
         </is>
       </c>
       <c r="C73" t="n">
@@ -1387,7 +1387,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>1309</t>
+          <t>1346</t>
         </is>
       </c>
       <c r="C74" t="n">
@@ -1400,7 +1400,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>1330</t>
+          <t>1369/1</t>
         </is>
       </c>
       <c r="C75" t="n">
@@ -1413,7 +1413,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>1334</t>
+          <t>194/4</t>
         </is>
       </c>
       <c r="C76" t="n">
@@ -1426,7 +1426,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>1346</t>
+          <t>254/2</t>
         </is>
       </c>
       <c r="C77" t="n">
@@ -1439,7 +1439,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>1369/1</t>
+          <t>337/5</t>
         </is>
       </c>
       <c r="C78" t="n">
@@ -1452,7 +1452,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>194/4</t>
+          <t>393/1</t>
         </is>
       </c>
       <c r="C79" t="n">
@@ -1465,7 +1465,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>254/2</t>
+          <t>393/2</t>
         </is>
       </c>
       <c r="C80" t="n">
@@ -1478,7 +1478,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>337/5</t>
+          <t>393/3</t>
         </is>
       </c>
       <c r="C81" t="n">
@@ -1491,7 +1491,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>393/1</t>
+          <t>465</t>
         </is>
       </c>
       <c r="C82" t="n">
@@ -1504,7 +1504,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>393/2</t>
+          <t>614</t>
         </is>
       </c>
       <c r="C83" t="n">
@@ -1517,7 +1517,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>393/3</t>
+          <t>384/1</t>
         </is>
       </c>
       <c r="C84" t="n">
@@ -1530,11 +1530,11 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>465</t>
+          <t>4523</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>193</v>
+        <v>404</v>
       </c>
     </row>
     <row r="86">
@@ -1543,11 +1543,11 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>614</t>
+          <t>1911/5</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>193</v>
+        <v>404</v>
       </c>
     </row>
     <row r="87">
@@ -1556,11 +1556,11 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>384/1</t>
+          <t>1912/5</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>193</v>
+        <v>404</v>
       </c>
     </row>
     <row r="88">
@@ -1569,49 +1569,10 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>4523</t>
+          <t>1912/5</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" s="1" t="n">
-        <v>87</v>
-      </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>1911/5</t>
-        </is>
-      </c>
-      <c r="C89" t="n">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" s="1" t="n">
-        <v>88</v>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>1912/5</t>
-        </is>
-      </c>
-      <c r="C90" t="n">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" s="1" t="n">
-        <v>89</v>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>1912/5</t>
-        </is>
-      </c>
-      <c r="C91" t="n">
         <v>404</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Latest data: Sun Mar 10 20:09:55 UTC 2024
</commit_message>
<xml_diff>
--- a/docs/particelle_non_trovate.xlsx
+++ b/docs/particelle_non_trovate.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Latest data: Tue Mar 26 12:15:08 UTC 2024
</commit_message>
<xml_diff>
--- a/docs/particelle_non_trovate.xlsx
+++ b/docs/particelle_non_trovate.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C76"/>
+  <dimension ref="A1:C73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,11 +451,11 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>277</t>
+          <t>2181/2</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3">
@@ -464,11 +464,11 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1018/2</t>
+          <t>9769/2</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>2</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4">
@@ -477,11 +477,11 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1040</t>
+          <t>9783/231</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>349</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5">
@@ -490,11 +490,11 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2181/2</t>
+          <t>13823</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>57</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6">
@@ -503,11 +503,11 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>9769/2</t>
+          <t>14724/2</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>44</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7">
@@ -516,11 +516,11 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>9783/231</t>
+          <t>8974/1</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>44</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8">
@@ -529,7 +529,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>13823</t>
+          <t>15380</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -542,11 +542,11 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>14724/2</t>
+          <t>466</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>154</v>
+        <v>213</v>
       </c>
     </row>
     <row r="10">
@@ -555,11 +555,11 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>8974/1</t>
+          <t>.315</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>154</v>
+        <v>282</v>
       </c>
     </row>
     <row r="11">
@@ -568,11 +568,11 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>15380</t>
+          <t>1900/4</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>154</v>
+        <v>317</v>
       </c>
     </row>
     <row r="12">
@@ -581,11 +581,11 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>466</t>
+          <t>754</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>213</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13">
@@ -594,11 +594,11 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>.315</t>
+          <t>755</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>282</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14">
@@ -607,11 +607,11 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>1900/4</t>
+          <t>825/63</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>317</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15">
@@ -620,11 +620,11 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>754</t>
+          <t>1272/3</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>97</v>
+        <v>390</v>
       </c>
     </row>
     <row r="16">
@@ -633,11 +633,11 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>755</t>
+          <t>765</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>97</v>
+        <v>404</v>
       </c>
     </row>
     <row r="17">
@@ -646,11 +646,11 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>825/63</t>
+          <t>94/6</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>97</v>
+        <v>251</v>
       </c>
     </row>
     <row r="18">
@@ -659,11 +659,11 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>1272/3</t>
+          <t>2681/1</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>390</v>
+        <v>442</v>
       </c>
     </row>
     <row r="19">
@@ -672,11 +672,11 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>765</t>
+          <t>789</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>404</v>
+        <v>443</v>
       </c>
     </row>
     <row r="20">
@@ -685,11 +685,11 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>94/6</t>
+          <t>384/1</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>251</v>
+        <v>193</v>
       </c>
     </row>
     <row r="21">
@@ -698,11 +698,11 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2681/1</t>
+          <t>1117/2</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>442</v>
+        <v>193</v>
       </c>
     </row>
     <row r="22">
@@ -711,11 +711,11 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>789</t>
+          <t>1230/100</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>443</v>
+        <v>193</v>
       </c>
     </row>
     <row r="23">
@@ -724,7 +724,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>384/1</t>
+          <t>1230/115</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -737,7 +737,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>1117/2</t>
+          <t>1230/85</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -750,7 +750,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>1230/100</t>
+          <t>1230/86</t>
         </is>
       </c>
       <c r="C25" t="n">
@@ -763,7 +763,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>1230/115</t>
+          <t>1230/87</t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -776,7 +776,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>1230/85</t>
+          <t>1230/88</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -789,7 +789,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>1230/86</t>
+          <t>1303/1</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -802,7 +802,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>1230/87</t>
+          <t>1303/2</t>
         </is>
       </c>
       <c r="C29" t="n">
@@ -815,7 +815,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>1230/88</t>
+          <t>1309</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -828,7 +828,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>1303/1</t>
+          <t>1330</t>
         </is>
       </c>
       <c r="C31" t="n">
@@ -841,7 +841,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>1303/2</t>
+          <t>1334</t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -854,7 +854,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>1309</t>
+          <t>1346</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -867,7 +867,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>1330</t>
+          <t>1369/1</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -880,7 +880,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>1334</t>
+          <t>194/4</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -893,7 +893,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>1346</t>
+          <t>254/2</t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -906,7 +906,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>1369/1</t>
+          <t>337/5</t>
         </is>
       </c>
       <c r="C37" t="n">
@@ -919,7 +919,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>194/4</t>
+          <t>393/1</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -932,7 +932,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>254/2</t>
+          <t>393/2</t>
         </is>
       </c>
       <c r="C39" t="n">
@@ -945,7 +945,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>337/5</t>
+          <t>393/3</t>
         </is>
       </c>
       <c r="C40" t="n">
@@ -958,7 +958,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>393/1</t>
+          <t>465</t>
         </is>
       </c>
       <c r="C41" t="n">
@@ -971,7 +971,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>393/2</t>
+          <t>614</t>
         </is>
       </c>
       <c r="C42" t="n">
@@ -984,11 +984,11 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>393/3</t>
+          <t>1038/2</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>193</v>
+        <v>215</v>
       </c>
     </row>
     <row r="44">
@@ -997,11 +997,11 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>465</t>
+          <t>420/101</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>193</v>
+        <v>215</v>
       </c>
     </row>
     <row r="45">
@@ -1010,11 +1010,11 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>614</t>
+          <t>420/102</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>193</v>
+        <v>215</v>
       </c>
     </row>
     <row r="46">
@@ -1023,7 +1023,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>1038/2</t>
+          <t>420/106</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -1036,7 +1036,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>420/101</t>
+          <t>420/107</t>
         </is>
       </c>
       <c r="C47" t="n">
@@ -1049,7 +1049,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>420/102</t>
+          <t>420/109</t>
         </is>
       </c>
       <c r="C48" t="n">
@@ -1062,7 +1062,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>420/106</t>
+          <t>420/110</t>
         </is>
       </c>
       <c r="C49" t="n">
@@ -1075,7 +1075,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>420/107</t>
+          <t>420/80</t>
         </is>
       </c>
       <c r="C50" t="n">
@@ -1088,7 +1088,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>420/109</t>
+          <t>420/92</t>
         </is>
       </c>
       <c r="C51" t="n">
@@ -1101,7 +1101,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>420/110</t>
+          <t>420/93</t>
         </is>
       </c>
       <c r="C52" t="n">
@@ -1114,7 +1114,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>420/80</t>
+          <t>420/94</t>
         </is>
       </c>
       <c r="C53" t="n">
@@ -1127,7 +1127,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>420/92</t>
+          <t>420/95</t>
         </is>
       </c>
       <c r="C54" t="n">
@@ -1140,7 +1140,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>420/93</t>
+          <t>420/96</t>
         </is>
       </c>
       <c r="C55" t="n">
@@ -1153,7 +1153,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>420/94</t>
+          <t>420/97</t>
         </is>
       </c>
       <c r="C56" t="n">
@@ -1166,7 +1166,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>420/95</t>
+          <t>454</t>
         </is>
       </c>
       <c r="C57" t="n">
@@ -1179,7 +1179,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>420/96</t>
+          <t>53</t>
         </is>
       </c>
       <c r="C58" t="n">
@@ -1192,7 +1192,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>420/97</t>
+          <t>705/11</t>
         </is>
       </c>
       <c r="C59" t="n">
@@ -1205,7 +1205,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>454</t>
+          <t>756</t>
         </is>
       </c>
       <c r="C60" t="n">
@@ -1218,7 +1218,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>798/3</t>
         </is>
       </c>
       <c r="C61" t="n">
@@ -1231,11 +1231,11 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>705/11</t>
+          <t>4523</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>215</v>
+        <v>404</v>
       </c>
     </row>
     <row r="63">
@@ -1244,11 +1244,11 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>756</t>
+          <t>1911/5</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>215</v>
+        <v>404</v>
       </c>
     </row>
     <row r="64">
@@ -1257,11 +1257,11 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>798/3</t>
+          <t>1912/5</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>215</v>
+        <v>404</v>
       </c>
     </row>
     <row r="65">
@@ -1270,7 +1270,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>4523</t>
+          <t>1912/5</t>
         </is>
       </c>
       <c r="C65" t="n">
@@ -1283,11 +1283,11 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>1911/5</t>
+          <t>3597/16</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>404</v>
+        <v>9</v>
       </c>
     </row>
     <row r="67">
@@ -1296,11 +1296,11 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>1912/5</t>
+          <t>3597/18</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>404</v>
+        <v>9</v>
       </c>
     </row>
     <row r="68">
@@ -1309,11 +1309,11 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>1912/5</t>
+          <t>3597/22</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>404</v>
+        <v>9</v>
       </c>
     </row>
     <row r="69">
@@ -1322,11 +1322,11 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>3597/16</t>
+          <t>2331/38</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>9</v>
+        <v>258</v>
       </c>
     </row>
     <row r="70">
@@ -1335,11 +1335,11 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>3597/18</t>
+          <t>2068/43</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>9</v>
+        <v>310</v>
       </c>
     </row>
     <row r="71">
@@ -1348,11 +1348,11 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>3597/22</t>
+          <t>2822/12</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>9</v>
+        <v>310</v>
       </c>
     </row>
     <row r="72">
@@ -1361,11 +1361,11 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>2331/38</t>
+          <t>2822/16</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>258</v>
+        <v>310</v>
       </c>
     </row>
     <row r="73">
@@ -1374,49 +1374,10 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>2068/43</t>
+          <t>2020/14</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" s="1" t="n">
-        <v>72</v>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>2822/12</t>
-        </is>
-      </c>
-      <c r="C74" t="n">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" s="1" t="n">
-        <v>73</v>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>2822/16</t>
-        </is>
-      </c>
-      <c r="C75" t="n">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" s="1" t="n">
-        <v>74</v>
-      </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>2020/14</t>
-        </is>
-      </c>
-      <c r="C76" t="n">
         <v>310</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Latest data: Tue Mar 26 16:12:15 UTC 2024
</commit_message>
<xml_diff>
--- a/docs/particelle_non_trovate.xlsx
+++ b/docs/particelle_non_trovate.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C73"/>
+  <dimension ref="A1:C71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,11 +451,11 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2181/2</t>
+          <t>9783/231</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>57</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3">
@@ -464,11 +464,11 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>9769/2</t>
+          <t>13823</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>44</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4">
@@ -477,11 +477,11 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>9783/231</t>
+          <t>14724/2</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>44</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5">
@@ -490,7 +490,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>13823</t>
+          <t>8974/1</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -503,7 +503,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>14724/2</t>
+          <t>15380</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -516,11 +516,11 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>8974/1</t>
+          <t>466</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>154</v>
+        <v>213</v>
       </c>
     </row>
     <row r="8">
@@ -529,11 +529,11 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>15380</t>
+          <t>.315</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>154</v>
+        <v>282</v>
       </c>
     </row>
     <row r="9">
@@ -542,11 +542,11 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>466</t>
+          <t>1900/4</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>213</v>
+        <v>317</v>
       </c>
     </row>
     <row r="10">
@@ -555,11 +555,11 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>.315</t>
+          <t>754</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>282</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11">
@@ -568,11 +568,11 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>1900/4</t>
+          <t>755</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>317</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12">
@@ -581,7 +581,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>754</t>
+          <t>825/63</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -594,11 +594,11 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>755</t>
+          <t>1272/3</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>97</v>
+        <v>390</v>
       </c>
     </row>
     <row r="14">
@@ -607,11 +607,11 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>825/63</t>
+          <t>765</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>97</v>
+        <v>404</v>
       </c>
     </row>
     <row r="15">
@@ -620,11 +620,11 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>1272/3</t>
+          <t>94/6</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>390</v>
+        <v>251</v>
       </c>
     </row>
     <row r="16">
@@ -633,11 +633,11 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>765</t>
+          <t>2681/1</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>404</v>
+        <v>442</v>
       </c>
     </row>
     <row r="17">
@@ -646,11 +646,11 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>94/6</t>
+          <t>789</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>251</v>
+        <v>443</v>
       </c>
     </row>
     <row r="18">
@@ -659,11 +659,11 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2681/1</t>
+          <t>384/1</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>442</v>
+        <v>193</v>
       </c>
     </row>
     <row r="19">
@@ -672,11 +672,11 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>789</t>
+          <t>1117/2</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>443</v>
+        <v>193</v>
       </c>
     </row>
     <row r="20">
@@ -685,7 +685,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>384/1</t>
+          <t>1230/100</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -698,7 +698,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>1117/2</t>
+          <t>1230/115</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -711,7 +711,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>1230/100</t>
+          <t>1230/85</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -724,7 +724,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>1230/115</t>
+          <t>1230/86</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -737,7 +737,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>1230/85</t>
+          <t>1230/87</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -750,7 +750,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>1230/86</t>
+          <t>1230/88</t>
         </is>
       </c>
       <c r="C25" t="n">
@@ -763,7 +763,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>1230/87</t>
+          <t>1303/1</t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -776,7 +776,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>1230/88</t>
+          <t>1303/2</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -789,7 +789,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>1303/1</t>
+          <t>1309</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -802,7 +802,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>1303/2</t>
+          <t>1330</t>
         </is>
       </c>
       <c r="C29" t="n">
@@ -815,7 +815,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>1309</t>
+          <t>1334</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -828,7 +828,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>1330</t>
+          <t>1346</t>
         </is>
       </c>
       <c r="C31" t="n">
@@ -841,7 +841,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>1334</t>
+          <t>1369/1</t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -854,7 +854,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>1346</t>
+          <t>194/4</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -867,7 +867,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>1369/1</t>
+          <t>254/2</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -880,7 +880,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>194/4</t>
+          <t>337/5</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -893,7 +893,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>254/2</t>
+          <t>393/1</t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -906,7 +906,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>337/5</t>
+          <t>393/2</t>
         </is>
       </c>
       <c r="C37" t="n">
@@ -919,7 +919,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>393/1</t>
+          <t>393/3</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -932,7 +932,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>393/2</t>
+          <t>465</t>
         </is>
       </c>
       <c r="C39" t="n">
@@ -945,7 +945,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>393/3</t>
+          <t>614</t>
         </is>
       </c>
       <c r="C40" t="n">
@@ -958,11 +958,11 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>465</t>
+          <t>1038/2</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>193</v>
+        <v>215</v>
       </c>
     </row>
     <row r="42">
@@ -971,11 +971,11 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>614</t>
+          <t>420/101</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>193</v>
+        <v>215</v>
       </c>
     </row>
     <row r="43">
@@ -984,7 +984,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>1038/2</t>
+          <t>420/102</t>
         </is>
       </c>
       <c r="C43" t="n">
@@ -997,7 +997,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>420/101</t>
+          <t>420/106</t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -1010,7 +1010,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>420/102</t>
+          <t>420/107</t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -1023,7 +1023,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>420/106</t>
+          <t>420/109</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -1036,7 +1036,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>420/107</t>
+          <t>420/110</t>
         </is>
       </c>
       <c r="C47" t="n">
@@ -1049,7 +1049,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>420/109</t>
+          <t>420/80</t>
         </is>
       </c>
       <c r="C48" t="n">
@@ -1062,7 +1062,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>420/110</t>
+          <t>420/92</t>
         </is>
       </c>
       <c r="C49" t="n">
@@ -1075,7 +1075,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>420/80</t>
+          <t>420/93</t>
         </is>
       </c>
       <c r="C50" t="n">
@@ -1088,7 +1088,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>420/92</t>
+          <t>420/94</t>
         </is>
       </c>
       <c r="C51" t="n">
@@ -1101,7 +1101,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>420/93</t>
+          <t>420/95</t>
         </is>
       </c>
       <c r="C52" t="n">
@@ -1114,7 +1114,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>420/94</t>
+          <t>420/96</t>
         </is>
       </c>
       <c r="C53" t="n">
@@ -1127,7 +1127,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>420/95</t>
+          <t>420/97</t>
         </is>
       </c>
       <c r="C54" t="n">
@@ -1140,7 +1140,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>420/96</t>
+          <t>454</t>
         </is>
       </c>
       <c r="C55" t="n">
@@ -1153,7 +1153,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>420/97</t>
+          <t>53</t>
         </is>
       </c>
       <c r="C56" t="n">
@@ -1166,7 +1166,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>454</t>
+          <t>705/11</t>
         </is>
       </c>
       <c r="C57" t="n">
@@ -1179,7 +1179,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>756</t>
         </is>
       </c>
       <c r="C58" t="n">
@@ -1192,7 +1192,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>705/11</t>
+          <t>798/3</t>
         </is>
       </c>
       <c r="C59" t="n">
@@ -1205,11 +1205,11 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>756</t>
+          <t>4523</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>215</v>
+        <v>404</v>
       </c>
     </row>
     <row r="61">
@@ -1218,11 +1218,11 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>798/3</t>
+          <t>1911/5</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>215</v>
+        <v>404</v>
       </c>
     </row>
     <row r="62">
@@ -1231,7 +1231,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>4523</t>
+          <t>1912/5</t>
         </is>
       </c>
       <c r="C62" t="n">
@@ -1244,7 +1244,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>1911/5</t>
+          <t>1912/5</t>
         </is>
       </c>
       <c r="C63" t="n">
@@ -1257,11 +1257,11 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>1912/5</t>
+          <t>3597/16</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>404</v>
+        <v>9</v>
       </c>
     </row>
     <row r="65">
@@ -1270,11 +1270,11 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>1912/5</t>
+          <t>3597/18</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>404</v>
+        <v>9</v>
       </c>
     </row>
     <row r="66">
@@ -1283,7 +1283,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>3597/16</t>
+          <t>3597/22</t>
         </is>
       </c>
       <c r="C66" t="n">
@@ -1296,11 +1296,11 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>3597/18</t>
+          <t>2331/38</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>9</v>
+        <v>258</v>
       </c>
     </row>
     <row r="68">
@@ -1309,11 +1309,11 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>3597/22</t>
+          <t>2068/43</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>9</v>
+        <v>310</v>
       </c>
     </row>
     <row r="69">
@@ -1322,11 +1322,11 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>2331/38</t>
+          <t>2822/12</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>258</v>
+        <v>310</v>
       </c>
     </row>
     <row r="70">
@@ -1335,7 +1335,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>2068/43</t>
+          <t>2822/16</t>
         </is>
       </c>
       <c r="C70" t="n">
@@ -1348,36 +1348,10 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>2822/12</t>
+          <t>2020/14</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" s="1" t="n">
-        <v>70</v>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>2822/16</t>
-        </is>
-      </c>
-      <c r="C72" t="n">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" s="1" t="n">
-        <v>71</v>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>2020/14</t>
-        </is>
-      </c>
-      <c r="C73" t="n">
         <v>310</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Latest data: Fri Mar 29 12:15:00 UTC 2024
</commit_message>
<xml_diff>
--- a/docs/particelle_non_trovate.xlsx
+++ b/docs/particelle_non_trovate.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C71"/>
+  <dimension ref="A1:C57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -542,11 +542,11 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>1900/4</t>
+          <t>1117/2</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>317</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10">
@@ -555,11 +555,11 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>754</t>
+          <t>1230/100</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>97</v>
+        <v>193</v>
       </c>
     </row>
     <row r="11">
@@ -568,11 +568,11 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>755</t>
+          <t>1230/115</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>97</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12">
@@ -581,11 +581,11 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>825/63</t>
+          <t>1230/85</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>97</v>
+        <v>193</v>
       </c>
     </row>
     <row r="13">
@@ -594,11 +594,11 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>1272/3</t>
+          <t>1230/86</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>390</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14">
@@ -607,11 +607,11 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>765</t>
+          <t>1230/87</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>404</v>
+        <v>193</v>
       </c>
     </row>
     <row r="15">
@@ -620,11 +620,11 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>94/6</t>
+          <t>1230/88</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>251</v>
+        <v>193</v>
       </c>
     </row>
     <row r="16">
@@ -633,11 +633,11 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2681/1</t>
+          <t>1303/1</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>442</v>
+        <v>193</v>
       </c>
     </row>
     <row r="17">
@@ -646,11 +646,11 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>789</t>
+          <t>1303/2</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>443</v>
+        <v>193</v>
       </c>
     </row>
     <row r="18">
@@ -659,7 +659,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>384/1</t>
+          <t>1309</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -672,7 +672,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>1117/2</t>
+          <t>1330</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -685,7 +685,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>1230/100</t>
+          <t>1334</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -698,7 +698,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>1230/115</t>
+          <t>1346</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -711,7 +711,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>1230/85</t>
+          <t>1369/1</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -724,7 +724,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>1230/86</t>
+          <t>194/4</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -737,7 +737,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>1230/87</t>
+          <t>254/2</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -750,7 +750,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>1230/88</t>
+          <t>337/5</t>
         </is>
       </c>
       <c r="C25" t="n">
@@ -763,7 +763,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>1303/1</t>
+          <t>393/1</t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -776,7 +776,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>1303/2</t>
+          <t>393/2</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -789,7 +789,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>1309</t>
+          <t>393/3</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -802,7 +802,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>1330</t>
+          <t>465</t>
         </is>
       </c>
       <c r="C29" t="n">
@@ -815,7 +815,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>1334</t>
+          <t>614</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -828,11 +828,11 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>1346</t>
+          <t>420/101</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>193</v>
+        <v>215</v>
       </c>
     </row>
     <row r="32">
@@ -841,11 +841,11 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>1369/1</t>
+          <t>420/102</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>193</v>
+        <v>215</v>
       </c>
     </row>
     <row r="33">
@@ -854,11 +854,11 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>194/4</t>
+          <t>420/106</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>193</v>
+        <v>215</v>
       </c>
     </row>
     <row r="34">
@@ -867,11 +867,11 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>254/2</t>
+          <t>420/107</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>193</v>
+        <v>215</v>
       </c>
     </row>
     <row r="35">
@@ -880,11 +880,11 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>337/5</t>
+          <t>420/109</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>193</v>
+        <v>215</v>
       </c>
     </row>
     <row r="36">
@@ -893,11 +893,11 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>393/1</t>
+          <t>420/110</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>193</v>
+        <v>215</v>
       </c>
     </row>
     <row r="37">
@@ -906,11 +906,11 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>393/2</t>
+          <t>420/80</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>193</v>
+        <v>215</v>
       </c>
     </row>
     <row r="38">
@@ -919,11 +919,11 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>393/3</t>
+          <t>420/92</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>193</v>
+        <v>215</v>
       </c>
     </row>
     <row r="39">
@@ -932,11 +932,11 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>465</t>
+          <t>420/93</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>193</v>
+        <v>215</v>
       </c>
     </row>
     <row r="40">
@@ -945,11 +945,11 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>614</t>
+          <t>420/94</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>193</v>
+        <v>215</v>
       </c>
     </row>
     <row r="41">
@@ -958,7 +958,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>1038/2</t>
+          <t>420/95</t>
         </is>
       </c>
       <c r="C41" t="n">
@@ -971,7 +971,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>420/101</t>
+          <t>420/96</t>
         </is>
       </c>
       <c r="C42" t="n">
@@ -984,7 +984,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>420/102</t>
+          <t>420/97</t>
         </is>
       </c>
       <c r="C43" t="n">
@@ -997,7 +997,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>420/106</t>
+          <t>454</t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -1010,7 +1010,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>420/107</t>
+          <t>53</t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -1023,7 +1023,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>420/109</t>
+          <t>705/11</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -1036,7 +1036,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>420/110</t>
+          <t>756</t>
         </is>
       </c>
       <c r="C47" t="n">
@@ -1049,7 +1049,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>420/80</t>
+          <t>798/3</t>
         </is>
       </c>
       <c r="C48" t="n">
@@ -1062,11 +1062,11 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>420/92</t>
+          <t>4523</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>215</v>
+        <v>404</v>
       </c>
     </row>
     <row r="50">
@@ -1075,11 +1075,11 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>420/93</t>
+          <t>3597/16</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>215</v>
+        <v>9</v>
       </c>
     </row>
     <row r="51">
@@ -1088,11 +1088,11 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>420/94</t>
+          <t>3597/18</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>215</v>
+        <v>9</v>
       </c>
     </row>
     <row r="52">
@@ -1101,11 +1101,11 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>420/95</t>
+          <t>3597/22</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>215</v>
+        <v>9</v>
       </c>
     </row>
     <row r="53">
@@ -1114,11 +1114,11 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>420/96</t>
+          <t>2331/38</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>215</v>
+        <v>258</v>
       </c>
     </row>
     <row r="54">
@@ -1127,11 +1127,11 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>420/97</t>
+          <t>2068/43</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>215</v>
+        <v>310</v>
       </c>
     </row>
     <row r="55">
@@ -1140,11 +1140,11 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>454</t>
+          <t>2822/12</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>215</v>
+        <v>310</v>
       </c>
     </row>
     <row r="56">
@@ -1153,11 +1153,11 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>2822/16</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>215</v>
+        <v>310</v>
       </c>
     </row>
     <row r="57">
@@ -1166,192 +1166,10 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>705/11</t>
+          <t>2020/14</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" s="1" t="n">
-        <v>56</v>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>756</t>
-        </is>
-      </c>
-      <c r="C58" t="n">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" s="1" t="n">
-        <v>57</v>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>798/3</t>
-        </is>
-      </c>
-      <c r="C59" t="n">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" s="1" t="n">
-        <v>58</v>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>4523</t>
-        </is>
-      </c>
-      <c r="C60" t="n">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" s="1" t="n">
-        <v>59</v>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>1911/5</t>
-        </is>
-      </c>
-      <c r="C61" t="n">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" s="1" t="n">
-        <v>60</v>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>1912/5</t>
-        </is>
-      </c>
-      <c r="C62" t="n">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" s="1" t="n">
-        <v>61</v>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>1912/5</t>
-        </is>
-      </c>
-      <c r="C63" t="n">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" s="1" t="n">
-        <v>62</v>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>3597/16</t>
-        </is>
-      </c>
-      <c r="C64" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" s="1" t="n">
-        <v>63</v>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>3597/18</t>
-        </is>
-      </c>
-      <c r="C65" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" s="1" t="n">
-        <v>64</v>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>3597/22</t>
-        </is>
-      </c>
-      <c r="C66" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" s="1" t="n">
-        <v>65</v>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>2331/38</t>
-        </is>
-      </c>
-      <c r="C67" t="n">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" s="1" t="n">
-        <v>66</v>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>2068/43</t>
-        </is>
-      </c>
-      <c r="C68" t="n">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" s="1" t="n">
-        <v>67</v>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>2822/12</t>
-        </is>
-      </c>
-      <c r="C69" t="n">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" s="1" t="n">
-        <v>68</v>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>2822/16</t>
-        </is>
-      </c>
-      <c r="C70" t="n">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" s="1" t="n">
-        <v>69</v>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>2020/14</t>
-        </is>
-      </c>
-      <c r="C71" t="n">
         <v>310</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Latest data: Fri Jun  7 04:15:13 UTC 2024
</commit_message>
<xml_diff>
--- a/docs/particelle_non_trovate.xlsx
+++ b/docs/particelle_non_trovate.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C57"/>
+  <dimension ref="A1:C240"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -542,7 +542,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>1117/2</t>
+          <t>1438</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -555,7 +555,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>1230/100</t>
+          <t>1439</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -568,7 +568,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>1230/115</t>
+          <t>1440</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -581,7 +581,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>1230/85</t>
+          <t>1441</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -594,7 +594,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>1230/86</t>
+          <t>1442</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -607,7 +607,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>1230/87</t>
+          <t>1466</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -620,7 +620,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>1230/88</t>
+          <t>1468/1</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -633,7 +633,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>1303/1</t>
+          <t>1470/1</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -646,7 +646,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>1303/2</t>
+          <t>1470/2</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -659,7 +659,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>1309</t>
+          <t>1471</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -672,7 +672,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>1330</t>
+          <t>1472</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -685,7 +685,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>1334</t>
+          <t>1473</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -698,7 +698,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>1346</t>
+          <t>1474/1</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -711,7 +711,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>1369/1</t>
+          <t>1474/3</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -724,7 +724,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>194/4</t>
+          <t>94</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -737,7 +737,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>254/2</t>
+          <t>108/1</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -750,7 +750,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>337/5</t>
+          <t>108/2</t>
         </is>
       </c>
       <c r="C25" t="n">
@@ -763,7 +763,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>393/1</t>
+          <t>109</t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -776,7 +776,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>393/2</t>
+          <t>132/1</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -789,7 +789,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>393/3</t>
+          <t>132/2</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -802,7 +802,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>465</t>
+          <t>132/3</t>
         </is>
       </c>
       <c r="C29" t="n">
@@ -815,7 +815,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>614</t>
+          <t>138</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -828,11 +828,11 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>420/101</t>
+          <t>149/1</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="32">
@@ -841,11 +841,11 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>420/102</t>
+          <t>149/2</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="33">
@@ -854,11 +854,11 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>420/106</t>
+          <t>149/3</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="34">
@@ -867,11 +867,11 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>420/107</t>
+          <t>152/1</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="35">
@@ -880,11 +880,11 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>420/109</t>
+          <t>152/3</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="36">
@@ -893,11 +893,11 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>420/110</t>
+          <t>152/3</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="37">
@@ -906,11 +906,11 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>420/80</t>
+          <t>152/4</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="38">
@@ -919,11 +919,11 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>420/92</t>
+          <t>152/5</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="39">
@@ -932,11 +932,11 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>420/93</t>
+          <t>163</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="40">
@@ -945,11 +945,11 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>420/94</t>
+          <t>169/2</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="41">
@@ -958,11 +958,11 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>420/95</t>
+          <t>173</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="42">
@@ -971,11 +971,11 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>420/96</t>
+          <t>182/1</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="43">
@@ -984,11 +984,11 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>420/97</t>
+          <t>183</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="44">
@@ -997,11 +997,11 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>454</t>
+          <t>204</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="45">
@@ -1010,11 +1010,11 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>205/1</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="46">
@@ -1023,11 +1023,11 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>705/11</t>
+          <t>205/2</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="47">
@@ -1036,11 +1036,11 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>756</t>
+          <t>205/3</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="48">
@@ -1049,11 +1049,11 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>798/3</t>
+          <t>251</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
     </row>
     <row r="49">
@@ -1062,11 +1062,11 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>4523</t>
+          <t>252</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>404</v>
+        <v>193</v>
       </c>
     </row>
     <row r="50">
@@ -1075,11 +1075,11 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>3597/16</t>
+          <t>254/1</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>9</v>
+        <v>193</v>
       </c>
     </row>
     <row r="51">
@@ -1088,11 +1088,11 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>3597/18</t>
+          <t>291/1</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>9</v>
+        <v>193</v>
       </c>
     </row>
     <row r="52">
@@ -1101,11 +1101,11 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>3597/22</t>
+          <t>291/6</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>9</v>
+        <v>193</v>
       </c>
     </row>
     <row r="53">
@@ -1114,11 +1114,11 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>2331/38</t>
+          <t>292/1</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>258</v>
+        <v>193</v>
       </c>
     </row>
     <row r="54">
@@ -1127,11 +1127,11 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>2068/43</t>
+          <t>292/2</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>310</v>
+        <v>193</v>
       </c>
     </row>
     <row r="55">
@@ -1140,11 +1140,11 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>2822/12</t>
+          <t>292/3</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>310</v>
+        <v>193</v>
       </c>
     </row>
     <row r="56">
@@ -1153,11 +1153,11 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>2822/16</t>
+          <t>315/1</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>310</v>
+        <v>193</v>
       </c>
     </row>
     <row r="57">
@@ -1166,10 +1166,2389 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
+          <t>323</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>327</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>335</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>336</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>337/1</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>337/6</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>337/7</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>337/8</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>337/9</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>348/1</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>348/3</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>348/5</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>348/6</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>348/7</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>388/1</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>393</t>
+        </is>
+      </c>
+      <c r="C72" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>446</t>
+        </is>
+      </c>
+      <c r="C73" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>451</t>
+        </is>
+      </c>
+      <c r="C74" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>465/1</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>614/1</t>
+        </is>
+      </c>
+      <c r="C76" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>616/2</t>
+        </is>
+      </c>
+      <c r="C77" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>1283/1</t>
+        </is>
+      </c>
+      <c r="C78" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>1283/64</t>
+        </is>
+      </c>
+      <c r="C79" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>1283/65</t>
+        </is>
+      </c>
+      <c r="C80" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>1283/70</t>
+        </is>
+      </c>
+      <c r="C81" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>1292</t>
+        </is>
+      </c>
+      <c r="C82" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>1299</t>
+        </is>
+      </c>
+      <c r="C83" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>1303</t>
+        </is>
+      </c>
+      <c r="C84" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>1323/1</t>
+        </is>
+      </c>
+      <c r="C85" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>1328</t>
+        </is>
+      </c>
+      <c r="C86" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>1353</t>
+        </is>
+      </c>
+      <c r="C87" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>1369/6</t>
+        </is>
+      </c>
+      <c r="C88" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>1369/7</t>
+        </is>
+      </c>
+      <c r="C89" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>1369/8</t>
+        </is>
+      </c>
+      <c r="C90" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>1381</t>
+        </is>
+      </c>
+      <c r="C91" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>1427/1</t>
+        </is>
+      </c>
+      <c r="C92" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>1427/2</t>
+        </is>
+      </c>
+      <c r="C93" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>1427/3</t>
+        </is>
+      </c>
+      <c r="C94" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="n">
+        <v>93</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>1427/4</t>
+        </is>
+      </c>
+      <c r="C95" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="n">
+        <v>94</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>1427/5</t>
+        </is>
+      </c>
+      <c r="C96" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>1427/6</t>
+        </is>
+      </c>
+      <c r="C97" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>1427/7</t>
+        </is>
+      </c>
+      <c r="C98" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>1427/8</t>
+        </is>
+      </c>
+      <c r="C99" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="n">
+        <v>98</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>1427/14</t>
+        </is>
+      </c>
+      <c r="C100" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>1427/21</t>
+        </is>
+      </c>
+      <c r="C101" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>1427/24</t>
+        </is>
+      </c>
+      <c r="C102" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>1427/25</t>
+        </is>
+      </c>
+      <c r="C103" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="n">
+        <v>102</v>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>1427/26</t>
+        </is>
+      </c>
+      <c r="C104" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="n">
+        <v>103</v>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>1427/27</t>
+        </is>
+      </c>
+      <c r="C105" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="n">
+        <v>104</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>1427/28</t>
+        </is>
+      </c>
+      <c r="C106" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="n">
+        <v>105</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>1427/29</t>
+        </is>
+      </c>
+      <c r="C107" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="n">
+        <v>106</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>1427/30</t>
+        </is>
+      </c>
+      <c r="C108" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="n">
+        <v>107</v>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>1427/43</t>
+        </is>
+      </c>
+      <c r="C109" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="n">
+        <v>108</v>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>1427/44</t>
+        </is>
+      </c>
+      <c r="C110" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="n">
+        <v>109</v>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>1427/45</t>
+        </is>
+      </c>
+      <c r="C111" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>1427/49</t>
+        </is>
+      </c>
+      <c r="C112" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="n">
+        <v>111</v>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>1427/50</t>
+        </is>
+      </c>
+      <c r="C113" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="n">
+        <v>112</v>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>1427/51</t>
+        </is>
+      </c>
+      <c r="C114" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="n">
+        <v>113</v>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>1427/52</t>
+        </is>
+      </c>
+      <c r="C115" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="n">
+        <v>114</v>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>1427/53</t>
+        </is>
+      </c>
+      <c r="C116" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="n">
+        <v>115</v>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>1427/54</t>
+        </is>
+      </c>
+      <c r="C117" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="n">
+        <v>116</v>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>1467</t>
+        </is>
+      </c>
+      <c r="C118" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="1" t="n">
+        <v>117</v>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>1474/2</t>
+        </is>
+      </c>
+      <c r="C119" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="1" t="n">
+        <v>118</v>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>1475</t>
+        </is>
+      </c>
+      <c r="C120" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="1" t="n">
+        <v>119</v>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>1476</t>
+        </is>
+      </c>
+      <c r="C121" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="1" t="n">
+        <v>120</v>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>1477</t>
+        </is>
+      </c>
+      <c r="C122" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="1" t="n">
+        <v>121</v>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>1564</t>
+        </is>
+      </c>
+      <c r="C123" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="1" t="n">
+        <v>122</v>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>.194/4</t>
+        </is>
+      </c>
+      <c r="C124" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="1" t="n">
+        <v>123</v>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>.521</t>
+        </is>
+      </c>
+      <c r="C125" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="1" t="n">
+        <v>124</v>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>.1232</t>
+        </is>
+      </c>
+      <c r="C126" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="1" t="n">
+        <v>125</v>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>.1236</t>
+        </is>
+      </c>
+      <c r="C127" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="1" t="n">
+        <v>126</v>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>.1237</t>
+        </is>
+      </c>
+      <c r="C128" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="1" t="n">
+        <v>127</v>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>.1253</t>
+        </is>
+      </c>
+      <c r="C129" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="1" t="n">
+        <v>128</v>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>.1297</t>
+        </is>
+      </c>
+      <c r="C130" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="1" t="n">
+        <v>129</v>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>.1358</t>
+        </is>
+      </c>
+      <c r="C131" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="1" t="n">
+        <v>130</v>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>.1439</t>
+        </is>
+      </c>
+      <c r="C132" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="1" t="n">
+        <v>131</v>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>.1492</t>
+        </is>
+      </c>
+      <c r="C133" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="1" t="n">
+        <v>132</v>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>.1518</t>
+        </is>
+      </c>
+      <c r="C134" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="1" t="n">
+        <v>133</v>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>.1540</t>
+        </is>
+      </c>
+      <c r="C135" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="1" t="n">
+        <v>134</v>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>.1649</t>
+        </is>
+      </c>
+      <c r="C136" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="1" t="n">
+        <v>135</v>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>.1676</t>
+        </is>
+      </c>
+      <c r="C137" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="1" t="n">
+        <v>136</v>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>.1677</t>
+        </is>
+      </c>
+      <c r="C138" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="1" t="n">
+        <v>137</v>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>.1678</t>
+        </is>
+      </c>
+      <c r="C139" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="1" t="n">
+        <v>138</v>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>.1679</t>
+        </is>
+      </c>
+      <c r="C140" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="1" t="n">
+        <v>139</v>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>.384/1</t>
+        </is>
+      </c>
+      <c r="C141" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>1379</t>
+        </is>
+      </c>
+      <c r="C142" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="1" t="n">
+        <v>141</v>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>1380</t>
+        </is>
+      </c>
+      <c r="C143" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="1" t="n">
+        <v>142</v>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>1285</t>
+        </is>
+      </c>
+      <c r="C144" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="1" t="n">
+        <v>143</v>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>110/2</t>
+        </is>
+      </c>
+      <c r="C145" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="1" t="n">
+        <v>144</v>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>112/3</t>
+        </is>
+      </c>
+      <c r="C146" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>128</t>
+        </is>
+      </c>
+      <c r="C147" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="1" t="n">
+        <v>146</v>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>1117/2</t>
+        </is>
+      </c>
+      <c r="C148" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="1" t="n">
+        <v>147</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>1180</t>
+        </is>
+      </c>
+      <c r="C149" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="1" t="n">
+        <v>148</v>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>1230/1</t>
+        </is>
+      </c>
+      <c r="C150" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="1" t="n">
+        <v>149</v>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>1230/100</t>
+        </is>
+      </c>
+      <c r="C151" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>1230/102</t>
+        </is>
+      </c>
+      <c r="C152" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="1" t="n">
+        <v>151</v>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>1230/104</t>
+        </is>
+      </c>
+      <c r="C153" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="1" t="n">
+        <v>152</v>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>1230/105</t>
+        </is>
+      </c>
+      <c r="C154" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="1" t="n">
+        <v>153</v>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>1230/115</t>
+        </is>
+      </c>
+      <c r="C155" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="1" t="n">
+        <v>154</v>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>1230/82</t>
+        </is>
+      </c>
+      <c r="C156" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="1" t="n">
+        <v>155</v>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>1230/85</t>
+        </is>
+      </c>
+      <c r="C157" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="1" t="n">
+        <v>156</v>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>1230/86</t>
+        </is>
+      </c>
+      <c r="C158" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="1" t="n">
+        <v>157</v>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>1230/87</t>
+        </is>
+      </c>
+      <c r="C159" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="1" t="n">
+        <v>158</v>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>1230/88</t>
+        </is>
+      </c>
+      <c r="C160" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="1" t="n">
+        <v>159</v>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>1255</t>
+        </is>
+      </c>
+      <c r="C161" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="1" t="n">
+        <v>160</v>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>1265/1</t>
+        </is>
+      </c>
+      <c r="C162" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="1" t="n">
+        <v>161</v>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>1274</t>
+        </is>
+      </c>
+      <c r="C163" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="1" t="n">
+        <v>162</v>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>1283/12</t>
+        </is>
+      </c>
+      <c r="C164" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="1" t="n">
+        <v>163</v>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>1284</t>
+        </is>
+      </c>
+      <c r="C165" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="1" t="n">
+        <v>164</v>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>1285</t>
+        </is>
+      </c>
+      <c r="C166" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="1" t="n">
+        <v>165</v>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>1303/1</t>
+        </is>
+      </c>
+      <c r="C167" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="1" t="n">
+        <v>166</v>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>1303/2</t>
+        </is>
+      </c>
+      <c r="C168" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="1" t="n">
+        <v>167</v>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>1309</t>
+        </is>
+      </c>
+      <c r="C169" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="1" t="n">
+        <v>168</v>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>1330</t>
+        </is>
+      </c>
+      <c r="C170" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" s="1" t="n">
+        <v>169</v>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>1334</t>
+        </is>
+      </c>
+      <c r="C171" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" s="1" t="n">
+        <v>170</v>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>1346</t>
+        </is>
+      </c>
+      <c r="C172" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" s="1" t="n">
+        <v>171</v>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>152/2</t>
+        </is>
+      </c>
+      <c r="C173" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" s="1" t="n">
+        <v>172</v>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>1369/1</t>
+        </is>
+      </c>
+      <c r="C174" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="1" t="n">
+        <v>173</v>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>194/4</t>
+        </is>
+      </c>
+      <c r="C175" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="1" t="n">
+        <v>174</v>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>169/1</t>
+        </is>
+      </c>
+      <c r="C176" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="1" t="n">
+        <v>175</v>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>170</t>
+        </is>
+      </c>
+      <c r="C177" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="1" t="n">
+        <v>176</v>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>253</t>
+        </is>
+      </c>
+      <c r="C178" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="1" t="n">
+        <v>177</v>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>254/2</t>
+        </is>
+      </c>
+      <c r="C179" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="1" t="n">
+        <v>178</v>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>291/2</t>
+        </is>
+      </c>
+      <c r="C180" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="1" t="n">
+        <v>179</v>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>291/3</t>
+        </is>
+      </c>
+      <c r="C181" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="1" t="n">
+        <v>180</v>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>337/5</t>
+        </is>
+      </c>
+      <c r="C182" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="1" t="n">
+        <v>181</v>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>348/2</t>
+        </is>
+      </c>
+      <c r="C183" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" s="1" t="n">
+        <v>182</v>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>348/4</t>
+        </is>
+      </c>
+      <c r="C184" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" s="1" t="n">
+        <v>183</v>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>393/1</t>
+        </is>
+      </c>
+      <c r="C185" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" s="1" t="n">
+        <v>184</v>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>393/2</t>
+        </is>
+      </c>
+      <c r="C186" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" s="1" t="n">
+        <v>185</v>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>393/3</t>
+        </is>
+      </c>
+      <c r="C187" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" s="1" t="n">
+        <v>186</v>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>432/1</t>
+        </is>
+      </c>
+      <c r="C188" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" s="1" t="n">
+        <v>187</v>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>432/1</t>
+        </is>
+      </c>
+      <c r="C189" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" s="1" t="n">
+        <v>188</v>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>465</t>
+        </is>
+      </c>
+      <c r="C190" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" s="1" t="n">
+        <v>189</v>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>471/1</t>
+        </is>
+      </c>
+      <c r="C191" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" s="1" t="n">
+        <v>190</v>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>471/2</t>
+        </is>
+      </c>
+      <c r="C192" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" s="1" t="n">
+        <v>191</v>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>614</t>
+        </is>
+      </c>
+      <c r="C193" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" s="1" t="n">
+        <v>192</v>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>642/1</t>
+        </is>
+      </c>
+      <c r="C194" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" s="1" t="n">
+        <v>193</v>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>87</t>
+        </is>
+      </c>
+      <c r="C195" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" s="1" t="n">
+        <v>194</v>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>88</t>
+        </is>
+      </c>
+      <c r="C196" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" s="1" t="n">
+        <v>195</v>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="C197" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" s="1" t="n">
+        <v>196</v>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>97/1</t>
+        </is>
+      </c>
+      <c r="C198" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" s="1" t="n">
+        <v>197</v>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>97/2</t>
+        </is>
+      </c>
+      <c r="C199" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" s="1" t="n">
+        <v>198</v>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>420/101</t>
+        </is>
+      </c>
+      <c r="C200" t="n">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" s="1" t="n">
+        <v>199</v>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>420/102</t>
+        </is>
+      </c>
+      <c r="C201" t="n">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>420/106</t>
+        </is>
+      </c>
+      <c r="C202" t="n">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" s="1" t="n">
+        <v>201</v>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>420/107</t>
+        </is>
+      </c>
+      <c r="C203" t="n">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" s="1" t="n">
+        <v>202</v>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>420/109</t>
+        </is>
+      </c>
+      <c r="C204" t="n">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" s="1" t="n">
+        <v>203</v>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>420/110</t>
+        </is>
+      </c>
+      <c r="C205" t="n">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" s="1" t="n">
+        <v>204</v>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>420/80</t>
+        </is>
+      </c>
+      <c r="C206" t="n">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" s="1" t="n">
+        <v>205</v>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>420/92</t>
+        </is>
+      </c>
+      <c r="C207" t="n">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" s="1" t="n">
+        <v>206</v>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>420/93</t>
+        </is>
+      </c>
+      <c r="C208" t="n">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" s="1" t="n">
+        <v>207</v>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>420/94</t>
+        </is>
+      </c>
+      <c r="C209" t="n">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" s="1" t="n">
+        <v>208</v>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>420/95</t>
+        </is>
+      </c>
+      <c r="C210" t="n">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" s="1" t="n">
+        <v>209</v>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>420/96</t>
+        </is>
+      </c>
+      <c r="C211" t="n">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" s="1" t="n">
+        <v>210</v>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>420/97</t>
+        </is>
+      </c>
+      <c r="C212" t="n">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" s="1" t="n">
+        <v>211</v>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>454</t>
+        </is>
+      </c>
+      <c r="C213" t="n">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" s="1" t="n">
+        <v>212</v>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="C214" t="n">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" s="1" t="n">
+        <v>213</v>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>705/11</t>
+        </is>
+      </c>
+      <c r="C215" t="n">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" s="1" t="n">
+        <v>214</v>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>756</t>
+        </is>
+      </c>
+      <c r="C216" t="n">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" s="1" t="n">
+        <v>215</v>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>798/3</t>
+        </is>
+      </c>
+      <c r="C217" t="n">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" s="1" t="n">
+        <v>216</v>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>4523</t>
+        </is>
+      </c>
+      <c r="C218" t="n">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" s="1" t="n">
+        <v>217</v>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>1438</t>
+        </is>
+      </c>
+      <c r="C219" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" s="1" t="n">
+        <v>218</v>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>1439</t>
+        </is>
+      </c>
+      <c r="C220" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" s="1" t="n">
+        <v>219</v>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>1440</t>
+        </is>
+      </c>
+      <c r="C221" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" s="1" t="n">
+        <v>220</v>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>1441</t>
+        </is>
+      </c>
+      <c r="C222" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" s="1" t="n">
+        <v>221</v>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>1442</t>
+        </is>
+      </c>
+      <c r="C223" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" s="1" t="n">
+        <v>222</v>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>1466</t>
+        </is>
+      </c>
+      <c r="C224" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" s="1" t="n">
+        <v>223</v>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>1468/1</t>
+        </is>
+      </c>
+      <c r="C225" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" s="1" t="n">
+        <v>224</v>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>1470/1</t>
+        </is>
+      </c>
+      <c r="C226" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" s="1" t="n">
+        <v>225</v>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>1470/2</t>
+        </is>
+      </c>
+      <c r="C227" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" s="1" t="n">
+        <v>226</v>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>1471</t>
+        </is>
+      </c>
+      <c r="C228" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" s="1" t="n">
+        <v>227</v>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>1472</t>
+        </is>
+      </c>
+      <c r="C229" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" s="1" t="n">
+        <v>228</v>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>1473</t>
+        </is>
+      </c>
+      <c r="C230" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" s="1" t="n">
+        <v>229</v>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>1474/1</t>
+        </is>
+      </c>
+      <c r="C231" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" s="1" t="n">
+        <v>230</v>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>1474/3</t>
+        </is>
+      </c>
+      <c r="C232" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" s="1" t="n">
+        <v>231</v>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>3597/16</t>
+        </is>
+      </c>
+      <c r="C233" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" s="1" t="n">
+        <v>232</v>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>3597/18</t>
+        </is>
+      </c>
+      <c r="C234" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" s="1" t="n">
+        <v>233</v>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>3597/22</t>
+        </is>
+      </c>
+      <c r="C235" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" s="1" t="n">
+        <v>234</v>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>2331/38</t>
+        </is>
+      </c>
+      <c r="C236" t="n">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" s="1" t="n">
+        <v>235</v>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>2068/43</t>
+        </is>
+      </c>
+      <c r="C237" t="n">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" s="1" t="n">
+        <v>236</v>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>2822/12</t>
+        </is>
+      </c>
+      <c r="C238" t="n">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" s="1" t="n">
+        <v>237</v>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>2822/16</t>
+        </is>
+      </c>
+      <c r="C239" t="n">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" s="1" t="n">
+        <v>238</v>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
           <t>2020/14</t>
         </is>
       </c>
-      <c r="C57" t="n">
+      <c r="C240" t="n">
         <v>310</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Latest data: Tue Jun 18 20:13:34 UTC 2024
</commit_message>
<xml_diff>
--- a/docs/particelle_non_trovate.xlsx
+++ b/docs/particelle_non_trovate.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C57"/>
+  <dimension ref="A1:C152"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1173,6 +1173,1241 @@
         <v>310</v>
       </c>
     </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>1146</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>719</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>857/2</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>859/2</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>1058/2</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>1064/3</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>1491</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>1583</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>1584</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>1517</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>71/2</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>71/2</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>1871</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>3798</t>
+        </is>
+      </c>
+      <c r="C72" t="n">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>353</t>
+        </is>
+      </c>
+      <c r="C73" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>236/2</t>
+        </is>
+      </c>
+      <c r="C74" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>236/3</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>68/4</t>
+        </is>
+      </c>
+      <c r="C76" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>455/1</t>
+        </is>
+      </c>
+      <c r="C77" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>929</t>
+        </is>
+      </c>
+      <c r="C78" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>933</t>
+        </is>
+      </c>
+      <c r="C79" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>934</t>
+        </is>
+      </c>
+      <c r="C80" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>935/1</t>
+        </is>
+      </c>
+      <c r="C81" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>1022/1</t>
+        </is>
+      </c>
+      <c r="C82" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>1030/1</t>
+        </is>
+      </c>
+      <c r="C83" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>1037/1</t>
+        </is>
+      </c>
+      <c r="C84" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>1038</t>
+        </is>
+      </c>
+      <c r="C85" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>1042</t>
+        </is>
+      </c>
+      <c r="C86" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>1043/1</t>
+        </is>
+      </c>
+      <c r="C87" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>1071</t>
+        </is>
+      </c>
+      <c r="C88" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>1093</t>
+        </is>
+      </c>
+      <c r="C89" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>923</t>
+        </is>
+      </c>
+      <c r="C90" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>673/2</t>
+        </is>
+      </c>
+      <c r="C91" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>209</t>
+        </is>
+      </c>
+      <c r="C92" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>870</t>
+        </is>
+      </c>
+      <c r="C93" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>877</t>
+        </is>
+      </c>
+      <c r="C94" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="n">
+        <v>93</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>878</t>
+        </is>
+      </c>
+      <c r="C95" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="n">
+        <v>94</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>884</t>
+        </is>
+      </c>
+      <c r="C96" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>3596</t>
+        </is>
+      </c>
+      <c r="C97" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>251</t>
+        </is>
+      </c>
+      <c r="C98" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>605</t>
+        </is>
+      </c>
+      <c r="C99" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="n">
+        <v>98</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>2074</t>
+        </is>
+      </c>
+      <c r="C100" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>406/3</t>
+        </is>
+      </c>
+      <c r="C101" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>674</t>
+        </is>
+      </c>
+      <c r="C102" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>938</t>
+        </is>
+      </c>
+      <c r="C103" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="n">
+        <v>102</v>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>996</t>
+        </is>
+      </c>
+      <c r="C104" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="n">
+        <v>103</v>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>657/1</t>
+        </is>
+      </c>
+      <c r="C105" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="n">
+        <v>104</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>765/3</t>
+        </is>
+      </c>
+      <c r="C106" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="n">
+        <v>105</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>2050</t>
+        </is>
+      </c>
+      <c r="C107" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="n">
+        <v>106</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>2065</t>
+        </is>
+      </c>
+      <c r="C108" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="n">
+        <v>107</v>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>2066</t>
+        </is>
+      </c>
+      <c r="C109" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="n">
+        <v>108</v>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>2153</t>
+        </is>
+      </c>
+      <c r="C110" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="n">
+        <v>109</v>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>2154</t>
+        </is>
+      </c>
+      <c r="C111" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>673/2</t>
+        </is>
+      </c>
+      <c r="C112" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="n">
+        <v>111</v>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>808</t>
+        </is>
+      </c>
+      <c r="C113" t="n">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="n">
+        <v>112</v>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>1419</t>
+        </is>
+      </c>
+      <c r="C114" t="n">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="n">
+        <v>113</v>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>1420</t>
+        </is>
+      </c>
+      <c r="C115" t="n">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="n">
+        <v>114</v>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>1421</t>
+        </is>
+      </c>
+      <c r="C116" t="n">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="n">
+        <v>115</v>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>1430</t>
+        </is>
+      </c>
+      <c r="C117" t="n">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="n">
+        <v>116</v>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>1431/1</t>
+        </is>
+      </c>
+      <c r="C118" t="n">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="1" t="n">
+        <v>117</v>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>1431/34</t>
+        </is>
+      </c>
+      <c r="C119" t="n">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="1" t="n">
+        <v>118</v>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>.950/1</t>
+        </is>
+      </c>
+      <c r="C120" t="n">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="1" t="n">
+        <v>119</v>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>.950/2</t>
+        </is>
+      </c>
+      <c r="C121" t="n">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="1" t="n">
+        <v>120</v>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>239</t>
+        </is>
+      </c>
+      <c r="C122" t="n">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="1" t="n">
+        <v>121</v>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>241</t>
+        </is>
+      </c>
+      <c r="C123" t="n">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="1" t="n">
+        <v>122</v>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>247</t>
+        </is>
+      </c>
+      <c r="C124" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="1" t="n">
+        <v>123</v>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>581/2</t>
+        </is>
+      </c>
+      <c r="C125" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="1" t="n">
+        <v>124</v>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>2841</t>
+        </is>
+      </c>
+      <c r="C126" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="1" t="n">
+        <v>125</v>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>2468/1</t>
+        </is>
+      </c>
+      <c r="C127" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="1" t="n">
+        <v>126</v>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>2468/2</t>
+        </is>
+      </c>
+      <c r="C128" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="1" t="n">
+        <v>127</v>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>2471</t>
+        </is>
+      </c>
+      <c r="C129" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="1" t="n">
+        <v>128</v>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>2472</t>
+        </is>
+      </c>
+      <c r="C130" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="1" t="n">
+        <v>129</v>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>2561</t>
+        </is>
+      </c>
+      <c r="C131" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="1" t="n">
+        <v>130</v>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>3585</t>
+        </is>
+      </c>
+      <c r="C132" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="1" t="n">
+        <v>131</v>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>3586</t>
+        </is>
+      </c>
+      <c r="C133" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="1" t="n">
+        <v>132</v>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>3587</t>
+        </is>
+      </c>
+      <c r="C134" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="1" t="n">
+        <v>133</v>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>3115/18</t>
+        </is>
+      </c>
+      <c r="C135" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="1" t="n">
+        <v>134</v>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>3115/21</t>
+        </is>
+      </c>
+      <c r="C136" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="1" t="n">
+        <v>135</v>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>3148/4</t>
+        </is>
+      </c>
+      <c r="C137" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="1" t="n">
+        <v>136</v>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>3148/8</t>
+        </is>
+      </c>
+      <c r="C138" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="1" t="n">
+        <v>137</v>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>759</t>
+        </is>
+      </c>
+      <c r="C139" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="1" t="n">
+        <v>138</v>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>1408</t>
+        </is>
+      </c>
+      <c r="C140" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="1" t="n">
+        <v>139</v>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>1411</t>
+        </is>
+      </c>
+      <c r="C141" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>1413</t>
+        </is>
+      </c>
+      <c r="C142" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="1" t="n">
+        <v>141</v>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>1419</t>
+        </is>
+      </c>
+      <c r="C143" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="1" t="n">
+        <v>142</v>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>1420</t>
+        </is>
+      </c>
+      <c r="C144" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="1" t="n">
+        <v>143</v>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>1421</t>
+        </is>
+      </c>
+      <c r="C145" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="1" t="n">
+        <v>144</v>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>1499</t>
+        </is>
+      </c>
+      <c r="C146" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>1502</t>
+        </is>
+      </c>
+      <c r="C147" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="1" t="n">
+        <v>146</v>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>1348/2</t>
+        </is>
+      </c>
+      <c r="C148" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="1" t="n">
+        <v>147</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>4189</t>
+        </is>
+      </c>
+      <c r="C149" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="1" t="n">
+        <v>148</v>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>1113</t>
+        </is>
+      </c>
+      <c r="C150" t="n">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="1" t="n">
+        <v>149</v>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>2052</t>
+        </is>
+      </c>
+      <c r="C151" t="n">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>2161</t>
+        </is>
+      </c>
+      <c r="C152" t="n">
+        <v>440</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Latest data: Fri Aug  9 20:14:51 UTC 2024
</commit_message>
<xml_diff>
--- a/docs/particelle_non_trovate.xlsx
+++ b/docs/particelle_non_trovate.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Latest data: Sun Sep  8 18:03:24 UTC 2024
</commit_message>
<xml_diff>
--- a/docs/particelle_non_trovate.xlsx
+++ b/docs/particelle_non_trovate.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Latest data: Mon Oct 14 12:21:53 UTC 2024
</commit_message>
<xml_diff>
--- a/docs/particelle_non_trovate.xlsx
+++ b/docs/particelle_non_trovate.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C114"/>
+  <dimension ref="A1:C116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1914,6 +1914,32 @@
         <v>444</v>
       </c>
     </row>
+    <row r="115">
+      <c r="A115" s="1" t="n">
+        <v>113</v>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>.451</t>
+        </is>
+      </c>
+      <c r="C115" t="n">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="n">
+        <v>114</v>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>1768</t>
+        </is>
+      </c>
+      <c r="C116" t="n">
+        <v>240</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Latest data: Fri Oct 18 12:21:48 UTC 2024
</commit_message>
<xml_diff>
--- a/docs/particelle_non_trovate.xlsx
+++ b/docs/particelle_non_trovate.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C116"/>
+  <dimension ref="A1:C114"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1907,37 +1907,11 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>.164/1 parte</t>
+          <t>.451</t>
         </is>
       </c>
       <c r="C114" t="n">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" s="1" t="n">
-        <v>113</v>
-      </c>
-      <c r="B115" t="inlineStr">
-        <is>
-          <t>.451</t>
-        </is>
-      </c>
-      <c r="C115" t="n">
         <v>88</v>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" s="1" t="n">
-        <v>114</v>
-      </c>
-      <c r="B116" t="inlineStr">
-        <is>
-          <t>1768</t>
-        </is>
-      </c>
-      <c r="C116" t="n">
-        <v>240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Latest data: Wed Nov 27 20:27:55 UTC 2024
</commit_message>
<xml_diff>
--- a/docs/particelle_non_trovate.xlsx
+++ b/docs/particelle_non_trovate.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C114"/>
+  <dimension ref="A1:C158"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1907,10 +1907,582 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
+          <t>215</t>
+        </is>
+      </c>
+      <c r="C114" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="n">
+        <v>113</v>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>260</t>
+        </is>
+      </c>
+      <c r="C115" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="n">
+        <v>114</v>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>268</t>
+        </is>
+      </c>
+      <c r="C116" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="n">
+        <v>115</v>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>288</t>
+        </is>
+      </c>
+      <c r="C117" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="n">
+        <v>116</v>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>355/1</t>
+        </is>
+      </c>
+      <c r="C118" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="1" t="n">
+        <v>117</v>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>356/1</t>
+        </is>
+      </c>
+      <c r="C119" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="1" t="n">
+        <v>118</v>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>356/2</t>
+        </is>
+      </c>
+      <c r="C120" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="1" t="n">
+        <v>119</v>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>356/5</t>
+        </is>
+      </c>
+      <c r="C121" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="1" t="n">
+        <v>120</v>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>356/25</t>
+        </is>
+      </c>
+      <c r="C122" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="1" t="n">
+        <v>121</v>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>356/27</t>
+        </is>
+      </c>
+      <c r="C123" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="1" t="n">
+        <v>122</v>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>356/28</t>
+        </is>
+      </c>
+      <c r="C124" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="1" t="n">
+        <v>123</v>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>356/29</t>
+        </is>
+      </c>
+      <c r="C125" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="1" t="n">
+        <v>124</v>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>357</t>
+        </is>
+      </c>
+      <c r="C126" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="1" t="n">
+        <v>125</v>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>358</t>
+        </is>
+      </c>
+      <c r="C127" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="1" t="n">
+        <v>126</v>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>361/1</t>
+        </is>
+      </c>
+      <c r="C128" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="1" t="n">
+        <v>127</v>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>361/2</t>
+        </is>
+      </c>
+      <c r="C129" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="1" t="n">
+        <v>128</v>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>362/1</t>
+        </is>
+      </c>
+      <c r="C130" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="1" t="n">
+        <v>129</v>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>362/31</t>
+        </is>
+      </c>
+      <c r="C131" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="1" t="n">
+        <v>130</v>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>362/33</t>
+        </is>
+      </c>
+      <c r="C132" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="1" t="n">
+        <v>131</v>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>362/34</t>
+        </is>
+      </c>
+      <c r="C133" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="1" t="n">
+        <v>132</v>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>362/35</t>
+        </is>
+      </c>
+      <c r="C134" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="1" t="n">
+        <v>133</v>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>362/36</t>
+        </is>
+      </c>
+      <c r="C135" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="1" t="n">
+        <v>134</v>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>363</t>
+        </is>
+      </c>
+      <c r="C136" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="1" t="n">
+        <v>135</v>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>364</t>
+        </is>
+      </c>
+      <c r="C137" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="1" t="n">
+        <v>136</v>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>388</t>
+        </is>
+      </c>
+      <c r="C138" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="1" t="n">
+        <v>137</v>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>389/1</t>
+        </is>
+      </c>
+      <c r="C139" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="1" t="n">
+        <v>138</v>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>389/10</t>
+        </is>
+      </c>
+      <c r="C140" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="1" t="n">
+        <v>139</v>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>390/1</t>
+        </is>
+      </c>
+      <c r="C141" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>390/9</t>
+        </is>
+      </c>
+      <c r="C142" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="1" t="n">
+        <v>141</v>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>390/10</t>
+        </is>
+      </c>
+      <c r="C143" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="1" t="n">
+        <v>142</v>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>391/1</t>
+        </is>
+      </c>
+      <c r="C144" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="1" t="n">
+        <v>143</v>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>391/38</t>
+        </is>
+      </c>
+      <c r="C145" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="1" t="n">
+        <v>144</v>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>391/45</t>
+        </is>
+      </c>
+      <c r="C146" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>392/1</t>
+        </is>
+      </c>
+      <c r="C147" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="1" t="n">
+        <v>146</v>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>392/6</t>
+        </is>
+      </c>
+      <c r="C148" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="1" t="n">
+        <v>147</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>392/7</t>
+        </is>
+      </c>
+      <c r="C149" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="1" t="n">
+        <v>148</v>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>475/21</t>
+        </is>
+      </c>
+      <c r="C150" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="1" t="n">
+        <v>149</v>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>475/31</t>
+        </is>
+      </c>
+      <c r="C151" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>729</t>
+        </is>
+      </c>
+      <c r="C152" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="1" t="n">
+        <v>151</v>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>.578</t>
+        </is>
+      </c>
+      <c r="C153" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="1" t="n">
+        <v>152</v>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>.579</t>
+        </is>
+      </c>
+      <c r="C154" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="1" t="n">
+        <v>153</v>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>.598</t>
+        </is>
+      </c>
+      <c r="C155" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="1" t="n">
+        <v>154</v>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>.607</t>
+        </is>
+      </c>
+      <c r="C156" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="1" t="n">
+        <v>155</v>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>.608</t>
+        </is>
+      </c>
+      <c r="C157" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="1" t="n">
+        <v>156</v>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
           <t>.451</t>
         </is>
       </c>
-      <c r="C114" t="n">
+      <c r="C158" t="n">
         <v>88</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Latest data: Thu Nov 28 00:48:59 UTC 2024
</commit_message>
<xml_diff>
--- a/docs/particelle_non_trovate.xlsx
+++ b/docs/particelle_non_trovate.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C158"/>
+  <dimension ref="A1:C114"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1907,582 +1907,10 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>215</t>
+          <t>.451</t>
         </is>
       </c>
       <c r="C114" t="n">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" s="1" t="n">
-        <v>113</v>
-      </c>
-      <c r="B115" t="inlineStr">
-        <is>
-          <t>260</t>
-        </is>
-      </c>
-      <c r="C115" t="n">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" s="1" t="n">
-        <v>114</v>
-      </c>
-      <c r="B116" t="inlineStr">
-        <is>
-          <t>268</t>
-        </is>
-      </c>
-      <c r="C116" t="n">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" s="1" t="n">
-        <v>115</v>
-      </c>
-      <c r="B117" t="inlineStr">
-        <is>
-          <t>288</t>
-        </is>
-      </c>
-      <c r="C117" t="n">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" s="1" t="n">
-        <v>116</v>
-      </c>
-      <c r="B118" t="inlineStr">
-        <is>
-          <t>355/1</t>
-        </is>
-      </c>
-      <c r="C118" t="n">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" s="1" t="n">
-        <v>117</v>
-      </c>
-      <c r="B119" t="inlineStr">
-        <is>
-          <t>356/1</t>
-        </is>
-      </c>
-      <c r="C119" t="n">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" s="1" t="n">
-        <v>118</v>
-      </c>
-      <c r="B120" t="inlineStr">
-        <is>
-          <t>356/2</t>
-        </is>
-      </c>
-      <c r="C120" t="n">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" s="1" t="n">
-        <v>119</v>
-      </c>
-      <c r="B121" t="inlineStr">
-        <is>
-          <t>356/5</t>
-        </is>
-      </c>
-      <c r="C121" t="n">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" s="1" t="n">
-        <v>120</v>
-      </c>
-      <c r="B122" t="inlineStr">
-        <is>
-          <t>356/25</t>
-        </is>
-      </c>
-      <c r="C122" t="n">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" s="1" t="n">
-        <v>121</v>
-      </c>
-      <c r="B123" t="inlineStr">
-        <is>
-          <t>356/27</t>
-        </is>
-      </c>
-      <c r="C123" t="n">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" s="1" t="n">
-        <v>122</v>
-      </c>
-      <c r="B124" t="inlineStr">
-        <is>
-          <t>356/28</t>
-        </is>
-      </c>
-      <c r="C124" t="n">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" s="1" t="n">
-        <v>123</v>
-      </c>
-      <c r="B125" t="inlineStr">
-        <is>
-          <t>356/29</t>
-        </is>
-      </c>
-      <c r="C125" t="n">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" s="1" t="n">
-        <v>124</v>
-      </c>
-      <c r="B126" t="inlineStr">
-        <is>
-          <t>357</t>
-        </is>
-      </c>
-      <c r="C126" t="n">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" s="1" t="n">
-        <v>125</v>
-      </c>
-      <c r="B127" t="inlineStr">
-        <is>
-          <t>358</t>
-        </is>
-      </c>
-      <c r="C127" t="n">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128" s="1" t="n">
-        <v>126</v>
-      </c>
-      <c r="B128" t="inlineStr">
-        <is>
-          <t>361/1</t>
-        </is>
-      </c>
-      <c r="C128" t="n">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="129">
-      <c r="A129" s="1" t="n">
-        <v>127</v>
-      </c>
-      <c r="B129" t="inlineStr">
-        <is>
-          <t>361/2</t>
-        </is>
-      </c>
-      <c r="C129" t="n">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130" s="1" t="n">
-        <v>128</v>
-      </c>
-      <c r="B130" t="inlineStr">
-        <is>
-          <t>362/1</t>
-        </is>
-      </c>
-      <c r="C130" t="n">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="131">
-      <c r="A131" s="1" t="n">
-        <v>129</v>
-      </c>
-      <c r="B131" t="inlineStr">
-        <is>
-          <t>362/31</t>
-        </is>
-      </c>
-      <c r="C131" t="n">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="132">
-      <c r="A132" s="1" t="n">
-        <v>130</v>
-      </c>
-      <c r="B132" t="inlineStr">
-        <is>
-          <t>362/33</t>
-        </is>
-      </c>
-      <c r="C132" t="n">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="133">
-      <c r="A133" s="1" t="n">
-        <v>131</v>
-      </c>
-      <c r="B133" t="inlineStr">
-        <is>
-          <t>362/34</t>
-        </is>
-      </c>
-      <c r="C133" t="n">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="134">
-      <c r="A134" s="1" t="n">
-        <v>132</v>
-      </c>
-      <c r="B134" t="inlineStr">
-        <is>
-          <t>362/35</t>
-        </is>
-      </c>
-      <c r="C134" t="n">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="135">
-      <c r="A135" s="1" t="n">
-        <v>133</v>
-      </c>
-      <c r="B135" t="inlineStr">
-        <is>
-          <t>362/36</t>
-        </is>
-      </c>
-      <c r="C135" t="n">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="136">
-      <c r="A136" s="1" t="n">
-        <v>134</v>
-      </c>
-      <c r="B136" t="inlineStr">
-        <is>
-          <t>363</t>
-        </is>
-      </c>
-      <c r="C136" t="n">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="137">
-      <c r="A137" s="1" t="n">
-        <v>135</v>
-      </c>
-      <c r="B137" t="inlineStr">
-        <is>
-          <t>364</t>
-        </is>
-      </c>
-      <c r="C137" t="n">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="138">
-      <c r="A138" s="1" t="n">
-        <v>136</v>
-      </c>
-      <c r="B138" t="inlineStr">
-        <is>
-          <t>388</t>
-        </is>
-      </c>
-      <c r="C138" t="n">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="139">
-      <c r="A139" s="1" t="n">
-        <v>137</v>
-      </c>
-      <c r="B139" t="inlineStr">
-        <is>
-          <t>389/1</t>
-        </is>
-      </c>
-      <c r="C139" t="n">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="140">
-      <c r="A140" s="1" t="n">
-        <v>138</v>
-      </c>
-      <c r="B140" t="inlineStr">
-        <is>
-          <t>389/10</t>
-        </is>
-      </c>
-      <c r="C140" t="n">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="141">
-      <c r="A141" s="1" t="n">
-        <v>139</v>
-      </c>
-      <c r="B141" t="inlineStr">
-        <is>
-          <t>390/1</t>
-        </is>
-      </c>
-      <c r="C141" t="n">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="142">
-      <c r="A142" s="1" t="n">
-        <v>140</v>
-      </c>
-      <c r="B142" t="inlineStr">
-        <is>
-          <t>390/9</t>
-        </is>
-      </c>
-      <c r="C142" t="n">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="143">
-      <c r="A143" s="1" t="n">
-        <v>141</v>
-      </c>
-      <c r="B143" t="inlineStr">
-        <is>
-          <t>390/10</t>
-        </is>
-      </c>
-      <c r="C143" t="n">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="144">
-      <c r="A144" s="1" t="n">
-        <v>142</v>
-      </c>
-      <c r="B144" t="inlineStr">
-        <is>
-          <t>391/1</t>
-        </is>
-      </c>
-      <c r="C144" t="n">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="145">
-      <c r="A145" s="1" t="n">
-        <v>143</v>
-      </c>
-      <c r="B145" t="inlineStr">
-        <is>
-          <t>391/38</t>
-        </is>
-      </c>
-      <c r="C145" t="n">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="146">
-      <c r="A146" s="1" t="n">
-        <v>144</v>
-      </c>
-      <c r="B146" t="inlineStr">
-        <is>
-          <t>391/45</t>
-        </is>
-      </c>
-      <c r="C146" t="n">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="147">
-      <c r="A147" s="1" t="n">
-        <v>145</v>
-      </c>
-      <c r="B147" t="inlineStr">
-        <is>
-          <t>392/1</t>
-        </is>
-      </c>
-      <c r="C147" t="n">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="148">
-      <c r="A148" s="1" t="n">
-        <v>146</v>
-      </c>
-      <c r="B148" t="inlineStr">
-        <is>
-          <t>392/6</t>
-        </is>
-      </c>
-      <c r="C148" t="n">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="149">
-      <c r="A149" s="1" t="n">
-        <v>147</v>
-      </c>
-      <c r="B149" t="inlineStr">
-        <is>
-          <t>392/7</t>
-        </is>
-      </c>
-      <c r="C149" t="n">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="150">
-      <c r="A150" s="1" t="n">
-        <v>148</v>
-      </c>
-      <c r="B150" t="inlineStr">
-        <is>
-          <t>475/21</t>
-        </is>
-      </c>
-      <c r="C150" t="n">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="151">
-      <c r="A151" s="1" t="n">
-        <v>149</v>
-      </c>
-      <c r="B151" t="inlineStr">
-        <is>
-          <t>475/31</t>
-        </is>
-      </c>
-      <c r="C151" t="n">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="152">
-      <c r="A152" s="1" t="n">
-        <v>150</v>
-      </c>
-      <c r="B152" t="inlineStr">
-        <is>
-          <t>729</t>
-        </is>
-      </c>
-      <c r="C152" t="n">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="153">
-      <c r="A153" s="1" t="n">
-        <v>151</v>
-      </c>
-      <c r="B153" t="inlineStr">
-        <is>
-          <t>.578</t>
-        </is>
-      </c>
-      <c r="C153" t="n">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="154">
-      <c r="A154" s="1" t="n">
-        <v>152</v>
-      </c>
-      <c r="B154" t="inlineStr">
-        <is>
-          <t>.579</t>
-        </is>
-      </c>
-      <c r="C154" t="n">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="155">
-      <c r="A155" s="1" t="n">
-        <v>153</v>
-      </c>
-      <c r="B155" t="inlineStr">
-        <is>
-          <t>.598</t>
-        </is>
-      </c>
-      <c r="C155" t="n">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="156">
-      <c r="A156" s="1" t="n">
-        <v>154</v>
-      </c>
-      <c r="B156" t="inlineStr">
-        <is>
-          <t>.607</t>
-        </is>
-      </c>
-      <c r="C156" t="n">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="157">
-      <c r="A157" s="1" t="n">
-        <v>155</v>
-      </c>
-      <c r="B157" t="inlineStr">
-        <is>
-          <t>.608</t>
-        </is>
-      </c>
-      <c r="C157" t="n">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="158">
-      <c r="A158" s="1" t="n">
-        <v>156</v>
-      </c>
-      <c r="B158" t="inlineStr">
-        <is>
-          <t>.451</t>
-        </is>
-      </c>
-      <c r="C158" t="n">
         <v>88</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Latest data: Wed Dec 18 12:23:20 UTC 2024
</commit_message>
<xml_diff>
--- a/docs/particelle_non_trovate.xlsx
+++ b/docs/particelle_non_trovate.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C114"/>
+  <dimension ref="A1:C117"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1914,6 +1914,45 @@
         <v>88</v>
       </c>
     </row>
+    <row r="115">
+      <c r="A115" s="1" t="n">
+        <v>113</v>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>703</t>
+        </is>
+      </c>
+      <c r="C115" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="n">
+        <v>114</v>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>.74</t>
+        </is>
+      </c>
+      <c r="C116" t="n">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="n">
+        <v>115</v>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>.207</t>
+        </is>
+      </c>
+      <c r="C117" t="n">
+        <v>388</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Latest data: Mon Dec 30 20:14:41 UTC 2024
</commit_message>
<xml_diff>
--- a/docs/particelle_non_trovate.xlsx
+++ b/docs/particelle_non_trovate.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1707"/>
+  <dimension ref="A1:C1510"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16751,22 +16751,40 @@
       <c r="A1256" s="1" t="n">
         <v>1254</v>
       </c>
-      <c r="B1256" t="inlineStr"/>
-      <c r="C1256" t="inlineStr"/>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>324337</t>
+        </is>
+      </c>
+      <c r="C1256" t="n">
+        <v>258</v>
+      </c>
     </row>
     <row r="1257">
       <c r="A1257" s="1" t="n">
         <v>1255</v>
       </c>
-      <c r="B1257" t="inlineStr"/>
-      <c r="C1257" t="inlineStr"/>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>655248</t>
+        </is>
+      </c>
+      <c r="C1257" t="n">
+        <v>258</v>
+      </c>
     </row>
     <row r="1258">
       <c r="A1258" s="1" t="n">
         <v>1256</v>
       </c>
-      <c r="B1258" t="inlineStr"/>
-      <c r="C1258" t="inlineStr"/>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>2331/38</t>
+        </is>
+      </c>
+      <c r="C1258" t="n">
+        <v>258</v>
+      </c>
     </row>
     <row r="1259">
       <c r="A1259" s="1" t="n">
@@ -17871,2613 +17889,1234 @@
       <c r="A1416" s="1" t="n">
         <v>1414</v>
       </c>
-      <c r="B1416" t="inlineStr"/>
-      <c r="C1416" t="inlineStr"/>
+      <c r="B1416" t="inlineStr">
+        <is>
+          <t>1146</t>
+        </is>
+      </c>
+      <c r="C1416" t="n">
+        <v>248</v>
+      </c>
     </row>
     <row r="1417">
       <c r="A1417" s="1" t="n">
         <v>1415</v>
       </c>
-      <c r="B1417" t="inlineStr"/>
-      <c r="C1417" t="inlineStr"/>
+      <c r="B1417" t="inlineStr">
+        <is>
+          <t>719</t>
+        </is>
+      </c>
+      <c r="C1417" t="n">
+        <v>248</v>
+      </c>
     </row>
     <row r="1418">
       <c r="A1418" s="1" t="n">
         <v>1416</v>
       </c>
-      <c r="B1418" t="inlineStr"/>
-      <c r="C1418" t="inlineStr"/>
+      <c r="B1418" t="inlineStr">
+        <is>
+          <t>857/2</t>
+        </is>
+      </c>
+      <c r="C1418" t="n">
+        <v>248</v>
+      </c>
     </row>
     <row r="1419">
       <c r="A1419" s="1" t="n">
         <v>1417</v>
       </c>
-      <c r="B1419" t="inlineStr"/>
-      <c r="C1419" t="inlineStr"/>
+      <c r="B1419" t="inlineStr">
+        <is>
+          <t>859/2</t>
+        </is>
+      </c>
+      <c r="C1419" t="n">
+        <v>248</v>
+      </c>
     </row>
     <row r="1420">
       <c r="A1420" s="1" t="n">
         <v>1418</v>
       </c>
-      <c r="B1420" t="inlineStr"/>
-      <c r="C1420" t="inlineStr"/>
+      <c r="B1420" t="inlineStr">
+        <is>
+          <t>1058/2</t>
+        </is>
+      </c>
+      <c r="C1420" t="n">
+        <v>248</v>
+      </c>
     </row>
     <row r="1421">
       <c r="A1421" s="1" t="n">
         <v>1419</v>
       </c>
-      <c r="B1421" t="inlineStr"/>
-      <c r="C1421" t="inlineStr"/>
+      <c r="B1421" t="inlineStr">
+        <is>
+          <t>1064/3</t>
+        </is>
+      </c>
+      <c r="C1421" t="n">
+        <v>248</v>
+      </c>
     </row>
     <row r="1422">
       <c r="A1422" s="1" t="n">
         <v>1420</v>
       </c>
-      <c r="B1422" t="inlineStr"/>
-      <c r="C1422" t="inlineStr"/>
+      <c r="B1422" t="inlineStr">
+        <is>
+          <t>1491</t>
+        </is>
+      </c>
+      <c r="C1422" t="n">
+        <v>248</v>
+      </c>
     </row>
     <row r="1423">
       <c r="A1423" s="1" t="n">
         <v>1421</v>
       </c>
-      <c r="B1423" t="inlineStr"/>
-      <c r="C1423" t="inlineStr"/>
+      <c r="B1423" t="inlineStr">
+        <is>
+          <t>1583</t>
+        </is>
+      </c>
+      <c r="C1423" t="n">
+        <v>248</v>
+      </c>
     </row>
     <row r="1424">
       <c r="A1424" s="1" t="n">
         <v>1422</v>
       </c>
-      <c r="B1424" t="inlineStr"/>
-      <c r="C1424" t="inlineStr"/>
+      <c r="B1424" t="inlineStr">
+        <is>
+          <t>1584</t>
+        </is>
+      </c>
+      <c r="C1424" t="n">
+        <v>248</v>
+      </c>
     </row>
     <row r="1425">
       <c r="A1425" s="1" t="n">
         <v>1423</v>
       </c>
-      <c r="B1425" t="inlineStr"/>
-      <c r="C1425" t="inlineStr"/>
+      <c r="B1425" t="inlineStr">
+        <is>
+          <t>1517</t>
+        </is>
+      </c>
+      <c r="C1425" t="n">
+        <v>248</v>
+      </c>
     </row>
     <row r="1426">
       <c r="A1426" s="1" t="n">
         <v>1424</v>
       </c>
-      <c r="B1426" t="inlineStr"/>
-      <c r="C1426" t="inlineStr"/>
+      <c r="B1426" t="inlineStr">
+        <is>
+          <t>71/2</t>
+        </is>
+      </c>
+      <c r="C1426" t="n">
+        <v>307</v>
+      </c>
     </row>
     <row r="1427">
       <c r="A1427" s="1" t="n">
         <v>1425</v>
       </c>
-      <c r="B1427" t="inlineStr"/>
-      <c r="C1427" t="inlineStr"/>
+      <c r="B1427" t="inlineStr">
+        <is>
+          <t>71/2</t>
+        </is>
+      </c>
+      <c r="C1427" t="n">
+        <v>307</v>
+      </c>
     </row>
     <row r="1428">
       <c r="A1428" s="1" t="n">
         <v>1426</v>
       </c>
-      <c r="B1428" t="inlineStr"/>
-      <c r="C1428" t="inlineStr"/>
+      <c r="B1428" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="C1428" t="n">
+        <v>307</v>
+      </c>
     </row>
     <row r="1429">
       <c r="A1429" s="1" t="n">
         <v>1427</v>
       </c>
-      <c r="B1429" t="inlineStr"/>
-      <c r="C1429" t="inlineStr"/>
+      <c r="B1429" t="inlineStr">
+        <is>
+          <t>1871</t>
+        </is>
+      </c>
+      <c r="C1429" t="n">
+        <v>307</v>
+      </c>
     </row>
     <row r="1430">
       <c r="A1430" s="1" t="n">
         <v>1428</v>
       </c>
-      <c r="B1430" t="inlineStr"/>
-      <c r="C1430" t="inlineStr"/>
+      <c r="B1430" t="inlineStr">
+        <is>
+          <t>3798</t>
+        </is>
+      </c>
+      <c r="C1430" t="n">
+        <v>307</v>
+      </c>
     </row>
     <row r="1431">
       <c r="A1431" s="1" t="n">
         <v>1429</v>
       </c>
-      <c r="B1431" t="inlineStr"/>
-      <c r="C1431" t="inlineStr"/>
+      <c r="B1431" t="inlineStr">
+        <is>
+          <t>353</t>
+        </is>
+      </c>
+      <c r="C1431" t="n">
+        <v>384</v>
+      </c>
     </row>
     <row r="1432">
       <c r="A1432" s="1" t="n">
         <v>1430</v>
       </c>
-      <c r="B1432" t="inlineStr"/>
-      <c r="C1432" t="inlineStr"/>
+      <c r="B1432" t="inlineStr">
+        <is>
+          <t>236/2</t>
+        </is>
+      </c>
+      <c r="C1432" t="n">
+        <v>384</v>
+      </c>
     </row>
     <row r="1433">
       <c r="A1433" s="1" t="n">
         <v>1431</v>
       </c>
-      <c r="B1433" t="inlineStr"/>
-      <c r="C1433" t="inlineStr"/>
+      <c r="B1433" t="inlineStr">
+        <is>
+          <t>236/3</t>
+        </is>
+      </c>
+      <c r="C1433" t="n">
+        <v>384</v>
+      </c>
     </row>
     <row r="1434">
       <c r="A1434" s="1" t="n">
         <v>1432</v>
       </c>
-      <c r="B1434" t="inlineStr"/>
-      <c r="C1434" t="inlineStr"/>
+      <c r="B1434" t="inlineStr">
+        <is>
+          <t>68/4</t>
+        </is>
+      </c>
+      <c r="C1434" t="n">
+        <v>384</v>
+      </c>
     </row>
     <row r="1435">
       <c r="A1435" s="1" t="n">
         <v>1433</v>
       </c>
-      <c r="B1435" t="inlineStr"/>
-      <c r="C1435" t="inlineStr"/>
+      <c r="B1435" t="inlineStr">
+        <is>
+          <t>455/1</t>
+        </is>
+      </c>
+      <c r="C1435" t="n">
+        <v>384</v>
+      </c>
     </row>
     <row r="1436">
       <c r="A1436" s="1" t="n">
         <v>1434</v>
       </c>
-      <c r="B1436" t="inlineStr"/>
-      <c r="C1436" t="inlineStr"/>
+      <c r="B1436" t="inlineStr">
+        <is>
+          <t>929</t>
+        </is>
+      </c>
+      <c r="C1436" t="n">
+        <v>384</v>
+      </c>
     </row>
     <row r="1437">
       <c r="A1437" s="1" t="n">
         <v>1435</v>
       </c>
-      <c r="B1437" t="inlineStr"/>
-      <c r="C1437" t="inlineStr"/>
+      <c r="B1437" t="inlineStr">
+        <is>
+          <t>933</t>
+        </is>
+      </c>
+      <c r="C1437" t="n">
+        <v>384</v>
+      </c>
     </row>
     <row r="1438">
       <c r="A1438" s="1" t="n">
         <v>1436</v>
       </c>
-      <c r="B1438" t="inlineStr"/>
-      <c r="C1438" t="inlineStr"/>
+      <c r="B1438" t="inlineStr">
+        <is>
+          <t>934</t>
+        </is>
+      </c>
+      <c r="C1438" t="n">
+        <v>384</v>
+      </c>
     </row>
     <row r="1439">
       <c r="A1439" s="1" t="n">
         <v>1437</v>
       </c>
-      <c r="B1439" t="inlineStr"/>
-      <c r="C1439" t="inlineStr"/>
+      <c r="B1439" t="inlineStr">
+        <is>
+          <t>935/1</t>
+        </is>
+      </c>
+      <c r="C1439" t="n">
+        <v>384</v>
+      </c>
     </row>
     <row r="1440">
       <c r="A1440" s="1" t="n">
         <v>1438</v>
       </c>
-      <c r="B1440" t="inlineStr"/>
-      <c r="C1440" t="inlineStr"/>
+      <c r="B1440" t="inlineStr">
+        <is>
+          <t>1022/1</t>
+        </is>
+      </c>
+      <c r="C1440" t="n">
+        <v>384</v>
+      </c>
     </row>
     <row r="1441">
       <c r="A1441" s="1" t="n">
         <v>1439</v>
       </c>
-      <c r="B1441" t="inlineStr"/>
-      <c r="C1441" t="inlineStr"/>
+      <c r="B1441" t="inlineStr">
+        <is>
+          <t>1030/1</t>
+        </is>
+      </c>
+      <c r="C1441" t="n">
+        <v>384</v>
+      </c>
     </row>
     <row r="1442">
       <c r="A1442" s="1" t="n">
         <v>1440</v>
       </c>
-      <c r="B1442" t="inlineStr"/>
-      <c r="C1442" t="inlineStr"/>
+      <c r="B1442" t="inlineStr">
+        <is>
+          <t>1037/1</t>
+        </is>
+      </c>
+      <c r="C1442" t="n">
+        <v>384</v>
+      </c>
     </row>
     <row r="1443">
       <c r="A1443" s="1" t="n">
         <v>1441</v>
       </c>
-      <c r="B1443" t="inlineStr"/>
-      <c r="C1443" t="inlineStr"/>
+      <c r="B1443" t="inlineStr">
+        <is>
+          <t>1038</t>
+        </is>
+      </c>
+      <c r="C1443" t="n">
+        <v>384</v>
+      </c>
     </row>
     <row r="1444">
       <c r="A1444" s="1" t="n">
         <v>1442</v>
       </c>
-      <c r="B1444" t="inlineStr"/>
-      <c r="C1444" t="inlineStr"/>
+      <c r="B1444" t="inlineStr">
+        <is>
+          <t>1042</t>
+        </is>
+      </c>
+      <c r="C1444" t="n">
+        <v>384</v>
+      </c>
     </row>
     <row r="1445">
       <c r="A1445" s="1" t="n">
         <v>1443</v>
       </c>
-      <c r="B1445" t="inlineStr"/>
-      <c r="C1445" t="inlineStr"/>
+      <c r="B1445" t="inlineStr">
+        <is>
+          <t>1043/1</t>
+        </is>
+      </c>
+      <c r="C1445" t="n">
+        <v>384</v>
+      </c>
     </row>
     <row r="1446">
       <c r="A1446" s="1" t="n">
         <v>1444</v>
       </c>
-      <c r="B1446" t="inlineStr"/>
-      <c r="C1446" t="inlineStr"/>
+      <c r="B1446" t="inlineStr">
+        <is>
+          <t>1071</t>
+        </is>
+      </c>
+      <c r="C1446" t="n">
+        <v>384</v>
+      </c>
     </row>
     <row r="1447">
       <c r="A1447" s="1" t="n">
         <v>1445</v>
       </c>
-      <c r="B1447" t="inlineStr"/>
-      <c r="C1447" t="inlineStr"/>
+      <c r="B1447" t="inlineStr">
+        <is>
+          <t>1093</t>
+        </is>
+      </c>
+      <c r="C1447" t="n">
+        <v>384</v>
+      </c>
     </row>
     <row r="1448">
       <c r="A1448" s="1" t="n">
         <v>1446</v>
       </c>
-      <c r="B1448" t="inlineStr"/>
-      <c r="C1448" t="inlineStr"/>
+      <c r="B1448" t="inlineStr">
+        <is>
+          <t>923</t>
+        </is>
+      </c>
+      <c r="C1448" t="n">
+        <v>384</v>
+      </c>
     </row>
     <row r="1449">
       <c r="A1449" s="1" t="n">
         <v>1447</v>
       </c>
-      <c r="B1449" t="inlineStr"/>
-      <c r="C1449" t="inlineStr"/>
+      <c r="B1449" t="inlineStr">
+        <is>
+          <t>673/2</t>
+        </is>
+      </c>
+      <c r="C1449" t="n">
+        <v>384</v>
+      </c>
     </row>
     <row r="1450">
       <c r="A1450" s="1" t="n">
         <v>1448</v>
       </c>
-      <c r="B1450" t="inlineStr"/>
-      <c r="C1450" t="inlineStr"/>
+      <c r="B1450" t="inlineStr">
+        <is>
+          <t>209</t>
+        </is>
+      </c>
+      <c r="C1450" t="n">
+        <v>384</v>
+      </c>
     </row>
     <row r="1451">
       <c r="A1451" s="1" t="n">
         <v>1449</v>
       </c>
-      <c r="B1451" t="inlineStr"/>
-      <c r="C1451" t="inlineStr"/>
+      <c r="B1451" t="inlineStr">
+        <is>
+          <t>870</t>
+        </is>
+      </c>
+      <c r="C1451" t="n">
+        <v>384</v>
+      </c>
     </row>
     <row r="1452">
       <c r="A1452" s="1" t="n">
         <v>1450</v>
       </c>
-      <c r="B1452" t="inlineStr"/>
-      <c r="C1452" t="inlineStr"/>
+      <c r="B1452" t="inlineStr">
+        <is>
+          <t>877</t>
+        </is>
+      </c>
+      <c r="C1452" t="n">
+        <v>384</v>
+      </c>
     </row>
     <row r="1453">
       <c r="A1453" s="1" t="n">
         <v>1451</v>
       </c>
-      <c r="B1453" t="inlineStr"/>
-      <c r="C1453" t="inlineStr"/>
+      <c r="B1453" t="inlineStr">
+        <is>
+          <t>878</t>
+        </is>
+      </c>
+      <c r="C1453" t="n">
+        <v>384</v>
+      </c>
     </row>
     <row r="1454">
       <c r="A1454" s="1" t="n">
         <v>1452</v>
       </c>
-      <c r="B1454" t="inlineStr"/>
-      <c r="C1454" t="inlineStr"/>
+      <c r="B1454" t="inlineStr">
+        <is>
+          <t>884</t>
+        </is>
+      </c>
+      <c r="C1454" t="n">
+        <v>384</v>
+      </c>
     </row>
     <row r="1455">
       <c r="A1455" s="1" t="n">
         <v>1453</v>
       </c>
-      <c r="B1455" t="inlineStr"/>
-      <c r="C1455" t="inlineStr"/>
+      <c r="B1455" t="inlineStr">
+        <is>
+          <t>3596</t>
+        </is>
+      </c>
+      <c r="C1455" t="n">
+        <v>384</v>
+      </c>
     </row>
     <row r="1456">
       <c r="A1456" s="1" t="n">
         <v>1454</v>
       </c>
-      <c r="B1456" t="inlineStr"/>
-      <c r="C1456" t="inlineStr"/>
+      <c r="B1456" t="inlineStr">
+        <is>
+          <t>251</t>
+        </is>
+      </c>
+      <c r="C1456" t="n">
+        <v>384</v>
+      </c>
     </row>
     <row r="1457">
       <c r="A1457" s="1" t="n">
         <v>1455</v>
       </c>
-      <c r="B1457" t="inlineStr"/>
-      <c r="C1457" t="inlineStr"/>
+      <c r="B1457" t="inlineStr">
+        <is>
+          <t>605</t>
+        </is>
+      </c>
+      <c r="C1457" t="n">
+        <v>384</v>
+      </c>
     </row>
     <row r="1458">
       <c r="A1458" s="1" t="n">
         <v>1456</v>
       </c>
-      <c r="B1458" t="inlineStr"/>
-      <c r="C1458" t="inlineStr"/>
+      <c r="B1458" t="inlineStr">
+        <is>
+          <t>2074</t>
+        </is>
+      </c>
+      <c r="C1458" t="n">
+        <v>384</v>
+      </c>
     </row>
     <row r="1459">
       <c r="A1459" s="1" t="n">
         <v>1457</v>
       </c>
-      <c r="B1459" t="inlineStr"/>
-      <c r="C1459" t="inlineStr"/>
+      <c r="B1459" t="inlineStr">
+        <is>
+          <t>406/3</t>
+        </is>
+      </c>
+      <c r="C1459" t="n">
+        <v>384</v>
+      </c>
     </row>
     <row r="1460">
       <c r="A1460" s="1" t="n">
         <v>1458</v>
       </c>
-      <c r="B1460" t="inlineStr"/>
-      <c r="C1460" t="inlineStr"/>
+      <c r="B1460" t="inlineStr">
+        <is>
+          <t>674</t>
+        </is>
+      </c>
+      <c r="C1460" t="n">
+        <v>384</v>
+      </c>
     </row>
     <row r="1461">
       <c r="A1461" s="1" t="n">
         <v>1459</v>
       </c>
-      <c r="B1461" t="inlineStr"/>
-      <c r="C1461" t="inlineStr"/>
+      <c r="B1461" t="inlineStr">
+        <is>
+          <t>938</t>
+        </is>
+      </c>
+      <c r="C1461" t="n">
+        <v>384</v>
+      </c>
     </row>
     <row r="1462">
       <c r="A1462" s="1" t="n">
         <v>1460</v>
       </c>
-      <c r="B1462" t="inlineStr"/>
-      <c r="C1462" t="inlineStr"/>
+      <c r="B1462" t="inlineStr">
+        <is>
+          <t>996</t>
+        </is>
+      </c>
+      <c r="C1462" t="n">
+        <v>384</v>
+      </c>
     </row>
     <row r="1463">
       <c r="A1463" s="1" t="n">
         <v>1461</v>
       </c>
-      <c r="B1463" t="inlineStr"/>
-      <c r="C1463" t="inlineStr"/>
+      <c r="B1463" t="inlineStr">
+        <is>
+          <t>657/1</t>
+        </is>
+      </c>
+      <c r="C1463" t="n">
+        <v>384</v>
+      </c>
     </row>
     <row r="1464">
       <c r="A1464" s="1" t="n">
         <v>1462</v>
       </c>
-      <c r="B1464" t="inlineStr"/>
-      <c r="C1464" t="inlineStr"/>
+      <c r="B1464" t="inlineStr">
+        <is>
+          <t>765/3</t>
+        </is>
+      </c>
+      <c r="C1464" t="n">
+        <v>384</v>
+      </c>
     </row>
     <row r="1465">
       <c r="A1465" s="1" t="n">
         <v>1463</v>
       </c>
-      <c r="B1465" t="inlineStr"/>
-      <c r="C1465" t="inlineStr"/>
+      <c r="B1465" t="inlineStr">
+        <is>
+          <t>2050</t>
+        </is>
+      </c>
+      <c r="C1465" t="n">
+        <v>384</v>
+      </c>
     </row>
     <row r="1466">
       <c r="A1466" s="1" t="n">
         <v>1464</v>
       </c>
-      <c r="B1466" t="inlineStr"/>
-      <c r="C1466" t="inlineStr"/>
+      <c r="B1466" t="inlineStr">
+        <is>
+          <t>2065</t>
+        </is>
+      </c>
+      <c r="C1466" t="n">
+        <v>384</v>
+      </c>
     </row>
     <row r="1467">
       <c r="A1467" s="1" t="n">
         <v>1465</v>
       </c>
-      <c r="B1467" t="inlineStr"/>
-      <c r="C1467" t="inlineStr"/>
+      <c r="B1467" t="inlineStr">
+        <is>
+          <t>2066</t>
+        </is>
+      </c>
+      <c r="C1467" t="n">
+        <v>384</v>
+      </c>
     </row>
     <row r="1468">
       <c r="A1468" s="1" t="n">
         <v>1466</v>
       </c>
-      <c r="B1468" t="inlineStr"/>
-      <c r="C1468" t="inlineStr"/>
+      <c r="B1468" t="inlineStr">
+        <is>
+          <t>2153</t>
+        </is>
+      </c>
+      <c r="C1468" t="n">
+        <v>384</v>
+      </c>
     </row>
     <row r="1469">
       <c r="A1469" s="1" t="n">
         <v>1467</v>
       </c>
-      <c r="B1469" t="inlineStr"/>
-      <c r="C1469" t="inlineStr"/>
+      <c r="B1469" t="inlineStr">
+        <is>
+          <t>2154</t>
+        </is>
+      </c>
+      <c r="C1469" t="n">
+        <v>384</v>
+      </c>
     </row>
     <row r="1470">
       <c r="A1470" s="1" t="n">
         <v>1468</v>
       </c>
-      <c r="B1470" t="inlineStr"/>
-      <c r="C1470" t="inlineStr"/>
+      <c r="B1470" t="inlineStr">
+        <is>
+          <t>673/2</t>
+        </is>
+      </c>
+      <c r="C1470" t="n">
+        <v>384</v>
+      </c>
     </row>
     <row r="1471">
       <c r="A1471" s="1" t="n">
         <v>1469</v>
       </c>
-      <c r="B1471" t="inlineStr"/>
-      <c r="C1471" t="inlineStr"/>
+      <c r="B1471" t="inlineStr">
+        <is>
+          <t>808</t>
+        </is>
+      </c>
+      <c r="C1471" t="n">
+        <v>287</v>
+      </c>
     </row>
     <row r="1472">
       <c r="A1472" s="1" t="n">
         <v>1470</v>
       </c>
-      <c r="B1472" t="inlineStr"/>
-      <c r="C1472" t="inlineStr"/>
+      <c r="B1472" t="inlineStr">
+        <is>
+          <t>1419</t>
+        </is>
+      </c>
+      <c r="C1472" t="n">
+        <v>287</v>
+      </c>
     </row>
     <row r="1473">
       <c r="A1473" s="1" t="n">
         <v>1471</v>
       </c>
-      <c r="B1473" t="inlineStr"/>
-      <c r="C1473" t="inlineStr"/>
+      <c r="B1473" t="inlineStr">
+        <is>
+          <t>1420</t>
+        </is>
+      </c>
+      <c r="C1473" t="n">
+        <v>287</v>
+      </c>
     </row>
     <row r="1474">
       <c r="A1474" s="1" t="n">
         <v>1472</v>
       </c>
-      <c r="B1474" t="inlineStr"/>
-      <c r="C1474" t="inlineStr"/>
+      <c r="B1474" t="inlineStr">
+        <is>
+          <t>1421</t>
+        </is>
+      </c>
+      <c r="C1474" t="n">
+        <v>287</v>
+      </c>
     </row>
     <row r="1475">
       <c r="A1475" s="1" t="n">
         <v>1473</v>
       </c>
-      <c r="B1475" t="inlineStr"/>
-      <c r="C1475" t="inlineStr"/>
+      <c r="B1475" t="inlineStr">
+        <is>
+          <t>1430</t>
+        </is>
+      </c>
+      <c r="C1475" t="n">
+        <v>287</v>
+      </c>
     </row>
     <row r="1476">
       <c r="A1476" s="1" t="n">
         <v>1474</v>
       </c>
-      <c r="B1476" t="inlineStr"/>
-      <c r="C1476" t="inlineStr"/>
+      <c r="B1476" t="inlineStr">
+        <is>
+          <t>1431/1</t>
+        </is>
+      </c>
+      <c r="C1476" t="n">
+        <v>287</v>
+      </c>
     </row>
     <row r="1477">
       <c r="A1477" s="1" t="n">
         <v>1475</v>
       </c>
-      <c r="B1477" t="inlineStr"/>
-      <c r="C1477" t="inlineStr"/>
+      <c r="B1477" t="inlineStr">
+        <is>
+          <t>1431/34</t>
+        </is>
+      </c>
+      <c r="C1477" t="n">
+        <v>287</v>
+      </c>
     </row>
     <row r="1478">
       <c r="A1478" s="1" t="n">
         <v>1476</v>
       </c>
-      <c r="B1478" t="inlineStr"/>
-      <c r="C1478" t="inlineStr"/>
+      <c r="B1478" t="inlineStr">
+        <is>
+          <t>.950/1</t>
+        </is>
+      </c>
+      <c r="C1478" t="n">
+        <v>287</v>
+      </c>
     </row>
     <row r="1479">
       <c r="A1479" s="1" t="n">
         <v>1477</v>
       </c>
-      <c r="B1479" t="inlineStr"/>
-      <c r="C1479" t="inlineStr"/>
+      <c r="B1479" t="inlineStr">
+        <is>
+          <t>.950/2</t>
+        </is>
+      </c>
+      <c r="C1479" t="n">
+        <v>287</v>
+      </c>
     </row>
     <row r="1480">
       <c r="A1480" s="1" t="n">
         <v>1478</v>
       </c>
-      <c r="B1480" t="inlineStr"/>
-      <c r="C1480" t="inlineStr"/>
+      <c r="B1480" t="inlineStr">
+        <is>
+          <t>239</t>
+        </is>
+      </c>
+      <c r="C1480" t="n">
+        <v>287</v>
+      </c>
     </row>
     <row r="1481">
       <c r="A1481" s="1" t="n">
         <v>1479</v>
       </c>
-      <c r="B1481" t="inlineStr"/>
-      <c r="C1481" t="inlineStr"/>
+      <c r="B1481" t="inlineStr">
+        <is>
+          <t>241</t>
+        </is>
+      </c>
+      <c r="C1481" t="n">
+        <v>287</v>
+      </c>
     </row>
     <row r="1482">
       <c r="A1482" s="1" t="n">
         <v>1480</v>
       </c>
-      <c r="B1482" t="inlineStr"/>
-      <c r="C1482" t="inlineStr"/>
+      <c r="B1482" t="inlineStr">
+        <is>
+          <t>247</t>
+        </is>
+      </c>
+      <c r="C1482" t="n">
+        <v>140</v>
+      </c>
     </row>
     <row r="1483">
       <c r="A1483" s="1" t="n">
         <v>1481</v>
       </c>
-      <c r="B1483" t="inlineStr"/>
-      <c r="C1483" t="inlineStr"/>
+      <c r="B1483" t="inlineStr">
+        <is>
+          <t>581/2</t>
+        </is>
+      </c>
+      <c r="C1483" t="n">
+        <v>140</v>
+      </c>
     </row>
     <row r="1484">
       <c r="A1484" s="1" t="n">
         <v>1482</v>
       </c>
-      <c r="B1484" t="inlineStr"/>
-      <c r="C1484" t="inlineStr"/>
+      <c r="B1484" t="inlineStr">
+        <is>
+          <t>2841</t>
+        </is>
+      </c>
+      <c r="C1484" t="n">
+        <v>140</v>
+      </c>
     </row>
     <row r="1485">
       <c r="A1485" s="1" t="n">
         <v>1483</v>
       </c>
-      <c r="B1485" t="inlineStr"/>
-      <c r="C1485" t="inlineStr"/>
+      <c r="B1485" t="inlineStr">
+        <is>
+          <t>2468/1</t>
+        </is>
+      </c>
+      <c r="C1485" t="n">
+        <v>140</v>
+      </c>
     </row>
     <row r="1486">
       <c r="A1486" s="1" t="n">
         <v>1484</v>
       </c>
-      <c r="B1486" t="inlineStr"/>
-      <c r="C1486" t="inlineStr"/>
+      <c r="B1486" t="inlineStr">
+        <is>
+          <t>2468/2</t>
+        </is>
+      </c>
+      <c r="C1486" t="n">
+        <v>140</v>
+      </c>
     </row>
     <row r="1487">
       <c r="A1487" s="1" t="n">
         <v>1485</v>
       </c>
-      <c r="B1487" t="inlineStr"/>
-      <c r="C1487" t="inlineStr"/>
+      <c r="B1487" t="inlineStr">
+        <is>
+          <t>2471</t>
+        </is>
+      </c>
+      <c r="C1487" t="n">
+        <v>140</v>
+      </c>
     </row>
     <row r="1488">
       <c r="A1488" s="1" t="n">
         <v>1486</v>
       </c>
-      <c r="B1488" t="inlineStr"/>
-      <c r="C1488" t="inlineStr"/>
+      <c r="B1488" t="inlineStr">
+        <is>
+          <t>2472</t>
+        </is>
+      </c>
+      <c r="C1488" t="n">
+        <v>140</v>
+      </c>
     </row>
     <row r="1489">
       <c r="A1489" s="1" t="n">
         <v>1487</v>
       </c>
-      <c r="B1489" t="inlineStr"/>
-      <c r="C1489" t="inlineStr"/>
+      <c r="B1489" t="inlineStr">
+        <is>
+          <t>2561</t>
+        </is>
+      </c>
+      <c r="C1489" t="n">
+        <v>140</v>
+      </c>
     </row>
     <row r="1490">
       <c r="A1490" s="1" t="n">
         <v>1488</v>
       </c>
-      <c r="B1490" t="inlineStr"/>
-      <c r="C1490" t="inlineStr"/>
+      <c r="B1490" t="inlineStr">
+        <is>
+          <t>3585</t>
+        </is>
+      </c>
+      <c r="C1490" t="n">
+        <v>140</v>
+      </c>
     </row>
     <row r="1491">
       <c r="A1491" s="1" t="n">
         <v>1489</v>
       </c>
-      <c r="B1491" t="inlineStr"/>
-      <c r="C1491" t="inlineStr"/>
+      <c r="B1491" t="inlineStr">
+        <is>
+          <t>3586</t>
+        </is>
+      </c>
+      <c r="C1491" t="n">
+        <v>140</v>
+      </c>
     </row>
     <row r="1492">
       <c r="A1492" s="1" t="n">
         <v>1490</v>
       </c>
-      <c r="B1492" t="inlineStr"/>
-      <c r="C1492" t="inlineStr"/>
+      <c r="B1492" t="inlineStr">
+        <is>
+          <t>3587</t>
+        </is>
+      </c>
+      <c r="C1492" t="n">
+        <v>140</v>
+      </c>
     </row>
     <row r="1493">
       <c r="A1493" s="1" t="n">
         <v>1491</v>
       </c>
-      <c r="B1493" t="inlineStr"/>
-      <c r="C1493" t="inlineStr"/>
+      <c r="B1493" t="inlineStr">
+        <is>
+          <t>3115/18</t>
+        </is>
+      </c>
+      <c r="C1493" t="n">
+        <v>140</v>
+      </c>
     </row>
     <row r="1494">
       <c r="A1494" s="1" t="n">
         <v>1492</v>
       </c>
-      <c r="B1494" t="inlineStr"/>
-      <c r="C1494" t="inlineStr"/>
+      <c r="B1494" t="inlineStr">
+        <is>
+          <t>3115/21</t>
+        </is>
+      </c>
+      <c r="C1494" t="n">
+        <v>140</v>
+      </c>
     </row>
     <row r="1495">
       <c r="A1495" s="1" t="n">
         <v>1493</v>
       </c>
-      <c r="B1495" t="inlineStr"/>
-      <c r="C1495" t="inlineStr"/>
+      <c r="B1495" t="inlineStr">
+        <is>
+          <t>3148/4</t>
+        </is>
+      </c>
+      <c r="C1495" t="n">
+        <v>140</v>
+      </c>
     </row>
     <row r="1496">
       <c r="A1496" s="1" t="n">
         <v>1494</v>
       </c>
-      <c r="B1496" t="inlineStr"/>
-      <c r="C1496" t="inlineStr"/>
+      <c r="B1496" t="inlineStr">
+        <is>
+          <t>3148/8</t>
+        </is>
+      </c>
+      <c r="C1496" t="n">
+        <v>140</v>
+      </c>
     </row>
     <row r="1497">
       <c r="A1497" s="1" t="n">
         <v>1495</v>
       </c>
-      <c r="B1497" t="inlineStr"/>
-      <c r="C1497" t="inlineStr"/>
+      <c r="B1497" t="inlineStr">
+        <is>
+          <t>759</t>
+        </is>
+      </c>
+      <c r="C1497" t="n">
+        <v>140</v>
+      </c>
     </row>
     <row r="1498">
       <c r="A1498" s="1" t="n">
         <v>1496</v>
       </c>
-      <c r="B1498" t="inlineStr"/>
-      <c r="C1498" t="inlineStr"/>
+      <c r="B1498" t="inlineStr">
+        <is>
+          <t>1408</t>
+        </is>
+      </c>
+      <c r="C1498" t="n">
+        <v>140</v>
+      </c>
     </row>
     <row r="1499">
       <c r="A1499" s="1" t="n">
         <v>1497</v>
       </c>
-      <c r="B1499" t="inlineStr"/>
-      <c r="C1499" t="inlineStr"/>
+      <c r="B1499" t="inlineStr">
+        <is>
+          <t>1411</t>
+        </is>
+      </c>
+      <c r="C1499" t="n">
+        <v>140</v>
+      </c>
     </row>
     <row r="1500">
       <c r="A1500" s="1" t="n">
         <v>1498</v>
       </c>
-      <c r="B1500" t="inlineStr"/>
-      <c r="C1500" t="inlineStr"/>
+      <c r="B1500" t="inlineStr">
+        <is>
+          <t>1413</t>
+        </is>
+      </c>
+      <c r="C1500" t="n">
+        <v>140</v>
+      </c>
     </row>
     <row r="1501">
       <c r="A1501" s="1" t="n">
         <v>1499</v>
       </c>
-      <c r="B1501" t="inlineStr"/>
-      <c r="C1501" t="inlineStr"/>
+      <c r="B1501" t="inlineStr">
+        <is>
+          <t>1419</t>
+        </is>
+      </c>
+      <c r="C1501" t="n">
+        <v>140</v>
+      </c>
     </row>
     <row r="1502">
       <c r="A1502" s="1" t="n">
         <v>1500</v>
       </c>
-      <c r="B1502" t="inlineStr"/>
-      <c r="C1502" t="inlineStr"/>
+      <c r="B1502" t="inlineStr">
+        <is>
+          <t>1420</t>
+        </is>
+      </c>
+      <c r="C1502" t="n">
+        <v>140</v>
+      </c>
     </row>
     <row r="1503">
       <c r="A1503" s="1" t="n">
         <v>1501</v>
       </c>
-      <c r="B1503" t="inlineStr"/>
-      <c r="C1503" t="inlineStr"/>
+      <c r="B1503" t="inlineStr">
+        <is>
+          <t>1421</t>
+        </is>
+      </c>
+      <c r="C1503" t="n">
+        <v>140</v>
+      </c>
     </row>
     <row r="1504">
       <c r="A1504" s="1" t="n">
         <v>1502</v>
       </c>
-      <c r="B1504" t="inlineStr"/>
-      <c r="C1504" t="inlineStr"/>
+      <c r="B1504" t="inlineStr">
+        <is>
+          <t>1499</t>
+        </is>
+      </c>
+      <c r="C1504" t="n">
+        <v>140</v>
+      </c>
     </row>
     <row r="1505">
       <c r="A1505" s="1" t="n">
         <v>1503</v>
       </c>
-      <c r="B1505" t="inlineStr"/>
-      <c r="C1505" t="inlineStr"/>
+      <c r="B1505" t="inlineStr">
+        <is>
+          <t>1502</t>
+        </is>
+      </c>
+      <c r="C1505" t="n">
+        <v>140</v>
+      </c>
     </row>
     <row r="1506">
       <c r="A1506" s="1" t="n">
         <v>1504</v>
       </c>
-      <c r="B1506" t="inlineStr"/>
-      <c r="C1506" t="inlineStr"/>
+      <c r="B1506" t="inlineStr">
+        <is>
+          <t>1348/2</t>
+        </is>
+      </c>
+      <c r="C1506" t="n">
+        <v>140</v>
+      </c>
     </row>
     <row r="1507">
       <c r="A1507" s="1" t="n">
         <v>1505</v>
       </c>
-      <c r="B1507" t="inlineStr"/>
-      <c r="C1507" t="inlineStr"/>
+      <c r="B1507" t="inlineStr">
+        <is>
+          <t>4189</t>
+        </is>
+      </c>
+      <c r="C1507" t="n">
+        <v>140</v>
+      </c>
     </row>
     <row r="1508">
       <c r="A1508" s="1" t="n">
         <v>1506</v>
       </c>
-      <c r="B1508" t="inlineStr"/>
-      <c r="C1508" t="inlineStr"/>
+      <c r="B1508" t="inlineStr">
+        <is>
+          <t>1113</t>
+        </is>
+      </c>
+      <c r="C1508" t="n">
+        <v>440</v>
+      </c>
     </row>
     <row r="1509">
       <c r="A1509" s="1" t="n">
         <v>1507</v>
       </c>
-      <c r="B1509" t="inlineStr"/>
-      <c r="C1509" t="inlineStr"/>
+      <c r="B1509" t="inlineStr">
+        <is>
+          <t>2052</t>
+        </is>
+      </c>
+      <c r="C1509" t="n">
+        <v>440</v>
+      </c>
     </row>
     <row r="1510">
       <c r="A1510" s="1" t="n">
         <v>1508</v>
       </c>
-      <c r="B1510" t="inlineStr"/>
-      <c r="C1510" t="inlineStr"/>
-    </row>
-    <row r="1511">
-      <c r="A1511" s="1" t="n">
-        <v>1509</v>
-      </c>
-      <c r="B1511" t="inlineStr"/>
-      <c r="C1511" t="inlineStr"/>
-    </row>
-    <row r="1512">
-      <c r="A1512" s="1" t="n">
-        <v>1510</v>
-      </c>
-      <c r="B1512" t="inlineStr"/>
-      <c r="C1512" t="inlineStr"/>
-    </row>
-    <row r="1513">
-      <c r="A1513" s="1" t="n">
-        <v>1511</v>
-      </c>
-      <c r="B1513" t="inlineStr"/>
-      <c r="C1513" t="inlineStr"/>
-    </row>
-    <row r="1514">
-      <c r="A1514" s="1" t="n">
-        <v>1512</v>
-      </c>
-      <c r="B1514" t="inlineStr"/>
-      <c r="C1514" t="inlineStr"/>
-    </row>
-    <row r="1515">
-      <c r="A1515" s="1" t="n">
-        <v>1513</v>
-      </c>
-      <c r="B1515" t="inlineStr"/>
-      <c r="C1515" t="inlineStr"/>
-    </row>
-    <row r="1516">
-      <c r="A1516" s="1" t="n">
-        <v>1514</v>
-      </c>
-      <c r="B1516" t="inlineStr"/>
-      <c r="C1516" t="inlineStr"/>
-    </row>
-    <row r="1517">
-      <c r="A1517" s="1" t="n">
-        <v>1515</v>
-      </c>
-      <c r="B1517" t="inlineStr"/>
-      <c r="C1517" t="inlineStr"/>
-    </row>
-    <row r="1518">
-      <c r="A1518" s="1" t="n">
-        <v>1516</v>
-      </c>
-      <c r="B1518" t="inlineStr"/>
-      <c r="C1518" t="inlineStr"/>
-    </row>
-    <row r="1519">
-      <c r="A1519" s="1" t="n">
-        <v>1517</v>
-      </c>
-      <c r="B1519" t="inlineStr"/>
-      <c r="C1519" t="inlineStr"/>
-    </row>
-    <row r="1520">
-      <c r="A1520" s="1" t="n">
-        <v>1518</v>
-      </c>
-      <c r="B1520" t="inlineStr"/>
-      <c r="C1520" t="inlineStr"/>
-    </row>
-    <row r="1521">
-      <c r="A1521" s="1" t="n">
-        <v>1519</v>
-      </c>
-      <c r="B1521" t="inlineStr"/>
-      <c r="C1521" t="inlineStr"/>
-    </row>
-    <row r="1522">
-      <c r="A1522" s="1" t="n">
-        <v>1520</v>
-      </c>
-      <c r="B1522" t="inlineStr"/>
-      <c r="C1522" t="inlineStr"/>
-    </row>
-    <row r="1523">
-      <c r="A1523" s="1" t="n">
-        <v>1521</v>
-      </c>
-      <c r="B1523" t="inlineStr"/>
-      <c r="C1523" t="inlineStr"/>
-    </row>
-    <row r="1524">
-      <c r="A1524" s="1" t="n">
-        <v>1522</v>
-      </c>
-      <c r="B1524" t="inlineStr"/>
-      <c r="C1524" t="inlineStr"/>
-    </row>
-    <row r="1525">
-      <c r="A1525" s="1" t="n">
-        <v>1523</v>
-      </c>
-      <c r="B1525" t="inlineStr"/>
-      <c r="C1525" t="inlineStr"/>
-    </row>
-    <row r="1526">
-      <c r="A1526" s="1" t="n">
-        <v>1524</v>
-      </c>
-      <c r="B1526" t="inlineStr"/>
-      <c r="C1526" t="inlineStr"/>
-    </row>
-    <row r="1527">
-      <c r="A1527" s="1" t="n">
-        <v>1525</v>
-      </c>
-      <c r="B1527" t="inlineStr"/>
-      <c r="C1527" t="inlineStr"/>
-    </row>
-    <row r="1528">
-      <c r="A1528" s="1" t="n">
-        <v>1526</v>
-      </c>
-      <c r="B1528" t="inlineStr"/>
-      <c r="C1528" t="inlineStr"/>
-    </row>
-    <row r="1529">
-      <c r="A1529" s="1" t="n">
-        <v>1527</v>
-      </c>
-      <c r="B1529" t="inlineStr"/>
-      <c r="C1529" t="inlineStr"/>
-    </row>
-    <row r="1530">
-      <c r="A1530" s="1" t="n">
-        <v>1528</v>
-      </c>
-      <c r="B1530" t="inlineStr"/>
-      <c r="C1530" t="inlineStr"/>
-    </row>
-    <row r="1531">
-      <c r="A1531" s="1" t="n">
-        <v>1529</v>
-      </c>
-      <c r="B1531" t="inlineStr"/>
-      <c r="C1531" t="inlineStr"/>
-    </row>
-    <row r="1532">
-      <c r="A1532" s="1" t="n">
-        <v>1530</v>
-      </c>
-      <c r="B1532" t="inlineStr"/>
-      <c r="C1532" t="inlineStr"/>
-    </row>
-    <row r="1533">
-      <c r="A1533" s="1" t="n">
-        <v>1531</v>
-      </c>
-      <c r="B1533" t="inlineStr"/>
-      <c r="C1533" t="inlineStr"/>
-    </row>
-    <row r="1534">
-      <c r="A1534" s="1" t="n">
-        <v>1532</v>
-      </c>
-      <c r="B1534" t="inlineStr"/>
-      <c r="C1534" t="inlineStr"/>
-    </row>
-    <row r="1535">
-      <c r="A1535" s="1" t="n">
-        <v>1533</v>
-      </c>
-      <c r="B1535" t="inlineStr"/>
-      <c r="C1535" t="inlineStr"/>
-    </row>
-    <row r="1536">
-      <c r="A1536" s="1" t="n">
-        <v>1534</v>
-      </c>
-      <c r="B1536" t="inlineStr"/>
-      <c r="C1536" t="inlineStr"/>
-    </row>
-    <row r="1537">
-      <c r="A1537" s="1" t="n">
-        <v>1535</v>
-      </c>
-      <c r="B1537" t="inlineStr"/>
-      <c r="C1537" t="inlineStr"/>
-    </row>
-    <row r="1538">
-      <c r="A1538" s="1" t="n">
-        <v>1536</v>
-      </c>
-      <c r="B1538" t="inlineStr"/>
-      <c r="C1538" t="inlineStr"/>
-    </row>
-    <row r="1539">
-      <c r="A1539" s="1" t="n">
-        <v>1537</v>
-      </c>
-      <c r="B1539" t="inlineStr"/>
-      <c r="C1539" t="inlineStr"/>
-    </row>
-    <row r="1540">
-      <c r="A1540" s="1" t="n">
-        <v>1538</v>
-      </c>
-      <c r="B1540" t="inlineStr"/>
-      <c r="C1540" t="inlineStr"/>
-    </row>
-    <row r="1541">
-      <c r="A1541" s="1" t="n">
-        <v>1539</v>
-      </c>
-      <c r="B1541" t="inlineStr"/>
-      <c r="C1541" t="inlineStr"/>
-    </row>
-    <row r="1542">
-      <c r="A1542" s="1" t="n">
-        <v>1540</v>
-      </c>
-      <c r="B1542" t="inlineStr"/>
-      <c r="C1542" t="inlineStr"/>
-    </row>
-    <row r="1543">
-      <c r="A1543" s="1" t="n">
-        <v>1541</v>
-      </c>
-      <c r="B1543" t="inlineStr"/>
-      <c r="C1543" t="inlineStr"/>
-    </row>
-    <row r="1544">
-      <c r="A1544" s="1" t="n">
-        <v>1542</v>
-      </c>
-      <c r="B1544" t="inlineStr"/>
-      <c r="C1544" t="inlineStr"/>
-    </row>
-    <row r="1545">
-      <c r="A1545" s="1" t="n">
-        <v>1543</v>
-      </c>
-      <c r="B1545" t="inlineStr"/>
-      <c r="C1545" t="inlineStr"/>
-    </row>
-    <row r="1546">
-      <c r="A1546" s="1" t="n">
-        <v>1544</v>
-      </c>
-      <c r="B1546" t="inlineStr"/>
-      <c r="C1546" t="inlineStr"/>
-    </row>
-    <row r="1547">
-      <c r="A1547" s="1" t="n">
-        <v>1545</v>
-      </c>
-      <c r="B1547" t="inlineStr"/>
-      <c r="C1547" t="inlineStr"/>
-    </row>
-    <row r="1548">
-      <c r="A1548" s="1" t="n">
-        <v>1546</v>
-      </c>
-      <c r="B1548" t="inlineStr"/>
-      <c r="C1548" t="inlineStr"/>
-    </row>
-    <row r="1549">
-      <c r="A1549" s="1" t="n">
-        <v>1547</v>
-      </c>
-      <c r="B1549" t="inlineStr"/>
-      <c r="C1549" t="inlineStr"/>
-    </row>
-    <row r="1550">
-      <c r="A1550" s="1" t="n">
-        <v>1548</v>
-      </c>
-      <c r="B1550" t="inlineStr"/>
-      <c r="C1550" t="inlineStr"/>
-    </row>
-    <row r="1551">
-      <c r="A1551" s="1" t="n">
-        <v>1549</v>
-      </c>
-      <c r="B1551" t="inlineStr"/>
-      <c r="C1551" t="inlineStr"/>
-    </row>
-    <row r="1552">
-      <c r="A1552" s="1" t="n">
-        <v>1550</v>
-      </c>
-      <c r="B1552" t="inlineStr"/>
-      <c r="C1552" t="inlineStr"/>
-    </row>
-    <row r="1553">
-      <c r="A1553" s="1" t="n">
-        <v>1551</v>
-      </c>
-      <c r="B1553" t="inlineStr"/>
-      <c r="C1553" t="inlineStr"/>
-    </row>
-    <row r="1554">
-      <c r="A1554" s="1" t="n">
-        <v>1552</v>
-      </c>
-      <c r="B1554" t="inlineStr"/>
-      <c r="C1554" t="inlineStr"/>
-    </row>
-    <row r="1555">
-      <c r="A1555" s="1" t="n">
-        <v>1553</v>
-      </c>
-      <c r="B1555" t="inlineStr"/>
-      <c r="C1555" t="inlineStr"/>
-    </row>
-    <row r="1556">
-      <c r="A1556" s="1" t="n">
-        <v>1554</v>
-      </c>
-      <c r="B1556" t="inlineStr"/>
-      <c r="C1556" t="inlineStr"/>
-    </row>
-    <row r="1557">
-      <c r="A1557" s="1" t="n">
-        <v>1555</v>
-      </c>
-      <c r="B1557" t="inlineStr"/>
-      <c r="C1557" t="inlineStr"/>
-    </row>
-    <row r="1558">
-      <c r="A1558" s="1" t="n">
-        <v>1556</v>
-      </c>
-      <c r="B1558" t="inlineStr"/>
-      <c r="C1558" t="inlineStr"/>
-    </row>
-    <row r="1559">
-      <c r="A1559" s="1" t="n">
-        <v>1557</v>
-      </c>
-      <c r="B1559" t="inlineStr"/>
-      <c r="C1559" t="inlineStr"/>
-    </row>
-    <row r="1560">
-      <c r="A1560" s="1" t="n">
-        <v>1558</v>
-      </c>
-      <c r="B1560" t="inlineStr"/>
-      <c r="C1560" t="inlineStr"/>
-    </row>
-    <row r="1561">
-      <c r="A1561" s="1" t="n">
-        <v>1559</v>
-      </c>
-      <c r="B1561" t="inlineStr"/>
-      <c r="C1561" t="inlineStr"/>
-    </row>
-    <row r="1562">
-      <c r="A1562" s="1" t="n">
-        <v>1560</v>
-      </c>
-      <c r="B1562" t="inlineStr"/>
-      <c r="C1562" t="inlineStr"/>
-    </row>
-    <row r="1563">
-      <c r="A1563" s="1" t="n">
-        <v>1561</v>
-      </c>
-      <c r="B1563" t="inlineStr"/>
-      <c r="C1563" t="inlineStr"/>
-    </row>
-    <row r="1564">
-      <c r="A1564" s="1" t="n">
-        <v>1562</v>
-      </c>
-      <c r="B1564" t="inlineStr"/>
-      <c r="C1564" t="inlineStr"/>
-    </row>
-    <row r="1565">
-      <c r="A1565" s="1" t="n">
-        <v>1563</v>
-      </c>
-      <c r="B1565" t="inlineStr"/>
-      <c r="C1565" t="inlineStr"/>
-    </row>
-    <row r="1566">
-      <c r="A1566" s="1" t="n">
-        <v>1564</v>
-      </c>
-      <c r="B1566" t="inlineStr"/>
-      <c r="C1566" t="inlineStr"/>
-    </row>
-    <row r="1567">
-      <c r="A1567" s="1" t="n">
-        <v>1565</v>
-      </c>
-      <c r="B1567" t="inlineStr"/>
-      <c r="C1567" t="inlineStr"/>
-    </row>
-    <row r="1568">
-      <c r="A1568" s="1" t="n">
-        <v>1566</v>
-      </c>
-      <c r="B1568" t="inlineStr"/>
-      <c r="C1568" t="inlineStr"/>
-    </row>
-    <row r="1569">
-      <c r="A1569" s="1" t="n">
-        <v>1567</v>
-      </c>
-      <c r="B1569" t="inlineStr"/>
-      <c r="C1569" t="inlineStr"/>
-    </row>
-    <row r="1570">
-      <c r="A1570" s="1" t="n">
-        <v>1568</v>
-      </c>
-      <c r="B1570" t="inlineStr"/>
-      <c r="C1570" t="inlineStr"/>
-    </row>
-    <row r="1571">
-      <c r="A1571" s="1" t="n">
-        <v>1569</v>
-      </c>
-      <c r="B1571" t="inlineStr"/>
-      <c r="C1571" t="inlineStr"/>
-    </row>
-    <row r="1572">
-      <c r="A1572" s="1" t="n">
-        <v>1570</v>
-      </c>
-      <c r="B1572" t="inlineStr"/>
-      <c r="C1572" t="inlineStr"/>
-    </row>
-    <row r="1573">
-      <c r="A1573" s="1" t="n">
-        <v>1571</v>
-      </c>
-      <c r="B1573" t="inlineStr"/>
-      <c r="C1573" t="inlineStr"/>
-    </row>
-    <row r="1574">
-      <c r="A1574" s="1" t="n">
-        <v>1572</v>
-      </c>
-      <c r="B1574" t="inlineStr"/>
-      <c r="C1574" t="inlineStr"/>
-    </row>
-    <row r="1575">
-      <c r="A1575" s="1" t="n">
-        <v>1573</v>
-      </c>
-      <c r="B1575" t="inlineStr"/>
-      <c r="C1575" t="inlineStr"/>
-    </row>
-    <row r="1576">
-      <c r="A1576" s="1" t="n">
-        <v>1574</v>
-      </c>
-      <c r="B1576" t="inlineStr"/>
-      <c r="C1576" t="inlineStr"/>
-    </row>
-    <row r="1577">
-      <c r="A1577" s="1" t="n">
-        <v>1575</v>
-      </c>
-      <c r="B1577" t="inlineStr"/>
-      <c r="C1577" t="inlineStr"/>
-    </row>
-    <row r="1578">
-      <c r="A1578" s="1" t="n">
-        <v>1576</v>
-      </c>
-      <c r="B1578" t="inlineStr"/>
-      <c r="C1578" t="inlineStr"/>
-    </row>
-    <row r="1579">
-      <c r="A1579" s="1" t="n">
-        <v>1577</v>
-      </c>
-      <c r="B1579" t="inlineStr"/>
-      <c r="C1579" t="inlineStr"/>
-    </row>
-    <row r="1580">
-      <c r="A1580" s="1" t="n">
-        <v>1578</v>
-      </c>
-      <c r="B1580" t="inlineStr"/>
-      <c r="C1580" t="inlineStr"/>
-    </row>
-    <row r="1581">
-      <c r="A1581" s="1" t="n">
-        <v>1579</v>
-      </c>
-      <c r="B1581" t="inlineStr"/>
-      <c r="C1581" t="inlineStr"/>
-    </row>
-    <row r="1582">
-      <c r="A1582" s="1" t="n">
-        <v>1580</v>
-      </c>
-      <c r="B1582" t="inlineStr"/>
-      <c r="C1582" t="inlineStr"/>
-    </row>
-    <row r="1583">
-      <c r="A1583" s="1" t="n">
-        <v>1581</v>
-      </c>
-      <c r="B1583" t="inlineStr"/>
-      <c r="C1583" t="inlineStr"/>
-    </row>
-    <row r="1584">
-      <c r="A1584" s="1" t="n">
-        <v>1582</v>
-      </c>
-      <c r="B1584" t="inlineStr"/>
-      <c r="C1584" t="inlineStr"/>
-    </row>
-    <row r="1585">
-      <c r="A1585" s="1" t="n">
-        <v>1583</v>
-      </c>
-      <c r="B1585" t="inlineStr"/>
-      <c r="C1585" t="inlineStr"/>
-    </row>
-    <row r="1586">
-      <c r="A1586" s="1" t="n">
-        <v>1584</v>
-      </c>
-      <c r="B1586" t="inlineStr"/>
-      <c r="C1586" t="inlineStr"/>
-    </row>
-    <row r="1587">
-      <c r="A1587" s="1" t="n">
-        <v>1585</v>
-      </c>
-      <c r="B1587" t="inlineStr"/>
-      <c r="C1587" t="inlineStr"/>
-    </row>
-    <row r="1588">
-      <c r="A1588" s="1" t="n">
-        <v>1586</v>
-      </c>
-      <c r="B1588" t="inlineStr"/>
-      <c r="C1588" t="inlineStr"/>
-    </row>
-    <row r="1589">
-      <c r="A1589" s="1" t="n">
-        <v>1587</v>
-      </c>
-      <c r="B1589" t="inlineStr"/>
-      <c r="C1589" t="inlineStr"/>
-    </row>
-    <row r="1590">
-      <c r="A1590" s="1" t="n">
-        <v>1588</v>
-      </c>
-      <c r="B1590" t="inlineStr"/>
-      <c r="C1590" t="inlineStr"/>
-    </row>
-    <row r="1591">
-      <c r="A1591" s="1" t="n">
-        <v>1589</v>
-      </c>
-      <c r="B1591" t="inlineStr"/>
-      <c r="C1591" t="inlineStr"/>
-    </row>
-    <row r="1592">
-      <c r="A1592" s="1" t="n">
-        <v>1590</v>
-      </c>
-      <c r="B1592" t="inlineStr"/>
-      <c r="C1592" t="inlineStr"/>
-    </row>
-    <row r="1593">
-      <c r="A1593" s="1" t="n">
-        <v>1591</v>
-      </c>
-      <c r="B1593" t="inlineStr"/>
-      <c r="C1593" t="inlineStr"/>
-    </row>
-    <row r="1594">
-      <c r="A1594" s="1" t="n">
-        <v>1592</v>
-      </c>
-      <c r="B1594" t="inlineStr"/>
-      <c r="C1594" t="inlineStr"/>
-    </row>
-    <row r="1595">
-      <c r="A1595" s="1" t="n">
-        <v>1593</v>
-      </c>
-      <c r="B1595" t="inlineStr"/>
-      <c r="C1595" t="inlineStr"/>
-    </row>
-    <row r="1596">
-      <c r="A1596" s="1" t="n">
-        <v>1594</v>
-      </c>
-      <c r="B1596" t="inlineStr"/>
-      <c r="C1596" t="inlineStr"/>
-    </row>
-    <row r="1597">
-      <c r="A1597" s="1" t="n">
-        <v>1595</v>
-      </c>
-      <c r="B1597" t="inlineStr"/>
-      <c r="C1597" t="inlineStr"/>
-    </row>
-    <row r="1598">
-      <c r="A1598" s="1" t="n">
-        <v>1596</v>
-      </c>
-      <c r="B1598" t="inlineStr"/>
-      <c r="C1598" t="inlineStr"/>
-    </row>
-    <row r="1599">
-      <c r="A1599" s="1" t="n">
-        <v>1597</v>
-      </c>
-      <c r="B1599" t="inlineStr"/>
-      <c r="C1599" t="inlineStr"/>
-    </row>
-    <row r="1600">
-      <c r="A1600" s="1" t="n">
-        <v>1598</v>
-      </c>
-      <c r="B1600" t="inlineStr"/>
-      <c r="C1600" t="inlineStr"/>
-    </row>
-    <row r="1601">
-      <c r="A1601" s="1" t="n">
-        <v>1599</v>
-      </c>
-      <c r="B1601" t="inlineStr"/>
-      <c r="C1601" t="inlineStr"/>
-    </row>
-    <row r="1602">
-      <c r="A1602" s="1" t="n">
-        <v>1600</v>
-      </c>
-      <c r="B1602" t="inlineStr"/>
-      <c r="C1602" t="inlineStr"/>
-    </row>
-    <row r="1603">
-      <c r="A1603" s="1" t="n">
-        <v>1601</v>
-      </c>
-      <c r="B1603" t="inlineStr"/>
-      <c r="C1603" t="inlineStr"/>
-    </row>
-    <row r="1604">
-      <c r="A1604" s="1" t="n">
-        <v>1602</v>
-      </c>
-      <c r="B1604" t="inlineStr"/>
-      <c r="C1604" t="inlineStr"/>
-    </row>
-    <row r="1605">
-      <c r="A1605" s="1" t="n">
-        <v>1603</v>
-      </c>
-      <c r="B1605" t="inlineStr"/>
-      <c r="C1605" t="inlineStr"/>
-    </row>
-    <row r="1606">
-      <c r="A1606" s="1" t="n">
-        <v>1604</v>
-      </c>
-      <c r="B1606" t="inlineStr"/>
-      <c r="C1606" t="inlineStr"/>
-    </row>
-    <row r="1607">
-      <c r="A1607" s="1" t="n">
-        <v>1605</v>
-      </c>
-      <c r="B1607" t="inlineStr"/>
-      <c r="C1607" t="inlineStr"/>
-    </row>
-    <row r="1608">
-      <c r="A1608" s="1" t="n">
-        <v>1606</v>
-      </c>
-      <c r="B1608" t="inlineStr"/>
-      <c r="C1608" t="inlineStr"/>
-    </row>
-    <row r="1609">
-      <c r="A1609" s="1" t="n">
-        <v>1607</v>
-      </c>
-      <c r="B1609" t="inlineStr"/>
-      <c r="C1609" t="inlineStr"/>
-    </row>
-    <row r="1610">
-      <c r="A1610" s="1" t="n">
-        <v>1608</v>
-      </c>
-      <c r="B1610" t="inlineStr"/>
-      <c r="C1610" t="inlineStr"/>
-    </row>
-    <row r="1611">
-      <c r="A1611" s="1" t="n">
-        <v>1609</v>
-      </c>
-      <c r="B1611" t="inlineStr"/>
-      <c r="C1611" t="inlineStr"/>
-    </row>
-    <row r="1612">
-      <c r="A1612" s="1" t="n">
-        <v>1610</v>
-      </c>
-      <c r="B1612" t="inlineStr"/>
-      <c r="C1612" t="inlineStr"/>
-    </row>
-    <row r="1613">
-      <c r="A1613" s="1" t="n">
-        <v>1611</v>
-      </c>
-      <c r="B1613" t="inlineStr">
-        <is>
-          <t>1146</t>
-        </is>
-      </c>
-      <c r="C1613" t="n">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="1614">
-      <c r="A1614" s="1" t="n">
-        <v>1612</v>
-      </c>
-      <c r="B1614" t="inlineStr">
-        <is>
-          <t>719</t>
-        </is>
-      </c>
-      <c r="C1614" t="n">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="1615">
-      <c r="A1615" s="1" t="n">
-        <v>1613</v>
-      </c>
-      <c r="B1615" t="inlineStr">
-        <is>
-          <t>857/2</t>
-        </is>
-      </c>
-      <c r="C1615" t="n">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="1616">
-      <c r="A1616" s="1" t="n">
-        <v>1614</v>
-      </c>
-      <c r="B1616" t="inlineStr">
-        <is>
-          <t>859/2</t>
-        </is>
-      </c>
-      <c r="C1616" t="n">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="1617">
-      <c r="A1617" s="1" t="n">
-        <v>1615</v>
-      </c>
-      <c r="B1617" t="inlineStr">
-        <is>
-          <t>1058/2</t>
-        </is>
-      </c>
-      <c r="C1617" t="n">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="1618">
-      <c r="A1618" s="1" t="n">
-        <v>1616</v>
-      </c>
-      <c r="B1618" t="inlineStr">
-        <is>
-          <t>1064/3</t>
-        </is>
-      </c>
-      <c r="C1618" t="n">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="1619">
-      <c r="A1619" s="1" t="n">
-        <v>1617</v>
-      </c>
-      <c r="B1619" t="inlineStr">
-        <is>
-          <t>1491</t>
-        </is>
-      </c>
-      <c r="C1619" t="n">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="1620">
-      <c r="A1620" s="1" t="n">
-        <v>1618</v>
-      </c>
-      <c r="B1620" t="inlineStr">
-        <is>
-          <t>1583</t>
-        </is>
-      </c>
-      <c r="C1620" t="n">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="1621">
-      <c r="A1621" s="1" t="n">
-        <v>1619</v>
-      </c>
-      <c r="B1621" t="inlineStr">
-        <is>
-          <t>1584</t>
-        </is>
-      </c>
-      <c r="C1621" t="n">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="1622">
-      <c r="A1622" s="1" t="n">
-        <v>1620</v>
-      </c>
-      <c r="B1622" t="inlineStr">
-        <is>
-          <t>1517</t>
-        </is>
-      </c>
-      <c r="C1622" t="n">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="1623">
-      <c r="A1623" s="1" t="n">
-        <v>1621</v>
-      </c>
-      <c r="B1623" t="inlineStr">
-        <is>
-          <t>71/2</t>
-        </is>
-      </c>
-      <c r="C1623" t="n">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="1624">
-      <c r="A1624" s="1" t="n">
-        <v>1622</v>
-      </c>
-      <c r="B1624" t="inlineStr">
-        <is>
-          <t>71/2</t>
-        </is>
-      </c>
-      <c r="C1624" t="n">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="1625">
-      <c r="A1625" s="1" t="n">
-        <v>1623</v>
-      </c>
-      <c r="B1625" t="inlineStr">
-        <is>
-          <t>91</t>
-        </is>
-      </c>
-      <c r="C1625" t="n">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="1626">
-      <c r="A1626" s="1" t="n">
-        <v>1624</v>
-      </c>
-      <c r="B1626" t="inlineStr">
-        <is>
-          <t>1871</t>
-        </is>
-      </c>
-      <c r="C1626" t="n">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="1627">
-      <c r="A1627" s="1" t="n">
-        <v>1625</v>
-      </c>
-      <c r="B1627" t="inlineStr">
-        <is>
-          <t>3798</t>
-        </is>
-      </c>
-      <c r="C1627" t="n">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="1628">
-      <c r="A1628" s="1" t="n">
-        <v>1626</v>
-      </c>
-      <c r="B1628" t="inlineStr">
-        <is>
-          <t>353</t>
-        </is>
-      </c>
-      <c r="C1628" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="1629">
-      <c r="A1629" s="1" t="n">
-        <v>1627</v>
-      </c>
-      <c r="B1629" t="inlineStr">
-        <is>
-          <t>236/2</t>
-        </is>
-      </c>
-      <c r="C1629" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="1630">
-      <c r="A1630" s="1" t="n">
-        <v>1628</v>
-      </c>
-      <c r="B1630" t="inlineStr">
-        <is>
-          <t>236/3</t>
-        </is>
-      </c>
-      <c r="C1630" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="1631">
-      <c r="A1631" s="1" t="n">
-        <v>1629</v>
-      </c>
-      <c r="B1631" t="inlineStr">
-        <is>
-          <t>68/4</t>
-        </is>
-      </c>
-      <c r="C1631" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="1632">
-      <c r="A1632" s="1" t="n">
-        <v>1630</v>
-      </c>
-      <c r="B1632" t="inlineStr">
-        <is>
-          <t>455/1</t>
-        </is>
-      </c>
-      <c r="C1632" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="1633">
-      <c r="A1633" s="1" t="n">
-        <v>1631</v>
-      </c>
-      <c r="B1633" t="inlineStr">
-        <is>
-          <t>929</t>
-        </is>
-      </c>
-      <c r="C1633" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="1634">
-      <c r="A1634" s="1" t="n">
-        <v>1632</v>
-      </c>
-      <c r="B1634" t="inlineStr">
-        <is>
-          <t>933</t>
-        </is>
-      </c>
-      <c r="C1634" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="1635">
-      <c r="A1635" s="1" t="n">
-        <v>1633</v>
-      </c>
-      <c r="B1635" t="inlineStr">
-        <is>
-          <t>934</t>
-        </is>
-      </c>
-      <c r="C1635" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="1636">
-      <c r="A1636" s="1" t="n">
-        <v>1634</v>
-      </c>
-      <c r="B1636" t="inlineStr">
-        <is>
-          <t>935/1</t>
-        </is>
-      </c>
-      <c r="C1636" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="1637">
-      <c r="A1637" s="1" t="n">
-        <v>1635</v>
-      </c>
-      <c r="B1637" t="inlineStr">
-        <is>
-          <t>1022/1</t>
-        </is>
-      </c>
-      <c r="C1637" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="1638">
-      <c r="A1638" s="1" t="n">
-        <v>1636</v>
-      </c>
-      <c r="B1638" t="inlineStr">
-        <is>
-          <t>1030/1</t>
-        </is>
-      </c>
-      <c r="C1638" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="1639">
-      <c r="A1639" s="1" t="n">
-        <v>1637</v>
-      </c>
-      <c r="B1639" t="inlineStr">
-        <is>
-          <t>1037/1</t>
-        </is>
-      </c>
-      <c r="C1639" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="1640">
-      <c r="A1640" s="1" t="n">
-        <v>1638</v>
-      </c>
-      <c r="B1640" t="inlineStr">
-        <is>
-          <t>1038</t>
-        </is>
-      </c>
-      <c r="C1640" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="1641">
-      <c r="A1641" s="1" t="n">
-        <v>1639</v>
-      </c>
-      <c r="B1641" t="inlineStr">
-        <is>
-          <t>1042</t>
-        </is>
-      </c>
-      <c r="C1641" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="1642">
-      <c r="A1642" s="1" t="n">
-        <v>1640</v>
-      </c>
-      <c r="B1642" t="inlineStr">
-        <is>
-          <t>1043/1</t>
-        </is>
-      </c>
-      <c r="C1642" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="1643">
-      <c r="A1643" s="1" t="n">
-        <v>1641</v>
-      </c>
-      <c r="B1643" t="inlineStr">
-        <is>
-          <t>1071</t>
-        </is>
-      </c>
-      <c r="C1643" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="1644">
-      <c r="A1644" s="1" t="n">
-        <v>1642</v>
-      </c>
-      <c r="B1644" t="inlineStr">
-        <is>
-          <t>1093</t>
-        </is>
-      </c>
-      <c r="C1644" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="1645">
-      <c r="A1645" s="1" t="n">
-        <v>1643</v>
-      </c>
-      <c r="B1645" t="inlineStr">
-        <is>
-          <t>923</t>
-        </is>
-      </c>
-      <c r="C1645" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="1646">
-      <c r="A1646" s="1" t="n">
-        <v>1644</v>
-      </c>
-      <c r="B1646" t="inlineStr">
-        <is>
-          <t>673/2</t>
-        </is>
-      </c>
-      <c r="C1646" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="1647">
-      <c r="A1647" s="1" t="n">
-        <v>1645</v>
-      </c>
-      <c r="B1647" t="inlineStr">
-        <is>
-          <t>209</t>
-        </is>
-      </c>
-      <c r="C1647" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="1648">
-      <c r="A1648" s="1" t="n">
-        <v>1646</v>
-      </c>
-      <c r="B1648" t="inlineStr">
-        <is>
-          <t>870</t>
-        </is>
-      </c>
-      <c r="C1648" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="1649">
-      <c r="A1649" s="1" t="n">
-        <v>1647</v>
-      </c>
-      <c r="B1649" t="inlineStr">
-        <is>
-          <t>877</t>
-        </is>
-      </c>
-      <c r="C1649" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="1650">
-      <c r="A1650" s="1" t="n">
-        <v>1648</v>
-      </c>
-      <c r="B1650" t="inlineStr">
-        <is>
-          <t>878</t>
-        </is>
-      </c>
-      <c r="C1650" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="1651">
-      <c r="A1651" s="1" t="n">
-        <v>1649</v>
-      </c>
-      <c r="B1651" t="inlineStr">
-        <is>
-          <t>884</t>
-        </is>
-      </c>
-      <c r="C1651" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="1652">
-      <c r="A1652" s="1" t="n">
-        <v>1650</v>
-      </c>
-      <c r="B1652" t="inlineStr">
-        <is>
-          <t>3596</t>
-        </is>
-      </c>
-      <c r="C1652" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="1653">
-      <c r="A1653" s="1" t="n">
-        <v>1651</v>
-      </c>
-      <c r="B1653" t="inlineStr">
-        <is>
-          <t>251</t>
-        </is>
-      </c>
-      <c r="C1653" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="1654">
-      <c r="A1654" s="1" t="n">
-        <v>1652</v>
-      </c>
-      <c r="B1654" t="inlineStr">
-        <is>
-          <t>605</t>
-        </is>
-      </c>
-      <c r="C1654" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="1655">
-      <c r="A1655" s="1" t="n">
-        <v>1653</v>
-      </c>
-      <c r="B1655" t="inlineStr">
-        <is>
-          <t>2074</t>
-        </is>
-      </c>
-      <c r="C1655" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="1656">
-      <c r="A1656" s="1" t="n">
-        <v>1654</v>
-      </c>
-      <c r="B1656" t="inlineStr">
-        <is>
-          <t>406/3</t>
-        </is>
-      </c>
-      <c r="C1656" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="1657">
-      <c r="A1657" s="1" t="n">
-        <v>1655</v>
-      </c>
-      <c r="B1657" t="inlineStr">
-        <is>
-          <t>674</t>
-        </is>
-      </c>
-      <c r="C1657" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="1658">
-      <c r="A1658" s="1" t="n">
-        <v>1656</v>
-      </c>
-      <c r="B1658" t="inlineStr">
-        <is>
-          <t>938</t>
-        </is>
-      </c>
-      <c r="C1658" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="1659">
-      <c r="A1659" s="1" t="n">
-        <v>1657</v>
-      </c>
-      <c r="B1659" t="inlineStr">
-        <is>
-          <t>996</t>
-        </is>
-      </c>
-      <c r="C1659" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="1660">
-      <c r="A1660" s="1" t="n">
-        <v>1658</v>
-      </c>
-      <c r="B1660" t="inlineStr">
-        <is>
-          <t>657/1</t>
-        </is>
-      </c>
-      <c r="C1660" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="1661">
-      <c r="A1661" s="1" t="n">
-        <v>1659</v>
-      </c>
-      <c r="B1661" t="inlineStr">
-        <is>
-          <t>765/3</t>
-        </is>
-      </c>
-      <c r="C1661" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="1662">
-      <c r="A1662" s="1" t="n">
-        <v>1660</v>
-      </c>
-      <c r="B1662" t="inlineStr">
-        <is>
-          <t>2050</t>
-        </is>
-      </c>
-      <c r="C1662" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="1663">
-      <c r="A1663" s="1" t="n">
-        <v>1661</v>
-      </c>
-      <c r="B1663" t="inlineStr">
-        <is>
-          <t>2065</t>
-        </is>
-      </c>
-      <c r="C1663" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="1664">
-      <c r="A1664" s="1" t="n">
-        <v>1662</v>
-      </c>
-      <c r="B1664" t="inlineStr">
-        <is>
-          <t>2066</t>
-        </is>
-      </c>
-      <c r="C1664" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="1665">
-      <c r="A1665" s="1" t="n">
-        <v>1663</v>
-      </c>
-      <c r="B1665" t="inlineStr">
-        <is>
-          <t>2153</t>
-        </is>
-      </c>
-      <c r="C1665" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="1666">
-      <c r="A1666" s="1" t="n">
-        <v>1664</v>
-      </c>
-      <c r="B1666" t="inlineStr">
-        <is>
-          <t>2154</t>
-        </is>
-      </c>
-      <c r="C1666" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="1667">
-      <c r="A1667" s="1" t="n">
-        <v>1665</v>
-      </c>
-      <c r="B1667" t="inlineStr">
-        <is>
-          <t>673/2</t>
-        </is>
-      </c>
-      <c r="C1667" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="1668">
-      <c r="A1668" s="1" t="n">
-        <v>1666</v>
-      </c>
-      <c r="B1668" t="inlineStr">
-        <is>
-          <t>808</t>
-        </is>
-      </c>
-      <c r="C1668" t="n">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="1669">
-      <c r="A1669" s="1" t="n">
-        <v>1667</v>
-      </c>
-      <c r="B1669" t="inlineStr">
-        <is>
-          <t>1419</t>
-        </is>
-      </c>
-      <c r="C1669" t="n">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="1670">
-      <c r="A1670" s="1" t="n">
-        <v>1668</v>
-      </c>
-      <c r="B1670" t="inlineStr">
-        <is>
-          <t>1420</t>
-        </is>
-      </c>
-      <c r="C1670" t="n">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="1671">
-      <c r="A1671" s="1" t="n">
-        <v>1669</v>
-      </c>
-      <c r="B1671" t="inlineStr">
-        <is>
-          <t>1421</t>
-        </is>
-      </c>
-      <c r="C1671" t="n">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="1672">
-      <c r="A1672" s="1" t="n">
-        <v>1670</v>
-      </c>
-      <c r="B1672" t="inlineStr">
-        <is>
-          <t>1430</t>
-        </is>
-      </c>
-      <c r="C1672" t="n">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="1673">
-      <c r="A1673" s="1" t="n">
-        <v>1671</v>
-      </c>
-      <c r="B1673" t="inlineStr">
-        <is>
-          <t>1431/1</t>
-        </is>
-      </c>
-      <c r="C1673" t="n">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="1674">
-      <c r="A1674" s="1" t="n">
-        <v>1672</v>
-      </c>
-      <c r="B1674" t="inlineStr">
-        <is>
-          <t>1431/34</t>
-        </is>
-      </c>
-      <c r="C1674" t="n">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="1675">
-      <c r="A1675" s="1" t="n">
-        <v>1673</v>
-      </c>
-      <c r="B1675" t="inlineStr">
-        <is>
-          <t>.950/1</t>
-        </is>
-      </c>
-      <c r="C1675" t="n">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="1676">
-      <c r="A1676" s="1" t="n">
-        <v>1674</v>
-      </c>
-      <c r="B1676" t="inlineStr">
-        <is>
-          <t>.950/2</t>
-        </is>
-      </c>
-      <c r="C1676" t="n">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="1677">
-      <c r="A1677" s="1" t="n">
-        <v>1675</v>
-      </c>
-      <c r="B1677" t="inlineStr">
-        <is>
-          <t>239</t>
-        </is>
-      </c>
-      <c r="C1677" t="n">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="1678">
-      <c r="A1678" s="1" t="n">
-        <v>1676</v>
-      </c>
-      <c r="B1678" t="inlineStr">
-        <is>
-          <t>241</t>
-        </is>
-      </c>
-      <c r="C1678" t="n">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="1679">
-      <c r="A1679" s="1" t="n">
-        <v>1677</v>
-      </c>
-      <c r="B1679" t="inlineStr">
-        <is>
-          <t>247</t>
-        </is>
-      </c>
-      <c r="C1679" t="n">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="1680">
-      <c r="A1680" s="1" t="n">
-        <v>1678</v>
-      </c>
-      <c r="B1680" t="inlineStr">
-        <is>
-          <t>581/2</t>
-        </is>
-      </c>
-      <c r="C1680" t="n">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="1681">
-      <c r="A1681" s="1" t="n">
-        <v>1679</v>
-      </c>
-      <c r="B1681" t="inlineStr">
-        <is>
-          <t>2841</t>
-        </is>
-      </c>
-      <c r="C1681" t="n">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="1682">
-      <c r="A1682" s="1" t="n">
-        <v>1680</v>
-      </c>
-      <c r="B1682" t="inlineStr">
-        <is>
-          <t>2468/1</t>
-        </is>
-      </c>
-      <c r="C1682" t="n">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="1683">
-      <c r="A1683" s="1" t="n">
-        <v>1681</v>
-      </c>
-      <c r="B1683" t="inlineStr">
-        <is>
-          <t>2468/2</t>
-        </is>
-      </c>
-      <c r="C1683" t="n">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="1684">
-      <c r="A1684" s="1" t="n">
-        <v>1682</v>
-      </c>
-      <c r="B1684" t="inlineStr">
-        <is>
-          <t>2471</t>
-        </is>
-      </c>
-      <c r="C1684" t="n">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="1685">
-      <c r="A1685" s="1" t="n">
-        <v>1683</v>
-      </c>
-      <c r="B1685" t="inlineStr">
-        <is>
-          <t>2472</t>
-        </is>
-      </c>
-      <c r="C1685" t="n">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="1686">
-      <c r="A1686" s="1" t="n">
-        <v>1684</v>
-      </c>
-      <c r="B1686" t="inlineStr">
-        <is>
-          <t>2561</t>
-        </is>
-      </c>
-      <c r="C1686" t="n">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="1687">
-      <c r="A1687" s="1" t="n">
-        <v>1685</v>
-      </c>
-      <c r="B1687" t="inlineStr">
-        <is>
-          <t>3585</t>
-        </is>
-      </c>
-      <c r="C1687" t="n">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="1688">
-      <c r="A1688" s="1" t="n">
-        <v>1686</v>
-      </c>
-      <c r="B1688" t="inlineStr">
-        <is>
-          <t>3586</t>
-        </is>
-      </c>
-      <c r="C1688" t="n">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="1689">
-      <c r="A1689" s="1" t="n">
-        <v>1687</v>
-      </c>
-      <c r="B1689" t="inlineStr">
-        <is>
-          <t>3587</t>
-        </is>
-      </c>
-      <c r="C1689" t="n">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="1690">
-      <c r="A1690" s="1" t="n">
-        <v>1688</v>
-      </c>
-      <c r="B1690" t="inlineStr">
-        <is>
-          <t>3115/18</t>
-        </is>
-      </c>
-      <c r="C1690" t="n">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="1691">
-      <c r="A1691" s="1" t="n">
-        <v>1689</v>
-      </c>
-      <c r="B1691" t="inlineStr">
-        <is>
-          <t>3115/21</t>
-        </is>
-      </c>
-      <c r="C1691" t="n">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="1692">
-      <c r="A1692" s="1" t="n">
-        <v>1690</v>
-      </c>
-      <c r="B1692" t="inlineStr">
-        <is>
-          <t>3148/4</t>
-        </is>
-      </c>
-      <c r="C1692" t="n">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="1693">
-      <c r="A1693" s="1" t="n">
-        <v>1691</v>
-      </c>
-      <c r="B1693" t="inlineStr">
-        <is>
-          <t>3148/8</t>
-        </is>
-      </c>
-      <c r="C1693" t="n">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="1694">
-      <c r="A1694" s="1" t="n">
-        <v>1692</v>
-      </c>
-      <c r="B1694" t="inlineStr">
-        <is>
-          <t>759</t>
-        </is>
-      </c>
-      <c r="C1694" t="n">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="1695">
-      <c r="A1695" s="1" t="n">
-        <v>1693</v>
-      </c>
-      <c r="B1695" t="inlineStr">
-        <is>
-          <t>1408</t>
-        </is>
-      </c>
-      <c r="C1695" t="n">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="1696">
-      <c r="A1696" s="1" t="n">
-        <v>1694</v>
-      </c>
-      <c r="B1696" t="inlineStr">
-        <is>
-          <t>1411</t>
-        </is>
-      </c>
-      <c r="C1696" t="n">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="1697">
-      <c r="A1697" s="1" t="n">
-        <v>1695</v>
-      </c>
-      <c r="B1697" t="inlineStr">
-        <is>
-          <t>1413</t>
-        </is>
-      </c>
-      <c r="C1697" t="n">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="1698">
-      <c r="A1698" s="1" t="n">
-        <v>1696</v>
-      </c>
-      <c r="B1698" t="inlineStr">
-        <is>
-          <t>1419</t>
-        </is>
-      </c>
-      <c r="C1698" t="n">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="1699">
-      <c r="A1699" s="1" t="n">
-        <v>1697</v>
-      </c>
-      <c r="B1699" t="inlineStr">
-        <is>
-          <t>1420</t>
-        </is>
-      </c>
-      <c r="C1699" t="n">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="1700">
-      <c r="A1700" s="1" t="n">
-        <v>1698</v>
-      </c>
-      <c r="B1700" t="inlineStr">
-        <is>
-          <t>1421</t>
-        </is>
-      </c>
-      <c r="C1700" t="n">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="1701">
-      <c r="A1701" s="1" t="n">
-        <v>1699</v>
-      </c>
-      <c r="B1701" t="inlineStr">
-        <is>
-          <t>1499</t>
-        </is>
-      </c>
-      <c r="C1701" t="n">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="1702">
-      <c r="A1702" s="1" t="n">
-        <v>1700</v>
-      </c>
-      <c r="B1702" t="inlineStr">
-        <is>
-          <t>1502</t>
-        </is>
-      </c>
-      <c r="C1702" t="n">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="1703">
-      <c r="A1703" s="1" t="n">
-        <v>1701</v>
-      </c>
-      <c r="B1703" t="inlineStr">
-        <is>
-          <t>1348/2</t>
-        </is>
-      </c>
-      <c r="C1703" t="n">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="1704">
-      <c r="A1704" s="1" t="n">
-        <v>1702</v>
-      </c>
-      <c r="B1704" t="inlineStr">
-        <is>
-          <t>4189</t>
-        </is>
-      </c>
-      <c r="C1704" t="n">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="1705">
-      <c r="A1705" s="1" t="n">
-        <v>1703</v>
-      </c>
-      <c r="B1705" t="inlineStr">
-        <is>
-          <t>1113</t>
-        </is>
-      </c>
-      <c r="C1705" t="n">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="1706">
-      <c r="A1706" s="1" t="n">
-        <v>1704</v>
-      </c>
-      <c r="B1706" t="inlineStr">
-        <is>
-          <t>2052</t>
-        </is>
-      </c>
-      <c r="C1706" t="n">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="1707">
-      <c r="A1707" s="1" t="n">
-        <v>1705</v>
-      </c>
-      <c r="B1707" t="inlineStr">
+      <c r="B1510" t="inlineStr">
         <is>
           <t>2161</t>
         </is>
       </c>
-      <c r="C1707" t="n">
+      <c r="C1510" t="n">
         <v>440</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Latest data: Fri Jan  3 16:18:20 UTC 2025
</commit_message>
<xml_diff>
--- a/docs/particelle_non_trovate.xlsx
+++ b/docs/particelle_non_trovate.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -796,6 +796,19 @@
         <v>140</v>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>.7.</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>187</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Latest data: Mon Jan  6 12:26:31 UTC 2025
</commit_message>
<xml_diff>
--- a/docs/particelle_non_trovate.xlsx
+++ b/docs/particelle_non_trovate.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -809,6 +809,32 @@
         <v>187</v>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>2727/1</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>.256</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>231</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Latest data: Mon Jan  6 16:18:43 UTC 2025
</commit_message>
<xml_diff>
--- a/docs/particelle_non_trovate.xlsx
+++ b/docs/particelle_non_trovate.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -835,6 +835,84 @@
         <v>231</v>
       </c>
     </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>47/3</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>302/1</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>2129/1</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>2129/2</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>2129/3</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>2103/7</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>394</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Latest data: Mon Jan  6 20:19:27 UTC 2025
</commit_message>
<xml_diff>
--- a/docs/particelle_non_trovate.xlsx
+++ b/docs/particelle_non_trovate.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -913,6 +913,409 @@
         <v>394</v>
       </c>
     </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>673/2</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>.372</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>.373</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>.374</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>673/2</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>406/3</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>605</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>657/1</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>674</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>765/3</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>938</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>996</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>2074</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>2050</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>2065</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>2066</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>2153</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>2154</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>1419</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>1420</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>1421</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>1430</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>1431/1</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>1431/34</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>.950/1</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>.950/2</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>239</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>241</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>773</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>.4046</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>.4047</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>307</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Latest data: Thu Feb  6 20:19:32 UTC 2025
</commit_message>
<xml_diff>
--- a/docs/particelle_non_trovate.xlsx
+++ b/docs/particelle_non_trovate.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C62"/>
+  <dimension ref="A1:C65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1238,6 +1238,45 @@
         <v>307</v>
       </c>
     </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>1133</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>1585/60</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>1064/3</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>248</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Latest data: Sun Mar 23 16:18:24 UTC 2025
</commit_message>
<xml_diff>
--- a/docs/particelle_non_trovate.xlsx
+++ b/docs/particelle_non_trovate.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C65"/>
+  <dimension ref="A1:C66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -555,11 +555,11 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>4523</t>
+          <t>3298</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>404</v>
+        <v>257</v>
       </c>
     </row>
     <row r="11">
@@ -568,11 +568,11 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>.451</t>
+          <t>4523</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>88</v>
+        <v>404</v>
       </c>
     </row>
     <row r="12">
@@ -581,11 +581,11 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>703</t>
+          <t>.451</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>61</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13">
@@ -594,11 +594,11 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>3597/16</t>
+          <t>703</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>9</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14">
@@ -607,7 +607,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>3597/18</t>
+          <t>3597/16</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -620,7 +620,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>3597/22</t>
+          <t>3597/18</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -633,7 +633,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>3697</t>
+          <t>3597/22</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -646,11 +646,11 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>324337</t>
+          <t>3697</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>258</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18">
@@ -659,7 +659,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>655248</t>
+          <t>324337</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -672,7 +672,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2331/38</t>
+          <t>655248</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -685,11 +685,11 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2068/43</t>
+          <t>2331/38</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>310</v>
+        <v>258</v>
       </c>
     </row>
     <row r="21">
@@ -698,7 +698,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2822/12</t>
+          <t>2068/43</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -711,7 +711,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2822/16</t>
+          <t>2822/12</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -724,7 +724,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2020/14</t>
+          <t>2822/16</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -737,11 +737,11 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>.384</t>
+          <t>2020/14</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>139</v>
+        <v>310</v>
       </c>
     </row>
     <row r="25">
@@ -750,11 +750,11 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>4052</t>
+          <t>.384</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>9</v>
+        <v>139</v>
       </c>
     </row>
     <row r="26">
@@ -763,11 +763,11 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>.1512</t>
+          <t>4052</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>140</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27">
@@ -776,11 +776,11 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>.7.</t>
+          <t>.1512</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>187</v>
+        <v>140</v>
       </c>
     </row>
     <row r="28">
@@ -789,11 +789,11 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2727/1</t>
+          <t>.7.</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="29">
@@ -802,11 +802,11 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>47/3</t>
+          <t>2727/1</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>277</v>
+        <v>189</v>
       </c>
     </row>
     <row r="30">
@@ -815,7 +815,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>302/1</t>
+          <t>47/3</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -828,11 +828,11 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2103/7</t>
+          <t>302/1</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>394</v>
+        <v>277</v>
       </c>
     </row>
     <row r="32">
@@ -841,11 +841,11 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>673/2</t>
+          <t>2103/7</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>384</v>
+        <v>394</v>
       </c>
     </row>
     <row r="33">
@@ -854,7 +854,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>.372</t>
+          <t>673/2</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -867,7 +867,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>.373</t>
+          <t>.372</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -880,7 +880,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>.374</t>
+          <t>.373</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -893,7 +893,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>673/2</t>
+          <t>.374</t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -906,7 +906,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>406/3</t>
+          <t>673/2</t>
         </is>
       </c>
       <c r="C37" t="n">
@@ -919,7 +919,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>605</t>
+          <t>406/3</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -932,7 +932,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>657/1</t>
+          <t>605</t>
         </is>
       </c>
       <c r="C39" t="n">
@@ -945,7 +945,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>674</t>
+          <t>657/1</t>
         </is>
       </c>
       <c r="C40" t="n">
@@ -958,7 +958,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>765/3</t>
+          <t>674</t>
         </is>
       </c>
       <c r="C41" t="n">
@@ -971,7 +971,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>938</t>
+          <t>765/3</t>
         </is>
       </c>
       <c r="C42" t="n">
@@ -984,7 +984,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>996</t>
+          <t>938</t>
         </is>
       </c>
       <c r="C43" t="n">
@@ -997,7 +997,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>2074</t>
+          <t>996</t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -1010,7 +1010,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>2050</t>
+          <t>2074</t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -1023,7 +1023,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>2065</t>
+          <t>2050</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -1036,7 +1036,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>2066</t>
+          <t>2065</t>
         </is>
       </c>
       <c r="C47" t="n">
@@ -1049,7 +1049,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>2153</t>
+          <t>2066</t>
         </is>
       </c>
       <c r="C48" t="n">
@@ -1062,7 +1062,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>2154</t>
+          <t>2153</t>
         </is>
       </c>
       <c r="C49" t="n">
@@ -1075,11 +1075,11 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>1419</t>
+          <t>2154</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>287</v>
+        <v>384</v>
       </c>
     </row>
     <row r="51">
@@ -1088,7 +1088,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>1420</t>
+          <t>1419</t>
         </is>
       </c>
       <c r="C51" t="n">
@@ -1101,7 +1101,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>1421</t>
+          <t>1420</t>
         </is>
       </c>
       <c r="C52" t="n">
@@ -1114,7 +1114,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>1430</t>
+          <t>1421</t>
         </is>
       </c>
       <c r="C53" t="n">
@@ -1127,7 +1127,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>1431/1</t>
+          <t>1430</t>
         </is>
       </c>
       <c r="C54" t="n">
@@ -1140,7 +1140,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>1431/34</t>
+          <t>1431/1</t>
         </is>
       </c>
       <c r="C55" t="n">
@@ -1153,7 +1153,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>.950/1</t>
+          <t>1431/34</t>
         </is>
       </c>
       <c r="C56" t="n">
@@ -1166,7 +1166,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>.950/2</t>
+          <t>.950/1</t>
         </is>
       </c>
       <c r="C57" t="n">
@@ -1179,7 +1179,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>239</t>
+          <t>.950/2</t>
         </is>
       </c>
       <c r="C58" t="n">
@@ -1192,7 +1192,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>241</t>
+          <t>239</t>
         </is>
       </c>
       <c r="C59" t="n">
@@ -1205,11 +1205,11 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>773</t>
+          <t>241</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>441</v>
+        <v>287</v>
       </c>
     </row>
     <row r="61">
@@ -1218,11 +1218,11 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>.4046</t>
+          <t>773</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>307</v>
+        <v>441</v>
       </c>
     </row>
     <row r="62">
@@ -1231,7 +1231,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>.4047</t>
+          <t>.4046</t>
         </is>
       </c>
       <c r="C62" t="n">
@@ -1244,11 +1244,11 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>1133</t>
+          <t>.4047</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>248</v>
+        <v>307</v>
       </c>
     </row>
     <row r="64">
@@ -1257,7 +1257,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>1585/60</t>
+          <t>1133</t>
         </is>
       </c>
       <c r="C64" t="n">
@@ -1270,10 +1270,23 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
+          <t>1585/60</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
           <t>1064/3</t>
         </is>
       </c>
-      <c r="C65" t="n">
+      <c r="C66" t="n">
         <v>248</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Latest data: Mon Jun  9 14:36:21 UTC 2025
</commit_message>
<xml_diff>
--- a/docs/particelle_non_trovate.xlsx
+++ b/docs/particelle_non_trovate.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Latest data: Sun Jul  6 19:07:39 UTC 2025
</commit_message>
<xml_diff>
--- a/docs/particelle_non_trovate.xlsx
+++ b/docs/particelle_non_trovate.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C66"/>
+  <dimension ref="A1:C67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -776,7 +776,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>.1512</t>
+          <t>766</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -789,11 +789,11 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>.7.</t>
+          <t>.1512</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>187</v>
+        <v>140</v>
       </c>
     </row>
     <row r="29">
@@ -802,11 +802,11 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2727/1</t>
+          <t>.7.</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="30">
@@ -815,11 +815,11 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>47/3</t>
+          <t>2727/1</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>277</v>
+        <v>189</v>
       </c>
     </row>
     <row r="31">
@@ -828,7 +828,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>302/1</t>
+          <t>47/3</t>
         </is>
       </c>
       <c r="C31" t="n">
@@ -841,11 +841,11 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2103/7</t>
+          <t>302/1</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>394</v>
+        <v>277</v>
       </c>
     </row>
     <row r="33">
@@ -854,11 +854,11 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>673/2</t>
+          <t>2103/7</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>384</v>
+        <v>394</v>
       </c>
     </row>
     <row r="34">
@@ -867,7 +867,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>.372</t>
+          <t>673/2</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -880,7 +880,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>.373</t>
+          <t>.372</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -893,7 +893,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>.374</t>
+          <t>.373</t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -906,7 +906,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>673/2</t>
+          <t>.374</t>
         </is>
       </c>
       <c r="C37" t="n">
@@ -919,7 +919,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>406/3</t>
+          <t>673/2</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -932,7 +932,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>605</t>
+          <t>406/3</t>
         </is>
       </c>
       <c r="C39" t="n">
@@ -945,7 +945,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>657/1</t>
+          <t>605</t>
         </is>
       </c>
       <c r="C40" t="n">
@@ -958,7 +958,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>674</t>
+          <t>657/1</t>
         </is>
       </c>
       <c r="C41" t="n">
@@ -971,7 +971,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>765/3</t>
+          <t>674</t>
         </is>
       </c>
       <c r="C42" t="n">
@@ -984,7 +984,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>938</t>
+          <t>765/3</t>
         </is>
       </c>
       <c r="C43" t="n">
@@ -997,7 +997,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>996</t>
+          <t>938</t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -1010,7 +1010,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>2074</t>
+          <t>996</t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -1023,7 +1023,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>2050</t>
+          <t>2074</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -1036,7 +1036,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>2065</t>
+          <t>2050</t>
         </is>
       </c>
       <c r="C47" t="n">
@@ -1049,7 +1049,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>2066</t>
+          <t>2065</t>
         </is>
       </c>
       <c r="C48" t="n">
@@ -1062,7 +1062,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>2153</t>
+          <t>2066</t>
         </is>
       </c>
       <c r="C49" t="n">
@@ -1075,7 +1075,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>2154</t>
+          <t>2153</t>
         </is>
       </c>
       <c r="C50" t="n">
@@ -1088,11 +1088,11 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>1419</t>
+          <t>2154</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>287</v>
+        <v>384</v>
       </c>
     </row>
     <row r="52">
@@ -1101,7 +1101,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>1420</t>
+          <t>1419</t>
         </is>
       </c>
       <c r="C52" t="n">
@@ -1114,7 +1114,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>1421</t>
+          <t>1420</t>
         </is>
       </c>
       <c r="C53" t="n">
@@ -1127,7 +1127,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>1430</t>
+          <t>1421</t>
         </is>
       </c>
       <c r="C54" t="n">
@@ -1140,7 +1140,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>1431/1</t>
+          <t>1430</t>
         </is>
       </c>
       <c r="C55" t="n">
@@ -1153,7 +1153,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>1431/34</t>
+          <t>1431/1</t>
         </is>
       </c>
       <c r="C56" t="n">
@@ -1166,7 +1166,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>.950/1</t>
+          <t>1431/34</t>
         </is>
       </c>
       <c r="C57" t="n">
@@ -1179,7 +1179,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>.950/2</t>
+          <t>.950/1</t>
         </is>
       </c>
       <c r="C58" t="n">
@@ -1192,7 +1192,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>239</t>
+          <t>.950/2</t>
         </is>
       </c>
       <c r="C59" t="n">
@@ -1205,7 +1205,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>241</t>
+          <t>239</t>
         </is>
       </c>
       <c r="C60" t="n">
@@ -1218,11 +1218,11 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>773</t>
+          <t>241</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>441</v>
+        <v>287</v>
       </c>
     </row>
     <row r="62">
@@ -1231,11 +1231,11 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>.4046</t>
+          <t>773</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>307</v>
+        <v>441</v>
       </c>
     </row>
     <row r="63">
@@ -1244,7 +1244,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>.4047</t>
+          <t>.4046</t>
         </is>
       </c>
       <c r="C63" t="n">
@@ -1257,11 +1257,11 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>1133</t>
+          <t>.4047</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>248</v>
+        <v>307</v>
       </c>
     </row>
     <row r="65">
@@ -1270,7 +1270,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>1585/60</t>
+          <t>1133</t>
         </is>
       </c>
       <c r="C65" t="n">
@@ -1283,10 +1283,23 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
+          <t>1585/60</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
           <t>1064/3</t>
         </is>
       </c>
-      <c r="C66" t="n">
+      <c r="C67" t="n">
         <v>248</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Latest data: Thu Aug 28 20:22:17 UTC 2025
</commit_message>
<xml_diff>
--- a/docs/particelle_non_trovate.xlsx
+++ b/docs/particelle_non_trovate.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C67"/>
+  <dimension ref="A1:C117"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -594,11 +594,11 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>703</t>
+          <t>240</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>61</v>
+        <v>362</v>
       </c>
     </row>
     <row r="14">
@@ -607,11 +607,11 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>3597/16</t>
+          <t>269/1</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>9</v>
+        <v>362</v>
       </c>
     </row>
     <row r="15">
@@ -620,11 +620,11 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>3597/18</t>
+          <t>269/22</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>9</v>
+        <v>362</v>
       </c>
     </row>
     <row r="16">
@@ -633,11 +633,11 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>3597/22</t>
+          <t>270/5</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>9</v>
+        <v>362</v>
       </c>
     </row>
     <row r="17">
@@ -646,11 +646,11 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>3697</t>
+          <t>279</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>9</v>
+        <v>362</v>
       </c>
     </row>
     <row r="18">
@@ -659,11 +659,11 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>324337</t>
+          <t>288</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>258</v>
+        <v>362</v>
       </c>
     </row>
     <row r="19">
@@ -672,11 +672,11 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>655248</t>
+          <t>333/1</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>258</v>
+        <v>362</v>
       </c>
     </row>
     <row r="20">
@@ -685,11 +685,11 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2331/38</t>
+          <t>333/2</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>258</v>
+        <v>362</v>
       </c>
     </row>
     <row r="21">
@@ -698,11 +698,11 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2068/43</t>
+          <t>333/3</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>310</v>
+        <v>362</v>
       </c>
     </row>
     <row r="22">
@@ -711,11 +711,11 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2822/12</t>
+          <t>409</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>310</v>
+        <v>362</v>
       </c>
     </row>
     <row r="23">
@@ -724,11 +724,11 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2822/16</t>
+          <t>812/1</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>310</v>
+        <v>362</v>
       </c>
     </row>
     <row r="24">
@@ -737,11 +737,11 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2020/14</t>
+          <t>856/1</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>310</v>
+        <v>362</v>
       </c>
     </row>
     <row r="25">
@@ -750,11 +750,11 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>.384</t>
+          <t>862</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>139</v>
+        <v>362</v>
       </c>
     </row>
     <row r="26">
@@ -763,11 +763,11 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>4052</t>
+          <t>863</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>9</v>
+        <v>362</v>
       </c>
     </row>
     <row r="27">
@@ -776,11 +776,11 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>766</t>
+          <t>864/1</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>140</v>
+        <v>362</v>
       </c>
     </row>
     <row r="28">
@@ -789,11 +789,11 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>.1512</t>
+          <t>864/2</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>140</v>
+        <v>362</v>
       </c>
     </row>
     <row r="29">
@@ -802,11 +802,11 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>.7.</t>
+          <t>1029</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>187</v>
+        <v>362</v>
       </c>
     </row>
     <row r="30">
@@ -815,11 +815,11 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>2727/1</t>
+          <t>1254</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>189</v>
+        <v>362</v>
       </c>
     </row>
     <row r="31">
@@ -828,11 +828,11 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>47/3</t>
+          <t>1256/3</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>277</v>
+        <v>362</v>
       </c>
     </row>
     <row r="32">
@@ -841,11 +841,11 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>302/1</t>
+          <t>1256/4</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>277</v>
+        <v>362</v>
       </c>
     </row>
     <row r="33">
@@ -854,11 +854,11 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>2103/7</t>
+          <t>1305</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>394</v>
+        <v>362</v>
       </c>
     </row>
     <row r="34">
@@ -867,11 +867,11 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>673/2</t>
+          <t>1343</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>384</v>
+        <v>362</v>
       </c>
     </row>
     <row r="35">
@@ -880,11 +880,11 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>.372</t>
+          <t>1344</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>384</v>
+        <v>362</v>
       </c>
     </row>
     <row r="36">
@@ -893,11 +893,11 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>.373</t>
+          <t>1345</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>384</v>
+        <v>362</v>
       </c>
     </row>
     <row r="37">
@@ -906,11 +906,11 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>.374</t>
+          <t>1346</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>384</v>
+        <v>362</v>
       </c>
     </row>
     <row r="38">
@@ -919,11 +919,11 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>673/2</t>
+          <t>1347/1</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>384</v>
+        <v>362</v>
       </c>
     </row>
     <row r="39">
@@ -932,11 +932,11 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>406/3</t>
+          <t>1347/2</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>384</v>
+        <v>362</v>
       </c>
     </row>
     <row r="40">
@@ -945,11 +945,11 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>605</t>
+          <t>1348</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>384</v>
+        <v>362</v>
       </c>
     </row>
     <row r="41">
@@ -958,11 +958,11 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>657/1</t>
+          <t>1383</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>384</v>
+        <v>362</v>
       </c>
     </row>
     <row r="42">
@@ -971,11 +971,11 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>674</t>
+          <t>1384</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>384</v>
+        <v>362</v>
       </c>
     </row>
     <row r="43">
@@ -984,11 +984,11 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>765/3</t>
+          <t>1830/1</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>384</v>
+        <v>362</v>
       </c>
     </row>
     <row r="44">
@@ -997,11 +997,11 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>938</t>
+          <t>1830/2</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>384</v>
+        <v>362</v>
       </c>
     </row>
     <row r="45">
@@ -1010,11 +1010,11 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>996</t>
+          <t>1830/6</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>384</v>
+        <v>362</v>
       </c>
     </row>
     <row r="46">
@@ -1023,11 +1023,11 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>2074</t>
+          <t>1830/13</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>384</v>
+        <v>362</v>
       </c>
     </row>
     <row r="47">
@@ -1036,11 +1036,11 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>2050</t>
+          <t>1830/14</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>384</v>
+        <v>362</v>
       </c>
     </row>
     <row r="48">
@@ -1049,11 +1049,11 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>2065</t>
+          <t>1830/18</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>384</v>
+        <v>362</v>
       </c>
     </row>
     <row r="49">
@@ -1062,11 +1062,11 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>2066</t>
+          <t>1830/25</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>384</v>
+        <v>362</v>
       </c>
     </row>
     <row r="50">
@@ -1075,11 +1075,11 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>2153</t>
+          <t>1830/32</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>384</v>
+        <v>362</v>
       </c>
     </row>
     <row r="51">
@@ -1088,11 +1088,11 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>2154</t>
+          <t>1830/34</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>384</v>
+        <v>362</v>
       </c>
     </row>
     <row r="52">
@@ -1101,11 +1101,11 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>1419</t>
+          <t>1830/35</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>287</v>
+        <v>362</v>
       </c>
     </row>
     <row r="53">
@@ -1114,11 +1114,11 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>1420</t>
+          <t>1831</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>287</v>
+        <v>362</v>
       </c>
     </row>
     <row r="54">
@@ -1127,11 +1127,11 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>1421</t>
+          <t>1832</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>287</v>
+        <v>362</v>
       </c>
     </row>
     <row r="55">
@@ -1140,11 +1140,11 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>1430</t>
+          <t>1833</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>287</v>
+        <v>362</v>
       </c>
     </row>
     <row r="56">
@@ -1153,11 +1153,11 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>1431/1</t>
+          <t>1834</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>287</v>
+        <v>362</v>
       </c>
     </row>
     <row r="57">
@@ -1166,11 +1166,11 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>1431/34</t>
+          <t>1836</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>287</v>
+        <v>362</v>
       </c>
     </row>
     <row r="58">
@@ -1179,11 +1179,11 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>.950/1</t>
+          <t>1838</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>287</v>
+        <v>362</v>
       </c>
     </row>
     <row r="59">
@@ -1192,11 +1192,11 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>.950/2</t>
+          <t>.158</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>287</v>
+        <v>362</v>
       </c>
     </row>
     <row r="60">
@@ -1205,11 +1205,11 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>239</t>
+          <t>.425</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>287</v>
+        <v>362</v>
       </c>
     </row>
     <row r="61">
@@ -1218,11 +1218,11 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>241</t>
+          <t>.436</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>287</v>
+        <v>362</v>
       </c>
     </row>
     <row r="62">
@@ -1231,11 +1231,11 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>773</t>
+          <t>.458</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>441</v>
+        <v>362</v>
       </c>
     </row>
     <row r="63">
@@ -1244,11 +1244,11 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>.4046</t>
+          <t>703</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>307</v>
+        <v>61</v>
       </c>
     </row>
     <row r="64">
@@ -1257,11 +1257,11 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>.4047</t>
+          <t>3597/16</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>307</v>
+        <v>9</v>
       </c>
     </row>
     <row r="65">
@@ -1270,11 +1270,11 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>1133</t>
+          <t>3597/18</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>248</v>
+        <v>9</v>
       </c>
     </row>
     <row r="66">
@@ -1283,11 +1283,11 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>1585/60</t>
+          <t>3597/22</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>248</v>
+        <v>9</v>
       </c>
     </row>
     <row r="67">
@@ -1296,10 +1296,660 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
+          <t>3697</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>324337</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>655248</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>2331/38</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>2068/43</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>2822/12</t>
+        </is>
+      </c>
+      <c r="C72" t="n">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>2822/16</t>
+        </is>
+      </c>
+      <c r="C73" t="n">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>2020/14</t>
+        </is>
+      </c>
+      <c r="C74" t="n">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>.384</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>4052</t>
+        </is>
+      </c>
+      <c r="C76" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>766</t>
+        </is>
+      </c>
+      <c r="C77" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>.1512</t>
+        </is>
+      </c>
+      <c r="C78" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>.7.</t>
+        </is>
+      </c>
+      <c r="C79" t="n">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>2727/1</t>
+        </is>
+      </c>
+      <c r="C80" t="n">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>47/3</t>
+        </is>
+      </c>
+      <c r="C81" t="n">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>302/1</t>
+        </is>
+      </c>
+      <c r="C82" t="n">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>2103/7</t>
+        </is>
+      </c>
+      <c r="C83" t="n">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>673/2</t>
+        </is>
+      </c>
+      <c r="C84" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>.372</t>
+        </is>
+      </c>
+      <c r="C85" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>.373</t>
+        </is>
+      </c>
+      <c r="C86" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>.374</t>
+        </is>
+      </c>
+      <c r="C87" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>673/2</t>
+        </is>
+      </c>
+      <c r="C88" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>406/3</t>
+        </is>
+      </c>
+      <c r="C89" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>605</t>
+        </is>
+      </c>
+      <c r="C90" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>657/1</t>
+        </is>
+      </c>
+      <c r="C91" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>674</t>
+        </is>
+      </c>
+      <c r="C92" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>765/3</t>
+        </is>
+      </c>
+      <c r="C93" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>938</t>
+        </is>
+      </c>
+      <c r="C94" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="n">
+        <v>93</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>996</t>
+        </is>
+      </c>
+      <c r="C95" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="n">
+        <v>94</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>2074</t>
+        </is>
+      </c>
+      <c r="C96" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>2050</t>
+        </is>
+      </c>
+      <c r="C97" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>2065</t>
+        </is>
+      </c>
+      <c r="C98" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>2066</t>
+        </is>
+      </c>
+      <c r="C99" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="n">
+        <v>98</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>2153</t>
+        </is>
+      </c>
+      <c r="C100" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>2154</t>
+        </is>
+      </c>
+      <c r="C101" t="n">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>1419</t>
+        </is>
+      </c>
+      <c r="C102" t="n">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>1420</t>
+        </is>
+      </c>
+      <c r="C103" t="n">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="n">
+        <v>102</v>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>1421</t>
+        </is>
+      </c>
+      <c r="C104" t="n">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="n">
+        <v>103</v>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>1430</t>
+        </is>
+      </c>
+      <c r="C105" t="n">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="n">
+        <v>104</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>1431/1</t>
+        </is>
+      </c>
+      <c r="C106" t="n">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="n">
+        <v>105</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>1431/34</t>
+        </is>
+      </c>
+      <c r="C107" t="n">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="n">
+        <v>106</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>.950/1</t>
+        </is>
+      </c>
+      <c r="C108" t="n">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="n">
+        <v>107</v>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>.950/2</t>
+        </is>
+      </c>
+      <c r="C109" t="n">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="n">
+        <v>108</v>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>239</t>
+        </is>
+      </c>
+      <c r="C110" t="n">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="n">
+        <v>109</v>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>241</t>
+        </is>
+      </c>
+      <c r="C111" t="n">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>773</t>
+        </is>
+      </c>
+      <c r="C112" t="n">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="n">
+        <v>111</v>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>.4046</t>
+        </is>
+      </c>
+      <c r="C113" t="n">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="n">
+        <v>112</v>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>.4047</t>
+        </is>
+      </c>
+      <c r="C114" t="n">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="n">
+        <v>113</v>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>1133</t>
+        </is>
+      </c>
+      <c r="C115" t="n">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="n">
+        <v>114</v>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>1585/60</t>
+        </is>
+      </c>
+      <c r="C116" t="n">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="n">
+        <v>115</v>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
           <t>1064/3</t>
         </is>
       </c>
-      <c r="C67" t="n">
+      <c r="C117" t="n">
         <v>248</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Latest data: Fri Aug 29 00:51:32 UTC 2025
</commit_message>
<xml_diff>
--- a/docs/particelle_non_trovate.xlsx
+++ b/docs/particelle_non_trovate.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C117"/>
+  <dimension ref="A1:C67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -594,11 +594,11 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>703</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>362</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14">
@@ -607,11 +607,11 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>269/1</t>
+          <t>3597/16</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>362</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15">
@@ -620,11 +620,11 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>269/22</t>
+          <t>3597/18</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>362</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16">
@@ -633,11 +633,11 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>270/5</t>
+          <t>3597/22</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>362</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17">
@@ -646,11 +646,11 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>279</t>
+          <t>3697</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>362</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18">
@@ -659,11 +659,11 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>288</t>
+          <t>324337</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>362</v>
+        <v>258</v>
       </c>
     </row>
     <row r="19">
@@ -672,11 +672,11 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>333/1</t>
+          <t>655248</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>362</v>
+        <v>258</v>
       </c>
     </row>
     <row r="20">
@@ -685,11 +685,11 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>333/2</t>
+          <t>2331/38</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>362</v>
+        <v>258</v>
       </c>
     </row>
     <row r="21">
@@ -698,11 +698,11 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>333/3</t>
+          <t>2068/43</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>362</v>
+        <v>310</v>
       </c>
     </row>
     <row r="22">
@@ -711,11 +711,11 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>409</t>
+          <t>2822/12</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>362</v>
+        <v>310</v>
       </c>
     </row>
     <row r="23">
@@ -724,11 +724,11 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>812/1</t>
+          <t>2822/16</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>362</v>
+        <v>310</v>
       </c>
     </row>
     <row r="24">
@@ -737,11 +737,11 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>856/1</t>
+          <t>2020/14</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>362</v>
+        <v>310</v>
       </c>
     </row>
     <row r="25">
@@ -750,11 +750,11 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>862</t>
+          <t>.384</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>362</v>
+        <v>139</v>
       </c>
     </row>
     <row r="26">
@@ -763,11 +763,11 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>863</t>
+          <t>4052</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>362</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27">
@@ -776,11 +776,11 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>864/1</t>
+          <t>766</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>362</v>
+        <v>140</v>
       </c>
     </row>
     <row r="28">
@@ -789,11 +789,11 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>864/2</t>
+          <t>.1512</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>362</v>
+        <v>140</v>
       </c>
     </row>
     <row r="29">
@@ -802,11 +802,11 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>1029</t>
+          <t>.7.</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>362</v>
+        <v>187</v>
       </c>
     </row>
     <row r="30">
@@ -815,11 +815,11 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>1254</t>
+          <t>2727/1</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>362</v>
+        <v>189</v>
       </c>
     </row>
     <row r="31">
@@ -828,11 +828,11 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>1256/3</t>
+          <t>47/3</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>362</v>
+        <v>277</v>
       </c>
     </row>
     <row r="32">
@@ -841,11 +841,11 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>1256/4</t>
+          <t>302/1</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>362</v>
+        <v>277</v>
       </c>
     </row>
     <row r="33">
@@ -854,11 +854,11 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>1305</t>
+          <t>2103/7</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>362</v>
+        <v>394</v>
       </c>
     </row>
     <row r="34">
@@ -867,11 +867,11 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>1343</t>
+          <t>673/2</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>362</v>
+        <v>384</v>
       </c>
     </row>
     <row r="35">
@@ -880,11 +880,11 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>1344</t>
+          <t>.372</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>362</v>
+        <v>384</v>
       </c>
     </row>
     <row r="36">
@@ -893,11 +893,11 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>1345</t>
+          <t>.373</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>362</v>
+        <v>384</v>
       </c>
     </row>
     <row r="37">
@@ -906,11 +906,11 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>1346</t>
+          <t>.374</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>362</v>
+        <v>384</v>
       </c>
     </row>
     <row r="38">
@@ -919,11 +919,11 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>1347/1</t>
+          <t>673/2</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>362</v>
+        <v>384</v>
       </c>
     </row>
     <row r="39">
@@ -932,11 +932,11 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>1347/2</t>
+          <t>406/3</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>362</v>
+        <v>384</v>
       </c>
     </row>
     <row r="40">
@@ -945,11 +945,11 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>1348</t>
+          <t>605</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>362</v>
+        <v>384</v>
       </c>
     </row>
     <row r="41">
@@ -958,11 +958,11 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>1383</t>
+          <t>657/1</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>362</v>
+        <v>384</v>
       </c>
     </row>
     <row r="42">
@@ -971,11 +971,11 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>1384</t>
+          <t>674</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>362</v>
+        <v>384</v>
       </c>
     </row>
     <row r="43">
@@ -984,11 +984,11 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>1830/1</t>
+          <t>765/3</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>362</v>
+        <v>384</v>
       </c>
     </row>
     <row r="44">
@@ -997,11 +997,11 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>1830/2</t>
+          <t>938</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>362</v>
+        <v>384</v>
       </c>
     </row>
     <row r="45">
@@ -1010,11 +1010,11 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>1830/6</t>
+          <t>996</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>362</v>
+        <v>384</v>
       </c>
     </row>
     <row r="46">
@@ -1023,11 +1023,11 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>1830/13</t>
+          <t>2074</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>362</v>
+        <v>384</v>
       </c>
     </row>
     <row r="47">
@@ -1036,11 +1036,11 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>1830/14</t>
+          <t>2050</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>362</v>
+        <v>384</v>
       </c>
     </row>
     <row r="48">
@@ -1049,11 +1049,11 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>1830/18</t>
+          <t>2065</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>362</v>
+        <v>384</v>
       </c>
     </row>
     <row r="49">
@@ -1062,11 +1062,11 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>1830/25</t>
+          <t>2066</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>362</v>
+        <v>384</v>
       </c>
     </row>
     <row r="50">
@@ -1075,11 +1075,11 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>1830/32</t>
+          <t>2153</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>362</v>
+        <v>384</v>
       </c>
     </row>
     <row r="51">
@@ -1088,11 +1088,11 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>1830/34</t>
+          <t>2154</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>362</v>
+        <v>384</v>
       </c>
     </row>
     <row r="52">
@@ -1101,11 +1101,11 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>1830/35</t>
+          <t>1419</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>362</v>
+        <v>287</v>
       </c>
     </row>
     <row r="53">
@@ -1114,11 +1114,11 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>1831</t>
+          <t>1420</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>362</v>
+        <v>287</v>
       </c>
     </row>
     <row r="54">
@@ -1127,11 +1127,11 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>1832</t>
+          <t>1421</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>362</v>
+        <v>287</v>
       </c>
     </row>
     <row r="55">
@@ -1140,11 +1140,11 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>1833</t>
+          <t>1430</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>362</v>
+        <v>287</v>
       </c>
     </row>
     <row r="56">
@@ -1153,11 +1153,11 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>1834</t>
+          <t>1431/1</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>362</v>
+        <v>287</v>
       </c>
     </row>
     <row r="57">
@@ -1166,11 +1166,11 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>1836</t>
+          <t>1431/34</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>362</v>
+        <v>287</v>
       </c>
     </row>
     <row r="58">
@@ -1179,11 +1179,11 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>1838</t>
+          <t>.950/1</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>362</v>
+        <v>287</v>
       </c>
     </row>
     <row r="59">
@@ -1192,11 +1192,11 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>.158</t>
+          <t>.950/2</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>362</v>
+        <v>287</v>
       </c>
     </row>
     <row r="60">
@@ -1205,11 +1205,11 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>.425</t>
+          <t>239</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>362</v>
+        <v>287</v>
       </c>
     </row>
     <row r="61">
@@ -1218,11 +1218,11 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>.436</t>
+          <t>241</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>362</v>
+        <v>287</v>
       </c>
     </row>
     <row r="62">
@@ -1231,11 +1231,11 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>.458</t>
+          <t>773</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>362</v>
+        <v>441</v>
       </c>
     </row>
     <row r="63">
@@ -1244,11 +1244,11 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>703</t>
+          <t>.4046</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>61</v>
+        <v>307</v>
       </c>
     </row>
     <row r="64">
@@ -1257,11 +1257,11 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>3597/16</t>
+          <t>.4047</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>9</v>
+        <v>307</v>
       </c>
     </row>
     <row r="65">
@@ -1270,11 +1270,11 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>3597/18</t>
+          <t>1133</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>9</v>
+        <v>248</v>
       </c>
     </row>
     <row r="66">
@@ -1283,11 +1283,11 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>3597/22</t>
+          <t>1585/60</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>9</v>
+        <v>248</v>
       </c>
     </row>
     <row r="67">
@@ -1296,660 +1296,10 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>3697</t>
+          <t>1064/3</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" s="1" t="n">
-        <v>66</v>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>324337</t>
-        </is>
-      </c>
-      <c r="C68" t="n">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" s="1" t="n">
-        <v>67</v>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>655248</t>
-        </is>
-      </c>
-      <c r="C69" t="n">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" s="1" t="n">
-        <v>68</v>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>2331/38</t>
-        </is>
-      </c>
-      <c r="C70" t="n">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" s="1" t="n">
-        <v>69</v>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>2068/43</t>
-        </is>
-      </c>
-      <c r="C71" t="n">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" s="1" t="n">
-        <v>70</v>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>2822/12</t>
-        </is>
-      </c>
-      <c r="C72" t="n">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" s="1" t="n">
-        <v>71</v>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>2822/16</t>
-        </is>
-      </c>
-      <c r="C73" t="n">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" s="1" t="n">
-        <v>72</v>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>2020/14</t>
-        </is>
-      </c>
-      <c r="C74" t="n">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" s="1" t="n">
-        <v>73</v>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>.384</t>
-        </is>
-      </c>
-      <c r="C75" t="n">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" s="1" t="n">
-        <v>74</v>
-      </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>4052</t>
-        </is>
-      </c>
-      <c r="C76" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>766</t>
-        </is>
-      </c>
-      <c r="C77" t="n">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" s="1" t="n">
-        <v>76</v>
-      </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>.1512</t>
-        </is>
-      </c>
-      <c r="C78" t="n">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" s="1" t="n">
-        <v>77</v>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>.7.</t>
-        </is>
-      </c>
-      <c r="C79" t="n">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" s="1" t="n">
-        <v>78</v>
-      </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>2727/1</t>
-        </is>
-      </c>
-      <c r="C80" t="n">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" s="1" t="n">
-        <v>79</v>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>47/3</t>
-        </is>
-      </c>
-      <c r="C81" t="n">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" s="1" t="n">
-        <v>80</v>
-      </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>302/1</t>
-        </is>
-      </c>
-      <c r="C82" t="n">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" s="1" t="n">
-        <v>81</v>
-      </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>2103/7</t>
-        </is>
-      </c>
-      <c r="C83" t="n">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" s="1" t="n">
-        <v>82</v>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>673/2</t>
-        </is>
-      </c>
-      <c r="C84" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" s="1" t="n">
-        <v>83</v>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>.372</t>
-        </is>
-      </c>
-      <c r="C85" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" s="1" t="n">
-        <v>84</v>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>.373</t>
-        </is>
-      </c>
-      <c r="C86" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" s="1" t="n">
-        <v>85</v>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>.374</t>
-        </is>
-      </c>
-      <c r="C87" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" s="1" t="n">
-        <v>86</v>
-      </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>673/2</t>
-        </is>
-      </c>
-      <c r="C88" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" s="1" t="n">
-        <v>87</v>
-      </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>406/3</t>
-        </is>
-      </c>
-      <c r="C89" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" s="1" t="n">
-        <v>88</v>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>605</t>
-        </is>
-      </c>
-      <c r="C90" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" s="1" t="n">
-        <v>89</v>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>657/1</t>
-        </is>
-      </c>
-      <c r="C91" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" s="1" t="n">
-        <v>90</v>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>674</t>
-        </is>
-      </c>
-      <c r="C92" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" s="1" t="n">
-        <v>91</v>
-      </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>765/3</t>
-        </is>
-      </c>
-      <c r="C93" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" s="1" t="n">
-        <v>92</v>
-      </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>938</t>
-        </is>
-      </c>
-      <c r="C94" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" s="1" t="n">
-        <v>93</v>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>996</t>
-        </is>
-      </c>
-      <c r="C95" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" s="1" t="n">
-        <v>94</v>
-      </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>2074</t>
-        </is>
-      </c>
-      <c r="C96" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" s="1" t="n">
-        <v>95</v>
-      </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>2050</t>
-        </is>
-      </c>
-      <c r="C97" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" s="1" t="n">
-        <v>96</v>
-      </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>2065</t>
-        </is>
-      </c>
-      <c r="C98" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" s="1" t="n">
-        <v>97</v>
-      </c>
-      <c r="B99" t="inlineStr">
-        <is>
-          <t>2066</t>
-        </is>
-      </c>
-      <c r="C99" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" s="1" t="n">
-        <v>98</v>
-      </c>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>2153</t>
-        </is>
-      </c>
-      <c r="C100" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" s="1" t="n">
-        <v>99</v>
-      </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>2154</t>
-        </is>
-      </c>
-      <c r="C101" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="B102" t="inlineStr">
-        <is>
-          <t>1419</t>
-        </is>
-      </c>
-      <c r="C102" t="n">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" s="1" t="n">
-        <v>101</v>
-      </c>
-      <c r="B103" t="inlineStr">
-        <is>
-          <t>1420</t>
-        </is>
-      </c>
-      <c r="C103" t="n">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" s="1" t="n">
-        <v>102</v>
-      </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>1421</t>
-        </is>
-      </c>
-      <c r="C104" t="n">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" s="1" t="n">
-        <v>103</v>
-      </c>
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>1430</t>
-        </is>
-      </c>
-      <c r="C105" t="n">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" s="1" t="n">
-        <v>104</v>
-      </c>
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>1431/1</t>
-        </is>
-      </c>
-      <c r="C106" t="n">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" s="1" t="n">
-        <v>105</v>
-      </c>
-      <c r="B107" t="inlineStr">
-        <is>
-          <t>1431/34</t>
-        </is>
-      </c>
-      <c r="C107" t="n">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" s="1" t="n">
-        <v>106</v>
-      </c>
-      <c r="B108" t="inlineStr">
-        <is>
-          <t>.950/1</t>
-        </is>
-      </c>
-      <c r="C108" t="n">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" s="1" t="n">
-        <v>107</v>
-      </c>
-      <c r="B109" t="inlineStr">
-        <is>
-          <t>.950/2</t>
-        </is>
-      </c>
-      <c r="C109" t="n">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" s="1" t="n">
-        <v>108</v>
-      </c>
-      <c r="B110" t="inlineStr">
-        <is>
-          <t>239</t>
-        </is>
-      </c>
-      <c r="C110" t="n">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" s="1" t="n">
-        <v>109</v>
-      </c>
-      <c r="B111" t="inlineStr">
-        <is>
-          <t>241</t>
-        </is>
-      </c>
-      <c r="C111" t="n">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" s="1" t="n">
-        <v>110</v>
-      </c>
-      <c r="B112" t="inlineStr">
-        <is>
-          <t>773</t>
-        </is>
-      </c>
-      <c r="C112" t="n">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" s="1" t="n">
-        <v>111</v>
-      </c>
-      <c r="B113" t="inlineStr">
-        <is>
-          <t>.4046</t>
-        </is>
-      </c>
-      <c r="C113" t="n">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" s="1" t="n">
-        <v>112</v>
-      </c>
-      <c r="B114" t="inlineStr">
-        <is>
-          <t>.4047</t>
-        </is>
-      </c>
-      <c r="C114" t="n">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" s="1" t="n">
-        <v>113</v>
-      </c>
-      <c r="B115" t="inlineStr">
-        <is>
-          <t>1133</t>
-        </is>
-      </c>
-      <c r="C115" t="n">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" s="1" t="n">
-        <v>114</v>
-      </c>
-      <c r="B116" t="inlineStr">
-        <is>
-          <t>1585/60</t>
-        </is>
-      </c>
-      <c r="C116" t="n">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" s="1" t="n">
-        <v>115</v>
-      </c>
-      <c r="B117" t="inlineStr">
-        <is>
-          <t>1064/3</t>
-        </is>
-      </c>
-      <c r="C117" t="n">
         <v>248</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Latest data: Tue Jan 20 12:34:36 UTC 2026
</commit_message>
<xml_diff>
--- a/docs/particelle_non_trovate.xlsx
+++ b/docs/particelle_non_trovate.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>